<commit_message>
Changed the servo rgulator PTH resistors to vertical mount 1/4W.
The resistance values required for the stock configuration are not available in a 1/6W PTH resistor, and mounting a 1/4W normally is not feasible for length reasons.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="363">
   <si>
     <t>Part</t>
   </si>
@@ -598,12 +598,6 @@
     <t>1.96K</t>
   </si>
   <si>
-    <t>RESISTORPTH-1/6W</t>
-  </si>
-  <si>
-    <t>1/6W-RES</t>
-  </si>
-  <si>
     <t>R38</t>
   </si>
   <si>
@@ -1082,6 +1076,33 @@
   </si>
   <si>
     <t>ERJ-3GEYJ2R2V</t>
+  </si>
+  <si>
+    <t>R-US_0207/5V</t>
+  </si>
+  <si>
+    <t>RNF14FTD1K96CT-ND</t>
+  </si>
+  <si>
+    <t>RNF14FTD1K96</t>
+  </si>
+  <si>
+    <t>RNF14FTD41K2CT-ND</t>
+  </si>
+  <si>
+    <t>RNF14FTD41K2</t>
+  </si>
+  <si>
+    <t>RNF14FTD66K5CT-ND</t>
+  </si>
+  <si>
+    <t>RNF14FTD66K5</t>
+  </si>
+  <si>
+    <t>RNF14FTD221KCT-ND</t>
+  </si>
+  <si>
+    <t>RNF14FTD221K</t>
   </si>
 </sst>
 </file>
@@ -1912,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,7 +2006,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J100)</f>
-        <v>155.09120000000001</v>
+        <v>155.69120000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2689,10 +2710,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G30" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3292,10 +3313,10 @@
         <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G50" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -3448,52 +3469,70 @@
         <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
       <c r="D55" t="s">
-        <v>195</v>
+        <v>131</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
+        <v>355</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>356</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
+      <c r="I55">
+        <v>0.15</v>
+      </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C56" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
       <c r="D56" t="s">
-        <v>195</v>
+        <v>131</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
+        <v>361</v>
       </c>
       <c r="G56" t="s">
-        <v>15</v>
+        <v>362</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
+      <c r="I56">
+        <v>0.15</v>
+      </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B57" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C57" t="s">
         <v>175</v>
@@ -3505,10 +3544,10 @@
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3523,7 +3562,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B58">
         <v>200</v>
@@ -3538,10 +3577,10 @@
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G58" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H58">
         <v>24</v>
@@ -3556,7 +3595,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B59">
         <v>100</v>
@@ -3571,10 +3610,10 @@
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G59" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H59">
         <v>10</v>
@@ -3589,10 +3628,10 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C60" t="s">
         <v>175</v>
@@ -3604,10 +3643,10 @@
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G60" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H60">
         <v>15</v>
@@ -3622,10 +3661,10 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B61" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C61" t="s">
         <v>175</v>
@@ -3637,10 +3676,10 @@
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G61" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H61">
         <v>6</v>
@@ -3655,10 +3694,10 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C62" t="s">
         <v>175</v>
@@ -3670,10 +3709,10 @@
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G62" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H62">
         <v>3</v>
@@ -3688,10 +3727,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C63" t="s">
         <v>175</v>
@@ -3703,10 +3742,10 @@
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G63" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H63">
         <v>4</v>
@@ -3721,10 +3760,10 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C64" t="s">
         <v>175</v>
@@ -3736,10 +3775,10 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -3754,10 +3793,10 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B65" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C65" t="s">
         <v>175</v>
@@ -3769,10 +3808,10 @@
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G65" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -3787,25 +3826,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B66">
         <v>0.3</v>
       </c>
       <c r="C66" t="s">
+        <v>231</v>
+      </c>
+      <c r="D66" t="s">
+        <v>232</v>
+      </c>
+      <c r="E66" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" t="s">
         <v>233</v>
       </c>
-      <c r="D66" t="s">
+      <c r="G66" t="s">
         <v>234</v>
-      </c>
-      <c r="E66" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" t="s">
-        <v>235</v>
-      </c>
-      <c r="G66" t="s">
-        <v>236</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -3820,10 +3859,10 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B67" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C67" t="s">
         <v>175</v>
@@ -3835,10 +3874,10 @@
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G67" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -3853,10 +3892,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B68" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C68" t="s">
         <v>175</v>
@@ -3868,10 +3907,10 @@
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G68" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -3886,10 +3925,10 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B69" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C69" t="s">
         <v>175</v>
@@ -3901,10 +3940,10 @@
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -3919,7 +3958,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
@@ -3946,10 +3985,10 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C71" t="s">
         <v>175</v>
@@ -3961,10 +4000,10 @@
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G71" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -3979,64 +4018,76 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B72" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C72" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
       <c r="D72" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="E72" t="s">
         <v>20</v>
       </c>
+      <c r="F72" t="s">
+        <v>357</v>
+      </c>
       <c r="G72" t="s">
-        <v>15</v>
+        <v>358</v>
       </c>
       <c r="H72">
         <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0.15</v>
       </c>
       <c r="J72">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B73" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
       <c r="D73" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
+      <c r="F73" t="s">
+        <v>359</v>
+      </c>
       <c r="G73" t="s">
-        <v>15</v>
+        <v>360</v>
       </c>
       <c r="H73">
         <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0.15</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B74" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C74" t="s">
         <v>175</v>
@@ -4048,10 +4099,10 @@
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G74" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4066,10 +4117,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B75" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C75" t="s">
         <v>175</v>
@@ -4081,10 +4132,10 @@
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G75" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4099,25 +4150,25 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>264</v>
+      </c>
+      <c r="B76" t="s">
+        <v>265</v>
+      </c>
+      <c r="C76" t="s">
+        <v>265</v>
+      </c>
+      <c r="D76" t="s">
         <v>266</v>
       </c>
-      <c r="B76" t="s">
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" t="s">
         <v>267</v>
       </c>
-      <c r="C76" t="s">
-        <v>267</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="G76" t="s">
         <v>268</v>
-      </c>
-      <c r="E76" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" t="s">
-        <v>269</v>
-      </c>
-      <c r="G76" t="s">
-        <v>270</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4132,25 +4183,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>269</v>
+      </c>
+      <c r="B77" t="s">
+        <v>270</v>
+      </c>
+      <c r="C77" t="s">
+        <v>270</v>
+      </c>
+      <c r="D77" t="s">
         <v>271</v>
       </c>
-      <c r="B77" t="s">
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
         <v>272</v>
       </c>
-      <c r="C77" t="s">
-        <v>272</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="G77" t="s">
         <v>273</v>
-      </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" t="s">
-        <v>274</v>
-      </c>
-      <c r="G77" t="s">
-        <v>275</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4165,25 +4216,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>274</v>
+      </c>
+      <c r="B78" t="s">
+        <v>275</v>
+      </c>
+      <c r="C78" t="s">
         <v>276</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>277</v>
       </c>
-      <c r="C78" t="s">
+      <c r="E78" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" t="s">
         <v>278</v>
       </c>
-      <c r="D78" t="s">
+      <c r="G78" t="s">
         <v>279</v>
-      </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="F78" t="s">
-        <v>280</v>
-      </c>
-      <c r="G78" t="s">
-        <v>281</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4198,25 +4249,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>280</v>
+      </c>
+      <c r="B79" t="s">
+        <v>281</v>
+      </c>
+      <c r="C79" t="s">
         <v>282</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>283</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" t="s">
         <v>284</v>
       </c>
-      <c r="D79" t="s">
+      <c r="G79" t="s">
         <v>285</v>
-      </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" t="s">
-        <v>286</v>
-      </c>
-      <c r="G79" t="s">
-        <v>287</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4231,25 +4282,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>286</v>
+      </c>
+      <c r="B80" t="s">
+        <v>287</v>
+      </c>
+      <c r="C80" t="s">
+        <v>287</v>
+      </c>
+      <c r="D80" t="s">
         <v>288</v>
       </c>
-      <c r="B80" t="s">
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" t="s">
         <v>289</v>
       </c>
-      <c r="C80" t="s">
-        <v>289</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="G80" t="s">
         <v>290</v>
-      </c>
-      <c r="E80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F80" t="s">
-        <v>291</v>
-      </c>
-      <c r="G80" t="s">
-        <v>292</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4264,25 +4315,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>291</v>
+      </c>
+      <c r="B81" t="s">
+        <v>292</v>
+      </c>
+      <c r="C81" t="s">
+        <v>292</v>
+      </c>
+      <c r="D81" t="s">
         <v>293</v>
       </c>
-      <c r="B81" t="s">
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" t="s">
         <v>294</v>
       </c>
-      <c r="C81" t="s">
-        <v>294</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="G81" t="s">
         <v>295</v>
-      </c>
-      <c r="E81" t="s">
-        <v>20</v>
-      </c>
-      <c r="F81" t="s">
-        <v>296</v>
-      </c>
-      <c r="G81" t="s">
-        <v>297</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4297,25 +4348,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>296</v>
+      </c>
+      <c r="B82" t="s">
+        <v>297</v>
+      </c>
+      <c r="C82" t="s">
+        <v>297</v>
+      </c>
+      <c r="D82" t="s">
         <v>298</v>
       </c>
-      <c r="B82" t="s">
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" t="s">
         <v>299</v>
       </c>
-      <c r="C82" t="s">
-        <v>299</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="G82" t="s">
         <v>300</v>
-      </c>
-      <c r="E82" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" t="s">
-        <v>301</v>
-      </c>
-      <c r="G82" t="s">
-        <v>302</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4330,25 +4381,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>301</v>
+      </c>
+      <c r="B83" t="s">
+        <v>302</v>
+      </c>
+      <c r="C83" t="s">
+        <v>302</v>
+      </c>
+      <c r="D83" t="s">
         <v>303</v>
       </c>
-      <c r="B83" t="s">
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" t="s">
         <v>304</v>
       </c>
-      <c r="C83" t="s">
-        <v>304</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="G83" t="s">
         <v>305</v>
-      </c>
-      <c r="E83" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" t="s">
-        <v>306</v>
-      </c>
-      <c r="G83" t="s">
-        <v>307</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4363,25 +4414,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>306</v>
+      </c>
+      <c r="B84" t="s">
+        <v>307</v>
+      </c>
+      <c r="C84" t="s">
+        <v>307</v>
+      </c>
+      <c r="D84" t="s">
         <v>308</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" t="s">
         <v>309</v>
       </c>
-      <c r="C84" t="s">
-        <v>309</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="G84" t="s">
         <v>310</v>
-      </c>
-      <c r="E84" t="s">
-        <v>20</v>
-      </c>
-      <c r="F84" t="s">
-        <v>311</v>
-      </c>
-      <c r="G84" t="s">
-        <v>312</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4396,16 +4447,16 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>311</v>
+      </c>
+      <c r="B85" t="s">
+        <v>312</v>
+      </c>
+      <c r="C85" t="s">
+        <v>312</v>
+      </c>
+      <c r="D85" t="s">
         <v>313</v>
-      </c>
-      <c r="B85" t="s">
-        <v>314</v>
-      </c>
-      <c r="C85" t="s">
-        <v>314</v>
-      </c>
-      <c r="D85" t="s">
-        <v>315</v>
       </c>
       <c r="G85" t="s">
         <v>15</v>
@@ -4418,30 +4469,30 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>315</v>
+      </c>
+      <c r="B86" t="s">
+        <v>316</v>
+      </c>
+      <c r="C86" t="s">
+        <v>316</v>
+      </c>
+      <c r="D86" t="s">
         <v>317</v>
       </c>
-      <c r="B86" t="s">
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" t="s">
         <v>318</v>
       </c>
-      <c r="C86" t="s">
-        <v>318</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
         <v>319</v>
-      </c>
-      <c r="E86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" t="s">
-        <v>320</v>
-      </c>
-      <c r="G86" t="s">
-        <v>321</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4456,25 +4507,25 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>320</v>
+      </c>
+      <c r="B87" t="s">
+        <v>321</v>
+      </c>
+      <c r="C87" t="s">
+        <v>321</v>
+      </c>
+      <c r="D87" t="s">
         <v>322</v>
       </c>
-      <c r="B87" t="s">
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" t="s">
         <v>323</v>
       </c>
-      <c r="C87" t="s">
-        <v>323</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>324</v>
-      </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>325</v>
-      </c>
-      <c r="G87" t="s">
-        <v>326</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4489,25 +4540,25 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>325</v>
+      </c>
+      <c r="B88" t="s">
+        <v>326</v>
+      </c>
+      <c r="C88" t="s">
+        <v>326</v>
+      </c>
+      <c r="D88" t="s">
         <v>327</v>
       </c>
-      <c r="B88" t="s">
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" t="s">
         <v>328</v>
       </c>
-      <c r="C88" t="s">
-        <v>328</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="G88" t="s">
         <v>329</v>
-      </c>
-      <c r="E88" t="s">
-        <v>20</v>
-      </c>
-      <c r="F88" t="s">
-        <v>330</v>
-      </c>
-      <c r="G88" t="s">
-        <v>331</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -4522,25 +4573,25 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>330</v>
+      </c>
+      <c r="B89" t="s">
+        <v>331</v>
+      </c>
+      <c r="C89" t="s">
+        <v>331</v>
+      </c>
+      <c r="D89" t="s">
         <v>332</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" t="s">
         <v>333</v>
       </c>
-      <c r="C89" t="s">
-        <v>333</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="G89" t="s">
         <v>334</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>335</v>
-      </c>
-      <c r="G89" t="s">
-        <v>336</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -4555,25 +4606,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>335</v>
+      </c>
+      <c r="B90" t="s">
+        <v>336</v>
+      </c>
+      <c r="C90" t="s">
+        <v>336</v>
+      </c>
+      <c r="D90" t="s">
         <v>337</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" t="s">
         <v>338</v>
       </c>
-      <c r="C90" t="s">
-        <v>338</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="F90" t="s">
         <v>339</v>
       </c>
-      <c r="E90" t="s">
+      <c r="G90" t="s">
         <v>340</v>
-      </c>
-      <c r="F90" t="s">
-        <v>341</v>
-      </c>
-      <c r="G90" t="s">
-        <v>342</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -4588,25 +4639,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>341</v>
+      </c>
+      <c r="B91" t="s">
+        <v>342</v>
+      </c>
+      <c r="C91" t="s">
+        <v>342</v>
+      </c>
+      <c r="D91" t="s">
         <v>343</v>
       </c>
-      <c r="B91" t="s">
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" t="s">
         <v>344</v>
       </c>
-      <c r="C91" t="s">
-        <v>344</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="G91" t="s">
         <v>345</v>
-      </c>
-      <c r="E91" t="s">
-        <v>20</v>
-      </c>
-      <c r="F91" t="s">
-        <v>346</v>
-      </c>
-      <c r="G91" t="s">
-        <v>347</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -4621,16 +4672,16 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>346</v>
+      </c>
+      <c r="B92" t="s">
+        <v>347</v>
+      </c>
+      <c r="C92" t="s">
         <v>348</v>
       </c>
-      <c r="B92" t="s">
+      <c r="D92" t="s">
         <v>349</v>
-      </c>
-      <c r="C92" t="s">
-        <v>350</v>
-      </c>
-      <c r="D92" t="s">
-        <v>351</v>
       </c>
       <c r="G92" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Duplicated 1x3 pin header DK PN and price for row 36.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="364">
   <si>
     <t>Part</t>
   </si>
@@ -1103,6 +1103,9 @@
   </si>
   <si>
     <t>RNF14FTD221K</t>
+  </si>
+  <si>
+    <t>Note: Redudndant line item</t>
   </si>
 </sst>
 </file>
@@ -1933,12 +1936,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
@@ -2006,7 +2010,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J100)</f>
-        <v>155.69120000000004</v>
+        <v>156.95120000000003</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2792,7 +2796,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2816,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2849,7 +2853,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -2873,7 +2877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -2886,15 +2890,30 @@
       <c r="D36" t="s">
         <v>110</v>
       </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" t="s">
+        <v>114</v>
+      </c>
       <c r="H36">
         <v>3</v>
       </c>
+      <c r="I36">
+        <v>0.42</v>
+      </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.26</v>
+      </c>
+      <c r="K36" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -2927,7 +2946,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -2960,7 +2979,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -2984,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -3017,7 +3036,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>128</v>
       </c>
@@ -3050,7 +3069,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>134</v>
       </c>
@@ -3083,7 +3102,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>140</v>
       </c>
@@ -3116,7 +3135,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -3140,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>149</v>
       </c>
@@ -3173,7 +3192,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>155</v>
       </c>
@@ -3206,7 +3225,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>160</v>
       </c>
@@ -3230,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
Updated rows 3 and 4 to higher voltage-rated parts.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -79,24 +79,12 @@
     <t>DK</t>
   </si>
   <si>
-    <t>490-1709-1-ND</t>
-  </si>
-  <si>
-    <t>GRM21BR61A106KE19L</t>
-  </si>
-  <si>
     <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56</t>
   </si>
   <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>490-1524-1-ND</t>
-  </si>
-  <si>
-    <t>GRM188R71E104KA01D</t>
-  </si>
-  <si>
     <t>C5, C6</t>
   </si>
   <si>
@@ -1124,6 +1112,18 @@
   </si>
   <si>
     <t>C1608X5R1E105K</t>
+  </si>
+  <si>
+    <t>490-5523-1-ND</t>
+  </si>
+  <si>
+    <t>GRM21BR61E106KA73L</t>
+  </si>
+  <si>
+    <t>311-1343-1-ND</t>
+  </si>
+  <si>
+    <t>CC0603ZRY5V9BB104</t>
   </si>
 </sst>
 </file>
@@ -1955,7 +1955,7 @@
   <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,10 +2020,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="G2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J100)</f>
-        <v>162.68120000000002</v>
+        <v>162.19720000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2057,28 +2057,28 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>366</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>367</v>
       </c>
       <c r="H3">
         <v>6</v>
       </c>
       <c r="I3">
-        <v>0.36</v>
+        <v>0.54</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J66" si="0">H3*I3</f>
-        <v>2.16</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -2090,28 +2090,28 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>368</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>369</v>
       </c>
       <c r="H4">
         <v>23</v>
       </c>
       <c r="I4">
-        <v>8.8999999999999996E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>2.0469999999999997</v>
+        <v>0.48300000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -2132,10 +2132,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -2156,10 +2156,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -2180,16 +2180,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -2204,16 +2204,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -2252,10 +2252,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2267,10 +2267,10 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -2333,10 +2333,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -2357,10 +2357,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -2381,16 +2381,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
         <v>15</v>
@@ -2405,16 +2405,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
@@ -2429,10 +2429,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -2453,16 +2453,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
@@ -2477,16 +2477,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
         <v>15</v>
@@ -2501,16 +2501,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G21" t="s">
         <v>15</v>
@@ -2525,16 +2525,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s">
         <v>15</v>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -2573,25 +2573,25 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H24">
         <v>26</v>
@@ -2606,25 +2606,25 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G25" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -2639,16 +2639,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G26" t="s">
         <v>15</v>
@@ -2663,16 +2663,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G27" t="s">
         <v>15</v>
@@ -2687,16 +2687,16 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G28" t="s">
         <v>15</v>
@@ -2711,16 +2711,16 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G29" t="s">
         <v>15</v>
@@ -2735,25 +2735,25 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G30" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -2768,25 +2768,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -2801,25 +2801,25 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -2834,16 +2834,16 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
         <v>15</v>
@@ -2858,25 +2858,25 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E34" t="s">
         <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -2891,25 +2891,25 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G35" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H35">
         <v>3</v>
@@ -2924,25 +2924,25 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
         <v>109</v>
       </c>
-      <c r="D36" t="s">
+      <c r="G36" t="s">
         <v>110</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
-        <v>113</v>
-      </c>
-      <c r="G36" t="s">
-        <v>114</v>
       </c>
       <c r="H36">
         <v>3</v>
@@ -2955,30 +2955,30 @@
         <v>1.26</v>
       </c>
       <c r="K36" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" t="s">
         <v>110</v>
-      </c>
-      <c r="E37" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" t="s">
-        <v>113</v>
-      </c>
-      <c r="G37" t="s">
-        <v>114</v>
       </c>
       <c r="H37">
         <v>10</v>
@@ -2993,25 +2993,25 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -3026,16 +3026,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G39" t="s">
         <v>15</v>
@@ -3050,25 +3050,25 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="s">
         <v>122</v>
       </c>
-      <c r="B40" t="s">
+      <c r="G40" t="s">
         <v>123</v>
-      </c>
-      <c r="C40" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" t="s">
-        <v>126</v>
-      </c>
-      <c r="G40" t="s">
-        <v>127</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -3083,25 +3083,25 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
         <v>128</v>
       </c>
-      <c r="B41" t="s">
+      <c r="G41" t="s">
         <v>129</v>
-      </c>
-      <c r="C41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" t="s">
-        <v>132</v>
-      </c>
-      <c r="G41" t="s">
-        <v>133</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -3116,25 +3116,25 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
         <v>134</v>
       </c>
-      <c r="B42" t="s">
+      <c r="G42" t="s">
         <v>135</v>
-      </c>
-      <c r="C42" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" t="s">
-        <v>137</v>
-      </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" t="s">
-        <v>139</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3149,25 +3149,25 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
         <v>140</v>
       </c>
-      <c r="B43" t="s">
+      <c r="G43" t="s">
         <v>141</v>
-      </c>
-      <c r="C43" t="s">
-        <v>142</v>
-      </c>
-      <c r="D43" t="s">
-        <v>143</v>
-      </c>
-      <c r="E43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" t="s">
-        <v>144</v>
-      </c>
-      <c r="G43" t="s">
-        <v>145</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3182,16 +3182,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G44" t="s">
         <v>15</v>
@@ -3206,25 +3206,25 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
         <v>149</v>
       </c>
-      <c r="B45" t="s">
+      <c r="G45" t="s">
         <v>150</v>
-      </c>
-      <c r="C45" t="s">
-        <v>151</v>
-      </c>
-      <c r="D45" t="s">
-        <v>152</v>
-      </c>
-      <c r="E45" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" t="s">
-        <v>153</v>
-      </c>
-      <c r="G45" t="s">
-        <v>154</v>
       </c>
       <c r="H45">
         <v>25</v>
@@ -3239,13 +3239,13 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -3254,10 +3254,10 @@
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G46" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H46">
         <v>2</v>
@@ -3272,16 +3272,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D47" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G47" t="s">
         <v>15</v>
@@ -3296,25 +3296,25 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B48" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G48" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -3329,25 +3329,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>167</v>
+      </c>
+      <c r="G49" t="s">
         <v>168</v>
-      </c>
-      <c r="B49" t="s">
-        <v>169</v>
-      </c>
-      <c r="C49" t="s">
-        <v>170</v>
-      </c>
-      <c r="D49" t="s">
-        <v>152</v>
-      </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" t="s">
-        <v>171</v>
-      </c>
-      <c r="G49" t="s">
-        <v>172</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -3362,25 +3362,25 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G50" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -3395,25 +3395,25 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C51" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" t="s">
         <v>175</v>
       </c>
-      <c r="D51" t="s">
+      <c r="G51" t="s">
         <v>176</v>
-      </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" t="s">
-        <v>179</v>
-      </c>
-      <c r="G51" t="s">
-        <v>180</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -3428,25 +3428,25 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B52">
         <v>470</v>
       </c>
       <c r="C52" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G52" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3461,25 +3461,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B53" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G53" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H53">
         <v>59</v>
@@ -3494,25 +3494,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B54" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C54" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G54" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H54">
         <v>4</v>
@@ -3527,25 +3527,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B55" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C55" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G55" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3560,25 +3560,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D56" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E56" t="s">
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G56" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3593,25 +3593,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B57" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C57" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G57" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3626,25 +3626,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B58">
         <v>200</v>
       </c>
       <c r="C58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G58" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H58">
         <v>24</v>
@@ -3659,25 +3659,25 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B59">
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G59" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H59">
         <v>10</v>
@@ -3692,25 +3692,25 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B60" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C60" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G60" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H60">
         <v>15</v>
@@ -3725,25 +3725,25 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G61" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H61">
         <v>6</v>
@@ -3758,25 +3758,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B62" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C62" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D62" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G62" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H62">
         <v>3</v>
@@ -3791,25 +3791,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C63" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G63" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H63">
         <v>4</v>
@@ -3824,25 +3824,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B64" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C64" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E64" t="s">
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G64" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -3857,25 +3857,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C65" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G65" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -3890,25 +3890,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B66">
         <v>0.3</v>
       </c>
       <c r="C66" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D66" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G66" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -3923,25 +3923,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B67" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C67" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E67" t="s">
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G67" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -3956,25 +3956,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B68" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C68" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G68" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -3989,25 +3989,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B69" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C69" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G69" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4022,16 +4022,16 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
       </c>
       <c r="C70" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
@@ -4049,25 +4049,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B71" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C71" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E71" t="s">
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G71" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4082,25 +4082,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B72" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C72" t="s">
+        <v>350</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" t="s">
+        <v>353</v>
+      </c>
+      <c r="G72" t="s">
         <v>354</v>
-      </c>
-      <c r="D72" t="s">
-        <v>131</v>
-      </c>
-      <c r="E72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" t="s">
-        <v>357</v>
-      </c>
-      <c r="G72" t="s">
-        <v>358</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4115,25 +4115,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B73" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C73" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D73" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
       <c r="F73" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G73" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4148,25 +4148,25 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B74" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C74" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E74" t="s">
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G74" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4181,25 +4181,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B75" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C75" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D75" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="G75" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4214,25 +4214,25 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>260</v>
+      </c>
+      <c r="B76" t="s">
+        <v>261</v>
+      </c>
+      <c r="C76" t="s">
+        <v>261</v>
+      </c>
+      <c r="D76" t="s">
+        <v>262</v>
+      </c>
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" t="s">
+        <v>263</v>
+      </c>
+      <c r="G76" t="s">
         <v>264</v>
-      </c>
-      <c r="B76" t="s">
-        <v>265</v>
-      </c>
-      <c r="C76" t="s">
-        <v>265</v>
-      </c>
-      <c r="D76" t="s">
-        <v>266</v>
-      </c>
-      <c r="E76" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" t="s">
-        <v>267</v>
-      </c>
-      <c r="G76" t="s">
-        <v>268</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4247,25 +4247,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>265</v>
+      </c>
+      <c r="B77" t="s">
+        <v>266</v>
+      </c>
+      <c r="C77" t="s">
+        <v>266</v>
+      </c>
+      <c r="D77" t="s">
+        <v>267</v>
+      </c>
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
+        <v>268</v>
+      </c>
+      <c r="G77" t="s">
         <v>269</v>
-      </c>
-      <c r="B77" t="s">
-        <v>270</v>
-      </c>
-      <c r="C77" t="s">
-        <v>270</v>
-      </c>
-      <c r="D77" t="s">
-        <v>271</v>
-      </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" t="s">
-        <v>272</v>
-      </c>
-      <c r="G77" t="s">
-        <v>273</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4280,25 +4280,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>270</v>
+      </c>
+      <c r="B78" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" t="s">
+        <v>272</v>
+      </c>
+      <c r="D78" t="s">
+        <v>273</v>
+      </c>
+      <c r="E78" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" t="s">
         <v>274</v>
       </c>
-      <c r="B78" t="s">
+      <c r="G78" t="s">
         <v>275</v>
-      </c>
-      <c r="C78" t="s">
-        <v>276</v>
-      </c>
-      <c r="D78" t="s">
-        <v>277</v>
-      </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="F78" t="s">
-        <v>278</v>
-      </c>
-      <c r="G78" t="s">
-        <v>279</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4313,25 +4313,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>276</v>
+      </c>
+      <c r="B79" t="s">
+        <v>277</v>
+      </c>
+      <c r="C79" t="s">
+        <v>278</v>
+      </c>
+      <c r="D79" t="s">
+        <v>279</v>
+      </c>
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" t="s">
         <v>280</v>
       </c>
-      <c r="B79" t="s">
+      <c r="G79" t="s">
         <v>281</v>
-      </c>
-      <c r="C79" t="s">
-        <v>282</v>
-      </c>
-      <c r="D79" t="s">
-        <v>283</v>
-      </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" t="s">
-        <v>284</v>
-      </c>
-      <c r="G79" t="s">
-        <v>285</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4346,25 +4346,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>282</v>
+      </c>
+      <c r="B80" t="s">
+        <v>283</v>
+      </c>
+      <c r="C80" t="s">
+        <v>283</v>
+      </c>
+      <c r="D80" t="s">
+        <v>284</v>
+      </c>
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" t="s">
+        <v>285</v>
+      </c>
+      <c r="G80" t="s">
         <v>286</v>
-      </c>
-      <c r="B80" t="s">
-        <v>287</v>
-      </c>
-      <c r="C80" t="s">
-        <v>287</v>
-      </c>
-      <c r="D80" t="s">
-        <v>288</v>
-      </c>
-      <c r="E80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F80" t="s">
-        <v>289</v>
-      </c>
-      <c r="G80" t="s">
-        <v>290</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4379,25 +4379,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>287</v>
+      </c>
+      <c r="B81" t="s">
+        <v>288</v>
+      </c>
+      <c r="C81" t="s">
+        <v>288</v>
+      </c>
+      <c r="D81" t="s">
+        <v>289</v>
+      </c>
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" t="s">
+        <v>290</v>
+      </c>
+      <c r="G81" t="s">
         <v>291</v>
-      </c>
-      <c r="B81" t="s">
-        <v>292</v>
-      </c>
-      <c r="C81" t="s">
-        <v>292</v>
-      </c>
-      <c r="D81" t="s">
-        <v>293</v>
-      </c>
-      <c r="E81" t="s">
-        <v>20</v>
-      </c>
-      <c r="F81" t="s">
-        <v>294</v>
-      </c>
-      <c r="G81" t="s">
-        <v>295</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4412,25 +4412,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>292</v>
+      </c>
+      <c r="B82" t="s">
+        <v>293</v>
+      </c>
+      <c r="C82" t="s">
+        <v>293</v>
+      </c>
+      <c r="D82" t="s">
+        <v>294</v>
+      </c>
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" t="s">
+        <v>295</v>
+      </c>
+      <c r="G82" t="s">
         <v>296</v>
-      </c>
-      <c r="B82" t="s">
-        <v>297</v>
-      </c>
-      <c r="C82" t="s">
-        <v>297</v>
-      </c>
-      <c r="D82" t="s">
-        <v>298</v>
-      </c>
-      <c r="E82" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" t="s">
-        <v>299</v>
-      </c>
-      <c r="G82" t="s">
-        <v>300</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4445,25 +4445,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>297</v>
+      </c>
+      <c r="B83" t="s">
+        <v>298</v>
+      </c>
+      <c r="C83" t="s">
+        <v>298</v>
+      </c>
+      <c r="D83" t="s">
+        <v>299</v>
+      </c>
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" t="s">
+        <v>300</v>
+      </c>
+      <c r="G83" t="s">
         <v>301</v>
-      </c>
-      <c r="B83" t="s">
-        <v>302</v>
-      </c>
-      <c r="C83" t="s">
-        <v>302</v>
-      </c>
-      <c r="D83" t="s">
-        <v>303</v>
-      </c>
-      <c r="E83" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" t="s">
-        <v>304</v>
-      </c>
-      <c r="G83" t="s">
-        <v>305</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4478,25 +4478,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>302</v>
+      </c>
+      <c r="B84" t="s">
+        <v>303</v>
+      </c>
+      <c r="C84" t="s">
+        <v>303</v>
+      </c>
+      <c r="D84" t="s">
+        <v>304</v>
+      </c>
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" t="s">
+        <v>305</v>
+      </c>
+      <c r="G84" t="s">
         <v>306</v>
-      </c>
-      <c r="B84" t="s">
-        <v>307</v>
-      </c>
-      <c r="C84" t="s">
-        <v>307</v>
-      </c>
-      <c r="D84" t="s">
-        <v>308</v>
-      </c>
-      <c r="E84" t="s">
-        <v>20</v>
-      </c>
-      <c r="F84" t="s">
-        <v>309</v>
-      </c>
-      <c r="G84" t="s">
-        <v>310</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4511,16 +4511,16 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B85" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C85" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D85" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G85" t="s">
         <v>15</v>
@@ -4533,30 +4533,30 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>311</v>
+      </c>
+      <c r="B86" t="s">
+        <v>312</v>
+      </c>
+      <c r="C86" t="s">
+        <v>312</v>
+      </c>
+      <c r="D86" t="s">
+        <v>313</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" t="s">
+        <v>314</v>
+      </c>
+      <c r="G86" t="s">
         <v>315</v>
-      </c>
-      <c r="B86" t="s">
-        <v>316</v>
-      </c>
-      <c r="C86" t="s">
-        <v>316</v>
-      </c>
-      <c r="D86" t="s">
-        <v>317</v>
-      </c>
-      <c r="E86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" t="s">
-        <v>318</v>
-      </c>
-      <c r="G86" t="s">
-        <v>319</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4571,25 +4571,25 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>316</v>
+      </c>
+      <c r="B87" t="s">
+        <v>317</v>
+      </c>
+      <c r="C87" t="s">
+        <v>317</v>
+      </c>
+      <c r="D87" t="s">
+        <v>318</v>
+      </c>
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" t="s">
+        <v>319</v>
+      </c>
+      <c r="G87" t="s">
         <v>320</v>
-      </c>
-      <c r="B87" t="s">
-        <v>321</v>
-      </c>
-      <c r="C87" t="s">
-        <v>321</v>
-      </c>
-      <c r="D87" t="s">
-        <v>322</v>
-      </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>323</v>
-      </c>
-      <c r="G87" t="s">
-        <v>324</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4604,25 +4604,25 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>321</v>
+      </c>
+      <c r="B88" t="s">
+        <v>322</v>
+      </c>
+      <c r="C88" t="s">
+        <v>322</v>
+      </c>
+      <c r="D88" t="s">
+        <v>323</v>
+      </c>
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" t="s">
+        <v>324</v>
+      </c>
+      <c r="G88" t="s">
         <v>325</v>
-      </c>
-      <c r="B88" t="s">
-        <v>326</v>
-      </c>
-      <c r="C88" t="s">
-        <v>326</v>
-      </c>
-      <c r="D88" t="s">
-        <v>327</v>
-      </c>
-      <c r="E88" t="s">
-        <v>20</v>
-      </c>
-      <c r="F88" t="s">
-        <v>328</v>
-      </c>
-      <c r="G88" t="s">
-        <v>329</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -4637,25 +4637,25 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>326</v>
+      </c>
+      <c r="B89" t="s">
+        <v>327</v>
+      </c>
+      <c r="C89" t="s">
+        <v>327</v>
+      </c>
+      <c r="D89" t="s">
+        <v>328</v>
+      </c>
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" t="s">
+        <v>329</v>
+      </c>
+      <c r="G89" t="s">
         <v>330</v>
-      </c>
-      <c r="B89" t="s">
-        <v>331</v>
-      </c>
-      <c r="C89" t="s">
-        <v>331</v>
-      </c>
-      <c r="D89" t="s">
-        <v>332</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>333</v>
-      </c>
-      <c r="G89" t="s">
-        <v>334</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -4670,25 +4670,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>331</v>
+      </c>
+      <c r="B90" t="s">
+        <v>332</v>
+      </c>
+      <c r="C90" t="s">
+        <v>332</v>
+      </c>
+      <c r="D90" t="s">
+        <v>333</v>
+      </c>
+      <c r="E90" t="s">
+        <v>334</v>
+      </c>
+      <c r="F90" t="s">
         <v>335</v>
       </c>
-      <c r="B90" t="s">
+      <c r="G90" t="s">
         <v>336</v>
-      </c>
-      <c r="C90" t="s">
-        <v>336</v>
-      </c>
-      <c r="D90" t="s">
-        <v>337</v>
-      </c>
-      <c r="E90" t="s">
-        <v>338</v>
-      </c>
-      <c r="F90" t="s">
-        <v>339</v>
-      </c>
-      <c r="G90" t="s">
-        <v>340</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -4703,25 +4703,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>337</v>
+      </c>
+      <c r="B91" t="s">
+        <v>338</v>
+      </c>
+      <c r="C91" t="s">
+        <v>338</v>
+      </c>
+      <c r="D91" t="s">
+        <v>339</v>
+      </c>
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" t="s">
+        <v>340</v>
+      </c>
+      <c r="G91" t="s">
         <v>341</v>
-      </c>
-      <c r="B91" t="s">
-        <v>342</v>
-      </c>
-      <c r="C91" t="s">
-        <v>342</v>
-      </c>
-      <c r="D91" t="s">
-        <v>343</v>
-      </c>
-      <c r="E91" t="s">
-        <v>20</v>
-      </c>
-      <c r="F91" t="s">
-        <v>344</v>
-      </c>
-      <c r="G91" t="s">
-        <v>345</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -4736,16 +4736,16 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B92" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C92" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D92" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G92" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
PTH 5mm axial capacitors.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="385">
   <si>
     <t>Part</t>
   </si>
@@ -1136,6 +1136,39 @@
   </si>
   <si>
     <t>C1608C0G1H301J</t>
+  </si>
+  <si>
+    <t>445-2904-ND</t>
+  </si>
+  <si>
+    <t>FK22Y5V1E226Z</t>
+  </si>
+  <si>
+    <t>445-2880-ND</t>
+  </si>
+  <si>
+    <t>FK26Y5V1E475Z</t>
+  </si>
+  <si>
+    <t>445-5257-ND</t>
+  </si>
+  <si>
+    <t>FK28X7R1H683K</t>
+  </si>
+  <si>
+    <t>445-5253-ND</t>
+  </si>
+  <si>
+    <t>FK28X7R1H153K</t>
+  </si>
+  <si>
+    <t>Real part value is 0.015uF</t>
+  </si>
+  <si>
+    <t>1292PH-ND</t>
+  </si>
+  <si>
+    <t>S680K29SL0N63J5R</t>
   </si>
 </sst>
 </file>
@@ -1967,7 +2000,7 @@
   <dimension ref="A1:L92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,7 +2086,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J100)</f>
-        <v>162.47720000000004</v>
+        <v>166.28720000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2219,15 +2252,24 @@
       <c r="D8" t="s">
         <v>32</v>
       </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>374</v>
+      </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>375</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
+      <c r="I8">
+        <v>1.25</v>
+      </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2243,15 +2285,24 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>376</v>
+      </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9">
+        <v>0.43</v>
+      </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2431,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2444,18 +2495,27 @@
       <c r="D17" t="s">
         <v>32</v>
       </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>378</v>
+      </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>379</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
+      <c r="I17">
+        <v>0.35</v>
+      </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2479,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2503,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2516,18 +2576,30 @@
       <c r="D20" t="s">
         <v>32</v>
       </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>380</v>
+      </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>381</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
+      <c r="I20">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -2540,18 +2612,27 @@
       <c r="D21" t="s">
         <v>32</v>
       </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>383</v>
+      </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>384</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
+      <c r="I21">
+        <v>0.24</v>
+      </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2575,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -2599,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -2632,7 +2713,7 @@
         <v>8.19</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2665,7 +2746,7 @@
         <v>1.0499999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2689,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2713,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -2737,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2761,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2794,7 +2875,7 @@
         <v>35.730000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2827,7 +2908,7 @@
         <v>7.97</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Rows 10, 12, 13, 14, and 15 filled in.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="399">
   <si>
     <t>Part</t>
   </si>
@@ -1169,6 +1169,48 @@
   </si>
   <si>
     <t>S680K29SL0N63J5R</t>
+  </si>
+  <si>
+    <t>445-1308-1-ND</t>
+  </si>
+  <si>
+    <t>C1608X7R1H102K</t>
+  </si>
+  <si>
+    <t>0.01uF = 10k pF</t>
+  </si>
+  <si>
+    <t>478-1227-1-ND</t>
+  </si>
+  <si>
+    <t>06035C103KAT2A</t>
+  </si>
+  <si>
+    <t>445-5191-1-ND</t>
+  </si>
+  <si>
+    <t>C1608X7R1E224K</t>
+  </si>
+  <si>
+    <t>10nF = 10k pF (redundant line item)</t>
+  </si>
+  <si>
+    <t>470nF = 0.47uF</t>
+  </si>
+  <si>
+    <t>445-3454-1-ND</t>
+  </si>
+  <si>
+    <t>C1608Y5V1E474Z</t>
+  </si>
+  <si>
+    <t>33nF = 33k pF = 0.033uF</t>
+  </si>
+  <si>
+    <t>445-5106-1-ND</t>
+  </si>
+  <si>
+    <t>C1608X7R1E333K</t>
   </si>
 </sst>
 </file>
@@ -2000,7 +2042,7 @@
   <dimension ref="A1:L92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +2053,7 @@
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2086,7 +2128,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J100)</f>
-        <v>166.28720000000001</v>
+        <v>167.43720000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2318,15 +2360,27 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>388</v>
+      </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>389</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
+      <c r="I10">
+        <v>0.06</v>
+      </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.06</v>
+      </c>
+      <c r="L10" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2375,15 +2429,24 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>390</v>
+      </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>391</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
+      <c r="I12">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2399,15 +2462,27 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>388</v>
+      </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>389</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
+      <c r="I13">
+        <v>0.06</v>
+      </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.06</v>
+      </c>
+      <c r="L13" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2423,15 +2498,27 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>394</v>
+      </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>395</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
+      <c r="I14">
+        <v>0.17</v>
+      </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.17</v>
+      </c>
+      <c r="L14" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2447,15 +2534,27 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>397</v>
+      </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>398</v>
       </c>
       <c r="H15">
         <v>3</v>
       </c>
+      <c r="I15">
+        <v>0.16</v>
+      </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.48</v>
+      </c>
+      <c r="L15" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2669,15 +2768,24 @@
       <c r="D23" t="s">
         <v>14</v>
       </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>385</v>
+      </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>386</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
+      <c r="I23">
+        <v>0.1</v>
+      </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed F1 to the next highest Ihold part (1.6A).
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="412">
   <si>
     <t>Part</t>
   </si>
@@ -295,9 +295,6 @@
     <t>A98442-ND</t>
   </si>
   <si>
-    <t>JARD</t>
-  </si>
-  <si>
     <t>ARDUINO_SHIELDNO_SILK</t>
   </si>
   <si>
@@ -1241,6 +1238,18 @@
   </si>
   <si>
     <t>RUEF1600</t>
+  </si>
+  <si>
+    <t>JARD - 6 pin headers</t>
+  </si>
+  <si>
+    <t>JARD-  8 pin headers</t>
+  </si>
+  <si>
+    <t>PRT-09280</t>
+  </si>
+  <si>
+    <t>PRT-09279</t>
   </si>
 </sst>
 </file>
@@ -2069,10 +2078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2130,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2141,10 +2150,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" t="s">
         <v>363</v>
-      </c>
-      <c r="G2" t="s">
-        <v>364</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2157,8 +2166,8 @@
         <v>0.27</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J100)</f>
-        <v>171.63720000000001</v>
+        <f>SUM(J2:J101)</f>
+        <v>173.63720000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2178,10 +2187,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" t="s">
         <v>365</v>
-      </c>
-      <c r="G3" t="s">
-        <v>366</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2190,7 +2199,7 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J67" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
@@ -2211,10 +2220,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>366</v>
+      </c>
+      <c r="G4" t="s">
         <v>367</v>
-      </c>
-      <c r="G4" t="s">
-        <v>368</v>
       </c>
       <c r="H4">
         <v>23</v>
@@ -2268,10 +2277,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>371</v>
+      </c>
+      <c r="G6" t="s">
         <v>372</v>
-      </c>
-      <c r="G6" t="s">
-        <v>373</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2284,7 +2293,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2328,10 +2337,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
+        <v>373</v>
+      </c>
+      <c r="G8" t="s">
         <v>374</v>
-      </c>
-      <c r="G8" t="s">
-        <v>375</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2361,10 +2370,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
+        <v>375</v>
+      </c>
+      <c r="G9" t="s">
         <v>376</v>
-      </c>
-      <c r="G9" t="s">
-        <v>377</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2394,10 +2403,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
+        <v>387</v>
+      </c>
+      <c r="G10" t="s">
         <v>388</v>
-      </c>
-      <c r="G10" t="s">
-        <v>389</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2410,7 +2419,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2463,10 +2472,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
+        <v>389</v>
+      </c>
+      <c r="G12" t="s">
         <v>390</v>
-      </c>
-      <c r="G12" t="s">
-        <v>391</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2496,10 +2505,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
+        <v>387</v>
+      </c>
+      <c r="G13" t="s">
         <v>388</v>
-      </c>
-      <c r="G13" t="s">
-        <v>389</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2512,7 +2521,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2532,10 +2541,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
+        <v>393</v>
+      </c>
+      <c r="G14" t="s">
         <v>394</v>
-      </c>
-      <c r="G14" t="s">
-        <v>395</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2548,7 +2557,7 @@
         <v>0.17</v>
       </c>
       <c r="L14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2568,10 +2577,10 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
+        <v>396</v>
+      </c>
+      <c r="G15" t="s">
         <v>397</v>
-      </c>
-      <c r="G15" t="s">
-        <v>398</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2584,7 +2593,7 @@
         <v>0.48</v>
       </c>
       <c r="L15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2628,10 +2637,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
+        <v>377</v>
+      </c>
+      <c r="G17" t="s">
         <v>378</v>
-      </c>
-      <c r="G17" t="s">
-        <v>379</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2709,10 +2718,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
+        <v>379</v>
+      </c>
+      <c r="G20" t="s">
         <v>380</v>
-      </c>
-      <c r="G20" t="s">
-        <v>381</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2725,7 +2734,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2745,10 +2754,10 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
+        <v>382</v>
+      </c>
+      <c r="G21" t="s">
         <v>383</v>
-      </c>
-      <c r="G21" t="s">
-        <v>384</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2802,10 +2811,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
+        <v>384</v>
+      </c>
+      <c r="G23" t="s">
         <v>385</v>
-      </c>
-      <c r="G23" t="s">
-        <v>386</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2868,10 +2877,10 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
+        <v>360</v>
+      </c>
+      <c r="G25" t="s">
         <v>361</v>
-      </c>
-      <c r="G25" t="s">
-        <v>362</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -2901,10 +2910,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
+        <v>406</v>
+      </c>
+      <c r="G26" t="s">
         <v>407</v>
-      </c>
-      <c r="G26" t="s">
-        <v>408</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2917,7 +2926,7 @@
         <v>0.4</v>
       </c>
       <c r="L26" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2937,10 +2946,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
+        <v>399</v>
+      </c>
+      <c r="G27" t="s">
         <v>400</v>
-      </c>
-      <c r="G27" t="s">
-        <v>401</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2970,10 +2979,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
+        <v>401</v>
+      </c>
+      <c r="G28" t="s">
         <v>402</v>
-      </c>
-      <c r="G28" t="s">
-        <v>403</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3003,10 +3012,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
+        <v>403</v>
+      </c>
+      <c r="G29" t="s">
         <v>404</v>
-      </c>
-      <c r="G29" t="s">
-        <v>405</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -3019,7 +3028,7 @@
         <v>2.7</v>
       </c>
       <c r="L29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3039,10 +3048,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
+        <v>345</v>
+      </c>
+      <c r="G30" t="s">
         <v>346</v>
-      </c>
-      <c r="G30" t="s">
-        <v>347</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3123,619 +3132,625 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>409</v>
+      </c>
+      <c r="B33" t="s">
         <v>93</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="G33" t="s">
-        <v>15</v>
+      <c r="E33" t="s">
+        <v>333</v>
+      </c>
+      <c r="F33" t="s">
+        <v>411</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>0.5</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>408</v>
       </c>
       <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" t="s">
+        <v>333</v>
+      </c>
+      <c r="F34" t="s">
+        <v>410</v>
+      </c>
+      <c r="G34" t="s">
         <v>15</v>
-      </c>
-      <c r="C34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" t="s">
-        <v>99</v>
-      </c>
-      <c r="G34" t="s">
-        <v>100</v>
       </c>
       <c r="H34">
         <v>2</v>
       </c>
       <c r="I34">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>359</v>
+        <v>98</v>
       </c>
       <c r="G35" t="s">
-        <v>360</v>
+        <v>99</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>358</v>
       </c>
       <c r="G36" t="s">
-        <v>110</v>
+        <v>359</v>
       </c>
       <c r="H36">
         <v>3</v>
       </c>
       <c r="I36">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L36" t="s">
-        <v>370</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
         <v>108</v>
       </c>
-      <c r="D37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>109</v>
       </c>
-      <c r="G37" t="s">
-        <v>110</v>
-      </c>
       <c r="H37">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I37">
         <v>0.42</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>1.26</v>
+      </c>
+      <c r="L37" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G38" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I38">
-        <v>3.65</v>
+        <v>0.42</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>111</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
+        <v>112</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>3.65</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>121</v>
-      </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G40" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40">
-        <v>2.13</v>
+        <v>5</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G42" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G43" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>138</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
+        <v>139</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="H44">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1.85</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G45" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="H45">
-        <v>25</v>
-      </c>
-      <c r="I45">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G46" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I46">
-        <v>0.84</v>
+        <v>0.3</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>15</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" t="s">
+        <v>153</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>0.84</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G48" t="s">
-        <v>163</v>
+        <v>15</v>
       </c>
       <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C49" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E49" t="s">
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G49" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>348</v>
+        <v>166</v>
       </c>
       <c r="G50" t="s">
-        <v>349</v>
+        <v>167</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C51" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" t="s">
         <v>171</v>
       </c>
-      <c r="D51" t="s">
-        <v>172</v>
-      </c>
       <c r="E51" t="s">
         <v>20</v>
       </c>
       <c r="F51" t="s">
-        <v>175</v>
+        <v>347</v>
       </c>
       <c r="G51" t="s">
-        <v>176</v>
+        <v>348</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>177</v>
-      </c>
-      <c r="B52">
-        <v>470</v>
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
+        <v>173</v>
       </c>
       <c r="C52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" t="s">
         <v>171</v>
       </c>
-      <c r="D52" t="s">
-        <v>172</v>
-      </c>
       <c r="E52" t="s">
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G52" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3750,124 +3765,124 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>180</v>
-      </c>
-      <c r="B53" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="B53">
+        <v>470</v>
       </c>
       <c r="C53" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" t="s">
         <v>171</v>
       </c>
-      <c r="D53" t="s">
-        <v>172</v>
-      </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G53" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H53">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="I53">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.81420000000000003</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" t="s">
         <v>171</v>
       </c>
-      <c r="D54" t="s">
-        <v>172</v>
-      </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G54" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H54">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="I54">
-        <v>0.04</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.81420000000000003</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B55" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C55" t="s">
-        <v>350</v>
+        <v>170</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>351</v>
+        <v>185</v>
       </c>
       <c r="G55" t="s">
-        <v>352</v>
+        <v>186</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I55">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B56" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C56" t="s">
+        <v>349</v>
+      </c>
+      <c r="D56" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
         <v>350</v>
       </c>
-      <c r="D56" t="s">
-        <v>127</v>
-      </c>
-      <c r="E56" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" t="s">
-        <v>357</v>
-      </c>
       <c r="G56" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3882,289 +3897,289 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>349</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>194</v>
+        <v>356</v>
       </c>
       <c r="G57" t="s">
-        <v>195</v>
+        <v>357</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
       <c r="I57">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>196</v>
-      </c>
-      <c r="B58">
-        <v>200</v>
+        <v>191</v>
+      </c>
+      <c r="B58" t="s">
+        <v>192</v>
       </c>
       <c r="C58" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" t="s">
         <v>171</v>
       </c>
-      <c r="D58" t="s">
-        <v>172</v>
-      </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G58" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H58">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B59">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C59" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" t="s">
         <v>171</v>
       </c>
-      <c r="D59" t="s">
-        <v>172</v>
-      </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G59" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H59">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>202</v>
-      </c>
-      <c r="B60" t="s">
-        <v>203</v>
+        <v>198</v>
+      </c>
+      <c r="B60">
+        <v>100</v>
       </c>
       <c r="C60" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" t="s">
         <v>171</v>
       </c>
-      <c r="D60" t="s">
-        <v>172</v>
-      </c>
       <c r="E60" t="s">
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G60" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H60">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I60">
         <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" t="s">
         <v>171</v>
       </c>
-      <c r="D61" t="s">
-        <v>172</v>
-      </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G61" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H61">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I61">
         <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C62" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" t="s">
         <v>171</v>
       </c>
-      <c r="D62" t="s">
-        <v>172</v>
-      </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G62" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C63" t="s">
+        <v>170</v>
+      </c>
+      <c r="D63" t="s">
         <v>171</v>
       </c>
-      <c r="D63" t="s">
-        <v>172</v>
-      </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G63" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C64" t="s">
+        <v>170</v>
+      </c>
+      <c r="D64" t="s">
         <v>171</v>
       </c>
-      <c r="D64" t="s">
-        <v>172</v>
-      </c>
       <c r="E64" t="s">
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G64" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B65" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C65" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" t="s">
         <v>171</v>
       </c>
-      <c r="D65" t="s">
-        <v>172</v>
-      </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G65" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -4179,91 +4194,91 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>226</v>
-      </c>
-      <c r="B66">
-        <v>0.3</v>
+        <v>221</v>
+      </c>
+      <c r="B66" t="s">
+        <v>222</v>
       </c>
       <c r="C66" t="s">
-        <v>227</v>
+        <v>170</v>
       </c>
       <c r="D66" t="s">
-        <v>228</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G66" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H66">
         <v>1</v>
       </c>
       <c r="I66">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>231</v>
-      </c>
-      <c r="B67" t="s">
-        <v>232</v>
+        <v>225</v>
+      </c>
+      <c r="B67">
+        <v>0.3</v>
       </c>
       <c r="C67" t="s">
-        <v>171</v>
+        <v>226</v>
       </c>
       <c r="D67" t="s">
-        <v>172</v>
+        <v>227</v>
       </c>
       <c r="E67" t="s">
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G67" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J92" si="1">H67*I67</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B68" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C68" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" t="s">
         <v>171</v>
       </c>
-      <c r="D68" t="s">
-        <v>172</v>
-      </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G68" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4272,31 +4287,31 @@
         <v>0.04</v>
       </c>
       <c r="J68">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J68:J93" si="1">H68*I68</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B69" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C69" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69" t="s">
         <v>171</v>
       </c>
-      <c r="D69" t="s">
-        <v>172</v>
-      </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G69" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4311,118 +4326,118 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>239</v>
       </c>
       <c r="C70" t="s">
+        <v>170</v>
+      </c>
+      <c r="D70" t="s">
         <v>171</v>
       </c>
-      <c r="D70" t="s">
-        <v>172</v>
-      </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
+      <c r="F70" t="s">
+        <v>240</v>
+      </c>
       <c r="G70" t="s">
-        <v>15</v>
+        <v>241</v>
       </c>
       <c r="H70">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B71" t="s">
-        <v>245</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
+        <v>170</v>
+      </c>
+      <c r="D71" t="s">
         <v>171</v>
       </c>
-      <c r="D71" t="s">
-        <v>172</v>
-      </c>
       <c r="E71" t="s">
         <v>20</v>
       </c>
-      <c r="F71" t="s">
-        <v>246</v>
-      </c>
       <c r="G71" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="H71">
-        <v>1</v>
-      </c>
-      <c r="I71">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J71">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B72" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C72" t="s">
-        <v>350</v>
+        <v>170</v>
       </c>
       <c r="D72" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="E72" t="s">
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>353</v>
+        <v>245</v>
       </c>
       <c r="G72" t="s">
-        <v>354</v>
+        <v>246</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B73" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C73" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
       <c r="F73" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G73" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4437,58 +4452,58 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B74" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C74" t="s">
-        <v>171</v>
+        <v>349</v>
       </c>
       <c r="D74" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="E74" t="s">
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>254</v>
+        <v>354</v>
       </c>
       <c r="G74" t="s">
-        <v>255</v>
+        <v>355</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B75" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C75" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" t="s">
         <v>171</v>
       </c>
-      <c r="D75" t="s">
-        <v>172</v>
-      </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G75" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4503,546 +4518,579 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B76" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C76" t="s">
-        <v>261</v>
+        <v>170</v>
       </c>
       <c r="D76" t="s">
-        <v>262</v>
+        <v>171</v>
       </c>
       <c r="E76" t="s">
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G76" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B77" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C77" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D77" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E77" t="s">
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G77" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B78" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C78" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D78" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E78" t="s">
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G78" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B79" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C79" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D79" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G79" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B80" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C80" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D80" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G80" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B81" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C81" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D81" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="G81" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B82" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C82" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D82" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G82" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B83" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C83" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D83" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="G83" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B84" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C84" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D84" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G84" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B85" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C85" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D85" t="s">
-        <v>309</v>
+        <v>303</v>
+      </c>
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" t="s">
+        <v>304</v>
       </c>
       <c r="G85" t="s">
-        <v>15</v>
+        <v>305</v>
       </c>
       <c r="H85">
         <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1.51</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K85" t="s">
-        <v>310</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B86" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C86" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D86" t="s">
-        <v>313</v>
-      </c>
-      <c r="E86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="G86" t="s">
-        <v>315</v>
+        <v>15</v>
       </c>
       <c r="H86">
         <v>1</v>
-      </c>
-      <c r="I86">
-        <v>0.47</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K86" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B87" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C87" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D87" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E87" t="s">
         <v>20</v>
       </c>
       <c r="F87" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G87" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B88" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C88" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D88" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E88" t="s">
         <v>20</v>
       </c>
       <c r="F88" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="G88" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B89" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C89" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D89" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E89" t="s">
         <v>20</v>
       </c>
       <c r="F89" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G89" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B90" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C90" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D90" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E90" t="s">
-        <v>334</v>
+        <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G90" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>1.5</v>
+        <v>12.95</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>12.95</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B91" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C91" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D91" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E91" t="s">
-        <v>20</v>
+        <v>333</v>
       </c>
       <c r="F91" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="G91" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>336</v>
+      </c>
+      <c r="B92" t="s">
+        <v>337</v>
+      </c>
+      <c r="C92" t="s">
+        <v>337</v>
+      </c>
+      <c r="D92" t="s">
+        <v>338</v>
+      </c>
+      <c r="E92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" t="s">
+        <v>339</v>
+      </c>
+      <c r="G92" t="s">
+        <v>340</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>2.96</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>341</v>
+      </c>
+      <c r="B93" t="s">
         <v>342</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C93" t="s">
         <v>343</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D93" t="s">
         <v>344</v>
       </c>
-      <c r="D92" t="s">
-        <v>345</v>
-      </c>
-      <c r="G92" t="s">
+      <c r="G93" t="s">
         <v>15</v>
       </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="J92">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="J93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Swapped out J1 for a cheaper part.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -280,12 +280,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>39910-0102</t>
-  </si>
-  <si>
-    <t>WM5964-ND</t>
-  </si>
-  <si>
     <t>J2, J3, J4</t>
   </si>
   <si>
@@ -1210,9 +1204,6 @@
     <t>C1608X7R1E333K</t>
   </si>
   <si>
-    <t>Ihold of 1.35A</t>
-  </si>
-  <si>
     <t>RUEF600-ND</t>
   </si>
   <si>
@@ -1250,6 +1241,15 @@
   </si>
   <si>
     <t>PRT-09279</t>
+  </si>
+  <si>
+    <t>Ihold of 1.60A</t>
+  </si>
+  <si>
+    <t>APC1274-ND</t>
+  </si>
+  <si>
+    <t>ESPM02200</t>
   </si>
 </sst>
 </file>
@@ -2080,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2130,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2150,10 +2150,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J101)</f>
-        <v>173.63720000000001</v>
+        <v>167.81719999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2187,10 +2187,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2220,10 +2220,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H4">
         <v>23</v>
@@ -2277,10 +2277,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2293,7 +2293,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2337,10 +2337,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2370,10 +2370,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2403,10 +2403,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2419,7 +2419,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2472,10 +2472,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2505,10 +2505,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2521,7 +2521,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2541,10 +2541,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2557,7 +2557,7 @@
         <v>0.17</v>
       </c>
       <c r="L14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2577,10 +2577,10 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2593,7 +2593,7 @@
         <v>0.48</v>
       </c>
       <c r="L15" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2637,10 +2637,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2718,10 +2718,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2734,7 +2734,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2754,10 +2754,10 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G21" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2811,10 +2811,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2877,10 +2877,10 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -2910,10 +2910,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G26" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2926,7 +2926,7 @@
         <v>0.4</v>
       </c>
       <c r="L26" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2946,10 +2946,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G27" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2979,10 +2979,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G28" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3012,10 +3012,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G29" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -3028,7 +3028,7 @@
         <v>2.7</v>
       </c>
       <c r="L29" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3048,10 +3048,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G30" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3069,55 +3069,55 @@
         <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>411</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>411</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>411</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>89</v>
+        <v>410</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>411</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31">
-        <v>7.97</v>
+        <v>2.15</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>7.97</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" t="s">
-        <v>92</v>
-      </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -3132,22 +3132,22 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F33" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -3162,22 +3162,22 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F34" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="G34" t="s">
         <v>15</v>
@@ -3195,25 +3195,25 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
         <v>96</v>
       </c>
-      <c r="D35" t="s">
+      <c r="G35" t="s">
         <v>97</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" t="s">
-        <v>98</v>
-      </c>
-      <c r="G35" t="s">
-        <v>99</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -3228,25 +3228,25 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G36" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H36">
         <v>3</v>
@@ -3261,25 +3261,25 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -3292,30 +3292,30 @@
         <v>1.26</v>
       </c>
       <c r="L37" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" t="s">
         <v>107</v>
-      </c>
-      <c r="D38" t="s">
-        <v>105</v>
-      </c>
-      <c r="E38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" t="s">
-        <v>109</v>
       </c>
       <c r="H38">
         <v>10</v>
@@ -3330,25 +3330,25 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
         <v>110</v>
       </c>
-      <c r="B39" t="s">
+      <c r="G39" t="s">
         <v>111</v>
-      </c>
-      <c r="C39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" t="s">
-        <v>111</v>
-      </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" t="s">
-        <v>112</v>
-      </c>
-      <c r="G39" t="s">
-        <v>113</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -3363,16 +3363,16 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G40" t="s">
         <v>15</v>
@@ -3387,25 +3387,25 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" t="s">
         <v>117</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>118</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
         <v>119</v>
       </c>
-      <c r="D41" t="s">
+      <c r="G41" t="s">
         <v>120</v>
-      </c>
-      <c r="E41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" t="s">
-        <v>121</v>
-      </c>
-      <c r="G41" t="s">
-        <v>122</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -3420,25 +3420,25 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>124</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
         <v>125</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>126</v>
-      </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
-        <v>127</v>
-      </c>
-      <c r="G42" t="s">
-        <v>128</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3453,25 +3453,25 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
         <v>129</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>130</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
         <v>131</v>
       </c>
-      <c r="D43" t="s">
+      <c r="G43" t="s">
         <v>132</v>
-      </c>
-      <c r="E43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" t="s">
-        <v>133</v>
-      </c>
-      <c r="G43" t="s">
-        <v>134</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3486,25 +3486,25 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" t="s">
         <v>135</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>136</v>
       </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
         <v>137</v>
       </c>
-      <c r="D44" t="s">
+      <c r="G44" t="s">
         <v>138</v>
-      </c>
-      <c r="E44" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G44" t="s">
-        <v>140</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3519,16 +3519,16 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G45" t="s">
         <v>15</v>
@@ -3543,25 +3543,25 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" t="s">
         <v>144</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>145</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
         <v>146</v>
       </c>
-      <c r="D46" t="s">
+      <c r="G46" t="s">
         <v>147</v>
-      </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" t="s">
-        <v>148</v>
-      </c>
-      <c r="G46" t="s">
-        <v>149</v>
       </c>
       <c r="H46">
         <v>25</v>
@@ -3576,13 +3576,13 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" t="s">
         <v>150</v>
-      </c>
-      <c r="B47" t="s">
-        <v>151</v>
-      </c>
-      <c r="C47" t="s">
-        <v>152</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
@@ -3591,10 +3591,10 @@
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G47" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -3609,16 +3609,16 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" t="s">
         <v>155</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>156</v>
-      </c>
-      <c r="C48" t="s">
-        <v>157</v>
-      </c>
-      <c r="D48" t="s">
-        <v>158</v>
       </c>
       <c r="G48" t="s">
         <v>15</v>
@@ -3633,25 +3633,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
         <v>159</v>
       </c>
-      <c r="B49" t="s">
+      <c r="G49" t="s">
         <v>160</v>
-      </c>
-      <c r="C49" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
-      </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" t="s">
-        <v>161</v>
-      </c>
-      <c r="G49" t="s">
-        <v>162</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -3666,25 +3666,25 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" t="s">
         <v>163</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
         <v>164</v>
       </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
         <v>165</v>
-      </c>
-      <c r="D50" t="s">
-        <v>147</v>
-      </c>
-      <c r="E50" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" t="s">
-        <v>166</v>
-      </c>
-      <c r="G50" t="s">
-        <v>167</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -3699,25 +3699,25 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" t="s">
         <v>168</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>169</v>
       </c>
-      <c r="C51" t="s">
-        <v>170</v>
-      </c>
-      <c r="D51" t="s">
-        <v>171</v>
-      </c>
       <c r="E51" t="s">
         <v>20</v>
       </c>
       <c r="F51" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G51" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -3732,25 +3732,25 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" t="s">
         <v>172</v>
       </c>
-      <c r="B52" t="s">
+      <c r="G52" t="s">
         <v>173</v>
-      </c>
-      <c r="C52" t="s">
-        <v>170</v>
-      </c>
-      <c r="D52" t="s">
-        <v>171</v>
-      </c>
-      <c r="E52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" t="s">
-        <v>174</v>
-      </c>
-      <c r="G52" t="s">
-        <v>175</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3765,25 +3765,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B53">
         <v>470</v>
       </c>
       <c r="C53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D53" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G53" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3798,25 +3798,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" t="s">
         <v>179</v>
       </c>
-      <c r="B54" t="s">
+      <c r="G54" t="s">
         <v>180</v>
-      </c>
-      <c r="C54" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" t="s">
-        <v>181</v>
-      </c>
-      <c r="G54" t="s">
-        <v>182</v>
       </c>
       <c r="H54">
         <v>59</v>
@@ -3831,25 +3831,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
         <v>183</v>
       </c>
-      <c r="B55" t="s">
+      <c r="G55" t="s">
         <v>184</v>
-      </c>
-      <c r="C55" t="s">
-        <v>170</v>
-      </c>
-      <c r="D55" t="s">
-        <v>171</v>
-      </c>
-      <c r="E55" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" t="s">
-        <v>185</v>
-      </c>
-      <c r="G55" t="s">
-        <v>186</v>
       </c>
       <c r="H55">
         <v>4</v>
@@ -3864,25 +3864,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C56" t="s">
+        <v>347</v>
+      </c>
+      <c r="D56" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
+        <v>348</v>
+      </c>
+      <c r="G56" t="s">
         <v>349</v>
-      </c>
-      <c r="D56" t="s">
-        <v>126</v>
-      </c>
-      <c r="E56" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" t="s">
-        <v>350</v>
-      </c>
-      <c r="G56" t="s">
-        <v>351</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3897,25 +3897,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C57" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G57" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3930,25 +3930,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>189</v>
+      </c>
+      <c r="B58" t="s">
+        <v>190</v>
+      </c>
+      <c r="C58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" t="s">
         <v>191</v>
       </c>
-      <c r="B58" t="s">
+      <c r="G58" t="s">
         <v>192</v>
-      </c>
-      <c r="C58" t="s">
-        <v>170</v>
-      </c>
-      <c r="D58" t="s">
-        <v>171</v>
-      </c>
-      <c r="E58" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" t="s">
-        <v>193</v>
-      </c>
-      <c r="G58" t="s">
-        <v>194</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -3963,25 +3963,25 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B59">
         <v>200</v>
       </c>
       <c r="C59" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D59" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G59" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H59">
         <v>24</v>
@@ -3996,25 +3996,25 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B60">
         <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D60" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E60" t="s">
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G60" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H60">
         <v>10</v>
@@ -4029,25 +4029,25 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" t="s">
         <v>201</v>
       </c>
-      <c r="B61" t="s">
+      <c r="G61" t="s">
         <v>202</v>
-      </c>
-      <c r="C61" t="s">
-        <v>170</v>
-      </c>
-      <c r="D61" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F61" t="s">
-        <v>203</v>
-      </c>
-      <c r="G61" t="s">
-        <v>204</v>
       </c>
       <c r="H61">
         <v>15</v>
@@ -4062,25 +4062,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" t="s">
+        <v>204</v>
+      </c>
+      <c r="C62" t="s">
+        <v>168</v>
+      </c>
+      <c r="D62" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" t="s">
         <v>205</v>
       </c>
-      <c r="B62" t="s">
+      <c r="G62" t="s">
         <v>206</v>
-      </c>
-      <c r="C62" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" t="s">
-        <v>171</v>
-      </c>
-      <c r="E62" t="s">
-        <v>20</v>
-      </c>
-      <c r="F62" t="s">
-        <v>207</v>
-      </c>
-      <c r="G62" t="s">
-        <v>208</v>
       </c>
       <c r="H62">
         <v>6</v>
@@ -4095,25 +4095,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" t="s">
+        <v>168</v>
+      </c>
+      <c r="D63" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" t="s">
         <v>209</v>
       </c>
-      <c r="B63" t="s">
+      <c r="G63" t="s">
         <v>210</v>
-      </c>
-      <c r="C63" t="s">
-        <v>170</v>
-      </c>
-      <c r="D63" t="s">
-        <v>171</v>
-      </c>
-      <c r="E63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" t="s">
-        <v>211</v>
-      </c>
-      <c r="G63" t="s">
-        <v>212</v>
       </c>
       <c r="H63">
         <v>3</v>
@@ -4128,25 +4128,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>211</v>
+      </c>
+      <c r="B64" t="s">
+        <v>212</v>
+      </c>
+      <c r="C64" t="s">
+        <v>168</v>
+      </c>
+      <c r="D64" t="s">
+        <v>169</v>
+      </c>
+      <c r="E64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" t="s">
         <v>213</v>
       </c>
-      <c r="B64" t="s">
+      <c r="G64" t="s">
         <v>214</v>
-      </c>
-      <c r="C64" t="s">
-        <v>170</v>
-      </c>
-      <c r="D64" t="s">
-        <v>171</v>
-      </c>
-      <c r="E64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" t="s">
-        <v>215</v>
-      </c>
-      <c r="G64" t="s">
-        <v>216</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4161,25 +4161,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>215</v>
+      </c>
+      <c r="B65" t="s">
+        <v>216</v>
+      </c>
+      <c r="C65" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" t="s">
         <v>217</v>
       </c>
-      <c r="B65" t="s">
+      <c r="G65" t="s">
         <v>218</v>
-      </c>
-      <c r="C65" t="s">
-        <v>170</v>
-      </c>
-      <c r="D65" t="s">
-        <v>171</v>
-      </c>
-      <c r="E65" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" t="s">
-        <v>219</v>
-      </c>
-      <c r="G65" t="s">
-        <v>220</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -4194,25 +4194,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B66" t="s">
+        <v>220</v>
+      </c>
+      <c r="C66" t="s">
+        <v>168</v>
+      </c>
+      <c r="D66" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" t="s">
         <v>221</v>
       </c>
-      <c r="B66" t="s">
+      <c r="G66" t="s">
         <v>222</v>
-      </c>
-      <c r="C66" t="s">
-        <v>170</v>
-      </c>
-      <c r="D66" t="s">
-        <v>171</v>
-      </c>
-      <c r="E66" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" t="s">
-        <v>223</v>
-      </c>
-      <c r="G66" t="s">
-        <v>224</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4227,25 +4227,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B67">
         <v>0.3</v>
       </c>
       <c r="C67" t="s">
+        <v>224</v>
+      </c>
+      <c r="D67" t="s">
+        <v>225</v>
+      </c>
+      <c r="E67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" t="s">
         <v>226</v>
       </c>
-      <c r="D67" t="s">
+      <c r="G67" t="s">
         <v>227</v>
-      </c>
-      <c r="E67" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67" t="s">
-        <v>228</v>
-      </c>
-      <c r="G67" t="s">
-        <v>229</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -4260,25 +4260,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>228</v>
+      </c>
+      <c r="B68" t="s">
+        <v>229</v>
+      </c>
+      <c r="C68" t="s">
+        <v>168</v>
+      </c>
+      <c r="D68" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" t="s">
         <v>230</v>
       </c>
-      <c r="B68" t="s">
+      <c r="G68" t="s">
         <v>231</v>
-      </c>
-      <c r="C68" t="s">
-        <v>170</v>
-      </c>
-      <c r="D68" t="s">
-        <v>171</v>
-      </c>
-      <c r="E68" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" t="s">
-        <v>232</v>
-      </c>
-      <c r="G68" t="s">
-        <v>233</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4293,25 +4293,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" t="s">
+        <v>233</v>
+      </c>
+      <c r="C69" t="s">
+        <v>168</v>
+      </c>
+      <c r="D69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" t="s">
         <v>234</v>
       </c>
-      <c r="B69" t="s">
+      <c r="G69" t="s">
         <v>235</v>
-      </c>
-      <c r="C69" t="s">
-        <v>170</v>
-      </c>
-      <c r="D69" t="s">
-        <v>171</v>
-      </c>
-      <c r="E69" t="s">
-        <v>20</v>
-      </c>
-      <c r="F69" t="s">
-        <v>236</v>
-      </c>
-      <c r="G69" t="s">
-        <v>237</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4326,25 +4326,25 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>236</v>
+      </c>
+      <c r="B70" t="s">
+        <v>237</v>
+      </c>
+      <c r="C70" t="s">
+        <v>168</v>
+      </c>
+      <c r="D70" t="s">
+        <v>169</v>
+      </c>
+      <c r="E70" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70" t="s">
         <v>238</v>
       </c>
-      <c r="B70" t="s">
+      <c r="G70" t="s">
         <v>239</v>
-      </c>
-      <c r="C70" t="s">
-        <v>170</v>
-      </c>
-      <c r="D70" t="s">
-        <v>171</v>
-      </c>
-      <c r="E70" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" t="s">
-        <v>240</v>
-      </c>
-      <c r="G70" t="s">
-        <v>241</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4359,16 +4359,16 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B71" t="s">
         <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D71" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E71" t="s">
         <v>20</v>
@@ -4386,25 +4386,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>241</v>
+      </c>
+      <c r="B72" t="s">
+        <v>242</v>
+      </c>
+      <c r="C72" t="s">
+        <v>168</v>
+      </c>
+      <c r="D72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" t="s">
         <v>243</v>
       </c>
-      <c r="B72" t="s">
+      <c r="G72" t="s">
         <v>244</v>
-      </c>
-      <c r="C72" t="s">
-        <v>170</v>
-      </c>
-      <c r="D72" t="s">
-        <v>171</v>
-      </c>
-      <c r="E72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" t="s">
-        <v>245</v>
-      </c>
-      <c r="G72" t="s">
-        <v>246</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4419,25 +4419,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B73" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C73" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D73" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
       <c r="F73" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G73" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4452,25 +4452,25 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C74" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D74" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E74" t="s">
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G74" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4485,25 +4485,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>249</v>
+      </c>
+      <c r="B75" t="s">
+        <v>250</v>
+      </c>
+      <c r="C75" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" t="s">
+        <v>169</v>
+      </c>
+      <c r="E75" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" t="s">
         <v>251</v>
       </c>
-      <c r="B75" t="s">
+      <c r="G75" t="s">
         <v>252</v>
-      </c>
-      <c r="C75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D75" t="s">
-        <v>171</v>
-      </c>
-      <c r="E75" t="s">
-        <v>20</v>
-      </c>
-      <c r="F75" t="s">
-        <v>253</v>
-      </c>
-      <c r="G75" t="s">
-        <v>254</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4518,25 +4518,25 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>253</v>
+      </c>
+      <c r="B76" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" t="s">
         <v>255</v>
       </c>
-      <c r="B76" t="s">
+      <c r="G76" t="s">
         <v>256</v>
-      </c>
-      <c r="C76" t="s">
-        <v>170</v>
-      </c>
-      <c r="D76" t="s">
-        <v>171</v>
-      </c>
-      <c r="E76" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" t="s">
-        <v>257</v>
-      </c>
-      <c r="G76" t="s">
-        <v>258</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4551,25 +4551,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>257</v>
+      </c>
+      <c r="B77" t="s">
+        <v>258</v>
+      </c>
+      <c r="C77" t="s">
+        <v>258</v>
+      </c>
+      <c r="D77" t="s">
         <v>259</v>
       </c>
-      <c r="B77" t="s">
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
         <v>260</v>
       </c>
-      <c r="C77" t="s">
-        <v>260</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="G77" t="s">
         <v>261</v>
-      </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" t="s">
-        <v>262</v>
-      </c>
-      <c r="G77" t="s">
-        <v>263</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4584,25 +4584,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>262</v>
+      </c>
+      <c r="B78" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78" t="s">
+        <v>263</v>
+      </c>
+      <c r="D78" t="s">
         <v>264</v>
       </c>
-      <c r="B78" t="s">
+      <c r="E78" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" t="s">
         <v>265</v>
       </c>
-      <c r="C78" t="s">
-        <v>265</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="G78" t="s">
         <v>266</v>
-      </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="F78" t="s">
-        <v>267</v>
-      </c>
-      <c r="G78" t="s">
-        <v>268</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4617,25 +4617,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>267</v>
+      </c>
+      <c r="B79" t="s">
+        <v>268</v>
+      </c>
+      <c r="C79" t="s">
         <v>269</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>270</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" t="s">
         <v>271</v>
       </c>
-      <c r="D79" t="s">
+      <c r="G79" t="s">
         <v>272</v>
-      </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" t="s">
-        <v>273</v>
-      </c>
-      <c r="G79" t="s">
-        <v>274</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4650,25 +4650,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>273</v>
+      </c>
+      <c r="B80" t="s">
+        <v>274</v>
+      </c>
+      <c r="C80" t="s">
         <v>275</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>276</v>
       </c>
-      <c r="C80" t="s">
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" t="s">
         <v>277</v>
       </c>
-      <c r="D80" t="s">
+      <c r="G80" t="s">
         <v>278</v>
-      </c>
-      <c r="E80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F80" t="s">
-        <v>279</v>
-      </c>
-      <c r="G80" t="s">
-        <v>280</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4683,25 +4683,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>279</v>
+      </c>
+      <c r="B81" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" t="s">
+        <v>280</v>
+      </c>
+      <c r="D81" t="s">
         <v>281</v>
       </c>
-      <c r="B81" t="s">
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" t="s">
         <v>282</v>
       </c>
-      <c r="C81" t="s">
-        <v>282</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="G81" t="s">
         <v>283</v>
-      </c>
-      <c r="E81" t="s">
-        <v>20</v>
-      </c>
-      <c r="F81" t="s">
-        <v>284</v>
-      </c>
-      <c r="G81" t="s">
-        <v>285</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4716,25 +4716,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>284</v>
+      </c>
+      <c r="B82" t="s">
+        <v>285</v>
+      </c>
+      <c r="C82" t="s">
+        <v>285</v>
+      </c>
+      <c r="D82" t="s">
         <v>286</v>
       </c>
-      <c r="B82" t="s">
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" t="s">
         <v>287</v>
       </c>
-      <c r="C82" t="s">
-        <v>287</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="G82" t="s">
         <v>288</v>
-      </c>
-      <c r="E82" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" t="s">
-        <v>289</v>
-      </c>
-      <c r="G82" t="s">
-        <v>290</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4749,25 +4749,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>289</v>
+      </c>
+      <c r="B83" t="s">
+        <v>290</v>
+      </c>
+      <c r="C83" t="s">
+        <v>290</v>
+      </c>
+      <c r="D83" t="s">
         <v>291</v>
       </c>
-      <c r="B83" t="s">
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" t="s">
         <v>292</v>
       </c>
-      <c r="C83" t="s">
-        <v>292</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="G83" t="s">
         <v>293</v>
-      </c>
-      <c r="E83" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" t="s">
-        <v>294</v>
-      </c>
-      <c r="G83" t="s">
-        <v>295</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4782,25 +4782,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>294</v>
+      </c>
+      <c r="B84" t="s">
+        <v>295</v>
+      </c>
+      <c r="C84" t="s">
+        <v>295</v>
+      </c>
+      <c r="D84" t="s">
         <v>296</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" t="s">
         <v>297</v>
       </c>
-      <c r="C84" t="s">
-        <v>297</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="G84" t="s">
         <v>298</v>
-      </c>
-      <c r="E84" t="s">
-        <v>20</v>
-      </c>
-      <c r="F84" t="s">
-        <v>299</v>
-      </c>
-      <c r="G84" t="s">
-        <v>300</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4815,25 +4815,25 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>299</v>
+      </c>
+      <c r="B85" t="s">
+        <v>300</v>
+      </c>
+      <c r="C85" t="s">
+        <v>300</v>
+      </c>
+      <c r="D85" t="s">
         <v>301</v>
       </c>
-      <c r="B85" t="s">
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" t="s">
         <v>302</v>
       </c>
-      <c r="C85" t="s">
-        <v>302</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="G85" t="s">
         <v>303</v>
-      </c>
-      <c r="E85" t="s">
-        <v>20</v>
-      </c>
-      <c r="F85" t="s">
-        <v>304</v>
-      </c>
-      <c r="G85" t="s">
-        <v>305</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4848,16 +4848,16 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>304</v>
+      </c>
+      <c r="B86" t="s">
+        <v>305</v>
+      </c>
+      <c r="C86" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" t="s">
         <v>306</v>
-      </c>
-      <c r="B86" t="s">
-        <v>307</v>
-      </c>
-      <c r="C86" t="s">
-        <v>307</v>
-      </c>
-      <c r="D86" t="s">
-        <v>308</v>
       </c>
       <c r="G86" t="s">
         <v>15</v>
@@ -4870,30 +4870,30 @@
         <v>0</v>
       </c>
       <c r="K86" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>308</v>
+      </c>
+      <c r="B87" t="s">
+        <v>309</v>
+      </c>
+      <c r="C87" t="s">
+        <v>309</v>
+      </c>
+      <c r="D87" t="s">
         <v>310</v>
       </c>
-      <c r="B87" t="s">
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" t="s">
         <v>311</v>
       </c>
-      <c r="C87" t="s">
-        <v>311</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>312</v>
-      </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>313</v>
-      </c>
-      <c r="G87" t="s">
-        <v>314</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4908,25 +4908,25 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>313</v>
+      </c>
+      <c r="B88" t="s">
+        <v>314</v>
+      </c>
+      <c r="C88" t="s">
+        <v>314</v>
+      </c>
+      <c r="D88" t="s">
         <v>315</v>
       </c>
-      <c r="B88" t="s">
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" t="s">
         <v>316</v>
       </c>
-      <c r="C88" t="s">
-        <v>316</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="G88" t="s">
         <v>317</v>
-      </c>
-      <c r="E88" t="s">
-        <v>20</v>
-      </c>
-      <c r="F88" t="s">
-        <v>318</v>
-      </c>
-      <c r="G88" t="s">
-        <v>319</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -4941,25 +4941,25 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>318</v>
+      </c>
+      <c r="B89" t="s">
+        <v>319</v>
+      </c>
+      <c r="C89" t="s">
+        <v>319</v>
+      </c>
+      <c r="D89" t="s">
         <v>320</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" t="s">
         <v>321</v>
       </c>
-      <c r="C89" t="s">
-        <v>321</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="G89" t="s">
         <v>322</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>323</v>
-      </c>
-      <c r="G89" t="s">
-        <v>324</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -4974,25 +4974,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>323</v>
+      </c>
+      <c r="B90" t="s">
+        <v>324</v>
+      </c>
+      <c r="C90" t="s">
+        <v>324</v>
+      </c>
+      <c r="D90" t="s">
         <v>325</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" t="s">
         <v>326</v>
       </c>
-      <c r="C90" t="s">
-        <v>326</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="G90" t="s">
         <v>327</v>
-      </c>
-      <c r="E90" t="s">
-        <v>20</v>
-      </c>
-      <c r="F90" t="s">
-        <v>328</v>
-      </c>
-      <c r="G90" t="s">
-        <v>329</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5007,25 +5007,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>328</v>
+      </c>
+      <c r="B91" t="s">
+        <v>329</v>
+      </c>
+      <c r="C91" t="s">
+        <v>329</v>
+      </c>
+      <c r="D91" t="s">
         <v>330</v>
       </c>
-      <c r="B91" t="s">
+      <c r="E91" t="s">
         <v>331</v>
       </c>
-      <c r="C91" t="s">
-        <v>331</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="F91" t="s">
         <v>332</v>
       </c>
-      <c r="E91" t="s">
+      <c r="G91" t="s">
         <v>333</v>
-      </c>
-      <c r="F91" t="s">
-        <v>334</v>
-      </c>
-      <c r="G91" t="s">
-        <v>335</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5040,25 +5040,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>334</v>
+      </c>
+      <c r="B92" t="s">
+        <v>335</v>
+      </c>
+      <c r="C92" t="s">
+        <v>335</v>
+      </c>
+      <c r="D92" t="s">
         <v>336</v>
       </c>
-      <c r="B92" t="s">
+      <c r="E92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" t="s">
         <v>337</v>
       </c>
-      <c r="C92" t="s">
-        <v>337</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="G92" t="s">
         <v>338</v>
-      </c>
-      <c r="E92" t="s">
-        <v>20</v>
-      </c>
-      <c r="F92" t="s">
-        <v>339</v>
-      </c>
-      <c r="G92" t="s">
-        <v>340</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5073,16 +5073,16 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>339</v>
+      </c>
+      <c r="B93" t="s">
+        <v>340</v>
+      </c>
+      <c r="C93" t="s">
         <v>341</v>
       </c>
-      <c r="B93" t="s">
+      <c r="D93" t="s">
         <v>342</v>
-      </c>
-      <c r="C93" t="s">
-        <v>343</v>
-      </c>
-      <c r="D93" t="s">
-        <v>344</v>
       </c>
       <c r="G93" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
AMS-39101 octal driver schematic added (U15).
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="421">
   <si>
     <t>Part</t>
   </si>
@@ -79,9 +79,6 @@
     <t>DK</t>
   </si>
   <si>
-    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56</t>
-  </si>
-  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -1250,6 +1247,36 @@
   </si>
   <si>
     <t>ESPM02200</t>
+  </si>
+  <si>
+    <t>C57</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>445-1310-1-ND</t>
+  </si>
+  <si>
+    <t>C1608X7R1H472K</t>
+  </si>
+  <si>
+    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C58, C59, C60, C61, C62, C63, C64, C65, C66, C67</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>AMIS-39101</t>
+  </si>
+  <si>
+    <t>766-1004-1-ND</t>
+  </si>
+  <si>
+    <t>SO-28W</t>
+  </si>
+  <si>
+    <t>AMIS39101PNPB4RG</t>
   </si>
 </sst>
 </file>
@@ -2078,10 +2105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2157,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2150,10 +2177,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G2" t="s">
         <v>360</v>
-      </c>
-      <c r="G2" t="s">
-        <v>361</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2166,8 +2193,8 @@
         <v>0.27</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J101)</f>
-        <v>167.81719999999999</v>
+        <f>SUM(J2:J103)</f>
+        <v>174.96719999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2187,10 +2214,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G3" t="s">
         <v>362</v>
-      </c>
-      <c r="G3" t="s">
-        <v>363</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2199,16 +2226,16 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J67" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J68" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -2220,28 +2247,28 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>363</v>
+      </c>
+      <c r="G4" t="s">
         <v>364</v>
       </c>
-      <c r="G4" t="s">
-        <v>365</v>
-      </c>
       <c r="H4">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="I4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.48300000000000004</v>
+        <v>0.69300000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -2262,10 +2289,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -2277,10 +2304,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G6" t="s">
         <v>369</v>
-      </c>
-      <c r="G6" t="s">
-        <v>370</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2293,15 +2320,15 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -2322,25 +2349,25 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s">
+        <v>370</v>
+      </c>
+      <c r="G8" t="s">
         <v>371</v>
-      </c>
-      <c r="G8" t="s">
-        <v>372</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2355,25 +2382,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
       <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
+        <v>372</v>
+      </c>
+      <c r="G9" t="s">
         <v>373</v>
-      </c>
-      <c r="G9" t="s">
-        <v>374</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2388,10 +2415,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -2403,10 +2430,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
+        <v>384</v>
+      </c>
+      <c r="G10" t="s">
         <v>385</v>
-      </c>
-      <c r="G10" t="s">
-        <v>386</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2419,15 +2446,15 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2439,10 +2466,10 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
         <v>38</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -2457,10 +2484,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -2472,10 +2499,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
+        <v>386</v>
+      </c>
+      <c r="G12" t="s">
         <v>387</v>
-      </c>
-      <c r="G12" t="s">
-        <v>388</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2490,10 +2517,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -2505,10 +2532,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
+        <v>384</v>
+      </c>
+      <c r="G13" t="s">
         <v>385</v>
-      </c>
-      <c r="G13" t="s">
-        <v>386</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2521,15 +2548,15 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -2541,10 +2568,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
+        <v>390</v>
+      </c>
+      <c r="G14" t="s">
         <v>391</v>
-      </c>
-      <c r="G14" t="s">
-        <v>392</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2557,15 +2584,15 @@
         <v>0.17</v>
       </c>
       <c r="L14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -2577,10 +2604,10 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
+        <v>393</v>
+      </c>
+      <c r="G15" t="s">
         <v>394</v>
-      </c>
-      <c r="G15" t="s">
-        <v>395</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2593,21 +2620,21 @@
         <v>0.48</v>
       </c>
       <c r="L15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
       </c>
       <c r="G16" t="s">
         <v>15</v>
@@ -2622,25 +2649,25 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
       <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17" t="s">
+        <v>374</v>
+      </c>
+      <c r="G17" t="s">
         <v>375</v>
-      </c>
-      <c r="G17" t="s">
-        <v>376</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2655,10 +2682,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -2679,16 +2706,16 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>58</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
@@ -2703,25 +2730,25 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
         <v>60</v>
       </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
       <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
-        <v>32</v>
-      </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20" t="s">
+        <v>376</v>
+      </c>
+      <c r="G20" t="s">
         <v>377</v>
-      </c>
-      <c r="G20" t="s">
-        <v>378</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2734,30 +2761,30 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
       <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
       <c r="E21" t="s">
         <v>20</v>
       </c>
       <c r="F21" t="s">
+        <v>379</v>
+      </c>
+      <c r="G21" t="s">
         <v>380</v>
-      </c>
-      <c r="G21" t="s">
-        <v>381</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2772,16 +2799,16 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
       <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
         <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
       </c>
       <c r="G22" t="s">
         <v>15</v>
@@ -2796,10 +2823,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
         <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -2811,10 +2838,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
+        <v>381</v>
+      </c>
+      <c r="G23" t="s">
         <v>382</v>
-      </c>
-      <c r="G23" t="s">
-        <v>383</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2829,335 +2856,338 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>411</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>412</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>413</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>414</v>
       </c>
       <c r="H24">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>0.315</v>
+        <v>0.1</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>8.19</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
         <v>70</v>
       </c>
-      <c r="E25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>358</v>
-      </c>
       <c r="G25" t="s">
-        <v>359</v>
+        <v>68</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="I25">
-        <v>0.35</v>
+        <v>0.315</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>403</v>
+        <v>357</v>
       </c>
       <c r="G26" t="s">
-        <v>404</v>
+        <v>358</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L26" t="s">
-        <v>409</v>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
         <v>76</v>
       </c>
-      <c r="D27" t="s">
-        <v>77</v>
-      </c>
       <c r="E27" t="s">
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="G27" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0.68</v>
+        <v>0.4</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
         <v>76</v>
       </c>
-      <c r="D28" t="s">
-        <v>77</v>
-      </c>
       <c r="E28" t="s">
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G28" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
         <v>76</v>
       </c>
-      <c r="D29" t="s">
-        <v>77</v>
-      </c>
       <c r="E29" t="s">
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G29" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>0.9</v>
+        <v>0.42</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="L29" t="s">
-        <v>402</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>399</v>
       </c>
       <c r="G30" t="s">
-        <v>344</v>
+        <v>400</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
       <c r="I30">
-        <v>11.91</v>
+        <v>0.9</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>2.7</v>
+      </c>
+      <c r="L30" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>411</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>411</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>411</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>410</v>
+        <v>342</v>
       </c>
       <c r="G31" t="s">
-        <v>411</v>
+        <v>343</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31">
-        <v>2.15</v>
+        <v>11.91</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>410</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>410</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>90</v>
+        <v>409</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>410</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>0.77</v>
+        <v>2.15</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>406</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E33" t="s">
-        <v>331</v>
+        <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>408</v>
+        <v>89</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3165,23 +3195,20 @@
         <v>405</v>
       </c>
       <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" t="s">
         <v>91</v>
       </c>
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" t="s">
-        <v>92</v>
-      </c>
       <c r="E34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F34" t="s">
         <v>407</v>
       </c>
-      <c r="G34" t="s">
-        <v>15</v>
-      </c>
       <c r="H34">
         <v>2</v>
       </c>
@@ -3195,595 +3222,595 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>404</v>
       </c>
       <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" t="s">
+        <v>330</v>
+      </c>
+      <c r="F35" t="s">
+        <v>406</v>
+      </c>
+      <c r="G35" t="s">
         <v>15</v>
-      </c>
-      <c r="C35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" t="s">
-        <v>95</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" t="s">
-        <v>97</v>
       </c>
       <c r="H35">
         <v>2</v>
       </c>
       <c r="I35">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>356</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>355</v>
       </c>
       <c r="G37" t="s">
-        <v>107</v>
+        <v>356</v>
       </c>
       <c r="H37">
         <v>3</v>
       </c>
       <c r="I37">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L37" t="s">
-        <v>367</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
         <v>105</v>
       </c>
-      <c r="D38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>106</v>
       </c>
-      <c r="G38" t="s">
-        <v>107</v>
-      </c>
       <c r="H38">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I38">
         <v>0.42</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>1.26</v>
+      </c>
+      <c r="L38" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
         <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I39">
-        <v>3.65</v>
+        <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>114</v>
+        <v>108</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="s">
+        <v>109</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="H40">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>3.65</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>118</v>
-      </c>
-      <c r="E41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G41" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
-        <v>2.13</v>
+        <v>5</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G42" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G43" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G44" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>135</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>136</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="H45">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1.85</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G46" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
       <c r="H46">
-        <v>25</v>
-      </c>
-      <c r="I46">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G47" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I47">
-        <v>0.84</v>
+        <v>0.3</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D48" t="s">
-        <v>156</v>
+        <v>15</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
+        <v>150</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="H48">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>0.84</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G49" t="s">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G50" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D51" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="E51" t="s">
         <v>20</v>
       </c>
       <c r="F51" t="s">
-        <v>345</v>
+        <v>163</v>
       </c>
       <c r="G51" t="s">
-        <v>346</v>
+        <v>164</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" t="s">
         <v>168</v>
       </c>
-      <c r="D52" t="s">
-        <v>169</v>
-      </c>
       <c r="E52" t="s">
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>172</v>
+        <v>344</v>
       </c>
       <c r="G52" t="s">
-        <v>173</v>
+        <v>345</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
-      </c>
-      <c r="B53">
-        <v>470</v>
+        <v>169</v>
+      </c>
+      <c r="B53" t="s">
+        <v>170</v>
       </c>
       <c r="C53" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" t="s">
         <v>168</v>
       </c>
-      <c r="D53" t="s">
-        <v>169</v>
-      </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G53" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3798,124 +3825,124 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>177</v>
-      </c>
-      <c r="B54" t="s">
-        <v>178</v>
+        <v>173</v>
+      </c>
+      <c r="B54">
+        <v>470</v>
       </c>
       <c r="C54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" t="s">
         <v>168</v>
       </c>
-      <c r="D54" t="s">
-        <v>169</v>
-      </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G54" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H54">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="I54">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.81420000000000003</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" t="s">
         <v>168</v>
       </c>
-      <c r="D55" t="s">
-        <v>169</v>
-      </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G55" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="I55">
-        <v>0.04</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.81420000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B56" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
-        <v>347</v>
+        <v>167</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="E56" t="s">
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>348</v>
+        <v>182</v>
       </c>
       <c r="G56" t="s">
-        <v>349</v>
+        <v>183</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I56">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C57" t="s">
+        <v>346</v>
+      </c>
+      <c r="D57" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" t="s">
         <v>347</v>
       </c>
-      <c r="D57" t="s">
-        <v>124</v>
-      </c>
-      <c r="E57" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" t="s">
-        <v>354</v>
-      </c>
       <c r="G57" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3930,289 +3957,289 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B58" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C58" t="s">
-        <v>168</v>
+        <v>346</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
+        <v>353</v>
       </c>
       <c r="G58" t="s">
-        <v>192</v>
+        <v>354</v>
       </c>
       <c r="H58">
         <v>1</v>
       </c>
       <c r="I58">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>193</v>
-      </c>
-      <c r="B59">
-        <v>200</v>
+        <v>188</v>
+      </c>
+      <c r="B59" t="s">
+        <v>189</v>
       </c>
       <c r="C59" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" t="s">
         <v>168</v>
       </c>
-      <c r="D59" t="s">
-        <v>169</v>
-      </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G59" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H59">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B60">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
         <v>168</v>
       </c>
-      <c r="D60" t="s">
-        <v>169</v>
-      </c>
       <c r="E60" t="s">
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G60" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H60">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I60">
         <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>199</v>
-      </c>
-      <c r="B61" t="s">
-        <v>200</v>
+        <v>195</v>
+      </c>
+      <c r="B61">
+        <v>100</v>
       </c>
       <c r="C61" t="s">
+        <v>167</v>
+      </c>
+      <c r="D61" t="s">
         <v>168</v>
       </c>
-      <c r="D61" t="s">
-        <v>169</v>
-      </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G61" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H61">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I61">
         <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B62" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C62" t="s">
+        <v>167</v>
+      </c>
+      <c r="D62" t="s">
         <v>168</v>
       </c>
-      <c r="D62" t="s">
-        <v>169</v>
-      </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G62" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H62">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D63" t="s">
         <v>168</v>
       </c>
-      <c r="D63" t="s">
-        <v>169</v>
-      </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G63" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H63">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D64" t="s">
         <v>168</v>
       </c>
-      <c r="D64" t="s">
-        <v>169</v>
-      </c>
       <c r="E64" t="s">
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G64" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" t="s">
         <v>168</v>
       </c>
-      <c r="D65" t="s">
-        <v>169</v>
-      </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G65" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B66" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C66" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" t="s">
         <v>168</v>
       </c>
-      <c r="D66" t="s">
-        <v>169</v>
-      </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G66" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4227,91 +4254,91 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>223</v>
-      </c>
-      <c r="B67">
-        <v>0.3</v>
+        <v>218</v>
+      </c>
+      <c r="B67" t="s">
+        <v>219</v>
       </c>
       <c r="C67" t="s">
-        <v>224</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>225</v>
+        <v>168</v>
       </c>
       <c r="E67" t="s">
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G67" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>228</v>
-      </c>
-      <c r="B68" t="s">
-        <v>229</v>
+        <v>222</v>
+      </c>
+      <c r="B68">
+        <v>0.3</v>
       </c>
       <c r="C68" t="s">
-        <v>168</v>
+        <v>223</v>
       </c>
       <c r="D68" t="s">
-        <v>169</v>
+        <v>224</v>
       </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G68" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H68">
         <v>1</v>
       </c>
       <c r="I68">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J68">
-        <f t="shared" ref="J68:J93" si="1">H68*I68</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B69" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D69" t="s">
         <v>168</v>
       </c>
-      <c r="D69" t="s">
-        <v>169</v>
-      </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G69" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4320,31 +4347,31 @@
         <v>0.04</v>
       </c>
       <c r="J69">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J69:J95" si="1">H69*I69</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C70" t="s">
+        <v>167</v>
+      </c>
+      <c r="D70" t="s">
         <v>168</v>
       </c>
-      <c r="D70" t="s">
-        <v>169</v>
-      </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G70" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4359,118 +4386,118 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>236</v>
       </c>
       <c r="C71" t="s">
+        <v>167</v>
+      </c>
+      <c r="D71" t="s">
         <v>168</v>
       </c>
-      <c r="D71" t="s">
-        <v>169</v>
-      </c>
       <c r="E71" t="s">
         <v>20</v>
       </c>
+      <c r="F71" t="s">
+        <v>237</v>
+      </c>
       <c r="G71" t="s">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="H71">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B72" t="s">
-        <v>242</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" t="s">
         <v>168</v>
       </c>
-      <c r="D72" t="s">
-        <v>169</v>
-      </c>
       <c r="E72" t="s">
         <v>20</v>
       </c>
-      <c r="F72" t="s">
-        <v>243</v>
-      </c>
       <c r="G72" t="s">
-        <v>244</v>
+        <v>15</v>
       </c>
       <c r="H72">
-        <v>1</v>
-      </c>
-      <c r="I72">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J72">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B73" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C73" t="s">
-        <v>347</v>
+        <v>167</v>
       </c>
       <c r="D73" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
       <c r="F73" t="s">
-        <v>350</v>
+        <v>242</v>
       </c>
       <c r="G73" t="s">
-        <v>351</v>
+        <v>243</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B74" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C74" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E74" t="s">
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G74" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4485,58 +4512,58 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B75" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>346</v>
       </c>
       <c r="D75" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>251</v>
+        <v>351</v>
       </c>
       <c r="G75" t="s">
-        <v>252</v>
+        <v>352</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B76" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C76" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" t="s">
         <v>168</v>
       </c>
-      <c r="D76" t="s">
-        <v>169</v>
-      </c>
       <c r="E76" t="s">
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="G76" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4551,546 +4578,612 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B77" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C77" t="s">
-        <v>258</v>
+        <v>167</v>
       </c>
       <c r="D77" t="s">
-        <v>259</v>
+        <v>168</v>
       </c>
       <c r="E77" t="s">
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G77" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B78" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C78" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D78" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E78" t="s">
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G78" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B79" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C79" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D79" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G79" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B80" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C80" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D80" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G80" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B81" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C81" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D81" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G81" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B82" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C82" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D82" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="G82" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B83" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C83" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D83" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="G83" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B84" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C84" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D84" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="G84" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B85" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C85" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D85" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="G85" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B86" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C86" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D86" t="s">
-        <v>306</v>
+        <v>300</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" t="s">
+        <v>301</v>
       </c>
       <c r="G86" t="s">
-        <v>15</v>
+        <v>302</v>
       </c>
       <c r="H86">
         <v>1</v>
+      </c>
+      <c r="I86">
+        <v>1.51</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K86" t="s">
-        <v>307</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B87" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C87" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D87" t="s">
-        <v>310</v>
-      </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="G87" t="s">
-        <v>312</v>
+        <v>15</v>
       </c>
       <c r="H87">
         <v>1</v>
-      </c>
-      <c r="I87">
-        <v>0.47</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K87" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B88" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C88" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D88" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E88" t="s">
         <v>20</v>
       </c>
       <c r="F88" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G88" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B89" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C89" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D89" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E89" t="s">
         <v>20</v>
       </c>
       <c r="F89" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G89" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B90" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C90" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D90" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E90" t="s">
         <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="G90" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B91" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C91" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D91" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E91" t="s">
-        <v>331</v>
+        <v>20</v>
       </c>
       <c r="F91" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="G91" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>1.5</v>
+        <v>12.95</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>12.95</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>334</v>
+        <v>416</v>
       </c>
       <c r="B92" t="s">
-        <v>335</v>
+        <v>417</v>
       </c>
       <c r="C92" t="s">
-        <v>335</v>
+        <v>417</v>
       </c>
       <c r="D92" t="s">
-        <v>336</v>
+        <v>419</v>
       </c>
       <c r="E92" t="s">
         <v>20</v>
       </c>
       <c r="F92" t="s">
-        <v>337</v>
+        <v>418</v>
       </c>
       <c r="G92" t="s">
-        <v>338</v>
+        <v>420</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>2.96</v>
+        <v>6.84</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>327</v>
+      </c>
+      <c r="B93" t="s">
+        <v>328</v>
+      </c>
+      <c r="C93" t="s">
+        <v>328</v>
+      </c>
+      <c r="D93" t="s">
+        <v>329</v>
+      </c>
+      <c r="E93" t="s">
+        <v>330</v>
+      </c>
+      <c r="F93" t="s">
+        <v>331</v>
+      </c>
+      <c r="G93" t="s">
+        <v>332</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>1.5</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>333</v>
+      </c>
+      <c r="B94" t="s">
+        <v>334</v>
+      </c>
+      <c r="C94" t="s">
+        <v>334</v>
+      </c>
+      <c r="D94" t="s">
+        <v>335</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94" t="s">
+        <v>336</v>
+      </c>
+      <c r="G94" t="s">
+        <v>337</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>2.96</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>338</v>
+      </c>
+      <c r="B95" t="s">
         <v>339</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C95" t="s">
         <v>340</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D95" t="s">
         <v>341</v>
       </c>
-      <c r="D93" t="s">
-        <v>342</v>
-      </c>
-      <c r="G93" t="s">
+      <c r="G95" t="s">
         <v>15</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="J93">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added JP25 to BOM.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="426">
   <si>
     <t>Part</t>
   </si>
@@ -1277,6 +1277,21 @@
   </si>
   <si>
     <t>AMIS39101PNPB4RG</t>
+  </si>
+  <si>
+    <t>JP25</t>
+  </si>
+  <si>
+    <t>PINHD-2X8</t>
+  </si>
+  <si>
+    <t>2X08</t>
+  </si>
+  <si>
+    <t>609-3364-ND</t>
+  </si>
+  <si>
+    <t>68602-116HLF</t>
   </si>
 </sst>
 </file>
@@ -2105,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,8 +2208,8 @@
         <v>0.27</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J103)</f>
-        <v>174.96719999999999</v>
+        <f>SUM(J2:J104)</f>
+        <v>175.6772</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2226,7 +2241,7 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J68" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J69" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
@@ -3447,292 +3462,289 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" t="s">
-        <v>115</v>
+        <v>421</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>422</v>
       </c>
       <c r="D42" t="s">
-        <v>117</v>
+        <v>423</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>424</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
+        <v>425</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
-        <v>2.13</v>
+        <v>0.71</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D43" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G43" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G44" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G45" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D46" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
+        <v>136</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="H46">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1.85</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
-      </c>
-      <c r="E47" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G47" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="H47">
-        <v>25</v>
-      </c>
-      <c r="I47">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G48" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I48">
-        <v>0.84</v>
+        <v>0.3</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C49" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>150</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="H49">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>0.84</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="D50" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G50" t="s">
-        <v>159</v>
+        <v>15</v>
       </c>
       <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D51" t="s">
         <v>144</v>
@@ -3741,61 +3753,61 @@
         <v>20</v>
       </c>
       <c r="F51" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G51" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>344</v>
+        <v>163</v>
       </c>
       <c r="G52" t="s">
-        <v>345</v>
+        <v>164</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B53" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C53" t="s">
         <v>167</v>
@@ -3807,28 +3819,28 @@
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>171</v>
+        <v>344</v>
       </c>
       <c r="G53" t="s">
-        <v>172</v>
+        <v>345</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>173</v>
-      </c>
-      <c r="B54">
-        <v>470</v>
+        <v>169</v>
+      </c>
+      <c r="B54" t="s">
+        <v>170</v>
       </c>
       <c r="C54" t="s">
         <v>167</v>
@@ -3840,10 +3852,10 @@
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G54" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3858,10 +3870,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>176</v>
-      </c>
-      <c r="B55" t="s">
-        <v>177</v>
+        <v>173</v>
+      </c>
+      <c r="B55">
+        <v>470</v>
       </c>
       <c r="C55" t="s">
         <v>167</v>
@@ -3873,28 +3885,28 @@
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G55" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H55">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="I55">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.81420000000000003</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C56" t="s">
         <v>167</v>
@@ -3906,61 +3918,61 @@
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G56" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H56">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="I56">
-        <v>0.04</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.81420000000000003</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>346</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>347</v>
+        <v>182</v>
       </c>
       <c r="G57" t="s">
-        <v>348</v>
+        <v>183</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I57">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B58" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C58" t="s">
         <v>346</v>
@@ -3972,10 +3984,10 @@
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G58" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -3990,43 +4002,43 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>346</v>
       </c>
       <c r="D59" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>190</v>
+        <v>353</v>
       </c>
       <c r="G59" t="s">
-        <v>191</v>
+        <v>354</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>192</v>
-      </c>
-      <c r="B60">
-        <v>200</v>
+        <v>188</v>
+      </c>
+      <c r="B60" t="s">
+        <v>189</v>
       </c>
       <c r="C60" t="s">
         <v>167</v>
@@ -4038,28 +4050,28 @@
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G60" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H60">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I60">
         <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B61">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C61" t="s">
         <v>167</v>
@@ -4071,28 +4083,28 @@
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G61" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H61">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I61">
         <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>198</v>
-      </c>
-      <c r="B62" t="s">
-        <v>199</v>
+        <v>195</v>
+      </c>
+      <c r="B62">
+        <v>100</v>
       </c>
       <c r="C62" t="s">
         <v>167</v>
@@ -4104,28 +4116,28 @@
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G62" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H62">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C63" t="s">
         <v>167</v>
@@ -4137,28 +4149,28 @@
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G63" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H63">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B64" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C64" t="s">
         <v>167</v>
@@ -4170,28 +4182,28 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G64" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H64">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C65" t="s">
         <v>167</v>
@@ -4203,28 +4215,28 @@
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G65" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B66" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C66" t="s">
         <v>167</v>
@@ -4236,28 +4248,28 @@
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G66" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B67" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C67" t="s">
         <v>167</v>
@@ -4269,10 +4281,10 @@
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G67" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -4287,76 +4299,76 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>222</v>
-      </c>
-      <c r="B68">
-        <v>0.3</v>
+        <v>218</v>
+      </c>
+      <c r="B68" t="s">
+        <v>219</v>
       </c>
       <c r="C68" t="s">
-        <v>223</v>
+        <v>167</v>
       </c>
       <c r="D68" t="s">
-        <v>224</v>
+        <v>168</v>
       </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G68" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H68">
         <v>1</v>
       </c>
       <c r="I68">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>227</v>
-      </c>
-      <c r="B69" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="B69">
+        <v>0.3</v>
       </c>
       <c r="C69" t="s">
-        <v>167</v>
+        <v>223</v>
       </c>
       <c r="D69" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G69" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H69">
         <v>1</v>
       </c>
       <c r="I69">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J69">
-        <f t="shared" ref="J69:J95" si="1">H69*I69</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B70" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C70" t="s">
         <v>167</v>
@@ -4368,10 +4380,10 @@
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G70" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4380,16 +4392,16 @@
         <v>0.04</v>
       </c>
       <c r="J70">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J70:J96" si="1">H70*I70</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B71" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C71" t="s">
         <v>167</v>
@@ -4401,10 +4413,10 @@
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G71" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4419,10 +4431,10 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
+        <v>236</v>
       </c>
       <c r="C72" t="s">
         <v>167</v>
@@ -4433,23 +4445,29 @@
       <c r="E72" t="s">
         <v>20</v>
       </c>
+      <c r="F72" t="s">
+        <v>237</v>
+      </c>
       <c r="G72" t="s">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="H72">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B73" t="s">
-        <v>241</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
         <v>167</v>
@@ -4460,62 +4478,56 @@
       <c r="E73" t="s">
         <v>20</v>
       </c>
-      <c r="F73" t="s">
-        <v>242</v>
-      </c>
       <c r="G73" t="s">
-        <v>243</v>
+        <v>15</v>
       </c>
       <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B74" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C74" t="s">
-        <v>346</v>
+        <v>167</v>
       </c>
       <c r="D74" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="E74" t="s">
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>349</v>
+        <v>242</v>
       </c>
       <c r="G74" t="s">
-        <v>350</v>
+        <v>243</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C75" t="s">
         <v>346</v>
@@ -4527,10 +4539,10 @@
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G75" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4545,43 +4557,43 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B76" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>346</v>
       </c>
       <c r="D76" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="E76" t="s">
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>250</v>
+        <v>351</v>
       </c>
       <c r="G76" t="s">
-        <v>251</v>
+        <v>352</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B77" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C77" t="s">
         <v>167</v>
@@ -4593,10 +4605,10 @@
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G77" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4611,579 +4623,612 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B78" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C78" t="s">
-        <v>257</v>
+        <v>167</v>
       </c>
       <c r="D78" t="s">
-        <v>258</v>
+        <v>168</v>
       </c>
       <c r="E78" t="s">
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G78" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B79" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C79" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D79" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G79" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B80" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C80" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D80" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G80" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B81" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C81" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D81" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G81" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B82" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C82" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D82" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G82" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B83" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C83" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D83" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G83" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B84" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C84" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D84" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G84" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B85" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C85" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D85" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G85" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B86" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C86" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D86" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E86" t="s">
         <v>20</v>
       </c>
       <c r="F86" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G86" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B87" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C87" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D87" t="s">
-        <v>305</v>
+        <v>300</v>
+      </c>
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" t="s">
+        <v>301</v>
       </c>
       <c r="G87" t="s">
-        <v>15</v>
+        <v>302</v>
       </c>
       <c r="H87">
         <v>1</v>
+      </c>
+      <c r="I87">
+        <v>1.51</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K87" t="s">
-        <v>306</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B88" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C88" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D88" t="s">
-        <v>309</v>
-      </c>
-      <c r="E88" t="s">
-        <v>20</v>
-      </c>
-      <c r="F88" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G88" t="s">
-        <v>311</v>
+        <v>15</v>
       </c>
       <c r="H88">
         <v>1</v>
-      </c>
-      <c r="I88">
-        <v>0.47</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K88" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B89" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C89" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D89" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E89" t="s">
         <v>20</v>
       </c>
       <c r="F89" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G89" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B90" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C90" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D90" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E90" t="s">
         <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="G90" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B91" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C91" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D91" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E91" t="s">
         <v>20</v>
       </c>
       <c r="F91" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="G91" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>416</v>
+        <v>322</v>
       </c>
       <c r="B92" t="s">
-        <v>417</v>
+        <v>323</v>
       </c>
       <c r="C92" t="s">
-        <v>417</v>
+        <v>323</v>
       </c>
       <c r="D92" t="s">
-        <v>419</v>
+        <v>324</v>
       </c>
       <c r="E92" t="s">
         <v>20</v>
       </c>
       <c r="F92" t="s">
-        <v>418</v>
+        <v>325</v>
       </c>
       <c r="G92" t="s">
-        <v>420</v>
+        <v>326</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>6.84</v>
+        <v>12.95</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>12.95</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>327</v>
+        <v>416</v>
       </c>
       <c r="B93" t="s">
-        <v>328</v>
+        <v>417</v>
       </c>
       <c r="C93" t="s">
-        <v>328</v>
+        <v>417</v>
       </c>
       <c r="D93" t="s">
-        <v>329</v>
+        <v>419</v>
       </c>
       <c r="E93" t="s">
-        <v>330</v>
+        <v>20</v>
       </c>
       <c r="F93" t="s">
-        <v>331</v>
+        <v>418</v>
       </c>
       <c r="G93" t="s">
-        <v>332</v>
+        <v>420</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B94" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C94" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D94" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E94" t="s">
-        <v>20</v>
+        <v>330</v>
       </c>
       <c r="F94" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G94" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>333</v>
+      </c>
+      <c r="B95" t="s">
+        <v>334</v>
+      </c>
+      <c r="C95" t="s">
+        <v>334</v>
+      </c>
+      <c r="D95" t="s">
+        <v>335</v>
+      </c>
+      <c r="E95" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" t="s">
+        <v>336</v>
+      </c>
+      <c r="G95" t="s">
+        <v>337</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>2.96</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>338</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>339</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>340</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>341</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>15</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="J95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Shuffled the names of JP22-JP30 so they line up nicely on the board.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="BOM-byvalue" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -325,9 +325,6 @@
     <t>1X03</t>
   </si>
   <si>
-    <t>JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19</t>
-  </si>
-  <si>
     <t>M03PTH</t>
   </si>
   <si>
@@ -349,9 +346,6 @@
     <t>HF-105-01-L-D-SM-LC</t>
   </si>
   <si>
-    <t>JP20, JP21, JP22, JP23, JP24</t>
-  </si>
-  <si>
     <t>M02PTH</t>
   </si>
   <si>
@@ -1279,9 +1273,6 @@
     <t>AMIS39101PNPB4RG</t>
   </si>
   <si>
-    <t>JP25</t>
-  </si>
-  <si>
     <t>PINHD-2X8</t>
   </si>
   <si>
@@ -1298,6 +1289,15 @@
   </si>
   <si>
     <t>XG8T-0231</t>
+  </si>
+  <si>
+    <t>JP20, JP21, JP22, JP29, JP30</t>
+  </si>
+  <si>
+    <t>JP23</t>
+  </si>
+  <si>
+    <t>JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19, JP24, JP25, JP26, JP27, JP28</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2178,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2198,10 +2198,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J104)</f>
-        <v>176.3272</v>
+        <v>178.4272</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2235,10 +2235,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2268,10 +2268,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2325,10 +2325,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2341,7 +2341,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2385,10 +2385,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2418,10 +2418,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2451,10 +2451,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2467,7 +2467,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2520,10 +2520,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2553,10 +2553,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2569,7 +2569,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2589,10 +2589,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2605,7 +2605,7 @@
         <v>0.17</v>
       </c>
       <c r="L14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2625,10 +2625,10 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2641,7 +2641,7 @@
         <v>0.48</v>
       </c>
       <c r="L15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2685,10 +2685,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2766,10 +2766,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G20" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2782,7 +2782,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L20" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2802,10 +2802,10 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G21" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2859,10 +2859,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2877,10 +2877,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B24" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
@@ -2892,10 +2892,10 @@
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G24" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2958,10 +2958,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -2991,10 +2991,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3007,7 +3007,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3027,10 +3027,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G28" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3060,10 +3060,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G29" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3093,10 +3093,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G30" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3109,7 +3109,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3129,10 +3129,10 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3150,22 +3150,22 @@
         <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C32" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D32" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G32" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B34" t="s">
         <v>90</v>
@@ -3225,10 +3225,10 @@
         <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F34" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B35" t="s">
         <v>90</v>
@@ -3255,10 +3255,10 @@
         <v>91</v>
       </c>
       <c r="E35" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F35" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G35" t="s">
         <v>15</v>
@@ -3324,10 +3324,10 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G37" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -3357,10 +3357,10 @@
         <v>20</v>
       </c>
       <c r="F38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G38" t="s">
         <v>105</v>
-      </c>
-      <c r="G38" t="s">
-        <v>106</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -3373,18 +3373,18 @@
         <v>1.26</v>
       </c>
       <c r="L38" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>427</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" t="s">
         <v>102</v>
@@ -3393,43 +3393,43 @@
         <v>20</v>
       </c>
       <c r="F39" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" t="s">
         <v>105</v>
       </c>
-      <c r="G39" t="s">
-        <v>106</v>
-      </c>
       <c r="H39">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I39">
         <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
         <v>107</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="s">
         <v>108</v>
       </c>
-      <c r="C40" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>109</v>
-      </c>
-      <c r="G40" t="s">
-        <v>110</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -3444,25 +3444,25 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>425</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G41" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="H41">
         <v>5</v>
@@ -3477,22 +3477,22 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>426</v>
+      </c>
+      <c r="C42" t="s">
+        <v>419</v>
+      </c>
+      <c r="D42" t="s">
+        <v>420</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
         <v>421</v>
       </c>
-      <c r="C42" t="s">
+      <c r="G42" t="s">
         <v>422</v>
-      </c>
-      <c r="D42" t="s">
-        <v>423</v>
-      </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
-        <v>424</v>
-      </c>
-      <c r="G42" t="s">
-        <v>425</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3507,25 +3507,25 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
         <v>114</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>115</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
         <v>116</v>
       </c>
-      <c r="D43" t="s">
+      <c r="G43" t="s">
         <v>117</v>
-      </c>
-      <c r="E43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" t="s">
-        <v>119</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3540,25 +3540,25 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
         <v>120</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>121</v>
       </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
         <v>122</v>
       </c>
-      <c r="D44" t="s">
+      <c r="G44" t="s">
         <v>123</v>
-      </c>
-      <c r="E44" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" t="s">
-        <v>124</v>
-      </c>
-      <c r="G44" t="s">
-        <v>125</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3573,25 +3573,25 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" t="s">
         <v>126</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>127</v>
       </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
         <v>128</v>
       </c>
-      <c r="D45" t="s">
+      <c r="G45" t="s">
         <v>129</v>
-      </c>
-      <c r="E45" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" t="s">
-        <v>130</v>
-      </c>
-      <c r="G45" t="s">
-        <v>131</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3606,25 +3606,25 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" t="s">
         <v>132</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>133</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
         <v>134</v>
       </c>
-      <c r="D46" t="s">
+      <c r="G46" t="s">
         <v>135</v>
-      </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" t="s">
-        <v>136</v>
-      </c>
-      <c r="G46" t="s">
-        <v>137</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -3639,16 +3639,16 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
         <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G47" t="s">
         <v>15</v>
@@ -3663,25 +3663,25 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" t="s">
         <v>141</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>142</v>
       </c>
-      <c r="C48" t="s">
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
         <v>143</v>
       </c>
-      <c r="D48" t="s">
+      <c r="G48" t="s">
         <v>144</v>
-      </c>
-      <c r="E48" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" t="s">
-        <v>146</v>
       </c>
       <c r="H48">
         <v>25</v>
@@ -3696,13 +3696,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
         <v>147</v>
-      </c>
-      <c r="B49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" t="s">
-        <v>149</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
@@ -3711,10 +3711,10 @@
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H49">
         <v>2</v>
@@ -3729,16 +3729,16 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" t="s">
         <v>152</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>153</v>
-      </c>
-      <c r="C50" t="s">
-        <v>154</v>
-      </c>
-      <c r="D50" t="s">
-        <v>155</v>
       </c>
       <c r="G50" t="s">
         <v>15</v>
@@ -3753,25 +3753,25 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" t="s">
+        <v>142</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" t="s">
         <v>156</v>
       </c>
-      <c r="B51" t="s">
+      <c r="G51" t="s">
         <v>157</v>
-      </c>
-      <c r="C51" t="s">
-        <v>143</v>
-      </c>
-      <c r="D51" t="s">
-        <v>144</v>
-      </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" t="s">
-        <v>158</v>
-      </c>
-      <c r="G51" t="s">
-        <v>159</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -3786,25 +3786,25 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" t="s">
         <v>160</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
+        <v>142</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" t="s">
         <v>161</v>
       </c>
-      <c r="C52" t="s">
+      <c r="G52" t="s">
         <v>162</v>
-      </c>
-      <c r="D52" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" t="s">
-        <v>163</v>
-      </c>
-      <c r="G52" t="s">
-        <v>164</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3819,25 +3819,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" t="s">
         <v>165</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>166</v>
       </c>
-      <c r="C53" t="s">
-        <v>167</v>
-      </c>
-      <c r="D53" t="s">
-        <v>168</v>
-      </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G53" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3852,25 +3852,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" t="s">
+        <v>168</v>
+      </c>
+      <c r="C54" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" t="s">
         <v>169</v>
       </c>
-      <c r="B54" t="s">
+      <c r="G54" t="s">
         <v>170</v>
-      </c>
-      <c r="C54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D54" t="s">
-        <v>168</v>
-      </c>
-      <c r="E54" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" t="s">
-        <v>171</v>
-      </c>
-      <c r="G54" t="s">
-        <v>172</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3885,25 +3885,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B55">
         <v>470</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G55" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3918,25 +3918,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" t="s">
+        <v>175</v>
+      </c>
+      <c r="C56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
         <v>176</v>
       </c>
-      <c r="B56" t="s">
+      <c r="G56" t="s">
         <v>177</v>
-      </c>
-      <c r="C56" t="s">
-        <v>167</v>
-      </c>
-      <c r="D56" t="s">
-        <v>168</v>
-      </c>
-      <c r="E56" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" t="s">
-        <v>178</v>
-      </c>
-      <c r="G56" t="s">
-        <v>179</v>
       </c>
       <c r="H56">
         <v>59</v>
@@ -3951,25 +3951,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" t="s">
+        <v>166</v>
+      </c>
+      <c r="E57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" t="s">
         <v>180</v>
       </c>
-      <c r="B57" t="s">
+      <c r="G57" t="s">
         <v>181</v>
-      </c>
-      <c r="C57" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" t="s">
-        <v>168</v>
-      </c>
-      <c r="E57" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" t="s">
-        <v>182</v>
-      </c>
-      <c r="G57" t="s">
-        <v>183</v>
       </c>
       <c r="H57">
         <v>4</v>
@@ -3984,25 +3984,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
+        <v>344</v>
+      </c>
+      <c r="D58" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" t="s">
+        <v>345</v>
+      </c>
+      <c r="G58" t="s">
         <v>346</v>
-      </c>
-      <c r="D58" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" t="s">
-        <v>347</v>
-      </c>
-      <c r="G58" t="s">
-        <v>348</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -4017,25 +4017,25 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G59" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4050,25 +4050,25 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" t="s">
         <v>188</v>
       </c>
-      <c r="B60" t="s">
+      <c r="G60" t="s">
         <v>189</v>
-      </c>
-      <c r="C60" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>168</v>
-      </c>
-      <c r="E60" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" t="s">
-        <v>190</v>
-      </c>
-      <c r="G60" t="s">
-        <v>191</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4083,25 +4083,25 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B61">
         <v>200</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G61" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H61">
         <v>24</v>
@@ -4116,25 +4116,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B62">
         <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G62" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H62">
         <v>10</v>
@@ -4149,25 +4149,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D63" t="s">
+        <v>166</v>
+      </c>
+      <c r="E63" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" t="s">
         <v>198</v>
       </c>
-      <c r="B63" t="s">
+      <c r="G63" t="s">
         <v>199</v>
-      </c>
-      <c r="C63" t="s">
-        <v>167</v>
-      </c>
-      <c r="D63" t="s">
-        <v>168</v>
-      </c>
-      <c r="E63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" t="s">
-        <v>200</v>
-      </c>
-      <c r="G63" t="s">
-        <v>201</v>
       </c>
       <c r="H63">
         <v>15</v>
@@ -4182,25 +4182,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>200</v>
+      </c>
+      <c r="B64" t="s">
+        <v>201</v>
+      </c>
+      <c r="C64" t="s">
+        <v>165</v>
+      </c>
+      <c r="D64" t="s">
+        <v>166</v>
+      </c>
+      <c r="E64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" t="s">
         <v>202</v>
       </c>
-      <c r="B64" t="s">
+      <c r="G64" t="s">
         <v>203</v>
-      </c>
-      <c r="C64" t="s">
-        <v>167</v>
-      </c>
-      <c r="D64" t="s">
-        <v>168</v>
-      </c>
-      <c r="E64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" t="s">
-        <v>204</v>
-      </c>
-      <c r="G64" t="s">
-        <v>205</v>
       </c>
       <c r="H64">
         <v>6</v>
@@ -4215,25 +4215,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" t="s">
+        <v>205</v>
+      </c>
+      <c r="C65" t="s">
+        <v>165</v>
+      </c>
+      <c r="D65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" t="s">
         <v>206</v>
       </c>
-      <c r="B65" t="s">
+      <c r="G65" t="s">
         <v>207</v>
-      </c>
-      <c r="C65" t="s">
-        <v>167</v>
-      </c>
-      <c r="D65" t="s">
-        <v>168</v>
-      </c>
-      <c r="E65" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" t="s">
-        <v>208</v>
-      </c>
-      <c r="G65" t="s">
-        <v>209</v>
       </c>
       <c r="H65">
         <v>3</v>
@@ -4248,25 +4248,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" t="s">
+        <v>165</v>
+      </c>
+      <c r="D66" t="s">
+        <v>166</v>
+      </c>
+      <c r="E66" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" t="s">
         <v>210</v>
       </c>
-      <c r="B66" t="s">
+      <c r="G66" t="s">
         <v>211</v>
-      </c>
-      <c r="C66" t="s">
-        <v>167</v>
-      </c>
-      <c r="D66" t="s">
-        <v>168</v>
-      </c>
-      <c r="E66" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" t="s">
-        <v>212</v>
-      </c>
-      <c r="G66" t="s">
-        <v>213</v>
       </c>
       <c r="H66">
         <v>4</v>
@@ -4281,25 +4281,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" t="s">
+        <v>165</v>
+      </c>
+      <c r="D67" t="s">
+        <v>166</v>
+      </c>
+      <c r="E67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" t="s">
         <v>214</v>
       </c>
-      <c r="B67" t="s">
+      <c r="G67" t="s">
         <v>215</v>
-      </c>
-      <c r="C67" t="s">
-        <v>167</v>
-      </c>
-      <c r="D67" t="s">
-        <v>168</v>
-      </c>
-      <c r="E67" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67" t="s">
-        <v>216</v>
-      </c>
-      <c r="G67" t="s">
-        <v>217</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -4314,25 +4314,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>216</v>
+      </c>
+      <c r="B68" t="s">
+        <v>217</v>
+      </c>
+      <c r="C68" t="s">
+        <v>165</v>
+      </c>
+      <c r="D68" t="s">
+        <v>166</v>
+      </c>
+      <c r="E68" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" t="s">
         <v>218</v>
       </c>
-      <c r="B68" t="s">
+      <c r="G68" t="s">
         <v>219</v>
-      </c>
-      <c r="C68" t="s">
-        <v>167</v>
-      </c>
-      <c r="D68" t="s">
-        <v>168</v>
-      </c>
-      <c r="E68" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" t="s">
-        <v>220</v>
-      </c>
-      <c r="G68" t="s">
-        <v>221</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4347,25 +4347,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B69">
         <v>0.3</v>
       </c>
       <c r="C69" t="s">
+        <v>221</v>
+      </c>
+      <c r="D69" t="s">
+        <v>222</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" t="s">
         <v>223</v>
       </c>
-      <c r="D69" t="s">
+      <c r="G69" t="s">
         <v>224</v>
-      </c>
-      <c r="E69" t="s">
-        <v>20</v>
-      </c>
-      <c r="F69" t="s">
-        <v>225</v>
-      </c>
-      <c r="G69" t="s">
-        <v>226</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4380,25 +4380,25 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>225</v>
+      </c>
+      <c r="B70" t="s">
+        <v>226</v>
+      </c>
+      <c r="C70" t="s">
+        <v>165</v>
+      </c>
+      <c r="D70" t="s">
+        <v>166</v>
+      </c>
+      <c r="E70" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70" t="s">
         <v>227</v>
       </c>
-      <c r="B70" t="s">
+      <c r="G70" t="s">
         <v>228</v>
-      </c>
-      <c r="C70" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" t="s">
-        <v>168</v>
-      </c>
-      <c r="E70" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" t="s">
-        <v>229</v>
-      </c>
-      <c r="G70" t="s">
-        <v>230</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4413,25 +4413,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>229</v>
+      </c>
+      <c r="B71" t="s">
+        <v>230</v>
+      </c>
+      <c r="C71" t="s">
+        <v>165</v>
+      </c>
+      <c r="D71" t="s">
+        <v>166</v>
+      </c>
+      <c r="E71" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
         <v>231</v>
       </c>
-      <c r="B71" t="s">
+      <c r="G71" t="s">
         <v>232</v>
-      </c>
-      <c r="C71" t="s">
-        <v>167</v>
-      </c>
-      <c r="D71" t="s">
-        <v>168</v>
-      </c>
-      <c r="E71" t="s">
-        <v>20</v>
-      </c>
-      <c r="F71" t="s">
-        <v>233</v>
-      </c>
-      <c r="G71" t="s">
-        <v>234</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4446,25 +4446,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>233</v>
+      </c>
+      <c r="B72" t="s">
+        <v>234</v>
+      </c>
+      <c r="C72" t="s">
+        <v>165</v>
+      </c>
+      <c r="D72" t="s">
+        <v>166</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" t="s">
         <v>235</v>
       </c>
-      <c r="B72" t="s">
+      <c r="G72" t="s">
         <v>236</v>
-      </c>
-      <c r="C72" t="s">
-        <v>167</v>
-      </c>
-      <c r="D72" t="s">
-        <v>168</v>
-      </c>
-      <c r="E72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" t="s">
-        <v>237</v>
-      </c>
-      <c r="G72" t="s">
-        <v>238</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4479,16 +4479,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D73" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
@@ -4506,25 +4506,25 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>238</v>
+      </c>
+      <c r="B74" t="s">
+        <v>239</v>
+      </c>
+      <c r="C74" t="s">
+        <v>165</v>
+      </c>
+      <c r="D74" t="s">
+        <v>166</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" t="s">
         <v>240</v>
       </c>
-      <c r="B74" t="s">
+      <c r="G74" t="s">
         <v>241</v>
-      </c>
-      <c r="C74" t="s">
-        <v>167</v>
-      </c>
-      <c r="D74" t="s">
-        <v>168</v>
-      </c>
-      <c r="E74" t="s">
-        <v>20</v>
-      </c>
-      <c r="F74" t="s">
-        <v>242</v>
-      </c>
-      <c r="G74" t="s">
-        <v>243</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4539,25 +4539,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B75" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C75" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G75" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4572,25 +4572,25 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B76" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C76" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E76" t="s">
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G76" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4605,25 +4605,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>246</v>
+      </c>
+      <c r="B77" t="s">
+        <v>247</v>
+      </c>
+      <c r="C77" t="s">
+        <v>165</v>
+      </c>
+      <c r="D77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
         <v>248</v>
       </c>
-      <c r="B77" t="s">
+      <c r="G77" t="s">
         <v>249</v>
-      </c>
-      <c r="C77" t="s">
-        <v>167</v>
-      </c>
-      <c r="D77" t="s">
-        <v>168</v>
-      </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" t="s">
-        <v>250</v>
-      </c>
-      <c r="G77" t="s">
-        <v>251</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4638,25 +4638,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>250</v>
+      </c>
+      <c r="B78" t="s">
+        <v>251</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78" t="s">
+        <v>166</v>
+      </c>
+      <c r="E78" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" t="s">
         <v>252</v>
       </c>
-      <c r="B78" t="s">
+      <c r="G78" t="s">
         <v>253</v>
-      </c>
-      <c r="C78" t="s">
-        <v>167</v>
-      </c>
-      <c r="D78" t="s">
-        <v>168</v>
-      </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="F78" t="s">
-        <v>254</v>
-      </c>
-      <c r="G78" t="s">
-        <v>255</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4671,25 +4671,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79" t="s">
+        <v>255</v>
+      </c>
+      <c r="C79" t="s">
+        <v>255</v>
+      </c>
+      <c r="D79" t="s">
         <v>256</v>
       </c>
-      <c r="B79" t="s">
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" t="s">
         <v>257</v>
       </c>
-      <c r="C79" t="s">
-        <v>257</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="G79" t="s">
         <v>258</v>
-      </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" t="s">
-        <v>259</v>
-      </c>
-      <c r="G79" t="s">
-        <v>260</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4704,25 +4704,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>259</v>
+      </c>
+      <c r="B80" t="s">
+        <v>260</v>
+      </c>
+      <c r="C80" t="s">
+        <v>260</v>
+      </c>
+      <c r="D80" t="s">
         <v>261</v>
       </c>
-      <c r="B80" t="s">
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" t="s">
         <v>262</v>
       </c>
-      <c r="C80" t="s">
-        <v>262</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="G80" t="s">
         <v>263</v>
-      </c>
-      <c r="E80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F80" t="s">
-        <v>264</v>
-      </c>
-      <c r="G80" t="s">
-        <v>265</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4737,25 +4737,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>264</v>
+      </c>
+      <c r="B81" t="s">
+        <v>265</v>
+      </c>
+      <c r="C81" t="s">
         <v>266</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>267</v>
       </c>
-      <c r="C81" t="s">
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" t="s">
         <v>268</v>
       </c>
-      <c r="D81" t="s">
+      <c r="G81" t="s">
         <v>269</v>
-      </c>
-      <c r="E81" t="s">
-        <v>20</v>
-      </c>
-      <c r="F81" t="s">
-        <v>270</v>
-      </c>
-      <c r="G81" t="s">
-        <v>271</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4770,25 +4770,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>270</v>
+      </c>
+      <c r="B82" t="s">
+        <v>271</v>
+      </c>
+      <c r="C82" t="s">
         <v>272</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>273</v>
       </c>
-      <c r="C82" t="s">
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" t="s">
         <v>274</v>
       </c>
-      <c r="D82" t="s">
+      <c r="G82" t="s">
         <v>275</v>
-      </c>
-      <c r="E82" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" t="s">
-        <v>276</v>
-      </c>
-      <c r="G82" t="s">
-        <v>277</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4803,25 +4803,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>276</v>
+      </c>
+      <c r="B83" t="s">
+        <v>277</v>
+      </c>
+      <c r="C83" t="s">
+        <v>277</v>
+      </c>
+      <c r="D83" t="s">
         <v>278</v>
       </c>
-      <c r="B83" t="s">
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" t="s">
         <v>279</v>
       </c>
-      <c r="C83" t="s">
-        <v>279</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="G83" t="s">
         <v>280</v>
-      </c>
-      <c r="E83" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" t="s">
-        <v>281</v>
-      </c>
-      <c r="G83" t="s">
-        <v>282</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4836,25 +4836,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>281</v>
+      </c>
+      <c r="B84" t="s">
+        <v>282</v>
+      </c>
+      <c r="C84" t="s">
+        <v>282</v>
+      </c>
+      <c r="D84" t="s">
         <v>283</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" t="s">
         <v>284</v>
       </c>
-      <c r="C84" t="s">
-        <v>284</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="G84" t="s">
         <v>285</v>
-      </c>
-      <c r="E84" t="s">
-        <v>20</v>
-      </c>
-      <c r="F84" t="s">
-        <v>286</v>
-      </c>
-      <c r="G84" t="s">
-        <v>287</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4869,25 +4869,25 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>286</v>
+      </c>
+      <c r="B85" t="s">
+        <v>287</v>
+      </c>
+      <c r="C85" t="s">
+        <v>287</v>
+      </c>
+      <c r="D85" t="s">
         <v>288</v>
       </c>
-      <c r="B85" t="s">
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" t="s">
         <v>289</v>
       </c>
-      <c r="C85" t="s">
-        <v>289</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="G85" t="s">
         <v>290</v>
-      </c>
-      <c r="E85" t="s">
-        <v>20</v>
-      </c>
-      <c r="F85" t="s">
-        <v>291</v>
-      </c>
-      <c r="G85" t="s">
-        <v>292</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4902,25 +4902,25 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>291</v>
+      </c>
+      <c r="B86" t="s">
+        <v>292</v>
+      </c>
+      <c r="C86" t="s">
+        <v>292</v>
+      </c>
+      <c r="D86" t="s">
         <v>293</v>
       </c>
-      <c r="B86" t="s">
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" t="s">
         <v>294</v>
       </c>
-      <c r="C86" t="s">
-        <v>294</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
         <v>295</v>
-      </c>
-      <c r="E86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" t="s">
-        <v>296</v>
-      </c>
-      <c r="G86" t="s">
-        <v>297</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4935,25 +4935,25 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>296</v>
+      </c>
+      <c r="B87" t="s">
+        <v>297</v>
+      </c>
+      <c r="C87" t="s">
+        <v>297</v>
+      </c>
+      <c r="D87" t="s">
         <v>298</v>
       </c>
-      <c r="B87" t="s">
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" t="s">
         <v>299</v>
       </c>
-      <c r="C87" t="s">
-        <v>299</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>300</v>
-      </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>301</v>
-      </c>
-      <c r="G87" t="s">
-        <v>302</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4968,16 +4968,16 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>301</v>
+      </c>
+      <c r="B88" t="s">
+        <v>302</v>
+      </c>
+      <c r="C88" t="s">
+        <v>302</v>
+      </c>
+      <c r="D88" t="s">
         <v>303</v>
-      </c>
-      <c r="B88" t="s">
-        <v>304</v>
-      </c>
-      <c r="C88" t="s">
-        <v>304</v>
-      </c>
-      <c r="D88" t="s">
-        <v>305</v>
       </c>
       <c r="G88" t="s">
         <v>15</v>
@@ -4990,30 +4990,30 @@
         <v>0</v>
       </c>
       <c r="K88" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>305</v>
+      </c>
+      <c r="B89" t="s">
+        <v>306</v>
+      </c>
+      <c r="C89" t="s">
+        <v>306</v>
+      </c>
+      <c r="D89" t="s">
         <v>307</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" t="s">
         <v>308</v>
       </c>
-      <c r="C89" t="s">
-        <v>308</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="G89" t="s">
         <v>309</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>310</v>
-      </c>
-      <c r="G89" t="s">
-        <v>311</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -5028,25 +5028,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>310</v>
+      </c>
+      <c r="B90" t="s">
+        <v>311</v>
+      </c>
+      <c r="C90" t="s">
+        <v>311</v>
+      </c>
+      <c r="D90" t="s">
         <v>312</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" t="s">
         <v>313</v>
       </c>
-      <c r="C90" t="s">
-        <v>313</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="G90" t="s">
         <v>314</v>
-      </c>
-      <c r="E90" t="s">
-        <v>20</v>
-      </c>
-      <c r="F90" t="s">
-        <v>315</v>
-      </c>
-      <c r="G90" t="s">
-        <v>316</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5061,25 +5061,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>315</v>
+      </c>
+      <c r="B91" t="s">
+        <v>316</v>
+      </c>
+      <c r="C91" t="s">
+        <v>316</v>
+      </c>
+      <c r="D91" t="s">
         <v>317</v>
       </c>
-      <c r="B91" t="s">
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" t="s">
         <v>318</v>
       </c>
-      <c r="C91" t="s">
-        <v>318</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="G91" t="s">
         <v>319</v>
-      </c>
-      <c r="E91" t="s">
-        <v>20</v>
-      </c>
-      <c r="F91" t="s">
-        <v>320</v>
-      </c>
-      <c r="G91" t="s">
-        <v>321</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5094,25 +5094,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>320</v>
+      </c>
+      <c r="B92" t="s">
+        <v>321</v>
+      </c>
+      <c r="C92" t="s">
+        <v>321</v>
+      </c>
+      <c r="D92" t="s">
         <v>322</v>
       </c>
-      <c r="B92" t="s">
+      <c r="E92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" t="s">
         <v>323</v>
       </c>
-      <c r="C92" t="s">
-        <v>323</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="G92" t="s">
         <v>324</v>
-      </c>
-      <c r="E92" t="s">
-        <v>20</v>
-      </c>
-      <c r="F92" t="s">
-        <v>325</v>
-      </c>
-      <c r="G92" t="s">
-        <v>326</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5127,25 +5127,25 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>414</v>
+      </c>
+      <c r="B93" t="s">
+        <v>415</v>
+      </c>
+      <c r="C93" t="s">
+        <v>415</v>
+      </c>
+      <c r="D93" t="s">
+        <v>417</v>
+      </c>
+      <c r="E93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" t="s">
         <v>416</v>
       </c>
-      <c r="B93" t="s">
-        <v>417</v>
-      </c>
-      <c r="C93" t="s">
-        <v>417</v>
-      </c>
-      <c r="D93" t="s">
-        <v>419</v>
-      </c>
-      <c r="E93" t="s">
-        <v>20</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>418</v>
-      </c>
-      <c r="G93" t="s">
-        <v>420</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5160,25 +5160,25 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>325</v>
+      </c>
+      <c r="B94" t="s">
+        <v>326</v>
+      </c>
+      <c r="C94" t="s">
+        <v>326</v>
+      </c>
+      <c r="D94" t="s">
         <v>327</v>
       </c>
-      <c r="B94" t="s">
+      <c r="E94" t="s">
         <v>328</v>
       </c>
-      <c r="C94" t="s">
-        <v>328</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="F94" t="s">
         <v>329</v>
       </c>
-      <c r="E94" t="s">
+      <c r="G94" t="s">
         <v>330</v>
-      </c>
-      <c r="F94" t="s">
-        <v>331</v>
-      </c>
-      <c r="G94" t="s">
-        <v>332</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5193,25 +5193,25 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>331</v>
+      </c>
+      <c r="B95" t="s">
+        <v>332</v>
+      </c>
+      <c r="C95" t="s">
+        <v>332</v>
+      </c>
+      <c r="D95" t="s">
         <v>333</v>
       </c>
-      <c r="B95" t="s">
+      <c r="E95" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" t="s">
         <v>334</v>
       </c>
-      <c r="C95" t="s">
-        <v>334</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="G95" t="s">
         <v>335</v>
-      </c>
-      <c r="E95" t="s">
-        <v>20</v>
-      </c>
-      <c r="F95" t="s">
-        <v>336</v>
-      </c>
-      <c r="G95" t="s">
-        <v>337</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -5226,16 +5226,16 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>336</v>
+      </c>
+      <c r="B96" t="s">
+        <v>337</v>
+      </c>
+      <c r="C96" t="s">
         <v>338</v>
       </c>
-      <c r="B96" t="s">
+      <c r="D96" t="s">
         <v>339</v>
-      </c>
-      <c r="C96" t="s">
-        <v>340</v>
-      </c>
-      <c r="D96" t="s">
-        <v>341</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Replaced the new IO headers and the DAC headers with a single 2x10 part.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="431">
   <si>
     <t>Part</t>
   </si>
@@ -298,9 +298,6 @@
     <t>PINHD-2X10</t>
   </si>
   <si>
-    <t>2X10</t>
-  </si>
-  <si>
     <t>S9180-ND</t>
   </si>
   <si>
@@ -1291,13 +1288,25 @@
     <t>XG8T-0231</t>
   </si>
   <si>
-    <t>JP20, JP21, JP22, JP29, JP30</t>
-  </si>
-  <si>
     <t>JP23</t>
   </si>
   <si>
-    <t>JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19, JP24, JP25, JP26, JP27, JP28</t>
+    <t>JP20, JP21, JP22</t>
+  </si>
+  <si>
+    <t>JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19</t>
+  </si>
+  <si>
+    <t>2X10 Right angle</t>
+  </si>
+  <si>
+    <t>JP24</t>
+  </si>
+  <si>
+    <t>A26460-ND</t>
+  </si>
+  <si>
+    <t>1-534206-0</t>
   </si>
 </sst>
 </file>
@@ -2126,10 +2135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2187,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2198,10 +2207,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G2" t="s">
         <v>357</v>
-      </c>
-      <c r="G2" t="s">
-        <v>358</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2214,8 +2223,8 @@
         <v>0.27</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J104)</f>
-        <v>178.4272</v>
+        <f>SUM(J2:J105)</f>
+        <v>179.21719999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2235,10 +2244,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>358</v>
+      </c>
+      <c r="G3" t="s">
         <v>359</v>
-      </c>
-      <c r="G3" t="s">
-        <v>360</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2247,13 +2256,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J69" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J70" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2268,10 +2277,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>360</v>
+      </c>
+      <c r="G4" t="s">
         <v>361</v>
-      </c>
-      <c r="G4" t="s">
-        <v>362</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2325,10 +2334,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>365</v>
+      </c>
+      <c r="G6" t="s">
         <v>366</v>
-      </c>
-      <c r="G6" t="s">
-        <v>367</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2341,7 +2350,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2385,10 +2394,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
+        <v>367</v>
+      </c>
+      <c r="G8" t="s">
         <v>368</v>
-      </c>
-      <c r="G8" t="s">
-        <v>369</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2418,10 +2427,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G9" t="s">
         <v>370</v>
-      </c>
-      <c r="G9" t="s">
-        <v>371</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2451,10 +2460,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
+        <v>381</v>
+      </c>
+      <c r="G10" t="s">
         <v>382</v>
-      </c>
-      <c r="G10" t="s">
-        <v>383</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2467,7 +2476,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2520,10 +2529,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
+        <v>383</v>
+      </c>
+      <c r="G12" t="s">
         <v>384</v>
-      </c>
-      <c r="G12" t="s">
-        <v>385</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2553,10 +2562,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
+        <v>381</v>
+      </c>
+      <c r="G13" t="s">
         <v>382</v>
-      </c>
-      <c r="G13" t="s">
-        <v>383</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2569,7 +2578,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2589,10 +2598,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
+        <v>387</v>
+      </c>
+      <c r="G14" t="s">
         <v>388</v>
-      </c>
-      <c r="G14" t="s">
-        <v>389</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2605,7 +2614,7 @@
         <v>0.17</v>
       </c>
       <c r="L14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2625,10 +2634,10 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
+        <v>390</v>
+      </c>
+      <c r="G15" t="s">
         <v>391</v>
-      </c>
-      <c r="G15" t="s">
-        <v>392</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2641,7 +2650,7 @@
         <v>0.48</v>
       </c>
       <c r="L15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2685,10 +2694,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
+        <v>371</v>
+      </c>
+      <c r="G17" t="s">
         <v>372</v>
-      </c>
-      <c r="G17" t="s">
-        <v>373</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2766,10 +2775,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
+        <v>373</v>
+      </c>
+      <c r="G20" t="s">
         <v>374</v>
-      </c>
-      <c r="G20" t="s">
-        <v>375</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2782,7 +2791,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2802,10 +2811,10 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
+        <v>376</v>
+      </c>
+      <c r="G21" t="s">
         <v>377</v>
-      </c>
-      <c r="G21" t="s">
-        <v>378</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2859,10 +2868,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
+        <v>378</v>
+      </c>
+      <c r="G23" t="s">
         <v>379</v>
-      </c>
-      <c r="G23" t="s">
-        <v>380</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2877,10 +2886,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>408</v>
+      </c>
+      <c r="B24" t="s">
         <v>409</v>
-      </c>
-      <c r="B24" t="s">
-        <v>410</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
@@ -2892,10 +2901,10 @@
         <v>20</v>
       </c>
       <c r="F24" t="s">
+        <v>410</v>
+      </c>
+      <c r="G24" t="s">
         <v>411</v>
-      </c>
-      <c r="G24" t="s">
-        <v>412</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2958,10 +2967,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
+        <v>354</v>
+      </c>
+      <c r="G26" t="s">
         <v>355</v>
-      </c>
-      <c r="G26" t="s">
-        <v>356</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -2991,10 +3000,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
+        <v>399</v>
+      </c>
+      <c r="G27" t="s">
         <v>400</v>
-      </c>
-      <c r="G27" t="s">
-        <v>401</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3007,7 +3016,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3027,10 +3036,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
+        <v>392</v>
+      </c>
+      <c r="G28" t="s">
         <v>393</v>
-      </c>
-      <c r="G28" t="s">
-        <v>394</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3060,10 +3069,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G29" t="s">
         <v>395</v>
-      </c>
-      <c r="G29" t="s">
-        <v>396</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3093,10 +3102,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
+        <v>396</v>
+      </c>
+      <c r="G30" t="s">
         <v>397</v>
-      </c>
-      <c r="G30" t="s">
-        <v>398</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3109,7 +3118,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3129,10 +3138,10 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
+        <v>339</v>
+      </c>
+      <c r="G31" t="s">
         <v>340</v>
-      </c>
-      <c r="G31" t="s">
-        <v>341</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3150,22 +3159,22 @@
         <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
+        <v>406</v>
+      </c>
+      <c r="G32" t="s">
         <v>407</v>
-      </c>
-      <c r="G32" t="s">
-        <v>408</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -3213,7 +3222,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B34" t="s">
         <v>90</v>
@@ -3225,10 +3234,10 @@
         <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F34" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -3243,7 +3252,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B35" t="s">
         <v>90</v>
@@ -3255,10 +3264,10 @@
         <v>91</v>
       </c>
       <c r="E35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G35" t="s">
         <v>15</v>
@@ -3285,16 +3294,16 @@
         <v>93</v>
       </c>
       <c r="D36" t="s">
+        <v>427</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
         <v>94</v>
       </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>95</v>
-      </c>
-      <c r="G36" t="s">
-        <v>96</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3309,25 +3318,25 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s">
         <v>98</v>
       </c>
-      <c r="D37" t="s">
-        <v>99</v>
-      </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
+        <v>352</v>
+      </c>
+      <c r="G37" t="s">
         <v>353</v>
-      </c>
-      <c r="G37" t="s">
-        <v>354</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -3342,25 +3351,25 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" t="s">
         <v>101</v>
       </c>
-      <c r="D38" t="s">
-        <v>102</v>
-      </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" t="s">
         <v>104</v>
-      </c>
-      <c r="G38" t="s">
-        <v>105</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -3373,63 +3382,63 @@
         <v>1.26</v>
       </c>
       <c r="L38" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
         <v>103</v>
       </c>
-      <c r="D39" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>104</v>
       </c>
-      <c r="G39" t="s">
-        <v>105</v>
-      </c>
       <c r="H39">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I39">
         <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>6.3</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
         <v>106</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="s">
         <v>107</v>
       </c>
-      <c r="C40" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>108</v>
-      </c>
-      <c r="G40" t="s">
-        <v>109</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -3450,49 +3459,49 @@
         <v>15</v>
       </c>
       <c r="C41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" t="s">
         <v>110</v>
       </c>
-      <c r="D41" t="s">
-        <v>111</v>
-      </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">
+        <v>422</v>
+      </c>
+      <c r="G41" t="s">
         <v>423</v>
       </c>
-      <c r="G41" t="s">
-        <v>424</v>
-      </c>
       <c r="H41">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I41">
         <v>0.13</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>0.65</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C42" t="s">
+        <v>418</v>
+      </c>
+      <c r="D42" t="s">
         <v>419</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
         <v>420</v>
       </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>421</v>
-      </c>
-      <c r="G42" t="s">
-        <v>422</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3507,403 +3516,400 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" t="s">
-        <v>113</v>
+        <v>428</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>427</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>429</v>
       </c>
       <c r="G43" t="s">
-        <v>117</v>
+        <v>430</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G44" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G45" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G46" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" t="s">
+        <v>133</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="H47">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1.85</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D48" t="s">
-        <v>142</v>
-      </c>
-      <c r="E48" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G48" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="H48">
-        <v>25</v>
-      </c>
-      <c r="I48">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="E49" t="s">
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G49" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I49">
-        <v>0.84</v>
+        <v>0.3</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>15</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
+        <v>147</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="H50">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>0.84</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>142</v>
-      </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G51" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G52" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D53" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>342</v>
+        <v>160</v>
       </c>
       <c r="G53" t="s">
-        <v>343</v>
+        <v>161</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B54" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" t="s">
         <v>165</v>
       </c>
-      <c r="D54" t="s">
-        <v>166</v>
-      </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>169</v>
+        <v>341</v>
       </c>
       <c r="G54" t="s">
-        <v>170</v>
+        <v>342</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>171</v>
-      </c>
-      <c r="B55">
-        <v>470</v>
+        <v>166</v>
+      </c>
+      <c r="B55" t="s">
+        <v>167</v>
       </c>
       <c r="C55" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" t="s">
         <v>165</v>
       </c>
-      <c r="D55" t="s">
-        <v>166</v>
-      </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G55" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3918,124 +3924,124 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>174</v>
-      </c>
-      <c r="B56" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="B56">
+        <v>470</v>
       </c>
       <c r="C56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" t="s">
         <v>165</v>
       </c>
-      <c r="D56" t="s">
-        <v>166</v>
-      </c>
       <c r="E56" t="s">
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G56" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H56">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="I56">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.81420000000000003</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" t="s">
         <v>165</v>
       </c>
-      <c r="D57" t="s">
-        <v>166</v>
-      </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G57" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="I57">
-        <v>0.04</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.81420000000000003</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C58" t="s">
-        <v>344</v>
+        <v>164</v>
       </c>
       <c r="D58" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>345</v>
+        <v>179</v>
       </c>
       <c r="G58" t="s">
-        <v>346</v>
+        <v>180</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I58">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C59" t="s">
+        <v>343</v>
+      </c>
+      <c r="D59" t="s">
+        <v>120</v>
+      </c>
+      <c r="E59" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" t="s">
         <v>344</v>
       </c>
-      <c r="D59" t="s">
-        <v>121</v>
-      </c>
-      <c r="E59" t="s">
-        <v>20</v>
-      </c>
-      <c r="F59" t="s">
-        <v>351</v>
-      </c>
       <c r="G59" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4050,289 +4056,289 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C60" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="D60" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="E60" t="s">
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>188</v>
+        <v>350</v>
       </c>
       <c r="G60" t="s">
-        <v>189</v>
+        <v>351</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>190</v>
-      </c>
-      <c r="B61">
-        <v>200</v>
+        <v>185</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
       </c>
       <c r="C61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" t="s">
         <v>165</v>
       </c>
-      <c r="D61" t="s">
-        <v>166</v>
-      </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G61" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H61">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I61">
         <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B62">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" t="s">
         <v>165</v>
       </c>
-      <c r="D62" t="s">
-        <v>166</v>
-      </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G62" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H62">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>196</v>
-      </c>
-      <c r="B63" t="s">
-        <v>197</v>
+        <v>192</v>
+      </c>
+      <c r="B63">
+        <v>100</v>
       </c>
       <c r="C63" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" t="s">
         <v>165</v>
       </c>
-      <c r="D63" t="s">
-        <v>166</v>
-      </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G63" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H63">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C64" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" t="s">
         <v>165</v>
       </c>
-      <c r="D64" t="s">
-        <v>166</v>
-      </c>
       <c r="E64" t="s">
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G64" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H64">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C65" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" t="s">
         <v>165</v>
       </c>
-      <c r="D65" t="s">
-        <v>166</v>
-      </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G65" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C66" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" t="s">
         <v>165</v>
       </c>
-      <c r="D66" t="s">
-        <v>166</v>
-      </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G66" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C67" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" t="s">
         <v>165</v>
       </c>
-      <c r="D67" t="s">
-        <v>166</v>
-      </c>
       <c r="E67" t="s">
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G67" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B68" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C68" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" t="s">
         <v>165</v>
       </c>
-      <c r="D68" t="s">
-        <v>166</v>
-      </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G68" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4347,91 +4353,91 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>220</v>
-      </c>
-      <c r="B69">
-        <v>0.3</v>
+        <v>215</v>
+      </c>
+      <c r="B69" t="s">
+        <v>216</v>
       </c>
       <c r="C69" t="s">
-        <v>221</v>
+        <v>164</v>
       </c>
       <c r="D69" t="s">
-        <v>222</v>
+        <v>165</v>
       </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G69" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="H69">
         <v>1</v>
       </c>
       <c r="I69">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>225</v>
-      </c>
-      <c r="B70" t="s">
-        <v>226</v>
+        <v>219</v>
+      </c>
+      <c r="B70">
+        <v>0.3</v>
       </c>
       <c r="C70" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="D70" t="s">
-        <v>166</v>
+        <v>221</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G70" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H70">
         <v>1</v>
       </c>
       <c r="I70">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J70">
-        <f t="shared" ref="J70:J96" si="1">H70*I70</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B71" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C71" t="s">
+        <v>164</v>
+      </c>
+      <c r="D71" t="s">
         <v>165</v>
       </c>
-      <c r="D71" t="s">
-        <v>166</v>
-      </c>
       <c r="E71" t="s">
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G71" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4440,31 +4446,31 @@
         <v>0.04</v>
       </c>
       <c r="J71">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J71:J97" si="1">H71*I71</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B72" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C72" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72" t="s">
         <v>165</v>
       </c>
-      <c r="D72" t="s">
-        <v>166</v>
-      </c>
       <c r="E72" t="s">
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G72" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4479,118 +4485,118 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B73" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" t="s">
         <v>165</v>
       </c>
-      <c r="D73" t="s">
-        <v>166</v>
-      </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
+      <c r="F73" t="s">
+        <v>234</v>
+      </c>
       <c r="G73" t="s">
-        <v>15</v>
+        <v>235</v>
       </c>
       <c r="H73">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B74" t="s">
-        <v>239</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
+        <v>164</v>
+      </c>
+      <c r="D74" t="s">
         <v>165</v>
       </c>
-      <c r="D74" t="s">
-        <v>166</v>
-      </c>
       <c r="E74" t="s">
         <v>20</v>
       </c>
-      <c r="F74" t="s">
-        <v>240</v>
-      </c>
       <c r="G74" t="s">
-        <v>241</v>
+        <v>15</v>
       </c>
       <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C75" t="s">
-        <v>344</v>
+        <v>164</v>
       </c>
       <c r="D75" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>347</v>
+        <v>239</v>
       </c>
       <c r="G75" t="s">
-        <v>348</v>
+        <v>240</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B76" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C76" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E76" t="s">
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G76" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4605,58 +4611,58 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C77" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="D77" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="E77" t="s">
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>248</v>
+        <v>348</v>
       </c>
       <c r="G77" t="s">
-        <v>249</v>
+        <v>349</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C78" t="s">
+        <v>164</v>
+      </c>
+      <c r="D78" t="s">
         <v>165</v>
       </c>
-      <c r="D78" t="s">
-        <v>166</v>
-      </c>
       <c r="E78" t="s">
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G78" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4671,579 +4677,612 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B79" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C79" t="s">
-        <v>255</v>
+        <v>164</v>
       </c>
       <c r="D79" t="s">
-        <v>256</v>
+        <v>165</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G79" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B80" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C80" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D80" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="G80" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B81" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C81" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D81" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="G81" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B82" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C82" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D82" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G82" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B83" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C83" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D83" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G83" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B84" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C84" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D84" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G84" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B85" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C85" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D85" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="G85" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B86" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C86" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D86" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E86" t="s">
         <v>20</v>
       </c>
       <c r="F86" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="G86" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B87" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C87" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D87" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E87" t="s">
         <v>20</v>
       </c>
       <c r="F87" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G87" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B88" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C88" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D88" t="s">
-        <v>303</v>
+        <v>297</v>
+      </c>
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" t="s">
+        <v>298</v>
       </c>
       <c r="G88" t="s">
-        <v>15</v>
+        <v>299</v>
       </c>
       <c r="H88">
         <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1.51</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K88" t="s">
-        <v>304</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B89" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C89" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D89" t="s">
-        <v>307</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G89" t="s">
-        <v>309</v>
+        <v>15</v>
       </c>
       <c r="H89">
         <v>1</v>
-      </c>
-      <c r="I89">
-        <v>0.47</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K89" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B90" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C90" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D90" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E90" t="s">
         <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="G90" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B91" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C91" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D91" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E91" t="s">
         <v>20</v>
       </c>
       <c r="F91" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G91" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B92" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C92" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D92" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E92" t="s">
         <v>20</v>
       </c>
       <c r="F92" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="G92" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>12.95</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>414</v>
+        <v>319</v>
       </c>
       <c r="B93" t="s">
-        <v>415</v>
+        <v>320</v>
       </c>
       <c r="C93" t="s">
-        <v>415</v>
+        <v>320</v>
       </c>
       <c r="D93" t="s">
-        <v>417</v>
+        <v>321</v>
       </c>
       <c r="E93" t="s">
         <v>20</v>
       </c>
       <c r="F93" t="s">
-        <v>416</v>
+        <v>322</v>
       </c>
       <c r="G93" t="s">
-        <v>418</v>
+        <v>323</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>6.84</v>
+        <v>12.95</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>12.95</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>325</v>
+        <v>413</v>
       </c>
       <c r="B94" t="s">
-        <v>326</v>
+        <v>414</v>
       </c>
       <c r="C94" t="s">
-        <v>326</v>
+        <v>414</v>
       </c>
       <c r="D94" t="s">
-        <v>327</v>
+        <v>416</v>
       </c>
       <c r="E94" t="s">
-        <v>328</v>
+        <v>20</v>
       </c>
       <c r="F94" t="s">
-        <v>329</v>
+        <v>415</v>
       </c>
       <c r="G94" t="s">
-        <v>330</v>
+        <v>417</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B95" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C95" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D95" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E95" t="s">
-        <v>20</v>
+        <v>327</v>
       </c>
       <c r="F95" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="G95" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>330</v>
+      </c>
+      <c r="B96" t="s">
+        <v>331</v>
+      </c>
+      <c r="C96" t="s">
+        <v>331</v>
+      </c>
+      <c r="D96" t="s">
+        <v>332</v>
+      </c>
+      <c r="E96" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" t="s">
+        <v>333</v>
+      </c>
+      <c r="G96" t="s">
+        <v>334</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>2.96</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>335</v>
+      </c>
+      <c r="B97" t="s">
         <v>336</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C97" t="s">
         <v>337</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D97" t="s">
         <v>338</v>
       </c>
-      <c r="D96" t="s">
-        <v>339</v>
-      </c>
-      <c r="G96" t="s">
+      <c r="G97" t="s">
         <v>15</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="J96">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Arduino analog pins 4 and 5 mode switcher redesigned.
The N/P MOSFET pairs (Q15 and Q16) would not have functioned correctly in a reverse voltage/current condition.
They have been replaced with 2:1 mux/demux ICs (IC4 and IC5) which are a much better fit for the configuration.
Q31 and Q32 have been renamed to Q15 and Q16 respectively to remove the gap in Q__ part names.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="432">
   <si>
     <t>Part</t>
   </si>
@@ -448,21 +448,6 @@
     <t>DMG1012UW-7</t>
   </si>
   <si>
-    <t>Q15, Q16</t>
-  </si>
-  <si>
-    <t>IRF7509</t>
-  </si>
-  <si>
-    <t>IRF7509",MICRO8"</t>
-  </si>
-  <si>
-    <t>IRF7509TRPBFCT-ND</t>
-  </si>
-  <si>
-    <t>IRF7509TRPBF</t>
-  </si>
-  <si>
     <t>Q17, Q25, Q30</t>
   </si>
   <si>
@@ -475,9 +460,6 @@
     <t>TO220V</t>
   </si>
   <si>
-    <t>Q31</t>
-  </si>
-  <si>
     <t>IRLML2402</t>
   </si>
   <si>
@@ -487,9 +469,6 @@
     <t>IRLML2402GTRPBF</t>
   </si>
   <si>
-    <t>Q32</t>
-  </si>
-  <si>
     <t>IRLML6402</t>
   </si>
   <si>
@@ -1307,6 +1286,30 @@
   </si>
   <si>
     <t>1-534206-0</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>IC4, IC5</t>
+  </si>
+  <si>
+    <t>741G3157DCKR</t>
+  </si>
+  <si>
+    <t>SN74LVC1G3157</t>
+  </si>
+  <si>
+    <t>SC-70-6</t>
+  </si>
+  <si>
+    <t>296-14909-1-ND</t>
+  </si>
+  <si>
+    <t>SN74LVC1G3157DCKR</t>
   </si>
 </sst>
 </file>
@@ -2137,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2190,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2207,10 +2210,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2224,7 +2227,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J105)</f>
-        <v>179.21719999999999</v>
+        <v>178.41719999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2244,10 +2247,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2277,10 +2280,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G4" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2334,10 +2337,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="G6" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2350,7 +2353,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2394,10 +2397,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="G8" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2427,10 +2430,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G9" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2460,10 +2463,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="G10" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2476,7 +2479,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2529,10 +2532,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G12" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2562,10 +2565,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="G13" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2578,7 +2581,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2598,10 +2601,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="G14" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2614,7 +2617,7 @@
         <v>0.17</v>
       </c>
       <c r="L14" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2634,10 +2637,10 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="G15" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2650,7 +2653,7 @@
         <v>0.48</v>
       </c>
       <c r="L15" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2694,10 +2697,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="G17" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2775,10 +2778,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="G20" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2791,7 +2794,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L20" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2811,10 +2814,10 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="G21" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2868,10 +2871,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="G23" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2886,10 +2889,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B24" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
@@ -2901,10 +2904,10 @@
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="G24" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2967,10 +2970,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="G26" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3000,10 +3003,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="G27" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3016,7 +3019,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3036,10 +3039,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="G28" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3069,10 +3072,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="G29" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3102,10 +3105,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G30" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3118,7 +3121,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3138,10 +3141,10 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="G31" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3156,103 +3159,106 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>426</v>
       </c>
       <c r="B32" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="C32" t="s">
-        <v>407</v>
+        <v>428</v>
       </c>
       <c r="D32" t="s">
-        <v>407</v>
+        <v>429</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>406</v>
+        <v>430</v>
       </c>
       <c r="G32" t="s">
-        <v>407</v>
+        <v>431</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>2.15</v>
+        <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>400</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>400</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>400</v>
       </c>
       <c r="E33" t="s">
         <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>399</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
+        <v>400</v>
       </c>
       <c r="H33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>0.77</v>
+        <v>2.15</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>402</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>327</v>
+        <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>404</v>
+        <v>89</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B35" t="s">
         <v>90</v>
@@ -3264,13 +3270,10 @@
         <v>91</v>
       </c>
       <c r="E35" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F35" t="s">
-        <v>403</v>
-      </c>
-      <c r="G35" t="s">
-        <v>15</v>
+        <v>397</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -3285,115 +3288,112 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>394</v>
       </c>
       <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" t="s">
+        <v>320</v>
+      </c>
+      <c r="F36" t="s">
+        <v>396</v>
+      </c>
+      <c r="G36" t="s">
         <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" t="s">
-        <v>427</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
-        <v>94</v>
-      </c>
-      <c r="G36" t="s">
-        <v>95</v>
       </c>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="I36">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>420</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>352</v>
+        <v>94</v>
       </c>
       <c r="G37" t="s">
-        <v>353</v>
+        <v>95</v>
       </c>
       <c r="H37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I37">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>345</v>
       </c>
       <c r="G38" t="s">
-        <v>104</v>
+        <v>346</v>
       </c>
       <c r="H38">
         <v>3</v>
       </c>
       <c r="I38">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L38" t="s">
-        <v>363</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>426</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
         <v>101</v>
@@ -3408,376 +3408,379 @@
         <v>104</v>
       </c>
       <c r="H39">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I39">
         <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>1.26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>419</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E40" t="s">
         <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G40" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I40">
-        <v>3.65</v>
+        <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>425</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>422</v>
+        <v>107</v>
       </c>
       <c r="G41" t="s">
-        <v>423</v>
+        <v>108</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>0.13</v>
+        <v>3.65</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>424</v>
+        <v>418</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>418</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>419</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="G42" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>0.71</v>
+        <v>0.13</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>411</v>
       </c>
       <c r="D43" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="G43" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" t="s">
-        <v>112</v>
+        <v>421</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
-        <v>114</v>
+        <v>420</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>115</v>
+        <v>422</v>
       </c>
       <c r="G44" t="s">
-        <v>116</v>
+        <v>423</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G45" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G46" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G47" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>132</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
+        <v>133</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1.85</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
-      </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G49" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="H49">
-        <v>25</v>
-      </c>
-      <c r="I49">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G50" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I50">
-        <v>0.84</v>
+        <v>0.3</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D51" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G51" t="s">
         <v>15</v>
@@ -3792,10 +3795,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>424</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
         <v>140</v>
@@ -3807,10 +3810,10 @@
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G52" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3825,13 +3828,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>157</v>
+        <v>425</v>
       </c>
       <c r="B53" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D53" t="s">
         <v>141</v>
@@ -3840,10 +3843,10 @@
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="G53" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3858,25 +3861,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="G54" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3891,25 +3894,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D55" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G55" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3924,25 +3927,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B56">
         <v>470</v>
       </c>
       <c r="C56" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" t="s">
+        <v>158</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
         <v>164</v>
       </c>
-      <c r="D56" t="s">
+      <c r="G56" t="s">
         <v>165</v>
-      </c>
-      <c r="E56" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" t="s">
-        <v>171</v>
-      </c>
-      <c r="G56" t="s">
-        <v>172</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3957,25 +3960,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G57" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H57">
         <v>59</v>
@@ -3990,25 +3993,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G58" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H58">
         <v>4</v>
@@ -4023,13 +4026,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D59" t="s">
         <v>120</v>
@@ -4038,10 +4041,10 @@
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="G59" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4056,13 +4059,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C60" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D60" t="s">
         <v>120</v>
@@ -4071,10 +4074,10 @@
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="G60" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4089,25 +4092,25 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G61" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4122,25 +4125,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B62">
         <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="G62" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H62">
         <v>24</v>
@@ -4155,25 +4158,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B63">
         <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D63" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G63" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H63">
         <v>10</v>
@@ -4188,25 +4191,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B64" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C64" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E64" t="s">
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G64" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="H64">
         <v>15</v>
@@ -4221,25 +4224,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D65" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G65" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H65">
         <v>6</v>
@@ -4254,25 +4257,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B66" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C66" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G66" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H66">
         <v>3</v>
@@ -4287,25 +4290,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B67" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C67" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D67" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E67" t="s">
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="G67" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H67">
         <v>4</v>
@@ -4320,25 +4323,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D68" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G68" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4353,25 +4356,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B69" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D69" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="G69" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4386,25 +4389,25 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B70">
         <v>0.3</v>
       </c>
       <c r="C70" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D70" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G70" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4419,25 +4422,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B71" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D71" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E71" t="s">
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G71" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4452,25 +4455,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B72" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C72" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D72" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E72" t="s">
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G72" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4485,25 +4488,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B73" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C73" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D73" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
       <c r="F73" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G73" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4518,16 +4521,16 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B74" t="s">
         <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D74" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E74" t="s">
         <v>20</v>
@@ -4545,25 +4548,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B75" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C75" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D75" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G75" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4578,13 +4581,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B76" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C76" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D76" t="s">
         <v>120</v>
@@ -4593,10 +4596,10 @@
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G76" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4611,13 +4614,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B77" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C77" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D77" t="s">
         <v>120</v>
@@ -4626,10 +4629,10 @@
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="G77" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4644,25 +4647,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C78" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E78" t="s">
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G78" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4677,25 +4680,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B79" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D79" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="G79" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4710,25 +4713,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B80" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C80" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D80" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="G80" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4743,25 +4746,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B81" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C81" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D81" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G81" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4776,25 +4779,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B82" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C82" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D82" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G82" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4809,25 +4812,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B83" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C83" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D83" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="G83" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4842,25 +4845,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B84" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C84" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D84" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="G84" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4875,25 +4878,25 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B85" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C85" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D85" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="G85" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4908,25 +4911,25 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B86" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C86" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D86" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E86" t="s">
         <v>20</v>
       </c>
       <c r="F86" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G86" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4941,25 +4944,25 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="B87" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C87" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D87" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E87" t="s">
         <v>20</v>
       </c>
       <c r="F87" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="G87" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4974,25 +4977,25 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B88" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C88" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D88" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E88" t="s">
         <v>20</v>
       </c>
       <c r="F88" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="G88" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -5007,16 +5010,16 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B89" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C89" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D89" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="G89" t="s">
         <v>15</v>
@@ -5029,30 +5032,30 @@
         <v>0</v>
       </c>
       <c r="K89" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B90" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C90" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D90" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E90" t="s">
         <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="G90" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5067,25 +5070,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B91" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C91" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D91" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E91" t="s">
         <v>20</v>
       </c>
       <c r="F91" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="G91" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5100,25 +5103,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B92" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C92" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D92" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E92" t="s">
         <v>20</v>
       </c>
       <c r="F92" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G92" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5133,25 +5136,25 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B93" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C93" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D93" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E93" t="s">
         <v>20</v>
       </c>
       <c r="F93" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="G93" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5166,25 +5169,25 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B94" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C94" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="D94" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="E94" t="s">
         <v>20</v>
       </c>
       <c r="F94" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="G94" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5199,25 +5202,25 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B95" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C95" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D95" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E95" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F95" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="G95" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -5232,25 +5235,25 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B96" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C96" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D96" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E96" t="s">
         <v>20</v>
       </c>
       <c r="F96" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G96" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -5265,16 +5268,16 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B97" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C97" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D97" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Updated gyro U14 to new model, the L3GD20.
C27 and R40 are noted in the schematic as DNP unless using an L3G4200D (they are pin and register compatible). They have also been removed from the BOM as the use of a L3G4200D will not be a standard configuration.
Added WHO_AM_I and slave address definitions to L3G4200D.h for both gyros.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="427">
   <si>
     <t>Part</t>
   </si>
@@ -145,12 +145,6 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>C27</t>
-  </si>
-  <si>
-    <t>470nF</t>
-  </si>
-  <si>
     <t>C31, C43, C46</t>
   </si>
   <si>
@@ -514,9 +508,6 @@
     <t>ERJ-3EKF4700V</t>
   </si>
   <si>
-    <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R40, R76, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96, R97, R98, R99, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -955,18 +946,9 @@
     <t>U14</t>
   </si>
   <si>
-    <t>L3G4200D</t>
-  </si>
-  <si>
     <t>LGA16-4X4</t>
   </si>
   <si>
-    <t>497-11071-1-ND</t>
-  </si>
-  <si>
-    <t>L3G4200DTR</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -1153,15 +1135,6 @@
     <t>10nF = 10k pF (redundant line item)</t>
   </si>
   <si>
-    <t>470nF = 0.47uF</t>
-  </si>
-  <si>
-    <t>445-3454-1-ND</t>
-  </si>
-  <si>
-    <t>C1608Y5V1E474Z</t>
-  </si>
-  <si>
     <t>33nF = 33k pF = 0.033uF</t>
   </si>
   <si>
@@ -1310,6 +1283,18 @@
   </si>
   <si>
     <t>SN74LVC1G3157DCKR</t>
+  </si>
+  <si>
+    <t>L3GD20</t>
+  </si>
+  <si>
+    <t>497-12081-1-ND</t>
+  </si>
+  <si>
+    <t>L3GD20TR</t>
+  </si>
+  <si>
+    <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96, R97, R98, R99, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
   </si>
 </sst>
 </file>
@@ -2138,10 +2123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,7 +2175,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2210,10 +2195,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2226,8 +2211,8 @@
         <v>0.27</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J105)</f>
-        <v>178.41719999999998</v>
+        <f>SUM(J2:J104)</f>
+        <v>173.76339999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2247,10 +2232,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="G3" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2259,13 +2244,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J70" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J69" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2280,10 +2265,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G4" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2337,10 +2322,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G6" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2353,7 +2338,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2397,10 +2382,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="G8" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2430,10 +2415,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G9" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2463,10 +2448,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="G10" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2479,7 +2464,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2532,10 +2517,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G12" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2565,10 +2550,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="G13" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2581,7 +2566,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2601,23 +2586,23 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="G14" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I14">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0.17</v>
+        <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2628,56 +2613,53 @@
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>383</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>384</v>
+        <v>15</v>
       </c>
       <c r="H15">
         <v>3</v>
       </c>
-      <c r="I15">
-        <v>0.16</v>
-      </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0.48</v>
-      </c>
-      <c r="L15" t="s">
-        <v>382</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>358</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>359</v>
       </c>
       <c r="H16">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0.35</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2688,29 +2670,20 @@
         <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>364</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>365</v>
+        <v>15</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>0.35</v>
-      </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2721,10 +2694,10 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
         <v>15</v>
@@ -2739,26 +2712,38 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>360</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>361</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
+      <c r="I19">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L19" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2778,23 +2763,20 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G20" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
-        <v>0.28999999999999998</v>
+        <v>0.24</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="L20" t="s">
-        <v>368</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2810,24 +2792,15 @@
       <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" t="s">
-        <v>369</v>
-      </c>
       <c r="G21" t="s">
-        <v>370</v>
+        <v>15</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21">
-        <v>0.24</v>
-      </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2838,28 +2811,37 @@
         <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>365</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>366</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
+      <c r="I22">
+        <v>0.1</v>
+      </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>392</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>393</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -2871,10 +2853,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="G23" t="s">
-        <v>372</v>
+        <v>395</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2889,68 +2871,68 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>401</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>402</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>403</v>
+        <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>404</v>
+        <v>66</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="I24">
-        <v>0.1</v>
+        <v>0.315</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
         <v>67</v>
       </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
       <c r="E25" t="s">
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>341</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>342</v>
       </c>
       <c r="H25">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="I25">
-        <v>0.315</v>
+        <v>0.35</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>8.19</v>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2961,65 +2943,65 @@
         <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>347</v>
+        <v>383</v>
       </c>
       <c r="G26" t="s">
-        <v>348</v>
+        <v>384</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>0.4</v>
+      </c>
+      <c r="L26" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
         <v>73</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" t="s">
-        <v>76</v>
-      </c>
       <c r="E27" t="s">
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="G27" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0.4</v>
+        <v>0.68</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L27" t="s">
-        <v>398</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3030,29 +3012,29 @@
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G28" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0.68</v>
+        <v>0.42</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3063,29 +3045,32 @@
         <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="G29" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29">
-        <v>0.42</v>
+        <v>0.9</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>2.7</v>
+      </c>
+      <c r="L29" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3096,136 +3081,133 @@
         <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>389</v>
+        <v>326</v>
       </c>
       <c r="G30" t="s">
-        <v>390</v>
+        <v>327</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
       <c r="I30">
-        <v>0.9</v>
+        <v>11.91</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="L30" t="s">
-        <v>391</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>417</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>418</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>419</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>420</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>332</v>
+        <v>421</v>
       </c>
       <c r="G31" t="s">
-        <v>333</v>
+        <v>422</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31">
-        <v>11.91</v>
+        <v>0.44</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>426</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>427</v>
+        <v>391</v>
       </c>
       <c r="C32" t="s">
-        <v>428</v>
+        <v>391</v>
       </c>
       <c r="D32" t="s">
-        <v>429</v>
+        <v>391</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="G32" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>0.44</v>
+        <v>2.15</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="B33" t="s">
-        <v>400</v>
-      </c>
       <c r="C33" t="s">
-        <v>400</v>
+        <v>86</v>
       </c>
       <c r="D33" t="s">
-        <v>400</v>
+        <v>86</v>
       </c>
       <c r="E33" t="s">
         <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>399</v>
+        <v>87</v>
       </c>
       <c r="G33" t="s">
-        <v>400</v>
+        <v>86</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>2.15</v>
+        <v>0.77</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>386</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
@@ -3234,46 +3216,46 @@
         <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>314</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" t="s">
-        <v>88</v>
+        <v>388</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34">
-        <v>0.77</v>
+        <v>0.5</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F35" t="s">
-        <v>397</v>
+        <v>387</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -3288,106 +3270,109 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>394</v>
+        <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>411</v>
       </c>
       <c r="E36" t="s">
-        <v>320</v>
+        <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>396</v>
+        <v>92</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="I36">
-        <v>0.5</v>
+        <v>0.93</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>420</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>339</v>
       </c>
       <c r="G37" t="s">
-        <v>95</v>
+        <v>340</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I37">
-        <v>0.93</v>
+        <v>1.47</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>345</v>
+        <v>101</v>
       </c>
       <c r="G38" t="s">
-        <v>346</v>
+        <v>102</v>
       </c>
       <c r="H38">
         <v>3</v>
       </c>
       <c r="I38">
-        <v>1.47</v>
+        <v>0.42</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>1.26</v>
+      </c>
+      <c r="L38" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>410</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -3396,139 +3381,133 @@
         <v>100</v>
       </c>
       <c r="D39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
         <v>101</v>
       </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" t="s">
-        <v>103</v>
-      </c>
       <c r="G39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I39">
         <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L39" t="s">
-        <v>356</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>419</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
         <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H40">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>0.42</v>
+        <v>3.65</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>409</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>107</v>
+        <v>406</v>
       </c>
       <c r="G41" t="s">
-        <v>108</v>
+        <v>407</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <v>3.65</v>
+        <v>0.13</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>418</v>
-      </c>
-      <c r="B42" t="s">
-        <v>15</v>
+        <v>408</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>402</v>
       </c>
       <c r="D42" t="s">
-        <v>110</v>
+        <v>403</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="G42" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0.13</v>
+        <v>0.71</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
         <v>411</v>
-      </c>
-      <c r="D43" t="s">
-        <v>412</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
@@ -3543,376 +3522,379 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>421</v>
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
-        <v>420</v>
+        <v>112</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>422</v>
+        <v>113</v>
       </c>
       <c r="G44" t="s">
-        <v>423</v>
+        <v>114</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>3.15</v>
+        <v>2.13</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G45" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D46" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G46" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G47" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G48" t="s">
-        <v>134</v>
+        <v>15</v>
       </c>
       <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48">
-        <v>1.85</v>
+        <v>8</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>140</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="H49">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="I49">
+        <v>0.3</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
-      </c>
-      <c r="E50" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G50" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="H50">
-        <v>25</v>
-      </c>
-      <c r="I50">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>415</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" t="s">
         <v>147</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="H51">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0.41</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G52" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>425</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>153</v>
+        <v>328</v>
       </c>
       <c r="G53" t="s">
-        <v>154</v>
+        <v>329</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" t="s">
         <v>155</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>156</v>
       </c>
-      <c r="C54" t="s">
-        <v>157</v>
-      </c>
-      <c r="D54" t="s">
-        <v>158</v>
-      </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>334</v>
+        <v>159</v>
       </c>
       <c r="G54" t="s">
-        <v>335</v>
+        <v>160</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="B55">
+        <v>470</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G55" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3927,115 +3909,115 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>163</v>
-      </c>
-      <c r="B56">
-        <v>470</v>
+        <v>426</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
       </c>
       <c r="C56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E56" t="s">
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="I56">
-        <v>0.04</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.8004</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G57" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H57">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="I57">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.81420000000000003</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>330</v>
       </c>
       <c r="D58" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>172</v>
+        <v>331</v>
       </c>
       <c r="G58" t="s">
-        <v>173</v>
+        <v>332</v>
       </c>
       <c r="H58">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I58">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" t="s">
         <v>174</v>
       </c>
-      <c r="B59" t="s">
-        <v>175</v>
-      </c>
       <c r="C59" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
@@ -4059,49 +4041,49 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" t="s">
         <v>176</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" t="s">
         <v>177</v>
       </c>
-      <c r="C60" t="s">
-        <v>336</v>
-      </c>
-      <c r="D60" t="s">
-        <v>120</v>
-      </c>
-      <c r="E60" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" t="s">
-        <v>343</v>
-      </c>
       <c r="G60" t="s">
-        <v>344</v>
+        <v>178</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>178</v>
-      </c>
-      <c r="B61" t="s">
         <v>179</v>
       </c>
+      <c r="B61">
+        <v>200</v>
+      </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D61" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
@@ -4113,14 +4095,14 @@
         <v>181</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I61">
         <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -4128,13 +4110,13 @@
         <v>182</v>
       </c>
       <c r="B62">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D62" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
@@ -4146,202 +4128,202 @@
         <v>184</v>
       </c>
       <c r="H62">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>185</v>
       </c>
-      <c r="B63">
-        <v>100</v>
+      <c r="B63" t="s">
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D63" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G63" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H63">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D64" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E64" t="s">
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G64" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H64">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B65" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D65" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G65" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C66" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G66" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H66">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D67" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E67" t="s">
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G67" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H67">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D68" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E68" t="s">
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G68" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4356,91 +4338,91 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>208</v>
-      </c>
-      <c r="B69" t="s">
         <v>209</v>
       </c>
+      <c r="B69">
+        <v>0.3</v>
+      </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G69" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H69">
         <v>1</v>
       </c>
       <c r="I69">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>212</v>
-      </c>
-      <c r="B70">
-        <v>0.3</v>
+        <v>214</v>
+      </c>
+      <c r="B70" t="s">
+        <v>215</v>
       </c>
       <c r="C70" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
       <c r="D70" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G70" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H70">
         <v>1</v>
       </c>
       <c r="I70">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J70">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" ref="J70:J96" si="1">H70*I70</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B71" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E71" t="s">
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G71" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4449,31 +4431,31 @@
         <v>0.04</v>
       </c>
       <c r="J71">
-        <f t="shared" ref="J71:J97" si="1">H71*I71</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C72" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D72" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E72" t="s">
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G72" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4488,118 +4470,118 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E73" t="s">
         <v>20</v>
       </c>
-      <c r="F73" t="s">
-        <v>227</v>
-      </c>
       <c r="G73" t="s">
-        <v>228</v>
+        <v>15</v>
       </c>
       <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>227</v>
+      </c>
+      <c r="B74" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" t="s">
+        <v>155</v>
+      </c>
+      <c r="D74" t="s">
+        <v>156</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" t="s">
         <v>229</v>
       </c>
-      <c r="B74" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" t="s">
-        <v>157</v>
-      </c>
-      <c r="D74" t="s">
-        <v>158</v>
-      </c>
-      <c r="E74" t="s">
-        <v>20</v>
-      </c>
       <c r="G74" t="s">
-        <v>15</v>
+        <v>230</v>
       </c>
       <c r="H74">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>330</v>
       </c>
       <c r="D75" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>232</v>
+        <v>333</v>
       </c>
       <c r="G75" t="s">
-        <v>233</v>
+        <v>334</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>233</v>
+      </c>
+      <c r="B76" t="s">
         <v>234</v>
       </c>
-      <c r="B76" t="s">
-        <v>235</v>
-      </c>
       <c r="C76" t="s">
+        <v>330</v>
+      </c>
+      <c r="D76" t="s">
+        <v>118</v>
+      </c>
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" t="s">
+        <v>335</v>
+      </c>
+      <c r="G76" t="s">
         <v>336</v>
-      </c>
-      <c r="D76" t="s">
-        <v>120</v>
-      </c>
-      <c r="E76" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" t="s">
-        <v>339</v>
-      </c>
-      <c r="G76" t="s">
-        <v>340</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4614,58 +4596,58 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>235</v>
+      </c>
+      <c r="B77" t="s">
         <v>236</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" t="s">
+        <v>156</v>
+      </c>
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
         <v>237</v>
       </c>
-      <c r="C77" t="s">
-        <v>336</v>
-      </c>
-      <c r="D77" t="s">
-        <v>120</v>
-      </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" t="s">
-        <v>341</v>
-      </c>
       <c r="G77" t="s">
-        <v>342</v>
+        <v>238</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B78" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E78" t="s">
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G78" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4680,524 +4662,524 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>244</v>
       </c>
       <c r="D79" t="s">
-        <v>158</v>
+        <v>245</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G79" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C80" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D80" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G80" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B81" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C81" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D81" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="G81" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>6.6</v>
+        <v>0.5</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B82" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C82" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D82" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G82" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.5</v>
+        <v>0.79</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B83" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C83" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="G83" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>0.79</v>
+        <v>0.67</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B84" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C84" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D84" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G84" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B85" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C85" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D85" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G85" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B86" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C86" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D86" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E86" t="s">
         <v>20</v>
       </c>
       <c r="F86" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G86" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B87" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C87" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D87" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E87" t="s">
         <v>20</v>
       </c>
       <c r="F87" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G87" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>5.88</v>
+        <v>1.51</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B88" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C88" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D88" t="s">
-        <v>290</v>
-      </c>
-      <c r="E88" t="s">
-        <v>20</v>
-      </c>
-      <c r="F88" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G88" t="s">
-        <v>292</v>
+        <v>15</v>
       </c>
       <c r="H88">
         <v>1</v>
-      </c>
-      <c r="I88">
-        <v>1.51</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>0</v>
+      </c>
+      <c r="K88" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B89" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C89" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D89" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" t="s">
+        <v>297</v>
       </c>
       <c r="G89" t="s">
-        <v>15</v>
+        <v>298</v>
       </c>
       <c r="H89">
         <v>1</v>
+      </c>
+      <c r="I89">
+        <v>0.47</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K89" t="s">
-        <v>296</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B90" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D90" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E90" t="s">
         <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G90" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>0.47</v>
+        <v>3.79</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B91" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C91" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D91" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E91" t="s">
         <v>20</v>
       </c>
       <c r="F91" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G91" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B92" t="s">
-        <v>308</v>
+        <v>423</v>
       </c>
       <c r="C92" t="s">
-        <v>308</v>
+        <v>423</v>
       </c>
       <c r="D92" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E92" t="s">
         <v>20</v>
       </c>
       <c r="F92" t="s">
-        <v>310</v>
+        <v>424</v>
       </c>
       <c r="G92" t="s">
-        <v>311</v>
+        <v>425</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="B93" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="C93" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="D93" t="s">
-        <v>314</v>
+        <v>400</v>
       </c>
       <c r="E93" t="s">
         <v>20</v>
       </c>
       <c r="F93" t="s">
-        <v>315</v>
+        <v>399</v>
       </c>
       <c r="G93" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>12.95</v>
+        <v>6.84</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>12.95</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>406</v>
+        <v>311</v>
       </c>
       <c r="B94" t="s">
-        <v>407</v>
+        <v>312</v>
       </c>
       <c r="C94" t="s">
-        <v>407</v>
+        <v>312</v>
       </c>
       <c r="D94" t="s">
-        <v>409</v>
+        <v>313</v>
       </c>
       <c r="E94" t="s">
-        <v>20</v>
+        <v>314</v>
       </c>
       <c r="F94" t="s">
-        <v>408</v>
+        <v>315</v>
       </c>
       <c r="G94" t="s">
-        <v>410</v>
+        <v>316</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>6.84</v>
+        <v>1.5</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -5214,31 +5196,31 @@
         <v>319</v>
       </c>
       <c r="E95" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" t="s">
         <v>320</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>321</v>
       </c>
-      <c r="G95" t="s">
-        <v>322</v>
-      </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>322</v>
+      </c>
+      <c r="B96" t="s">
         <v>323</v>
-      </c>
-      <c r="B96" t="s">
-        <v>324</v>
       </c>
       <c r="C96" t="s">
         <v>324</v>
@@ -5246,46 +5228,13 @@
       <c r="D96" t="s">
         <v>325</v>
       </c>
-      <c r="E96" t="s">
-        <v>20</v>
-      </c>
-      <c r="F96" t="s">
-        <v>326</v>
-      </c>
       <c r="G96" t="s">
-        <v>327</v>
+        <v>15</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
-      <c r="I96">
-        <v>2.96</v>
-      </c>
       <c r="J96">
-        <f t="shared" si="1"/>
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>328</v>
-      </c>
-      <c r="B97" t="s">
-        <v>329</v>
-      </c>
-      <c r="C97" t="s">
-        <v>330</v>
-      </c>
-      <c r="D97" t="s">
-        <v>331</v>
-      </c>
-      <c r="G97" t="s">
-        <v>15</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="J97">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Made the Pmod current limit resistors (R41-R64) a 0402 package.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -556,12 +556,6 @@
     <t>R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64</t>
   </si>
   <si>
-    <t>P200HCT-ND</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF2000V</t>
-  </si>
-  <si>
     <t>R65, R66, R67, R68, R100, R101, R102, R103, R104, R105</t>
   </si>
   <si>
@@ -1295,6 +1289,12 @@
   </si>
   <si>
     <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96, R97, R98, R99, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
+  </si>
+  <si>
+    <t>P200JCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ201X</t>
   </si>
 </sst>
 </file>
@@ -2125,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2175,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2195,10 +2195,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J104)</f>
-        <v>173.76339999999999</v>
+        <v>172.80339999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2232,10 +2232,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2265,10 +2265,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2322,10 +2322,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2338,7 +2338,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2382,10 +2382,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2415,10 +2415,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2448,10 +2448,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2464,7 +2464,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2517,10 +2517,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2550,10 +2550,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2566,7 +2566,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,10 +2586,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2602,7 +2602,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2646,10 +2646,10 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G16" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2727,10 +2727,10 @@
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2743,7 +2743,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2763,10 +2763,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G20" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2820,10 +2820,10 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G22" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2838,10 +2838,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B23" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -2853,10 +2853,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G23" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2919,10 +2919,10 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -2952,10 +2952,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G26" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2968,7 +2968,7 @@
         <v>0.4</v>
       </c>
       <c r="L26" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2988,10 +2988,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G27" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3021,10 +3021,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G28" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3054,10 +3054,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G29" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -3070,7 +3070,7 @@
         <v>2.7</v>
       </c>
       <c r="L29" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3090,10 +3090,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G30" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3108,25 +3108,25 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>415</v>
+      </c>
+      <c r="B31" t="s">
+        <v>416</v>
+      </c>
+      <c r="C31" t="s">
         <v>417</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>418</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" t="s">
         <v>419</v>
       </c>
-      <c r="D31" t="s">
+      <c r="G31" t="s">
         <v>420</v>
-      </c>
-      <c r="E31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" t="s">
-        <v>421</v>
-      </c>
-      <c r="G31" t="s">
-        <v>422</v>
       </c>
       <c r="H31">
         <v>2</v>
@@ -3144,22 +3144,22 @@
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
@@ -3219,10 +3219,10 @@
         <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F34" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
@@ -3249,10 +3249,10 @@
         <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F35" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G35" t="s">
         <v>15</v>
@@ -3279,7 +3279,7 @@
         <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
@@ -3318,10 +3318,10 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G37" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -3367,12 +3367,12 @@
         <v>1.26</v>
       </c>
       <c r="L38" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
@@ -3453,10 +3453,10 @@
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G41" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H41">
         <v>3</v>
@@ -3471,22 +3471,22 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C42" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" t="s">
+        <v>401</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
         <v>402</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>403</v>
-      </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
-        <v>404</v>
-      </c>
-      <c r="G42" t="s">
-        <v>405</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3501,22 +3501,22 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C43" t="s">
         <v>91</v>
       </c>
       <c r="D43" t="s">
+        <v>409</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
         <v>411</v>
       </c>
-      <c r="E43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" t="s">
-        <v>413</v>
-      </c>
       <c r="G43" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3744,7 +3744,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B51" t="s">
         <v>146</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B52" t="s">
         <v>149</v>
@@ -3825,10 +3825,10 @@
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G53" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B56" t="s">
         <v>164</v>
@@ -3981,7 +3981,7 @@
         <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D58" t="s">
         <v>118</v>
@@ -3990,10 +3990,10 @@
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G58" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -4014,7 +4014,7 @@
         <v>174</v>
       </c>
       <c r="C59" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D59" t="s">
         <v>118</v>
@@ -4023,10 +4023,10 @@
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G59" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4080,34 +4080,34 @@
         <v>200</v>
       </c>
       <c r="C61" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>180</v>
+        <v>425</v>
       </c>
       <c r="G61" t="s">
-        <v>181</v>
+        <v>426</v>
       </c>
       <c r="H61">
         <v>24</v>
       </c>
       <c r="I61">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B62">
         <v>100</v>
@@ -4122,10 +4122,10 @@
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G62" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H62">
         <v>10</v>
@@ -4140,10 +4140,10 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C63" t="s">
         <v>155</v>
@@ -4155,10 +4155,10 @@
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H63">
         <v>15</v>
@@ -4173,10 +4173,10 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B64" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C64" t="s">
         <v>155</v>
@@ -4188,10 +4188,10 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G64" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H64">
         <v>6</v>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B65" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C65" t="s">
         <v>155</v>
@@ -4221,10 +4221,10 @@
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G65" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H65">
         <v>3</v>
@@ -4239,10 +4239,10 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C66" t="s">
         <v>155</v>
@@ -4254,10 +4254,10 @@
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H66">
         <v>4</v>
@@ -4272,10 +4272,10 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C67" t="s">
         <v>155</v>
@@ -4287,10 +4287,10 @@
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G67" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -4305,10 +4305,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C68" t="s">
         <v>155</v>
@@ -4320,10 +4320,10 @@
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G68" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4338,25 +4338,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B69">
         <v>0.3</v>
       </c>
       <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="D69" t="s">
+        <v>209</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" t="s">
         <v>210</v>
       </c>
-      <c r="D69" t="s">
+      <c r="G69" t="s">
         <v>211</v>
-      </c>
-      <c r="E69" t="s">
-        <v>20</v>
-      </c>
-      <c r="F69" t="s">
-        <v>212</v>
-      </c>
-      <c r="G69" t="s">
-        <v>213</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4371,10 +4371,10 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C70" t="s">
         <v>155</v>
@@ -4386,10 +4386,10 @@
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G70" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4404,10 +4404,10 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
         <v>155</v>
@@ -4419,10 +4419,10 @@
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G71" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4437,10 +4437,10 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B72" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C72" t="s">
         <v>155</v>
@@ -4452,10 +4452,10 @@
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G72" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
@@ -4497,10 +4497,10 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B74" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C74" t="s">
         <v>155</v>
@@ -4512,10 +4512,10 @@
         <v>20</v>
       </c>
       <c r="F74" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4530,13 +4530,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C75" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D75" t="s">
         <v>118</v>
@@ -4545,10 +4545,10 @@
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G75" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4563,13 +4563,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B76" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C76" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D76" t="s">
         <v>118</v>
@@ -4578,10 +4578,10 @@
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G76" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4596,10 +4596,10 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B77" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C77" t="s">
         <v>155</v>
@@ -4611,10 +4611,10 @@
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G77" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4629,10 +4629,10 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B78" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C78" t="s">
         <v>155</v>
@@ -4644,10 +4644,10 @@
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G78" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4662,25 +4662,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>241</v>
+      </c>
+      <c r="B79" t="s">
+        <v>242</v>
+      </c>
+      <c r="C79" t="s">
+        <v>242</v>
+      </c>
+      <c r="D79" t="s">
         <v>243</v>
       </c>
-      <c r="B79" t="s">
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" t="s">
         <v>244</v>
       </c>
-      <c r="C79" t="s">
-        <v>244</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="G79" t="s">
         <v>245</v>
-      </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" t="s">
-        <v>246</v>
-      </c>
-      <c r="G79" t="s">
-        <v>247</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4695,25 +4695,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>246</v>
+      </c>
+      <c r="B80" t="s">
+        <v>247</v>
+      </c>
+      <c r="C80" t="s">
+        <v>247</v>
+      </c>
+      <c r="D80" t="s">
         <v>248</v>
       </c>
-      <c r="B80" t="s">
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" t="s">
         <v>249</v>
       </c>
-      <c r="C80" t="s">
-        <v>249</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="G80" t="s">
         <v>250</v>
-      </c>
-      <c r="E80" t="s">
-        <v>20</v>
-      </c>
-      <c r="F80" t="s">
-        <v>251</v>
-      </c>
-      <c r="G80" t="s">
-        <v>252</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4728,25 +4728,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>251</v>
+      </c>
+      <c r="B81" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" t="s">
         <v>253</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>254</v>
       </c>
-      <c r="C81" t="s">
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" t="s">
         <v>255</v>
       </c>
-      <c r="D81" t="s">
+      <c r="G81" t="s">
         <v>256</v>
-      </c>
-      <c r="E81" t="s">
-        <v>20</v>
-      </c>
-      <c r="F81" t="s">
-        <v>257</v>
-      </c>
-      <c r="G81" t="s">
-        <v>258</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4761,25 +4761,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>257</v>
+      </c>
+      <c r="B82" t="s">
+        <v>258</v>
+      </c>
+      <c r="C82" t="s">
         <v>259</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>260</v>
       </c>
-      <c r="C82" t="s">
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" t="s">
         <v>261</v>
       </c>
-      <c r="D82" t="s">
+      <c r="G82" t="s">
         <v>262</v>
-      </c>
-      <c r="E82" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" t="s">
-        <v>263</v>
-      </c>
-      <c r="G82" t="s">
-        <v>264</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4794,25 +4794,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>263</v>
+      </c>
+      <c r="B83" t="s">
+        <v>264</v>
+      </c>
+      <c r="C83" t="s">
+        <v>264</v>
+      </c>
+      <c r="D83" t="s">
         <v>265</v>
       </c>
-      <c r="B83" t="s">
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" t="s">
         <v>266</v>
       </c>
-      <c r="C83" t="s">
-        <v>266</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="G83" t="s">
         <v>267</v>
-      </c>
-      <c r="E83" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" t="s">
-        <v>268</v>
-      </c>
-      <c r="G83" t="s">
-        <v>269</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4827,25 +4827,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>268</v>
+      </c>
+      <c r="B84" t="s">
+        <v>269</v>
+      </c>
+      <c r="C84" t="s">
+        <v>269</v>
+      </c>
+      <c r="D84" t="s">
         <v>270</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" t="s">
         <v>271</v>
       </c>
-      <c r="C84" t="s">
-        <v>271</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="G84" t="s">
         <v>272</v>
-      </c>
-      <c r="E84" t="s">
-        <v>20</v>
-      </c>
-      <c r="F84" t="s">
-        <v>273</v>
-      </c>
-      <c r="G84" t="s">
-        <v>274</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4860,25 +4860,25 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>273</v>
+      </c>
+      <c r="B85" t="s">
+        <v>274</v>
+      </c>
+      <c r="C85" t="s">
+        <v>274</v>
+      </c>
+      <c r="D85" t="s">
         <v>275</v>
       </c>
-      <c r="B85" t="s">
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" t="s">
         <v>276</v>
       </c>
-      <c r="C85" t="s">
-        <v>276</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="G85" t="s">
         <v>277</v>
-      </c>
-      <c r="E85" t="s">
-        <v>20</v>
-      </c>
-      <c r="F85" t="s">
-        <v>278</v>
-      </c>
-      <c r="G85" t="s">
-        <v>279</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4893,25 +4893,25 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>278</v>
+      </c>
+      <c r="B86" t="s">
+        <v>279</v>
+      </c>
+      <c r="C86" t="s">
+        <v>279</v>
+      </c>
+      <c r="D86" t="s">
         <v>280</v>
       </c>
-      <c r="B86" t="s">
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" t="s">
         <v>281</v>
       </c>
-      <c r="C86" t="s">
-        <v>281</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
         <v>282</v>
-      </c>
-      <c r="E86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" t="s">
-        <v>283</v>
-      </c>
-      <c r="G86" t="s">
-        <v>284</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4926,25 +4926,25 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>283</v>
+      </c>
+      <c r="B87" t="s">
+        <v>284</v>
+      </c>
+      <c r="C87" t="s">
+        <v>284</v>
+      </c>
+      <c r="D87" t="s">
         <v>285</v>
       </c>
-      <c r="B87" t="s">
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" t="s">
         <v>286</v>
       </c>
-      <c r="C87" t="s">
-        <v>286</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>287</v>
-      </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="F87" t="s">
-        <v>288</v>
-      </c>
-      <c r="G87" t="s">
-        <v>289</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4959,16 +4959,16 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>288</v>
+      </c>
+      <c r="B88" t="s">
+        <v>289</v>
+      </c>
+      <c r="C88" t="s">
+        <v>289</v>
+      </c>
+      <c r="D88" t="s">
         <v>290</v>
-      </c>
-      <c r="B88" t="s">
-        <v>291</v>
-      </c>
-      <c r="C88" t="s">
-        <v>291</v>
-      </c>
-      <c r="D88" t="s">
-        <v>292</v>
       </c>
       <c r="G88" t="s">
         <v>15</v>
@@ -4981,30 +4981,30 @@
         <v>0</v>
       </c>
       <c r="K88" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>292</v>
+      </c>
+      <c r="B89" t="s">
+        <v>293</v>
+      </c>
+      <c r="C89" t="s">
+        <v>293</v>
+      </c>
+      <c r="D89" t="s">
         <v>294</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" t="s">
         <v>295</v>
       </c>
-      <c r="C89" t="s">
-        <v>295</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="G89" t="s">
         <v>296</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>297</v>
-      </c>
-      <c r="G89" t="s">
-        <v>298</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -5019,25 +5019,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>297</v>
+      </c>
+      <c r="B90" t="s">
+        <v>298</v>
+      </c>
+      <c r="C90" t="s">
+        <v>298</v>
+      </c>
+      <c r="D90" t="s">
         <v>299</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" t="s">
         <v>300</v>
       </c>
-      <c r="C90" t="s">
-        <v>300</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="G90" t="s">
         <v>301</v>
-      </c>
-      <c r="E90" t="s">
-        <v>20</v>
-      </c>
-      <c r="F90" t="s">
-        <v>302</v>
-      </c>
-      <c r="G90" t="s">
-        <v>303</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5052,25 +5052,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>302</v>
+      </c>
+      <c r="B91" t="s">
+        <v>303</v>
+      </c>
+      <c r="C91" t="s">
+        <v>303</v>
+      </c>
+      <c r="D91" t="s">
         <v>304</v>
       </c>
-      <c r="B91" t="s">
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" t="s">
         <v>305</v>
       </c>
-      <c r="C91" t="s">
-        <v>305</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="G91" t="s">
         <v>306</v>
-      </c>
-      <c r="E91" t="s">
-        <v>20</v>
-      </c>
-      <c r="F91" t="s">
-        <v>307</v>
-      </c>
-      <c r="G91" t="s">
-        <v>308</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5085,25 +5085,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B92" t="s">
+        <v>421</v>
+      </c>
+      <c r="C92" t="s">
+        <v>421</v>
+      </c>
+      <c r="D92" t="s">
+        <v>308</v>
+      </c>
+      <c r="E92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" t="s">
+        <v>422</v>
+      </c>
+      <c r="G92" t="s">
         <v>423</v>
-      </c>
-      <c r="C92" t="s">
-        <v>423</v>
-      </c>
-      <c r="D92" t="s">
-        <v>310</v>
-      </c>
-      <c r="E92" t="s">
-        <v>20</v>
-      </c>
-      <c r="F92" t="s">
-        <v>424</v>
-      </c>
-      <c r="G92" t="s">
-        <v>425</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5118,25 +5118,25 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>395</v>
+      </c>
+      <c r="B93" t="s">
+        <v>396</v>
+      </c>
+      <c r="C93" t="s">
+        <v>396</v>
+      </c>
+      <c r="D93" t="s">
+        <v>398</v>
+      </c>
+      <c r="E93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" t="s">
         <v>397</v>
       </c>
-      <c r="B93" t="s">
-        <v>398</v>
-      </c>
-      <c r="C93" t="s">
-        <v>398</v>
-      </c>
-      <c r="D93" t="s">
-        <v>400</v>
-      </c>
-      <c r="E93" t="s">
-        <v>20</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>399</v>
-      </c>
-      <c r="G93" t="s">
-        <v>401</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5151,25 +5151,25 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>309</v>
+      </c>
+      <c r="B94" t="s">
+        <v>310</v>
+      </c>
+      <c r="C94" t="s">
+        <v>310</v>
+      </c>
+      <c r="D94" t="s">
         <v>311</v>
       </c>
-      <c r="B94" t="s">
+      <c r="E94" t="s">
         <v>312</v>
       </c>
-      <c r="C94" t="s">
-        <v>312</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="F94" t="s">
         <v>313</v>
       </c>
-      <c r="E94" t="s">
+      <c r="G94" t="s">
         <v>314</v>
-      </c>
-      <c r="F94" t="s">
-        <v>315</v>
-      </c>
-      <c r="G94" t="s">
-        <v>316</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5184,25 +5184,25 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>315</v>
+      </c>
+      <c r="B95" t="s">
+        <v>316</v>
+      </c>
+      <c r="C95" t="s">
+        <v>316</v>
+      </c>
+      <c r="D95" t="s">
         <v>317</v>
       </c>
-      <c r="B95" t="s">
+      <c r="E95" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" t="s">
         <v>318</v>
       </c>
-      <c r="C95" t="s">
-        <v>318</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="G95" t="s">
         <v>319</v>
-      </c>
-      <c r="E95" t="s">
-        <v>20</v>
-      </c>
-      <c r="F95" t="s">
-        <v>320</v>
-      </c>
-      <c r="G95" t="s">
-        <v>321</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -5217,16 +5217,16 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>320</v>
+      </c>
+      <c r="B96" t="s">
+        <v>321</v>
+      </c>
+      <c r="C96" t="s">
         <v>322</v>
       </c>
-      <c r="B96" t="s">
+      <c r="D96" t="s">
         <v>323</v>
-      </c>
-      <c r="C96" t="s">
-        <v>324</v>
-      </c>
-      <c r="D96" t="s">
-        <v>325</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Changed R65-R68 to a 0402 package.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="430">
   <si>
     <t>Part</t>
   </si>
@@ -556,9 +556,6 @@
     <t>R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64</t>
   </si>
   <si>
-    <t>R65, R66, R67, R68, R100, R101, R102, R103, R104, R105</t>
-  </si>
-  <si>
     <t>P100HCT-ND</t>
   </si>
   <si>
@@ -1295,6 +1292,18 @@
   </si>
   <si>
     <t>ERJ-2GEJ201X</t>
+  </si>
+  <si>
+    <t>R65, R66, R67, R68</t>
+  </si>
+  <si>
+    <t>R100, R101, R102, R103, R104, R105</t>
+  </si>
+  <si>
+    <t>P100JCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ101X</t>
   </si>
 </sst>
 </file>
@@ -2123,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2184,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2195,10 +2204,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" t="s">
         <v>341</v>
-      </c>
-      <c r="G2" t="s">
-        <v>342</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2211,7 +2220,7 @@
         <v>0.27</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J104)</f>
+        <f>SUM(J2:J105)</f>
         <v>172.80339999999998</v>
       </c>
     </row>
@@ -2232,10 +2241,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G3" t="s">
         <v>343</v>
-      </c>
-      <c r="G3" t="s">
-        <v>344</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2244,13 +2253,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J69" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J70" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2265,10 +2274,10 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G4" t="s">
         <v>345</v>
-      </c>
-      <c r="G4" t="s">
-        <v>346</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2322,10 +2331,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>349</v>
+      </c>
+      <c r="G6" t="s">
         <v>350</v>
-      </c>
-      <c r="G6" t="s">
-        <v>351</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2338,7 +2347,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2382,10 +2391,10 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
+        <v>351</v>
+      </c>
+      <c r="G8" t="s">
         <v>352</v>
-      </c>
-      <c r="G8" t="s">
-        <v>353</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2415,10 +2424,10 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
+        <v>353</v>
+      </c>
+      <c r="G9" t="s">
         <v>354</v>
-      </c>
-      <c r="G9" t="s">
-        <v>355</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2448,10 +2457,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G10" t="s">
         <v>366</v>
-      </c>
-      <c r="G10" t="s">
-        <v>367</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2464,7 +2473,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2517,10 +2526,10 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
+        <v>367</v>
+      </c>
+      <c r="G12" t="s">
         <v>368</v>
-      </c>
-      <c r="G12" t="s">
-        <v>369</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2550,10 +2559,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
+        <v>365</v>
+      </c>
+      <c r="G13" t="s">
         <v>366</v>
-      </c>
-      <c r="G13" t="s">
-        <v>367</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2566,7 +2575,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,10 +2595,10 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
+        <v>371</v>
+      </c>
+      <c r="G14" t="s">
         <v>372</v>
-      </c>
-      <c r="G14" t="s">
-        <v>373</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2602,7 +2611,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2646,10 +2655,10 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G16" t="s">
         <v>356</v>
-      </c>
-      <c r="G16" t="s">
-        <v>357</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2727,10 +2736,10 @@
         <v>20</v>
       </c>
       <c r="F19" t="s">
+        <v>357</v>
+      </c>
+      <c r="G19" t="s">
         <v>358</v>
-      </c>
-      <c r="G19" t="s">
-        <v>359</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2743,7 +2752,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2763,10 +2772,10 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
+        <v>360</v>
+      </c>
+      <c r="G20" t="s">
         <v>361</v>
-      </c>
-      <c r="G20" t="s">
-        <v>362</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2820,10 +2829,10 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
+        <v>362</v>
+      </c>
+      <c r="G22" t="s">
         <v>363</v>
-      </c>
-      <c r="G22" t="s">
-        <v>364</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2838,10 +2847,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>389</v>
+      </c>
+      <c r="B23" t="s">
         <v>390</v>
-      </c>
-      <c r="B23" t="s">
-        <v>391</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -2853,10 +2862,10 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
+        <v>391</v>
+      </c>
+      <c r="G23" t="s">
         <v>392</v>
-      </c>
-      <c r="G23" t="s">
-        <v>393</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2919,10 +2928,10 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
+        <v>338</v>
+      </c>
+      <c r="G25" t="s">
         <v>339</v>
-      </c>
-      <c r="G25" t="s">
-        <v>340</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -2952,10 +2961,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
+        <v>380</v>
+      </c>
+      <c r="G26" t="s">
         <v>381</v>
-      </c>
-      <c r="G26" t="s">
-        <v>382</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2968,7 +2977,7 @@
         <v>0.4</v>
       </c>
       <c r="L26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2988,10 +2997,10 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
+        <v>373</v>
+      </c>
+      <c r="G27" t="s">
         <v>374</v>
-      </c>
-      <c r="G27" t="s">
-        <v>375</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3021,10 +3030,10 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
+        <v>375</v>
+      </c>
+      <c r="G28" t="s">
         <v>376</v>
-      </c>
-      <c r="G28" t="s">
-        <v>377</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3054,10 +3063,10 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
+        <v>377</v>
+      </c>
+      <c r="G29" t="s">
         <v>378</v>
-      </c>
-      <c r="G29" t="s">
-        <v>379</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -3070,7 +3079,7 @@
         <v>2.7</v>
       </c>
       <c r="L29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3090,10 +3099,10 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
+        <v>323</v>
+      </c>
+      <c r="G30" t="s">
         <v>324</v>
-      </c>
-      <c r="G30" t="s">
-        <v>325</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3108,25 +3117,25 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>414</v>
+      </c>
+      <c r="B31" t="s">
         <v>415</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>416</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>417</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" t="s">
         <v>418</v>
       </c>
-      <c r="E31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>419</v>
-      </c>
-      <c r="G31" t="s">
-        <v>420</v>
       </c>
       <c r="H31">
         <v>2</v>
@@ -3144,22 +3153,22 @@
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
+        <v>387</v>
+      </c>
+      <c r="G32" t="s">
         <v>388</v>
-      </c>
-      <c r="G32" t="s">
-        <v>389</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -3207,7 +3216,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
@@ -3219,10 +3228,10 @@
         <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F34" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -3237,7 +3246,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
@@ -3249,10 +3258,10 @@
         <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G35" t="s">
         <v>15</v>
@@ -3279,7 +3288,7 @@
         <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
@@ -3318,10 +3327,10 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
+        <v>336</v>
+      </c>
+      <c r="G37" t="s">
         <v>337</v>
-      </c>
-      <c r="G37" t="s">
-        <v>338</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -3367,12 +3376,12 @@
         <v>1.26</v>
       </c>
       <c r="L38" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -3438,7 +3447,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
@@ -3453,10 +3462,10 @@
         <v>20</v>
       </c>
       <c r="F41" t="s">
+        <v>403</v>
+      </c>
+      <c r="G41" t="s">
         <v>404</v>
-      </c>
-      <c r="G41" t="s">
-        <v>405</v>
       </c>
       <c r="H41">
         <v>3</v>
@@ -3471,22 +3480,22 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C42" t="s">
+        <v>399</v>
+      </c>
+      <c r="D42" t="s">
         <v>400</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
         <v>401</v>
       </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>402</v>
-      </c>
-      <c r="G42" t="s">
-        <v>403</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3501,22 +3510,22 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C43" t="s">
         <v>91</v>
       </c>
       <c r="D43" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
+        <v>410</v>
+      </c>
+      <c r="G43" t="s">
         <v>411</v>
-      </c>
-      <c r="G43" t="s">
-        <v>412</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3744,7 +3753,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B51" t="s">
         <v>146</v>
@@ -3777,7 +3786,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B52" t="s">
         <v>149</v>
@@ -3825,10 +3834,10 @@
         <v>20</v>
       </c>
       <c r="F53" t="s">
+        <v>325</v>
+      </c>
+      <c r="G53" t="s">
         <v>326</v>
-      </c>
-      <c r="G53" t="s">
-        <v>327</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3909,7 +3918,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B56" t="s">
         <v>164</v>
@@ -3981,7 +3990,7 @@
         <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D58" t="s">
         <v>118</v>
@@ -3990,10 +3999,10 @@
         <v>20</v>
       </c>
       <c r="F58" t="s">
+        <v>328</v>
+      </c>
+      <c r="G58" t="s">
         <v>329</v>
-      </c>
-      <c r="G58" t="s">
-        <v>330</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -4014,7 +4023,7 @@
         <v>174</v>
       </c>
       <c r="C59" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D59" t="s">
         <v>118</v>
@@ -4023,10 +4032,10 @@
         <v>20</v>
       </c>
       <c r="F59" t="s">
+        <v>334</v>
+      </c>
+      <c r="G59" t="s">
         <v>335</v>
-      </c>
-      <c r="G59" t="s">
-        <v>336</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4080,19 +4089,19 @@
         <v>200</v>
       </c>
       <c r="C61" t="s">
+        <v>207</v>
+      </c>
+      <c r="D61" t="s">
         <v>208</v>
       </c>
-      <c r="D61" t="s">
-        <v>209</v>
-      </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
+        <v>424</v>
+      </c>
+      <c r="G61" t="s">
         <v>425</v>
-      </c>
-      <c r="G61" t="s">
-        <v>426</v>
       </c>
       <c r="H61">
         <v>24</v>
@@ -4107,43 +4116,43 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>426</v>
       </c>
       <c r="B62">
         <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>181</v>
+        <v>428</v>
       </c>
       <c r="G62" t="s">
-        <v>182</v>
+        <v>429</v>
       </c>
       <c r="H62">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" t="s">
-        <v>184</v>
+        <v>427</v>
+      </c>
+      <c r="B63">
+        <v>100</v>
       </c>
       <c r="C63" t="s">
         <v>155</v>
@@ -4155,28 +4164,28 @@
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G63" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H63">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
         <v>155</v>
@@ -4188,28 +4197,28 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G64" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H64">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
         <v>155</v>
@@ -4221,28 +4230,28 @@
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G65" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B66" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C66" t="s">
         <v>155</v>
@@ -4254,28 +4263,28 @@
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G66" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B67" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C67" t="s">
         <v>155</v>
@@ -4287,28 +4296,28 @@
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G67" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B68" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s">
         <v>155</v>
@@ -4320,10 +4329,10 @@
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G68" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -4338,76 +4347,76 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>207</v>
-      </c>
-      <c r="B69">
-        <v>0.3</v>
+        <v>202</v>
+      </c>
+      <c r="B69" t="s">
+        <v>203</v>
       </c>
       <c r="C69" t="s">
-        <v>208</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>209</v>
+        <v>156</v>
       </c>
       <c r="E69" t="s">
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G69" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H69">
         <v>1</v>
       </c>
       <c r="I69">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>212</v>
-      </c>
-      <c r="B70" t="s">
-        <v>213</v>
+        <v>206</v>
+      </c>
+      <c r="B70">
+        <v>0.3</v>
       </c>
       <c r="C70" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="D70" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
       <c r="F70" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G70" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H70">
         <v>1</v>
       </c>
       <c r="I70">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J70">
-        <f t="shared" ref="J70:J96" si="1">H70*I70</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C71" t="s">
         <v>155</v>
@@ -4419,10 +4428,10 @@
         <v>20</v>
       </c>
       <c r="F71" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G71" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4431,16 +4440,16 @@
         <v>0.04</v>
       </c>
       <c r="J71">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J71:J97" si="1">H71*I71</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C72" t="s">
         <v>155</v>
@@ -4452,10 +4461,10 @@
         <v>20</v>
       </c>
       <c r="F72" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G72" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4470,10 +4479,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B73" t="s">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
         <v>155</v>
@@ -4484,23 +4493,29 @@
       <c r="E73" t="s">
         <v>20</v>
       </c>
+      <c r="F73" t="s">
+        <v>221</v>
+      </c>
       <c r="G73" t="s">
-        <v>15</v>
+        <v>222</v>
       </c>
       <c r="H73">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B74" t="s">
-        <v>226</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
         <v>155</v>
@@ -4511,65 +4526,59 @@
       <c r="E74" t="s">
         <v>20</v>
       </c>
-      <c r="F74" t="s">
-        <v>227</v>
-      </c>
       <c r="G74" t="s">
-        <v>228</v>
+        <v>15</v>
       </c>
       <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B75" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
-        <v>328</v>
+        <v>155</v>
       </c>
       <c r="D75" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
       </c>
       <c r="F75" t="s">
-        <v>331</v>
+        <v>226</v>
       </c>
       <c r="G75" t="s">
-        <v>332</v>
+        <v>227</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B76" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C76" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D76" t="s">
         <v>118</v>
@@ -4578,10 +4587,10 @@
         <v>20</v>
       </c>
       <c r="F76" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G76" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4596,43 +4605,43 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B77" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>327</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="E77" t="s">
         <v>20</v>
       </c>
       <c r="F77" t="s">
-        <v>235</v>
+        <v>332</v>
       </c>
       <c r="G77" t="s">
-        <v>236</v>
+        <v>333</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B78" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C78" t="s">
         <v>155</v>
@@ -4644,10 +4653,10 @@
         <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G78" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4662,579 +4671,612 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B79" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C79" t="s">
-        <v>242</v>
+        <v>155</v>
       </c>
       <c r="D79" t="s">
-        <v>243</v>
+        <v>156</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="G79" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C80" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D80" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G80" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D81" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G81" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D82" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E82" t="s">
         <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G82" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B83" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C83" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E83" t="s">
         <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G83" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B84" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C84" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D84" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G84" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B85" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C85" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D85" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G85" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B86" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C86" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D86" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E86" t="s">
         <v>20</v>
       </c>
       <c r="F86" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G86" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B87" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C87" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D87" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E87" t="s">
         <v>20</v>
       </c>
       <c r="F87" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="G87" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B88" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C88" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D88" t="s">
-        <v>290</v>
+        <v>284</v>
+      </c>
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" t="s">
+        <v>285</v>
       </c>
       <c r="G88" t="s">
-        <v>15</v>
+        <v>286</v>
       </c>
       <c r="H88">
         <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1.51</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K88" t="s">
-        <v>291</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B89" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C89" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D89" t="s">
-        <v>294</v>
-      </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G89" t="s">
-        <v>296</v>
+        <v>15</v>
       </c>
       <c r="H89">
         <v>1</v>
-      </c>
-      <c r="I89">
-        <v>0.47</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K89" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B90" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D90" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E90" t="s">
         <v>20</v>
       </c>
       <c r="F90" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="G90" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B91" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C91" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D91" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E91" t="s">
         <v>20</v>
       </c>
       <c r="F91" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G91" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B92" t="s">
-        <v>421</v>
+        <v>302</v>
       </c>
       <c r="C92" t="s">
-        <v>421</v>
+        <v>302</v>
       </c>
       <c r="D92" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E92" t="s">
         <v>20</v>
       </c>
       <c r="F92" t="s">
-        <v>422</v>
+        <v>304</v>
       </c>
       <c r="G92" t="s">
-        <v>423</v>
+        <v>305</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>8.48</v>
+        <v>1.57</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>395</v>
+        <v>306</v>
       </c>
       <c r="B93" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="C93" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="D93" t="s">
-        <v>398</v>
+        <v>307</v>
       </c>
       <c r="E93" t="s">
         <v>20</v>
       </c>
       <c r="F93" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="G93" t="s">
-        <v>399</v>
+        <v>422</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>6.84</v>
+        <v>8.48</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>309</v>
+        <v>394</v>
       </c>
       <c r="B94" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="C94" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="D94" t="s">
-        <v>311</v>
+        <v>397</v>
       </c>
       <c r="E94" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="F94" t="s">
-        <v>313</v>
+        <v>396</v>
       </c>
       <c r="G94" t="s">
-        <v>314</v>
+        <v>398</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="B95" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C95" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D95" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E95" t="s">
-        <v>20</v>
+        <v>311</v>
       </c>
       <c r="F95" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G95" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>314</v>
+      </c>
+      <c r="B96" t="s">
+        <v>315</v>
+      </c>
+      <c r="C96" t="s">
+        <v>315</v>
+      </c>
+      <c r="D96" t="s">
+        <v>316</v>
+      </c>
+      <c r="E96" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" t="s">
+        <v>317</v>
+      </c>
+      <c r="G96" t="s">
+        <v>318</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>2.96</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>319</v>
+      </c>
+      <c r="B97" t="s">
         <v>320</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C97" t="s">
         <v>321</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D97" t="s">
         <v>322</v>
       </c>
-      <c r="D96" t="s">
-        <v>323</v>
-      </c>
-      <c r="G96" t="s">
+      <c r="G97" t="s">
         <v>15</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="J96">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added C68 and C69 to BOM.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="434">
   <si>
     <t>Part</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">TOTAL: </t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -1304,6 +1301,21 @@
   </si>
   <si>
     <t>JP3, JP4, JP5, JP25</t>
+  </si>
+  <si>
+    <t>C1, C68</t>
+  </si>
+  <si>
+    <t>C69</t>
+  </si>
+  <si>
+    <t>8.2pF</t>
+  </si>
+  <si>
+    <t>445-5045-1-ND</t>
+  </si>
+  <si>
+    <t>C1608C0G1H8R2D</t>
   </si>
 </sst>
 </file>
@@ -2132,10 +2144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,67 +2196,67 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" t="s">
         <v>339</v>
       </c>
-      <c r="G2" t="s">
-        <v>340</v>
-      </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>0.27</v>
       </c>
       <c r="J2">
         <f>H2*I2</f>
-        <v>0.27</v>
+        <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J105)</f>
-        <v>174.27339999999998</v>
+        <f>SUM(J2:J106)</f>
+        <v>174.66339999999997</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G3" t="s">
         <v>341</v>
-      </c>
-      <c r="G3" t="s">
-        <v>342</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2253,31 +2265,31 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J70" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J71" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>342</v>
+      </c>
+      <c r="G4" t="s">
         <v>343</v>
-      </c>
-      <c r="G4" t="s">
-        <v>344</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2292,19 +2304,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -2316,25 +2328,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>347</v>
+      </c>
+      <c r="G6" t="s">
         <v>348</v>
-      </c>
-      <c r="G6" t="s">
-        <v>349</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2347,24 +2359,24 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2376,25 +2388,25 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>349</v>
+      </c>
+      <c r="G8" t="s">
         <v>350</v>
-      </c>
-      <c r="G8" t="s">
-        <v>351</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2409,25 +2421,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
       <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>351</v>
+      </c>
+      <c r="G9" t="s">
         <v>352</v>
-      </c>
-      <c r="G9" t="s">
-        <v>353</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2442,25 +2454,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>363</v>
+      </c>
+      <c r="G10" t="s">
         <v>364</v>
-      </c>
-      <c r="G10" t="s">
-        <v>365</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2473,30 +2485,30 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -2511,25 +2523,25 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>365</v>
+      </c>
+      <c r="G12" t="s">
         <v>366</v>
-      </c>
-      <c r="G12" t="s">
-        <v>367</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2544,25 +2556,25 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
       <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>363</v>
+      </c>
+      <c r="G13" t="s">
         <v>364</v>
-      </c>
-      <c r="G13" t="s">
-        <v>365</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2575,30 +2587,30 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>369</v>
+      </c>
+      <c r="G14" t="s">
         <v>370</v>
-      </c>
-      <c r="G14" t="s">
-        <v>371</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2611,24 +2623,24 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2640,25 +2652,25 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>353</v>
+      </c>
+      <c r="G16" t="s">
         <v>354</v>
-      </c>
-      <c r="G16" t="s">
-        <v>355</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2673,19 +2685,19 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
       <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2697,19 +2709,19 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -2721,25 +2733,25 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
         <v>57</v>
       </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
       <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>355</v>
+      </c>
+      <c r="G19" t="s">
         <v>356</v>
-      </c>
-      <c r="G19" t="s">
-        <v>357</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2752,30 +2764,30 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
       <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>358</v>
+      </c>
+      <c r="G20" t="s">
         <v>359</v>
-      </c>
-      <c r="G20" t="s">
-        <v>360</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2790,19 +2802,19 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
       <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2814,25 +2826,25 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
       <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>360</v>
+      </c>
+      <c r="G22" t="s">
         <v>361</v>
-      </c>
-      <c r="G22" t="s">
-        <v>362</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2847,25 +2859,25 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>387</v>
+      </c>
+      <c r="B23" t="s">
         <v>388</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
         <v>389</v>
       </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>390</v>
-      </c>
-      <c r="G23" t="s">
-        <v>391</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2880,368 +2892,371 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>430</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>431</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>432</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>433</v>
       </c>
       <c r="H24">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>0.315</v>
+        <v>0.12</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>8.19</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
         <v>67</v>
       </c>
-      <c r="E25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>337</v>
-      </c>
       <c r="G25" t="s">
-        <v>338</v>
+        <v>65</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="I25">
-        <v>0.35</v>
+        <v>0.315</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>379</v>
+        <v>336</v>
       </c>
       <c r="G26" t="s">
-        <v>380</v>
+        <v>337</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L26" t="s">
-        <v>385</v>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
         <v>73</v>
       </c>
-      <c r="D27" t="s">
-        <v>74</v>
-      </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="G27" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0.68</v>
+        <v>0.4</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
         <v>73</v>
       </c>
-      <c r="D28" t="s">
-        <v>74</v>
-      </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G28" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
         <v>73</v>
       </c>
-      <c r="D29" t="s">
-        <v>74</v>
-      </c>
       <c r="E29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>0.9</v>
+        <v>0.42</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="L29" t="s">
-        <v>378</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>322</v>
+        <v>375</v>
       </c>
       <c r="G30" t="s">
-        <v>323</v>
+        <v>376</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
       <c r="I30">
-        <v>11.91</v>
+        <v>0.9</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>2.7</v>
+      </c>
+      <c r="L30" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>413</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>414</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>415</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>416</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>417</v>
+        <v>321</v>
       </c>
       <c r="G31" t="s">
-        <v>418</v>
+        <v>322</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31">
-        <v>0.44</v>
+        <v>11.91</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>412</v>
       </c>
       <c r="B32" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="C32" t="s">
-        <v>387</v>
+        <v>414</v>
       </c>
       <c r="D32" t="s">
-        <v>387</v>
+        <v>415</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>386</v>
+        <v>416</v>
       </c>
       <c r="G32" t="s">
-        <v>387</v>
+        <v>417</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>2.15</v>
+        <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>386</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>386</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>386</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>385</v>
       </c>
       <c r="G33" t="s">
-        <v>86</v>
+        <v>386</v>
       </c>
       <c r="H33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>0.77</v>
+        <v>2.15</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E34" t="s">
-        <v>310</v>
+        <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>384</v>
+        <v>86</v>
+      </c>
+      <c r="G34" t="s">
+        <v>85</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -3249,23 +3264,20 @@
         <v>381</v>
       </c>
       <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
         <v>88</v>
       </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>89</v>
-      </c>
       <c r="E35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F35" t="s">
         <v>383</v>
       </c>
-      <c r="G35" t="s">
-        <v>15</v>
-      </c>
       <c r="H35">
         <v>2</v>
       </c>
@@ -3279,631 +3291,631 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>380</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>407</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>382</v>
       </c>
       <c r="G36" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="I36">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>429</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>406</v>
       </c>
       <c r="E37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F37" t="s">
-        <v>335</v>
+        <v>91</v>
       </c>
       <c r="G37" t="s">
-        <v>336</v>
+        <v>92</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I37">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>5.88</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>428</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>334</v>
       </c>
       <c r="G38" t="s">
-        <v>101</v>
+        <v>335</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I38">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L38" t="s">
-        <v>346</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>406</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
         <v>99</v>
       </c>
-      <c r="D39" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>100</v>
       </c>
-      <c r="G39" t="s">
-        <v>101</v>
-      </c>
       <c r="H39">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I39">
         <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>1.26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>405</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I40">
-        <v>3.65</v>
+        <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>405</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>402</v>
+        <v>103</v>
       </c>
       <c r="G41" t="s">
-        <v>403</v>
+        <v>104</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>0.13</v>
+        <v>3.65</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>404</v>
       </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
       <c r="C42" t="s">
-        <v>398</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>399</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G42" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>0.71</v>
+        <v>0.13</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>397</v>
       </c>
       <c r="D43" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="G43" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>108</v>
-      </c>
-      <c r="B44" t="s">
-        <v>109</v>
+        <v>407</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>406</v>
       </c>
       <c r="E44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>112</v>
+        <v>408</v>
       </c>
       <c r="G44" t="s">
-        <v>113</v>
+        <v>409</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G45" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G46" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G47" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D48" t="s">
-        <v>134</v>
+        <v>128</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>129</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1.85</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>138</v>
-      </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G49" t="s">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="H49">
-        <v>25</v>
-      </c>
-      <c r="I49">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>144</v>
+        <v>137</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>138</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="H50">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="I50">
+        <v>0.3</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>411</v>
+        <v>140</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
-      </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G51" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G52" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>411</v>
       </c>
       <c r="B53" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="E53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>324</v>
+        <v>149</v>
       </c>
       <c r="G53" t="s">
-        <v>325</v>
+        <v>150</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" t="s">
         <v>154</v>
       </c>
-      <c r="D54" t="s">
-        <v>155</v>
-      </c>
       <c r="E54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>158</v>
+        <v>323</v>
       </c>
       <c r="G54" t="s">
-        <v>159</v>
+        <v>324</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>160</v>
-      </c>
-      <c r="B55">
-        <v>470</v>
+        <v>155</v>
+      </c>
+      <c r="B55" t="s">
+        <v>156</v>
       </c>
       <c r="C55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" t="s">
         <v>154</v>
       </c>
-      <c r="D55" t="s">
-        <v>155</v>
-      </c>
       <c r="E55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G55" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3918,124 +3930,124 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>422</v>
-      </c>
-      <c r="B56" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+      <c r="B56">
+        <v>470</v>
       </c>
       <c r="C56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" t="s">
         <v>154</v>
       </c>
-      <c r="D56" t="s">
-        <v>155</v>
-      </c>
       <c r="E56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G56" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H56">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="I56">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.8004</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>421</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C57" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" t="s">
         <v>154</v>
       </c>
-      <c r="D57" t="s">
-        <v>155</v>
-      </c>
       <c r="E57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G57" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="I57">
-        <v>0.04</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.8004</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C58" t="s">
-        <v>326</v>
+        <v>153</v>
       </c>
       <c r="D58" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>327</v>
+        <v>167</v>
       </c>
       <c r="G58" t="s">
-        <v>328</v>
+        <v>168</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I58">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C59" t="s">
+        <v>325</v>
+      </c>
+      <c r="D59" t="s">
+        <v>116</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
         <v>326</v>
       </c>
-      <c r="D59" t="s">
-        <v>117</v>
-      </c>
-      <c r="E59" t="s">
-        <v>20</v>
-      </c>
-      <c r="F59" t="s">
-        <v>333</v>
-      </c>
       <c r="G59" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4050,322 +4062,322 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>154</v>
+        <v>325</v>
       </c>
       <c r="D60" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>176</v>
+        <v>332</v>
       </c>
       <c r="G60" t="s">
-        <v>177</v>
+        <v>333</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>178</v>
-      </c>
-      <c r="B61">
-        <v>200</v>
+        <v>173</v>
+      </c>
+      <c r="B61" t="s">
+        <v>174</v>
       </c>
       <c r="C61" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="D61" t="s">
-        <v>207</v>
+        <v>154</v>
       </c>
       <c r="E61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>423</v>
+        <v>175</v>
       </c>
       <c r="G61" t="s">
-        <v>424</v>
+        <v>176</v>
       </c>
       <c r="H61">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>425</v>
+        <v>177</v>
       </c>
       <c r="B62">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" t="s">
         <v>206</v>
       </c>
-      <c r="D62" t="s">
-        <v>207</v>
-      </c>
       <c r="E62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G62" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="H62">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I62">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B63">
         <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="E63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>179</v>
+        <v>426</v>
       </c>
       <c r="G63" t="s">
-        <v>180</v>
+        <v>427</v>
       </c>
       <c r="H63">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" t="s">
-        <v>182</v>
+        <v>425</v>
+      </c>
+      <c r="B64">
+        <v>100</v>
       </c>
       <c r="C64" t="s">
+        <v>153</v>
+      </c>
+      <c r="D64" t="s">
         <v>154</v>
       </c>
-      <c r="D64" t="s">
-        <v>155</v>
-      </c>
       <c r="E64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G64" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H64">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C65" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" t="s">
         <v>154</v>
       </c>
-      <c r="D65" t="s">
-        <v>155</v>
-      </c>
       <c r="E65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G65" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C66" t="s">
+        <v>153</v>
+      </c>
+      <c r="D66" t="s">
         <v>154</v>
       </c>
-      <c r="D66" t="s">
-        <v>155</v>
-      </c>
       <c r="E66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G66" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H66">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B67" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C67" t="s">
+        <v>153</v>
+      </c>
+      <c r="D67" t="s">
         <v>154</v>
       </c>
-      <c r="D67" t="s">
-        <v>155</v>
-      </c>
       <c r="E67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G67" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C68" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" t="s">
         <v>154</v>
       </c>
-      <c r="D68" t="s">
-        <v>155</v>
-      </c>
       <c r="E68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G68" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B69" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C69" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" t="s">
         <v>154</v>
       </c>
-      <c r="D69" t="s">
-        <v>155</v>
-      </c>
       <c r="E69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G69" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -4380,91 +4392,91 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>205</v>
-      </c>
-      <c r="B70">
-        <v>0.3</v>
+        <v>200</v>
+      </c>
+      <c r="B70" t="s">
+        <v>201</v>
       </c>
       <c r="C70" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="D70" t="s">
-        <v>207</v>
+        <v>154</v>
       </c>
       <c r="E70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G70" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="H70">
         <v>1</v>
       </c>
       <c r="I70">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>210</v>
-      </c>
-      <c r="B71" t="s">
-        <v>211</v>
+        <v>204</v>
+      </c>
+      <c r="B71">
+        <v>0.3</v>
       </c>
       <c r="C71" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="E71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G71" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H71">
         <v>1</v>
       </c>
       <c r="I71">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J71">
-        <f t="shared" ref="J71:J97" si="1">H71*I71</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B72" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s">
+        <v>153</v>
+      </c>
+      <c r="D72" t="s">
         <v>154</v>
       </c>
-      <c r="D72" t="s">
-        <v>155</v>
-      </c>
       <c r="E72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G72" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4473,31 +4485,31 @@
         <v>0.04</v>
       </c>
       <c r="J72">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J72:J98" si="1">H72*I72</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B73" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C73" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" t="s">
         <v>154</v>
       </c>
-      <c r="D73" t="s">
-        <v>155</v>
-      </c>
       <c r="E73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G73" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4512,118 +4524,118 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B74" t="s">
-        <v>15</v>
+        <v>218</v>
       </c>
       <c r="C74" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74" t="s">
         <v>154</v>
       </c>
-      <c r="D74" t="s">
-        <v>155</v>
-      </c>
       <c r="E74" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
+        <v>219</v>
       </c>
       <c r="G74" t="s">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="H74">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B75" t="s">
-        <v>224</v>
+        <v>14</v>
       </c>
       <c r="C75" t="s">
+        <v>153</v>
+      </c>
+      <c r="D75" t="s">
         <v>154</v>
       </c>
-      <c r="D75" t="s">
-        <v>155</v>
-      </c>
       <c r="E75" t="s">
-        <v>20</v>
-      </c>
-      <c r="F75" t="s">
-        <v>225</v>
+        <v>19</v>
       </c>
       <c r="G75" t="s">
-        <v>226</v>
+        <v>14</v>
       </c>
       <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B76" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>326</v>
+        <v>153</v>
       </c>
       <c r="D76" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="E76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F76" t="s">
-        <v>329</v>
+        <v>224</v>
       </c>
       <c r="G76" t="s">
-        <v>330</v>
+        <v>225</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B77" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C77" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G77" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4638,58 +4650,58 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C78" t="s">
-        <v>154</v>
+        <v>325</v>
       </c>
       <c r="D78" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>233</v>
+        <v>330</v>
       </c>
       <c r="G78" t="s">
-        <v>234</v>
+        <v>331</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B79" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C79" t="s">
+        <v>153</v>
+      </c>
+      <c r="D79" t="s">
         <v>154</v>
       </c>
-      <c r="D79" t="s">
-        <v>155</v>
-      </c>
       <c r="E79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G79" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4704,579 +4716,612 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B80" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C80" t="s">
-        <v>240</v>
+        <v>153</v>
       </c>
       <c r="D80" t="s">
-        <v>241</v>
+        <v>154</v>
       </c>
       <c r="E80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="G80" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B81" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C81" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D81" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G81" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C82" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D82" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G82" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B83" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C83" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D83" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="E83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G83" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B84" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C84" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D84" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="G84" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B85" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C85" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D85" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G85" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B86" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C86" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D86" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E86" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G86" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B87" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C87" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D87" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E87" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G87" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B88" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C88" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D88" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="E88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G88" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B89" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C89" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D89" t="s">
-        <v>288</v>
+        <v>282</v>
+      </c>
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
+        <v>283</v>
       </c>
       <c r="G89" t="s">
-        <v>15</v>
+        <v>284</v>
       </c>
       <c r="H89">
         <v>1</v>
+      </c>
+      <c r="I89">
+        <v>1.51</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K89" t="s">
-        <v>289</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B90" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C90" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D90" t="s">
-        <v>292</v>
-      </c>
-      <c r="E90" t="s">
-        <v>20</v>
-      </c>
-      <c r="F90" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="G90" t="s">
-        <v>294</v>
+        <v>14</v>
       </c>
       <c r="H90">
         <v>1</v>
-      </c>
-      <c r="I90">
-        <v>0.47</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K90" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B91" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C91" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D91" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F91" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="G91" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B92" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C92" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D92" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="G92" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B93" t="s">
-        <v>419</v>
+        <v>300</v>
       </c>
       <c r="C93" t="s">
-        <v>419</v>
+        <v>300</v>
       </c>
       <c r="D93" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>420</v>
+        <v>302</v>
       </c>
       <c r="G93" t="s">
-        <v>421</v>
+        <v>303</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>8.48</v>
+        <v>1.57</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>393</v>
+        <v>304</v>
       </c>
       <c r="B94" t="s">
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="C94" t="s">
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="D94" t="s">
-        <v>396</v>
+        <v>305</v>
       </c>
       <c r="E94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="G94" t="s">
-        <v>397</v>
+        <v>420</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>6.84</v>
+        <v>8.48</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>307</v>
+        <v>392</v>
       </c>
       <c r="B95" t="s">
-        <v>308</v>
+        <v>393</v>
       </c>
       <c r="C95" t="s">
-        <v>308</v>
+        <v>393</v>
       </c>
       <c r="D95" t="s">
-        <v>309</v>
+        <v>395</v>
       </c>
       <c r="E95" t="s">
-        <v>310</v>
+        <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>311</v>
+        <v>394</v>
       </c>
       <c r="G95" t="s">
-        <v>312</v>
+        <v>396</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="B96" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C96" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D96" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E96" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="F96" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G96" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="I96">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>312</v>
+      </c>
+      <c r="B97" t="s">
+        <v>313</v>
+      </c>
+      <c r="C97" t="s">
+        <v>313</v>
+      </c>
+      <c r="D97" t="s">
+        <v>314</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
+        <v>315</v>
+      </c>
+      <c r="G97" t="s">
+        <v>316</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>2.96</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>317</v>
+      </c>
+      <c r="B98" t="s">
         <v>318</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C98" t="s">
         <v>319</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D98" t="s">
         <v>320</v>
       </c>
-      <c r="D97" t="s">
-        <v>321</v>
-      </c>
-      <c r="G97" t="s">
-        <v>15</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="J97">
+      <c r="G98" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added XBee SMD headers to BOM.
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="439">
   <si>
     <t>Part</t>
   </si>
@@ -1316,6 +1316,21 @@
   </si>
   <si>
     <t>C1608C0G1H8R2D</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>XBEE-1B3</t>
+  </si>
+  <si>
+    <t>XBEE-SMD</t>
+  </si>
+  <si>
+    <t>PRT-10030</t>
+  </si>
+  <si>
+    <t>NPPN101BFLD-RC</t>
   </si>
 </sst>
 </file>
@@ -2144,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,8 +2247,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J106)</f>
-        <v>174.66339999999997</v>
+        <f>SUM(J2:J107)</f>
+        <v>176.56339999999997</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4485,7 +4500,7 @@
         <v>0.04</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72:J98" si="1">H72*I72</f>
+        <f t="shared" ref="J72:J99" si="1">H72*I72</f>
         <v>0.04</v>
       </c>
     </row>
@@ -5304,24 +5319,57 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>434</v>
+      </c>
+      <c r="B98" t="s">
+        <v>435</v>
+      </c>
+      <c r="C98" t="s">
+        <v>436</v>
+      </c>
+      <c r="D98" t="s">
+        <v>436</v>
+      </c>
+      <c r="E98" t="s">
+        <v>309</v>
+      </c>
+      <c r="F98" t="s">
+        <v>437</v>
+      </c>
+      <c r="G98" t="s">
+        <v>438</v>
+      </c>
+      <c r="H98">
+        <v>2</v>
+      </c>
+      <c r="I98">
+        <v>0.95</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>317</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>318</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>319</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>320</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G99" t="s">
         <v>14</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="J98">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated BOM with ICs changed in this branch.
Passives have not been kept track of, will generate a new BOM file for that later.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="436">
   <si>
     <t>Part</t>
   </si>
@@ -733,21 +733,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>XS1-L2-SPLIT</t>
-  </si>
-  <si>
-    <t>124QFN</t>
-  </si>
-  <si>
-    <t>880-1004-ND</t>
-  </si>
-  <si>
-    <t>XS1-L02A-QF124-C4</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>STM32L15XVX</t>
   </si>
   <si>
@@ -760,27 +745,6 @@
     <t>STM32L151V8T6</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>NC7SZU04</t>
-  </si>
-  <si>
-    <t>INVERTER"</t>
-  </si>
-  <si>
-    <t>SC70</t>
-  </si>
-  <si>
-    <t>NC7SZU04M5XCT-ND</t>
-  </si>
-  <si>
-    <t>NC7SZU04M5X</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
     <t>SST25VF010A</t>
   </si>
   <si>
@@ -859,18 +823,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>MCP23017SS</t>
-  </si>
-  <si>
-    <t>SSOP28</t>
-  </si>
-  <si>
-    <t>MCP23017-E/SS-ND</t>
-  </si>
-  <si>
-    <t>MCP23017-E/SS</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -973,12 +925,6 @@
     <t>20M</t>
   </si>
   <si>
-    <t>CRYSTALHC49US</t>
-  </si>
-  <si>
-    <t>HC49US</t>
-  </si>
-  <si>
     <t>497-4501-1-ND</t>
   </si>
   <si>
@@ -1331,6 +1277,51 @@
   </si>
   <si>
     <t>NPPN101BFLD-RC</t>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>XS1-L1-128TQFP</t>
+  </si>
+  <si>
+    <t>TQFP-128</t>
+  </si>
+  <si>
+    <t>880-1002-ND</t>
+  </si>
+  <si>
+    <t>XS1-L01A-TQ128-C4</t>
+  </si>
+  <si>
+    <t>U2, U3, U4</t>
+  </si>
+  <si>
+    <t>880-1035-ND</t>
+  </si>
+  <si>
+    <t>XS1-L01A-TQ48-C4</t>
+  </si>
+  <si>
+    <t>XS1-L1-TQFP48</t>
+  </si>
+  <si>
+    <t>XS1-L1-48TQFP</t>
+  </si>
+  <si>
+    <t>TQFP48</t>
+  </si>
+  <si>
+    <t>ASFL1</t>
+  </si>
+  <si>
+    <t>ASF</t>
+  </si>
+  <si>
+    <t>535-10816-1-ND</t>
+  </si>
+  <si>
+    <t>ASFL1-20.000MHZ-L-T</t>
   </si>
 </sst>
 </file>
@@ -2159,10 +2150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:K96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,12 +2202,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2231,10 +2222,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="G2" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2247,8 +2238,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J107)</f>
-        <v>176.56339999999997</v>
+        <f>SUM(J2:J106)</f>
+        <v>191.14339999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2268,10 +2259,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="G3" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2286,7 +2277,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2301,10 +2292,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="G4" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2358,10 +2349,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="G6" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2374,7 +2365,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2418,10 +2409,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="G8" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2451,10 +2442,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="G9" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2484,10 +2475,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="G10" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2500,7 +2491,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2553,10 +2544,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="G12" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2586,10 +2577,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="G13" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2602,7 +2593,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2622,10 +2613,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="G14" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2638,7 +2629,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2682,10 +2673,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="G16" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2763,10 +2754,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="G19" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2779,7 +2770,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2799,10 +2790,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="G20" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2856,10 +2847,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="G22" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2874,10 +2865,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B23" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2889,10 +2880,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="G23" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2907,10 +2898,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="B24" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2922,10 +2913,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="G24" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2988,10 +2979,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="G26" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3021,10 +3012,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="G27" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3037,7 +3028,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3057,10 +3048,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="G28" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3090,10 +3081,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="G29" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3123,10 +3114,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="G30" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3139,7 +3130,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3159,10 +3150,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="G31" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3177,25 +3168,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="B32" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="C32" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="D32" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="G32" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -3213,22 +3204,22 @@
         <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="C33" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="D33" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="G33" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3276,7 +3267,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="B35" t="s">
         <v>87</v>
@@ -3288,10 +3279,10 @@
         <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="F35" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -3306,7 +3297,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3318,10 +3309,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="F36" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
@@ -3348,7 +3339,7 @@
         <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -3372,7 +3363,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -3387,10 +3378,10 @@
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="G38" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="H38">
         <v>4</v>
@@ -3436,12 +3427,12 @@
         <v>1.26</v>
       </c>
       <c r="L39" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3507,7 +3498,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
@@ -3522,10 +3513,10 @@
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="G42" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="H42">
         <v>3</v>
@@ -3540,22 +3531,22 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="C43" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="D43" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="G43" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3570,22 +3561,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="G44" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3813,7 +3804,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="B52" t="s">
         <v>144</v>
@@ -3846,7 +3837,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="B53" t="s">
         <v>147</v>
@@ -3894,10 +3885,10 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="G54" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3978,7 +3969,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="B57" t="s">
         <v>162</v>
@@ -4050,7 +4041,7 @@
         <v>170</v>
       </c>
       <c r="C59" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="D59" t="s">
         <v>116</v>
@@ -4059,10 +4050,10 @@
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="G59" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4083,7 +4074,7 @@
         <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4092,10 +4083,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="G60" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4158,10 +4149,10 @@
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="G62" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="H62">
         <v>24</v>
@@ -4176,7 +4167,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="B63">
         <v>100</v>
@@ -4191,10 +4182,10 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="G63" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="H63">
         <v>4</v>
@@ -4209,7 +4200,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -4500,7 +4491,7 @@
         <v>0.04</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72:J99" si="1">H72*I72</f>
+        <f t="shared" ref="J72:J98" si="1">H72*I72</f>
         <v>0.04</v>
       </c>
     </row>
@@ -4638,7 +4629,7 @@
         <v>227</v>
       </c>
       <c r="C77" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="D77" t="s">
         <v>116</v>
@@ -4647,10 +4638,10 @@
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="G77" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4671,7 +4662,7 @@
         <v>229</v>
       </c>
       <c r="C78" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4680,10 +4671,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="G78" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4767,65 +4758,65 @@
         <v>238</v>
       </c>
       <c r="B81" t="s">
-        <v>239</v>
+        <v>422</v>
       </c>
       <c r="C81" t="s">
-        <v>239</v>
+        <v>422</v>
       </c>
       <c r="D81" t="s">
-        <v>240</v>
+        <v>423</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>241</v>
+        <v>424</v>
       </c>
       <c r="G81" t="s">
-        <v>242</v>
+        <v>425</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>15.1</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>243</v>
+        <v>426</v>
       </c>
       <c r="B82" t="s">
-        <v>244</v>
+        <v>429</v>
       </c>
       <c r="C82" t="s">
-        <v>244</v>
+        <v>430</v>
       </c>
       <c r="D82" t="s">
-        <v>245</v>
+        <v>431</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>246</v>
+        <v>427</v>
       </c>
       <c r="G82" t="s">
-        <v>247</v>
+        <v>428</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I82">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -4833,55 +4824,55 @@
         <v>248</v>
       </c>
       <c r="B83" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C83" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D83" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="G83" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>0.5</v>
+        <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>H83*I83</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C84" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D84" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="G84" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4890,488 +4881,464 @@
         <v>0.79</v>
       </c>
       <c r="J84">
-        <f t="shared" si="1"/>
+        <f>H84*I84</f>
         <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="D85" t="s">
-        <v>262</v>
-      </c>
-      <c r="E85" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="G85" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
-      <c r="I85">
-        <v>0.67</v>
-      </c>
       <c r="J85">
-        <f t="shared" si="1"/>
-        <v>0.67</v>
+        <f>H85*I85</f>
+        <v>0</v>
+      </c>
+      <c r="K85" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B86" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C86" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="D86" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="G86" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>6.63</v>
+        <v>0.47</v>
       </c>
       <c r="J86">
-        <f t="shared" si="1"/>
-        <v>6.63</v>
+        <f>H86*I86</f>
+        <v>0.47</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B87" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C87" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="D87" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="G87" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>1.67</v>
+        <v>0.67</v>
       </c>
       <c r="J87">
-        <f t="shared" si="1"/>
-        <v>1.67</v>
+        <f>H87*I87</f>
+        <v>0.67</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B88" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="C88" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="D88" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="G88" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>5.88</v>
+        <v>6.63</v>
       </c>
       <c r="J88">
-        <f t="shared" si="1"/>
-        <v>5.88</v>
+        <f>H88*I88</f>
+        <v>6.63</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B89" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="C89" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="D89" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="G89" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>1.51</v>
+        <v>1.67</v>
       </c>
       <c r="J89">
-        <f t="shared" si="1"/>
-        <v>1.51</v>
+        <f>H89*I89</f>
+        <v>1.67</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B90" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="C90" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>287</v>
+        <v>265</v>
+      </c>
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
+        <v>266</v>
       </c>
       <c r="G90" t="s">
-        <v>14</v>
+        <v>267</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
+      <c r="I90">
+        <v>5.88</v>
+      </c>
       <c r="J90">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K90" t="s">
-        <v>288</v>
+        <f>H90*I90</f>
+        <v>5.88</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B91" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C91" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D91" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
       </c>
       <c r="F91" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="G91" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>0.47</v>
+        <v>3.79</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B92" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C92" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D92" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="G92" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>374</v>
       </c>
       <c r="B93" t="s">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="C93" t="s">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D93" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>302</v>
+        <v>401</v>
       </c>
       <c r="G93" t="s">
-        <v>303</v>
+        <v>402</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>304</v>
+        <v>421</v>
       </c>
       <c r="B94" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
       <c r="C94" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
       <c r="D94" t="s">
-        <v>305</v>
+        <v>377</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="G94" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>392</v>
+        <v>290</v>
       </c>
       <c r="B95" t="s">
-        <v>393</v>
+        <v>291</v>
       </c>
       <c r="C95" t="s">
-        <v>393</v>
+        <v>291</v>
       </c>
       <c r="D95" t="s">
-        <v>395</v>
+        <v>292</v>
       </c>
       <c r="E95" t="s">
-        <v>19</v>
+        <v>293</v>
       </c>
       <c r="F95" t="s">
-        <v>394</v>
+        <v>294</v>
       </c>
       <c r="G95" t="s">
-        <v>396</v>
+        <v>295</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>6.84</v>
+        <v>1.5</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B96" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C96" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D96" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E96" t="s">
-        <v>309</v>
+        <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="G96" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="I96">
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>312</v>
+        <v>416</v>
       </c>
       <c r="B97" t="s">
-        <v>313</v>
+        <v>417</v>
       </c>
       <c r="C97" t="s">
-        <v>313</v>
+        <v>418</v>
       </c>
       <c r="D97" t="s">
-        <v>314</v>
+        <v>418</v>
       </c>
       <c r="E97" t="s">
-        <v>19</v>
+        <v>293</v>
       </c>
       <c r="F97" t="s">
-        <v>315</v>
+        <v>419</v>
       </c>
       <c r="G97" t="s">
-        <v>316</v>
+        <v>420</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I97">
-        <v>2.96</v>
+        <v>0.95</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>301</v>
+      </c>
+      <c r="B98" t="s">
+        <v>302</v>
+      </c>
+      <c r="C98" t="s">
+        <v>432</v>
+      </c>
+      <c r="D98" t="s">
+        <v>433</v>
+      </c>
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>434</v>
       </c>
-      <c r="B98" t="s">
+      <c r="G98" t="s">
         <v>435</v>
       </c>
-      <c r="C98" t="s">
-        <v>436</v>
-      </c>
-      <c r="D98" t="s">
-        <v>436</v>
-      </c>
-      <c r="E98" t="s">
-        <v>309</v>
-      </c>
-      <c r="F98" t="s">
-        <v>437</v>
-      </c>
-      <c r="G98" t="s">
-        <v>438</v>
-      </c>
       <c r="H98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I98">
-        <v>0.95</v>
+        <v>1.99</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>317</v>
-      </c>
-      <c r="B99" t="s">
-        <v>318</v>
-      </c>
-      <c r="C99" t="s">
-        <v>319</v>
-      </c>
-      <c r="D99" t="s">
-        <v>320</v>
-      </c>
-      <c r="G99" t="s">
-        <v>14</v>
-      </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="J99">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redesigned Gadgeteer logic translation circuitry.
The old pullup/FET setup has been removed in favor of logic translator ICs.
U3_P1A (assuming no changed to the U3 assignments) will be used to select I2C/non-I2C operation modes for the Gadgeteer socket.
Set U3_P1A high for I2C operation. This controls the select input of the IC6 and IC7 multiplexers, as well as the enable inputs of the translators (U17's enable input is inverted via IC8).

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="451">
   <si>
     <t>Part</t>
   </si>
@@ -418,9 +418,6 @@
     <t>CHIPLED_0603</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q18, Q19, Q20, Q21, Q22, Q23, Q24, Q26, Q27, Q28, Q29</t>
-  </si>
-  <si>
     <t>DMG1012UW</t>
   </si>
   <si>
@@ -1198,9 +1195,6 @@
     <t>Q16</t>
   </si>
   <si>
-    <t>IC4, IC5</t>
-  </si>
-  <si>
     <t>741G3157DCKR</t>
   </si>
   <si>
@@ -1225,9 +1219,6 @@
     <t>L3GD20TR</t>
   </si>
   <si>
-    <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96, R97, R98, R99, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
-  </si>
-  <si>
     <t>P200JCT-ND</t>
   </si>
   <si>
@@ -1282,6 +1273,9 @@
     <t>U16</t>
   </si>
   <si>
+    <t>U18</t>
+  </si>
+  <si>
     <t>XS1-L1-128TQFP</t>
   </si>
   <si>
@@ -1322,6 +1316,57 @@
   </si>
   <si>
     <t>ASFL1-20.000MHZ-L-T</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>PW_R-PDSO-G20</t>
+  </si>
+  <si>
+    <t>TXB0108</t>
+  </si>
+  <si>
+    <t>DCT-R-PDSO-G8</t>
+  </si>
+  <si>
+    <t>TXS0102</t>
+  </si>
+  <si>
+    <t>296-21527-1-ND</t>
+  </si>
+  <si>
+    <t>TXB0108PWR</t>
+  </si>
+  <si>
+    <t>296-21978-1-ND</t>
+  </si>
+  <si>
+    <t>TXS0102DCTR</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q24, Q26, Q27, Q28, Q29</t>
+  </si>
+  <si>
+    <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
+  </si>
+  <si>
+    <t>IC4, IC5, IC6, IC7</t>
+  </si>
+  <si>
+    <t>IC8</t>
+  </si>
+  <si>
+    <t>568-4822-1-ND</t>
+  </si>
+  <si>
+    <t>74AHC1G04GV,125</t>
+  </si>
+  <si>
+    <t>74AHC1G04DCK</t>
+  </si>
+  <si>
+    <t>SC70-5</t>
   </si>
 </sst>
 </file>
@@ -2150,10 +2195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:K96"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,12 +2247,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2222,10 +2267,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G2" t="s">
         <v>320</v>
-      </c>
-      <c r="G2" t="s">
-        <v>321</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2238,8 +2283,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J106)</f>
-        <v>191.14339999999999</v>
+        <f>SUM(J2:J109)</f>
+        <v>195.31300000000005</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2259,10 +2304,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" t="s">
         <v>322</v>
-      </c>
-      <c r="G3" t="s">
-        <v>323</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2271,13 +2316,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J71" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2292,10 +2337,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>323</v>
+      </c>
+      <c r="G4" t="s">
         <v>324</v>
-      </c>
-      <c r="G4" t="s">
-        <v>325</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2349,10 +2394,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>328</v>
+      </c>
+      <c r="G6" t="s">
         <v>329</v>
-      </c>
-      <c r="G6" t="s">
-        <v>330</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2365,7 +2410,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2409,10 +2454,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>330</v>
+      </c>
+      <c r="G8" t="s">
         <v>331</v>
-      </c>
-      <c r="G8" t="s">
-        <v>332</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2442,10 +2487,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>332</v>
+      </c>
+      <c r="G9" t="s">
         <v>333</v>
-      </c>
-      <c r="G9" t="s">
-        <v>334</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2475,10 +2520,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>344</v>
+      </c>
+      <c r="G10" t="s">
         <v>345</v>
-      </c>
-      <c r="G10" t="s">
-        <v>346</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2491,7 +2536,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2544,10 +2589,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>346</v>
+      </c>
+      <c r="G12" t="s">
         <v>347</v>
-      </c>
-      <c r="G12" t="s">
-        <v>348</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2577,10 +2622,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G13" t="s">
         <v>345</v>
-      </c>
-      <c r="G13" t="s">
-        <v>346</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2593,7 +2638,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2613,10 +2658,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>350</v>
+      </c>
+      <c r="G14" t="s">
         <v>351</v>
-      </c>
-      <c r="G14" t="s">
-        <v>352</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2629,7 +2674,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2673,10 +2718,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>334</v>
+      </c>
+      <c r="G16" t="s">
         <v>335</v>
-      </c>
-      <c r="G16" t="s">
-        <v>336</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2754,10 +2799,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>336</v>
+      </c>
+      <c r="G19" t="s">
         <v>337</v>
-      </c>
-      <c r="G19" t="s">
-        <v>338</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2770,7 +2815,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2790,10 +2835,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>339</v>
+      </c>
+      <c r="G20" t="s">
         <v>340</v>
-      </c>
-      <c r="G20" t="s">
-        <v>341</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2847,10 +2892,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>341</v>
+      </c>
+      <c r="G22" t="s">
         <v>342</v>
-      </c>
-      <c r="G22" t="s">
-        <v>343</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2865,10 +2910,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" t="s">
         <v>369</v>
-      </c>
-      <c r="B23" t="s">
-        <v>370</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2880,10 +2925,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>370</v>
+      </c>
+      <c r="G23" t="s">
         <v>371</v>
-      </c>
-      <c r="G23" t="s">
-        <v>372</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2898,10 +2943,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B24" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2913,10 +2958,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G24" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2979,10 +3024,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
+        <v>317</v>
+      </c>
+      <c r="G26" t="s">
         <v>318</v>
-      </c>
-      <c r="G26" t="s">
-        <v>319</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3012,10 +3057,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>359</v>
+      </c>
+      <c r="G27" t="s">
         <v>360</v>
-      </c>
-      <c r="G27" t="s">
-        <v>361</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3028,7 +3073,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3048,10 +3093,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
+        <v>352</v>
+      </c>
+      <c r="G28" t="s">
         <v>353</v>
-      </c>
-      <c r="G28" t="s">
-        <v>354</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3081,10 +3126,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>354</v>
+      </c>
+      <c r="G29" t="s">
         <v>355</v>
-      </c>
-      <c r="G29" t="s">
-        <v>356</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3114,10 +3159,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>356</v>
+      </c>
+      <c r="G30" t="s">
         <v>357</v>
-      </c>
-      <c r="G30" t="s">
-        <v>358</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3130,7 +3175,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3150,10 +3195,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>302</v>
+      </c>
+      <c r="G31" t="s">
         <v>303</v>
-      </c>
-      <c r="G31" t="s">
-        <v>304</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3168,131 +3213,134 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>445</v>
+      </c>
+      <c r="B32" t="s">
+        <v>393</v>
+      </c>
+      <c r="C32" t="s">
         <v>394</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>395</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>396</v>
       </c>
-      <c r="D32" t="s">
+      <c r="G32" t="s">
         <v>397</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
-        <v>398</v>
-      </c>
-      <c r="G32" t="s">
-        <v>399</v>
-      </c>
       <c r="H32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I32">
         <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>446</v>
       </c>
       <c r="B33" t="s">
-        <v>368</v>
+        <v>449</v>
       </c>
       <c r="C33" t="s">
-        <v>368</v>
+        <v>449</v>
       </c>
       <c r="D33" t="s">
-        <v>368</v>
+        <v>450</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>367</v>
+        <v>447</v>
       </c>
       <c r="G33" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
-        <v>2.15</v>
+        <v>0.38</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>367</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>367</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>367</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>86</v>
+        <v>366</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>367</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>0.77</v>
+        <v>2.15</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>363</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>293</v>
+        <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>365</v>
+        <v>86</v>
+      </c>
+      <c r="G35" t="s">
+        <v>85</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3309,14 +3357,11 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F36" t="s">
         <v>364</v>
       </c>
-      <c r="G36" t="s">
-        <v>14</v>
-      </c>
       <c r="H36">
         <v>2</v>
       </c>
@@ -3330,115 +3375,112 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>361</v>
       </c>
       <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" t="s">
+        <v>292</v>
+      </c>
+      <c r="F37" t="s">
+        <v>363</v>
+      </c>
+      <c r="G37" t="s">
         <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" t="s">
-        <v>388</v>
-      </c>
-      <c r="E37" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" t="s">
-        <v>92</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="I37">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>410</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>387</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>316</v>
+        <v>91</v>
       </c>
       <c r="G38" t="s">
-        <v>317</v>
+        <v>92</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I38">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>5.88</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>407</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>99</v>
+        <v>315</v>
       </c>
       <c r="G39" t="s">
-        <v>100</v>
+        <v>316</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I39">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L39" t="s">
-        <v>327</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>387</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
         <v>97</v>
@@ -3453,508 +3495,511 @@
         <v>100</v>
       </c>
       <c r="H40">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I40">
         <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>1.26</v>
+      </c>
+      <c r="L40" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>386</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G41" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I41">
-        <v>3.65</v>
+        <v>0.42</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>386</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>383</v>
+        <v>103</v>
       </c>
       <c r="G42" t="s">
-        <v>384</v>
+        <v>104</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0.13</v>
+        <v>3.65</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>385</v>
       </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
       <c r="C43" t="s">
-        <v>379</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
-        <v>380</v>
+        <v>106</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G43" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I43">
-        <v>0.71</v>
+        <v>0.13</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>378</v>
       </c>
       <c r="D44" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="G44" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>107</v>
-      </c>
-      <c r="B45" t="s">
-        <v>108</v>
+        <v>388</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>387</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>111</v>
+        <v>389</v>
       </c>
       <c r="G45" t="s">
-        <v>112</v>
+        <v>390</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G46" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G47" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G48" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>129</v>
       </c>
       <c r="G49" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="H49">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1.85</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
-      </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G50" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="H50">
-        <v>25</v>
-      </c>
-      <c r="I50">
-        <v>0.3</v>
+        <v>8</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>140</v>
+        <v>443</v>
       </c>
       <c r="B51" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>137</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="H51">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="I51">
+        <v>0.3</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.3999999999999995</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>392</v>
+        <v>139</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G52" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
         <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G53" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>151</v>
+        <v>392</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D54" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>305</v>
+        <v>148</v>
       </c>
       <c r="G54" t="s">
-        <v>306</v>
+        <v>149</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" t="s">
         <v>153</v>
       </c>
-      <c r="D55" t="s">
-        <v>154</v>
-      </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>157</v>
+        <v>304</v>
       </c>
       <c r="G55" t="s">
-        <v>158</v>
+        <v>305</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>159</v>
-      </c>
-      <c r="B56">
-        <v>470</v>
+        <v>154</v>
+      </c>
+      <c r="B56" t="s">
+        <v>155</v>
       </c>
       <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" t="s">
         <v>153</v>
       </c>
-      <c r="D56" t="s">
-        <v>154</v>
-      </c>
       <c r="E56" t="s">
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G56" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3969,112 +4014,112 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>403</v>
-      </c>
-      <c r="B57" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="B57">
+        <v>470</v>
       </c>
       <c r="C57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" t="s">
         <v>153</v>
       </c>
-      <c r="D57" t="s">
-        <v>154</v>
-      </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G57" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H57">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="I57">
-        <v>1.38E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.8004</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>444</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C58" t="s">
+        <v>152</v>
+      </c>
+      <c r="D58" t="s">
         <v>153</v>
       </c>
-      <c r="D58" t="s">
-        <v>154</v>
-      </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G58" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H58">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B59" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C59" t="s">
-        <v>307</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>308</v>
+        <v>166</v>
       </c>
       <c r="G59" t="s">
-        <v>309</v>
+        <v>167</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I59">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4083,10 +4128,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G60" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4101,322 +4146,322 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>306</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
       <c r="G61" t="s">
-        <v>176</v>
+        <v>314</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>177</v>
-      </c>
-      <c r="B62">
-        <v>200</v>
+        <v>172</v>
+      </c>
+      <c r="B62" t="s">
+        <v>173</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
       <c r="D62" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>404</v>
+        <v>174</v>
       </c>
       <c r="G62" t="s">
-        <v>405</v>
+        <v>175</v>
       </c>
       <c r="H62">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>406</v>
+        <v>176</v>
       </c>
       <c r="B63">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C63" t="s">
+        <v>204</v>
+      </c>
+      <c r="D63" t="s">
         <v>205</v>
       </c>
-      <c r="D63" t="s">
-        <v>206</v>
-      </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="G63" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="H63">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I63">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
       <c r="D64" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>178</v>
+        <v>405</v>
       </c>
       <c r="G64" t="s">
-        <v>179</v>
+        <v>406</v>
       </c>
       <c r="H64">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B65" t="s">
-        <v>181</v>
+        <v>404</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
       </c>
       <c r="C65" t="s">
+        <v>152</v>
+      </c>
+      <c r="D65" t="s">
         <v>153</v>
       </c>
-      <c r="D65" t="s">
-        <v>154</v>
-      </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G65" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H65">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" t="s">
         <v>153</v>
       </c>
-      <c r="D66" t="s">
-        <v>154</v>
-      </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G66" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H66">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C67" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" t="s">
         <v>153</v>
       </c>
-      <c r="D67" t="s">
-        <v>154</v>
-      </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G67" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H67">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B68" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C68" t="s">
+        <v>152</v>
+      </c>
+      <c r="D68" t="s">
         <v>153</v>
       </c>
-      <c r="D68" t="s">
-        <v>154</v>
-      </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G68" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B69" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" t="s">
         <v>153</v>
       </c>
-      <c r="D69" t="s">
-        <v>154</v>
-      </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G69" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C70" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" t="s">
         <v>153</v>
       </c>
-      <c r="D70" t="s">
-        <v>154</v>
-      </c>
       <c r="E70" t="s">
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G70" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4431,91 +4476,91 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>204</v>
-      </c>
-      <c r="B71">
-        <v>0.3</v>
+        <v>199</v>
+      </c>
+      <c r="B71" t="s">
+        <v>200</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
       <c r="D71" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G71" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H71">
         <v>1</v>
       </c>
       <c r="I71">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>209</v>
-      </c>
-      <c r="B72" t="s">
-        <v>210</v>
+        <v>203</v>
+      </c>
+      <c r="B72">
+        <v>0.3</v>
       </c>
       <c r="C72" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
       <c r="D72" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G72" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72:J98" si="1">H72*I72</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C73" t="s">
+        <v>152</v>
+      </c>
+      <c r="D73" t="s">
         <v>153</v>
       </c>
-      <c r="D73" t="s">
-        <v>154</v>
-      </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G73" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4524,31 +4569,31 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B74" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C74" t="s">
+        <v>152</v>
+      </c>
+      <c r="D74" t="s">
         <v>153</v>
       </c>
-      <c r="D74" t="s">
-        <v>154</v>
-      </c>
       <c r="E74" t="s">
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G74" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4563,106 +4608,106 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>217</v>
       </c>
       <c r="C75" t="s">
+        <v>152</v>
+      </c>
+      <c r="D75" t="s">
         <v>153</v>
       </c>
-      <c r="D75" t="s">
-        <v>154</v>
-      </c>
       <c r="E75" t="s">
         <v>19</v>
       </c>
+      <c r="F75" t="s">
+        <v>218</v>
+      </c>
       <c r="G75" t="s">
-        <v>14</v>
+        <v>219</v>
       </c>
       <c r="H75">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>0.04</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s">
+        <v>152</v>
+      </c>
+      <c r="D76" t="s">
         <v>153</v>
       </c>
-      <c r="D76" t="s">
-        <v>154</v>
-      </c>
       <c r="E76" t="s">
         <v>19</v>
       </c>
-      <c r="F76" t="s">
-        <v>224</v>
-      </c>
       <c r="G76" t="s">
-        <v>225</v>
+        <v>14</v>
       </c>
       <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B77" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C77" t="s">
-        <v>307</v>
+        <v>152</v>
       </c>
       <c r="D77" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>310</v>
+        <v>223</v>
       </c>
       <c r="G77" t="s">
-        <v>311</v>
+        <v>224</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B78" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4671,10 +4716,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G78" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4689,58 +4734,58 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B79" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
+        <v>306</v>
       </c>
       <c r="D79" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>232</v>
+        <v>311</v>
       </c>
       <c r="G79" t="s">
-        <v>233</v>
+        <v>312</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B80" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C80" t="s">
+        <v>152</v>
+      </c>
+      <c r="D80" t="s">
         <v>153</v>
       </c>
-      <c r="D80" t="s">
-        <v>154</v>
-      </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G80" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4755,588 +4800,687 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B81" t="s">
-        <v>422</v>
+        <v>234</v>
       </c>
       <c r="C81" t="s">
-        <v>422</v>
+        <v>152</v>
       </c>
       <c r="D81" t="s">
-        <v>423</v>
+        <v>153</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>424</v>
+        <v>235</v>
       </c>
       <c r="G81" t="s">
-        <v>425</v>
+        <v>236</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>8.6999999999999993</v>
+        <v>0.04</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>8.6999999999999993</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>426</v>
+        <v>237</v>
       </c>
       <c r="B82" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C82" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="D82" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G82" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="H82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I82">
-        <v>7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>248</v>
+        <v>424</v>
       </c>
       <c r="B83" t="s">
-        <v>239</v>
+        <v>427</v>
       </c>
       <c r="C83" t="s">
-        <v>239</v>
+        <v>428</v>
       </c>
       <c r="D83" t="s">
-        <v>240</v>
+        <v>429</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>241</v>
+        <v>425</v>
       </c>
       <c r="G83" t="s">
-        <v>242</v>
+        <v>426</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I83">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="J83">
-        <f>H83*I83</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B84" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C84" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D84" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G84" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.79</v>
+        <v>6.6</v>
       </c>
       <c r="J84">
         <f>H84*I84</f>
-        <v>0.79</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B85" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="C85" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="D85" t="s">
-        <v>271</v>
+        <v>244</v>
+      </c>
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
+        <v>245</v>
       </c>
       <c r="G85" t="s">
-        <v>14</v>
+        <v>246</v>
       </c>
       <c r="H85">
         <v>1</v>
+      </c>
+      <c r="I85">
+        <v>0.79</v>
       </c>
       <c r="J85">
         <f>H85*I85</f>
-        <v>0</v>
-      </c>
-      <c r="K85" t="s">
-        <v>272</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B86" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C86" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D86" t="s">
-        <v>275</v>
-      </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G86" t="s">
-        <v>277</v>
+        <v>14</v>
       </c>
       <c r="H86">
         <v>1</v>
-      </c>
-      <c r="I86">
-        <v>0.47</v>
       </c>
       <c r="J86">
         <f>H86*I86</f>
-        <v>0.47</v>
+        <v>0</v>
+      </c>
+      <c r="K86" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B87" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="C87" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="D87" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="G87" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>0.67</v>
+        <v>0.47</v>
       </c>
       <c r="J87">
         <f>H87*I87</f>
-        <v>0.67</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B88" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C88" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D88" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G88" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
       <c r="J88">
         <f>H88*I88</f>
-        <v>6.63</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B89" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C89" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D89" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G89" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
       <c r="J89">
         <f>H89*I89</f>
-        <v>1.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B90" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C90" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D90" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G90" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
       <c r="J90">
         <f>H90*I90</f>
-        <v>5.88</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B91" t="s">
+        <v>263</v>
+      </c>
+      <c r="C91" t="s">
+        <v>263</v>
+      </c>
+      <c r="D91" t="s">
+        <v>264</v>
+      </c>
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
+        <v>265</v>
+      </c>
+      <c r="G91" t="s">
+        <v>266</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>5.88</v>
+      </c>
+      <c r="J91">
+        <f>H91*I91</f>
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>282</v>
+      </c>
+      <c r="B92" t="s">
+        <v>278</v>
+      </c>
+      <c r="C92" t="s">
+        <v>278</v>
+      </c>
+      <c r="D92" t="s">
         <v>279</v>
       </c>
-      <c r="C91" t="s">
-        <v>279</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>280</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="G92" t="s">
         <v>281</v>
       </c>
-      <c r="G91" t="s">
-        <v>282</v>
-      </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>3.79</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>288</v>
-      </c>
-      <c r="B92" t="s">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>287</v>
+      </c>
+      <c r="B93" t="s">
+        <v>283</v>
+      </c>
+      <c r="C93" t="s">
+        <v>283</v>
+      </c>
+      <c r="D93" t="s">
         <v>284</v>
       </c>
-      <c r="C92" t="s">
-        <v>284</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>285</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G93" t="s">
         <v>286</v>
       </c>
-      <c r="G92" t="s">
-        <v>287</v>
-      </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>1.57</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>374</v>
-      </c>
-      <c r="B93" t="s">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>373</v>
+      </c>
+      <c r="B94" t="s">
+        <v>398</v>
+      </c>
+      <c r="C94" t="s">
+        <v>398</v>
+      </c>
+      <c r="D94" t="s">
+        <v>288</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
+        <v>399</v>
+      </c>
+      <c r="G94" t="s">
         <v>400</v>
       </c>
-      <c r="C93" t="s">
-        <v>400</v>
-      </c>
-      <c r="D93" t="s">
-        <v>289</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
-        <v>401</v>
-      </c>
-      <c r="G93" t="s">
-        <v>402</v>
-      </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>8.48</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>421</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>418</v>
+      </c>
+      <c r="B95" t="s">
+        <v>374</v>
+      </c>
+      <c r="C95" t="s">
+        <v>374</v>
+      </c>
+      <c r="D95" t="s">
+        <v>376</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>375</v>
       </c>
-      <c r="C94" t="s">
-        <v>375</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="G95" t="s">
         <v>377</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>376</v>
-      </c>
-      <c r="G94" t="s">
-        <v>378</v>
-      </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>6.84</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>434</v>
+      </c>
+      <c r="B96" t="s">
+        <v>436</v>
+      </c>
+      <c r="C96" t="s">
+        <v>436</v>
+      </c>
+      <c r="D96" t="s">
+        <v>435</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
+        <v>439</v>
+      </c>
+      <c r="G96" t="s">
+        <v>440</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>2.8</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>419</v>
+      </c>
+      <c r="B97" t="s">
+        <v>438</v>
+      </c>
+      <c r="C97" t="s">
+        <v>438</v>
+      </c>
+      <c r="D97" t="s">
+        <v>437</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
+        <v>441</v>
+      </c>
+      <c r="G97" t="s">
+        <v>442</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>1.25</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>289</v>
+      </c>
+      <c r="B98" t="s">
         <v>290</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C98" t="s">
+        <v>290</v>
+      </c>
+      <c r="D98" t="s">
         <v>291</v>
       </c>
-      <c r="C95" t="s">
-        <v>291</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E98" t="s">
         <v>292</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F98" t="s">
         <v>293</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G98" t="s">
         <v>294</v>
       </c>
-      <c r="G95" t="s">
-        <v>295</v>
-      </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>1.5</v>
       </c>
-      <c r="J95">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>295</v>
+      </c>
+      <c r="B99" t="s">
         <v>296</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C99" t="s">
+        <v>296</v>
+      </c>
+      <c r="D99" t="s">
         <v>297</v>
       </c>
-      <c r="C96" t="s">
-        <v>297</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>298</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="G99" t="s">
         <v>299</v>
       </c>
-      <c r="G96" t="s">
-        <v>300</v>
-      </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>2.96</v>
       </c>
-      <c r="J96">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>413</v>
+      </c>
+      <c r="B100" t="s">
+        <v>414</v>
+      </c>
+      <c r="C100" t="s">
+        <v>415</v>
+      </c>
+      <c r="D100" t="s">
+        <v>415</v>
+      </c>
+      <c r="E100" t="s">
+        <v>292</v>
+      </c>
+      <c r="F100" t="s">
         <v>416</v>
       </c>
-      <c r="B97" t="s">
+      <c r="G100" t="s">
         <v>417</v>
       </c>
-      <c r="C97" t="s">
-        <v>418</v>
-      </c>
-      <c r="D97" t="s">
-        <v>418</v>
-      </c>
-      <c r="E97" t="s">
-        <v>293</v>
-      </c>
-      <c r="F97" t="s">
-        <v>419</v>
-      </c>
-      <c r="G97" t="s">
-        <v>420</v>
-      </c>
-      <c r="H97">
+      <c r="H100">
         <v>2</v>
       </c>
-      <c r="I97">
+      <c r="I100">
         <v>0.95</v>
       </c>
-      <c r="J97">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>300</v>
+      </c>
+      <c r="B101" t="s">
         <v>301</v>
       </c>
-      <c r="B98" t="s">
-        <v>302</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="C101" t="s">
+        <v>430</v>
+      </c>
+      <c r="D101" t="s">
+        <v>431</v>
+      </c>
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>432</v>
       </c>
-      <c r="D98" t="s">
+      <c r="G101" t="s">
         <v>433</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
-        <v>434</v>
-      </c>
-      <c r="G98" t="s">
-        <v>435</v>
-      </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
         <v>1.99</v>
       </c>
-      <c r="J98">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Gadgeteer signals rearranged to align nicely with the new logic translators.
U17 package changed to QFN-20 variant.
U18 package changed to XBGA-8 variant.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1321,30 +1321,12 @@
     <t>U17</t>
   </si>
   <si>
-    <t>PW_R-PDSO-G20</t>
-  </si>
-  <si>
     <t>TXB0108</t>
   </si>
   <si>
-    <t>DCT-R-PDSO-G8</t>
-  </si>
-  <si>
     <t>TXS0102</t>
   </si>
   <si>
-    <t>296-21527-1-ND</t>
-  </si>
-  <si>
-    <t>TXB0108PWR</t>
-  </si>
-  <si>
-    <t>296-21978-1-ND</t>
-  </si>
-  <si>
-    <t>TXS0102DCTR</t>
-  </si>
-  <si>
     <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q24, Q26, Q27, Q28, Q29</t>
   </si>
   <si>
@@ -1367,6 +1349,24 @@
   </si>
   <si>
     <t>SC70-5</t>
+  </si>
+  <si>
+    <t>QFN20_3,5X4,5</t>
+  </si>
+  <si>
+    <t>296-21528-1-ND</t>
+  </si>
+  <si>
+    <t>TXB0108RGYR</t>
+  </si>
+  <si>
+    <t>YZP-R-XBGA-N8</t>
+  </si>
+  <si>
+    <t>296-21932-1-ND</t>
+  </si>
+  <si>
+    <t>TXS0102YZPR</t>
   </si>
 </sst>
 </file>
@@ -2197,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J109)</f>
-        <v>195.31300000000005</v>
+        <v>195.39300000000006</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3213,7 +3213,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B32" t="s">
         <v>393</v>
@@ -3246,25 +3246,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="B33" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C33" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D33" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="G33" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -5292,22 +5292,22 @@
         <v>434</v>
       </c>
       <c r="B96" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C96" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D96" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="G96" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -5325,32 +5325,32 @@
         <v>419</v>
       </c>
       <c r="B97" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C97" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D97" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="G97" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>1.25</v>
+        <v>1.33</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added two more TXB0108 level shifters for the motor drivers.
The 3.3V side of the translators has been defined to line up with
available pins on U1. PWM signals go to the 1-bit ports, while the
rest use 4-bit ports and the upper half of P8D.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -2197,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J109)</f>
-        <v>195.39300000000006</v>
+        <v>200.99300000000005</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>6.6</v>
       </c>
       <c r="J84">
-        <f>H84*I84</f>
+        <f t="shared" ref="J84:J91" si="2">H84*I84</f>
         <v>6.6</v>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
         <v>0.79</v>
       </c>
       <c r="J85">
-        <f>H85*I85</f>
+        <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
         <v>1</v>
       </c>
       <c r="J86">
-        <f>H86*I86</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K86" t="s">
@@ -5019,7 +5019,7 @@
         <v>0.47</v>
       </c>
       <c r="J87">
-        <f>H87*I87</f>
+        <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
@@ -5052,7 +5052,7 @@
         <v>0.67</v>
       </c>
       <c r="J88">
-        <f>H88*I88</f>
+        <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
         <v>6.63</v>
       </c>
       <c r="J89">
-        <f>H89*I89</f>
+        <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
@@ -5118,7 +5118,7 @@
         <v>1.67</v>
       </c>
       <c r="J90">
-        <f>H90*I90</f>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
@@ -5151,7 +5151,7 @@
         <v>5.88</v>
       </c>
       <c r="J91">
-        <f>H91*I91</f>
+        <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
@@ -5310,14 +5310,14 @@
         <v>447</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I96">
         <v>2.8</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>8.3999999999999986</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added U21, a 1:4 clock fanout buffer.
The old CLK net is connected to the input of U21.
The outputs of U21 (Q1 to Q4) each connect to the CLK inputs of U1-U4.
This will ensure that all four XMOS chips receive an accurate, synchronized clock.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="456">
   <si>
     <t>Part</t>
   </si>
@@ -1367,6 +1367,21 @@
   </si>
   <si>
     <t>TXS0102YZPR</t>
+  </si>
+  <si>
+    <t>U21</t>
+  </si>
+  <si>
+    <t>NB3N551</t>
+  </si>
+  <si>
+    <t>SOIC8</t>
+  </si>
+  <si>
+    <t>NB3N551DGOS-ND</t>
+  </si>
+  <si>
+    <t>NB3N551DG</t>
   </si>
 </sst>
 </file>
@@ -2195,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95"/>
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,8 +2298,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J109)</f>
-        <v>200.99300000000005</v>
+        <f>SUM(J2:J110)</f>
+        <v>202.85300000000007</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4569,7 +4584,7 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
+        <f t="shared" ref="J73:J102" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
@@ -5355,132 +5370,165 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>289</v>
+        <v>451</v>
       </c>
       <c r="B98" t="s">
-        <v>290</v>
+        <v>452</v>
       </c>
       <c r="C98" t="s">
-        <v>290</v>
+        <v>452</v>
       </c>
       <c r="D98" t="s">
-        <v>291</v>
+        <v>453</v>
       </c>
       <c r="E98" t="s">
-        <v>292</v>
+        <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>293</v>
+        <v>454</v>
       </c>
       <c r="G98" t="s">
-        <v>294</v>
+        <v>455</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>1.5</v>
+        <v>1.86</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B99" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C99" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D99" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E99" t="s">
-        <v>19</v>
+        <v>292</v>
       </c>
       <c r="F99" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G99" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>413</v>
+        <v>295</v>
       </c>
       <c r="B100" t="s">
-        <v>414</v>
+        <v>296</v>
       </c>
       <c r="C100" t="s">
-        <v>415</v>
+        <v>296</v>
       </c>
       <c r="D100" t="s">
-        <v>415</v>
+        <v>297</v>
       </c>
       <c r="E100" t="s">
-        <v>292</v>
+        <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>416</v>
+        <v>298</v>
       </c>
       <c r="G100" t="s">
-        <v>417</v>
+        <v>299</v>
       </c>
       <c r="H100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I100">
-        <v>0.95</v>
+        <v>2.96</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>1.9</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>413</v>
+      </c>
+      <c r="B101" t="s">
+        <v>414</v>
+      </c>
+      <c r="C101" t="s">
+        <v>415</v>
+      </c>
+      <c r="D101" t="s">
+        <v>415</v>
+      </c>
+      <c r="E101" t="s">
+        <v>292</v>
+      </c>
+      <c r="F101" t="s">
+        <v>416</v>
+      </c>
+      <c r="G101" t="s">
+        <v>417</v>
+      </c>
+      <c r="H101">
+        <v>2</v>
+      </c>
+      <c r="I101">
+        <v>0.95</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>300</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>301</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>430</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>431</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>432</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" t="s">
         <v>433</v>
       </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>1.99</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Updated XMOS chips in BOM.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="450">
   <si>
     <t>Part</t>
   </si>
@@ -727,9 +727,6 @@
     <t>ERJ-3EKF3902V</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>STM32L15XVX</t>
   </si>
   <si>
@@ -1276,36 +1273,6 @@
     <t>U18</t>
   </si>
   <si>
-    <t>XS1-L1-128TQFP</t>
-  </si>
-  <si>
-    <t>TQFP-128</t>
-  </si>
-  <si>
-    <t>880-1002-ND</t>
-  </si>
-  <si>
-    <t>XS1-L01A-TQ128-C4</t>
-  </si>
-  <si>
-    <t>U2, U3, U4</t>
-  </si>
-  <si>
-    <t>880-1035-ND</t>
-  </si>
-  <si>
-    <t>XS1-L01A-TQ48-C4</t>
-  </si>
-  <si>
-    <t>XS1-L1-TQFP48</t>
-  </si>
-  <si>
-    <t>XS1-L1-48TQFP</t>
-  </si>
-  <si>
-    <t>TQFP48</t>
-  </si>
-  <si>
     <t>ASFL1</t>
   </si>
   <si>
@@ -1382,6 +1349,21 @@
   </si>
   <si>
     <t>NB3N551DG</t>
+  </si>
+  <si>
+    <t>XS2-L2-124QFN</t>
+  </si>
+  <si>
+    <t>TQFN-124</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>880-1004-ND</t>
+  </si>
+  <si>
+    <t>XS1-L02A-QF124-C4</t>
   </si>
 </sst>
 </file>
@@ -2210,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,12 +2244,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2282,10 +2264,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" t="s">
         <v>319</v>
-      </c>
-      <c r="G2" t="s">
-        <v>320</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2298,8 +2280,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J110)</f>
-        <v>202.85300000000007</v>
+        <f>SUM(J2:J109)</f>
+        <v>188.25300000000004</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2319,10 +2301,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G3" t="s">
         <v>321</v>
-      </c>
-      <c r="G3" t="s">
-        <v>322</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2337,7 +2319,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2352,10 +2334,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>322</v>
+      </c>
+      <c r="G4" t="s">
         <v>323</v>
-      </c>
-      <c r="G4" t="s">
-        <v>324</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2409,10 +2391,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>327</v>
+      </c>
+      <c r="G6" t="s">
         <v>328</v>
-      </c>
-      <c r="G6" t="s">
-        <v>329</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2425,7 +2407,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2469,10 +2451,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>329</v>
+      </c>
+      <c r="G8" t="s">
         <v>330</v>
-      </c>
-      <c r="G8" t="s">
-        <v>331</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2502,10 +2484,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>331</v>
+      </c>
+      <c r="G9" t="s">
         <v>332</v>
-      </c>
-      <c r="G9" t="s">
-        <v>333</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2535,10 +2517,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>343</v>
+      </c>
+      <c r="G10" t="s">
         <v>344</v>
-      </c>
-      <c r="G10" t="s">
-        <v>345</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2551,7 +2533,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2604,10 +2586,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G12" t="s">
         <v>346</v>
-      </c>
-      <c r="G12" t="s">
-        <v>347</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2637,10 +2619,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>343</v>
+      </c>
+      <c r="G13" t="s">
         <v>344</v>
-      </c>
-      <c r="G13" t="s">
-        <v>345</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2653,7 +2635,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2673,10 +2655,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>349</v>
+      </c>
+      <c r="G14" t="s">
         <v>350</v>
-      </c>
-      <c r="G14" t="s">
-        <v>351</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2689,7 +2671,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2733,10 +2715,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>333</v>
+      </c>
+      <c r="G16" t="s">
         <v>334</v>
-      </c>
-      <c r="G16" t="s">
-        <v>335</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2814,10 +2796,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>335</v>
+      </c>
+      <c r="G19" t="s">
         <v>336</v>
-      </c>
-      <c r="G19" t="s">
-        <v>337</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2830,7 +2812,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2850,10 +2832,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>338</v>
+      </c>
+      <c r="G20" t="s">
         <v>339</v>
-      </c>
-      <c r="G20" t="s">
-        <v>340</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2907,10 +2889,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>340</v>
+      </c>
+      <c r="G22" t="s">
         <v>341</v>
-      </c>
-      <c r="G22" t="s">
-        <v>342</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2925,10 +2907,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>367</v>
+      </c>
+      <c r="B23" t="s">
         <v>368</v>
-      </c>
-      <c r="B23" t="s">
-        <v>369</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2940,10 +2922,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>369</v>
+      </c>
+      <c r="G23" t="s">
         <v>370</v>
-      </c>
-      <c r="G23" t="s">
-        <v>371</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2958,10 +2940,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>408</v>
+      </c>
+      <c r="B24" t="s">
         <v>409</v>
-      </c>
-      <c r="B24" t="s">
-        <v>410</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2973,10 +2955,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>410</v>
+      </c>
+      <c r="G24" t="s">
         <v>411</v>
-      </c>
-      <c r="G24" t="s">
-        <v>412</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3039,10 +3021,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
+        <v>316</v>
+      </c>
+      <c r="G26" t="s">
         <v>317</v>
-      </c>
-      <c r="G26" t="s">
-        <v>318</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3072,10 +3054,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>358</v>
+      </c>
+      <c r="G27" t="s">
         <v>359</v>
-      </c>
-      <c r="G27" t="s">
-        <v>360</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3088,7 +3070,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3108,10 +3090,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
+        <v>351</v>
+      </c>
+      <c r="G28" t="s">
         <v>352</v>
-      </c>
-      <c r="G28" t="s">
-        <v>353</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3141,10 +3123,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>353</v>
+      </c>
+      <c r="G29" t="s">
         <v>354</v>
-      </c>
-      <c r="G29" t="s">
-        <v>355</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3174,10 +3156,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>355</v>
+      </c>
+      <c r="G30" t="s">
         <v>356</v>
-      </c>
-      <c r="G30" t="s">
-        <v>357</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3190,7 +3172,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3210,10 +3192,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>301</v>
+      </c>
+      <c r="G31" t="s">
         <v>302</v>
-      </c>
-      <c r="G31" t="s">
-        <v>303</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3228,25 +3210,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="B32" t="s">
+        <v>392</v>
+      </c>
+      <c r="C32" t="s">
         <v>393</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>394</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>395</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>396</v>
-      </c>
-      <c r="G32" t="s">
-        <v>397</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -3261,25 +3243,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="B33" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="C33" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="D33" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="G33" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3297,22 +3279,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
+        <v>365</v>
+      </c>
+      <c r="G34" t="s">
         <v>366</v>
-      </c>
-      <c r="G34" t="s">
-        <v>367</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3360,7 +3342,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3372,10 +3354,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3390,7 +3372,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3402,10 +3384,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3432,7 +3414,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3456,7 +3438,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3471,10 +3453,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
+        <v>314</v>
+      </c>
+      <c r="G39" t="s">
         <v>315</v>
-      </c>
-      <c r="G39" t="s">
-        <v>316</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -3520,12 +3502,12 @@
         <v>1.26</v>
       </c>
       <c r="L40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3591,7 +3573,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3606,10 +3588,10 @@
         <v>19</v>
       </c>
       <c r="F43" t="s">
+        <v>381</v>
+      </c>
+      <c r="G43" t="s">
         <v>382</v>
-      </c>
-      <c r="G43" t="s">
-        <v>383</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3624,22 +3606,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C44" t="s">
+        <v>377</v>
+      </c>
+      <c r="D44" t="s">
         <v>378</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>379</v>
       </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>380</v>
-      </c>
-      <c r="G44" t="s">
-        <v>381</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3654,22 +3636,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
+        <v>388</v>
+      </c>
+      <c r="G45" t="s">
         <v>389</v>
-      </c>
-      <c r="G45" t="s">
-        <v>390</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3840,7 +3822,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -3897,7 +3879,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
@@ -3930,7 +3912,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B54" t="s">
         <v>146</v>
@@ -3978,10 +3960,10 @@
         <v>19</v>
       </c>
       <c r="F55" t="s">
+        <v>303</v>
+      </c>
+      <c r="G55" t="s">
         <v>304</v>
-      </c>
-      <c r="G55" t="s">
-        <v>305</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4062,7 +4044,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -4134,7 +4116,7 @@
         <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4143,10 +4125,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
+        <v>306</v>
+      </c>
+      <c r="G60" t="s">
         <v>307</v>
-      </c>
-      <c r="G60" t="s">
-        <v>308</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4167,7 +4149,7 @@
         <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D61" t="s">
         <v>116</v>
@@ -4176,10 +4158,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
+        <v>312</v>
+      </c>
+      <c r="G61" t="s">
         <v>313</v>
-      </c>
-      <c r="G61" t="s">
-        <v>314</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4242,10 +4224,10 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
+        <v>400</v>
+      </c>
+      <c r="G63" t="s">
         <v>401</v>
-      </c>
-      <c r="G63" t="s">
-        <v>402</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4260,7 +4242,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -4275,10 +4257,10 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
+        <v>404</v>
+      </c>
+      <c r="G64" t="s">
         <v>405</v>
-      </c>
-      <c r="G64" t="s">
-        <v>406</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4293,7 +4275,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -4584,7 +4566,7 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J102" si="1">H73*I73</f>
+        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
@@ -4722,7 +4704,7 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4731,10 +4713,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
+        <v>308</v>
+      </c>
+      <c r="G78" t="s">
         <v>309</v>
-      </c>
-      <c r="G78" t="s">
-        <v>310</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4755,7 +4737,7 @@
         <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D79" t="s">
         <v>116</v>
@@ -4764,10 +4746,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
+        <v>310</v>
+      </c>
+      <c r="G79" t="s">
         <v>311</v>
-      </c>
-      <c r="G79" t="s">
-        <v>312</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4848,194 +4830,194 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>237</v>
+        <v>447</v>
       </c>
       <c r="B82" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="C82" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="D82" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>422</v>
+        <v>448</v>
       </c>
       <c r="G82" t="s">
-        <v>423</v>
+        <v>449</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>8.6999999999999993</v>
+        <v>15.1</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>8.6999999999999993</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>424</v>
+        <v>246</v>
       </c>
       <c r="B83" t="s">
-        <v>427</v>
+        <v>237</v>
       </c>
       <c r="C83" t="s">
-        <v>428</v>
+        <v>237</v>
       </c>
       <c r="D83" t="s">
-        <v>429</v>
+        <v>238</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>425</v>
+        <v>239</v>
       </c>
       <c r="G83" t="s">
-        <v>426</v>
+        <v>240</v>
       </c>
       <c r="H83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I83">
-        <v>7</v>
+        <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" ref="J83:J90" si="2">H83*I83</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B84" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C84" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D84" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="G84" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J84">
-        <f t="shared" ref="J84:J91" si="2">H84*I84</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B85" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="C85" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="D85" t="s">
-        <v>244</v>
-      </c>
-      <c r="E85" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="G85" t="s">
-        <v>246</v>
+        <v>14</v>
       </c>
       <c r="H85">
         <v>1</v>
-      </c>
-      <c r="I85">
-        <v>0.79</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0</v>
+      </c>
+      <c r="K85" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B86" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C86" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D86" t="s">
-        <v>270</v>
+        <v>273</v>
+      </c>
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
+        <v>274</v>
       </c>
       <c r="G86" t="s">
-        <v>14</v>
+        <v>275</v>
       </c>
       <c r="H86">
         <v>1</v>
+      </c>
+      <c r="I86">
+        <v>0.47</v>
       </c>
       <c r="J86">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K86" t="s">
-        <v>271</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B87" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="C87" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="D87" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="G87" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -5043,492 +5025,459 @@
         <v>267</v>
       </c>
       <c r="B88" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C88" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D88" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G88" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J88">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B89" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C89" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D89" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="G89" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B90" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C90" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D90" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="G90" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>281</v>
+      </c>
+      <c r="B91" t="s">
         <v>277</v>
       </c>
-      <c r="B91" t="s">
-        <v>263</v>
-      </c>
       <c r="C91" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="D91" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
       </c>
       <c r="F91" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="G91" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>5.88</v>
+        <v>3.79</v>
       </c>
       <c r="J91">
-        <f t="shared" si="2"/>
-        <v>5.88</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>286</v>
+      </c>
+      <c r="B92" t="s">
         <v>282</v>
       </c>
-      <c r="B92" t="s">
-        <v>278</v>
-      </c>
       <c r="C92" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D92" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G92" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>372</v>
+      </c>
+      <c r="B93" t="s">
+        <v>397</v>
+      </c>
+      <c r="C93" t="s">
+        <v>397</v>
+      </c>
+      <c r="D93" t="s">
         <v>287</v>
       </c>
-      <c r="B93" t="s">
-        <v>283</v>
-      </c>
-      <c r="C93" t="s">
-        <v>283</v>
-      </c>
-      <c r="D93" t="s">
-        <v>284</v>
-      </c>
       <c r="E93" t="s">
         <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>285</v>
+        <v>398</v>
       </c>
       <c r="G93" t="s">
-        <v>286</v>
+        <v>399</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>417</v>
+      </c>
+      <c r="B94" t="s">
         <v>373</v>
       </c>
-      <c r="B94" t="s">
-        <v>398</v>
-      </c>
       <c r="C94" t="s">
-        <v>398</v>
+        <v>373</v>
       </c>
       <c r="D94" t="s">
-        <v>288</v>
+        <v>375</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>399</v>
+        <v>374</v>
       </c>
       <c r="G94" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B95" t="s">
-        <v>374</v>
+        <v>424</v>
       </c>
       <c r="C95" t="s">
-        <v>374</v>
+        <v>424</v>
       </c>
       <c r="D95" t="s">
-        <v>376</v>
+        <v>434</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="G95" t="s">
-        <v>377</v>
+        <v>436</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I95">
-        <v>6.84</v>
+        <v>2.8</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>8.3999999999999986</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="B96" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C96" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="D96" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="G96" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="H96">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I96">
-        <v>2.8</v>
+        <v>1.33</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>8.3999999999999986</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>419</v>
+        <v>440</v>
       </c>
       <c r="B97" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="C97" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="D97" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="G97" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>1.33</v>
+        <v>1.86</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>1.33</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>451</v>
+        <v>288</v>
       </c>
       <c r="B98" t="s">
-        <v>452</v>
+        <v>289</v>
       </c>
       <c r="C98" t="s">
-        <v>452</v>
+        <v>289</v>
       </c>
       <c r="D98" t="s">
-        <v>453</v>
+        <v>290</v>
       </c>
       <c r="E98" t="s">
-        <v>19</v>
+        <v>291</v>
       </c>
       <c r="F98" t="s">
-        <v>454</v>
+        <v>292</v>
       </c>
       <c r="G98" t="s">
-        <v>455</v>
+        <v>293</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>1.86</v>
+        <v>1.5</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B99" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C99" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D99" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E99" t="s">
-        <v>292</v>
+        <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G99" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>295</v>
+        <v>412</v>
       </c>
       <c r="B100" t="s">
-        <v>296</v>
+        <v>413</v>
       </c>
       <c r="C100" t="s">
-        <v>296</v>
+        <v>414</v>
       </c>
       <c r="D100" t="s">
-        <v>297</v>
+        <v>414</v>
       </c>
       <c r="E100" t="s">
-        <v>19</v>
+        <v>291</v>
       </c>
       <c r="F100" t="s">
-        <v>298</v>
+        <v>415</v>
       </c>
       <c r="G100" t="s">
-        <v>299</v>
+        <v>416</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100">
-        <v>2.96</v>
+        <v>0.95</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>413</v>
+        <v>299</v>
       </c>
       <c r="B101" t="s">
-        <v>414</v>
+        <v>300</v>
       </c>
       <c r="C101" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D101" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="E101" t="s">
-        <v>292</v>
+        <v>19</v>
       </c>
       <c r="F101" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G101" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I101">
-        <v>0.95</v>
+        <v>1.99</v>
       </c>
       <c r="J101">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>300</v>
-      </c>
-      <c r="B102" t="s">
-        <v>301</v>
-      </c>
-      <c r="C102" t="s">
-        <v>430</v>
-      </c>
-      <c r="D102" t="s">
-        <v>431</v>
-      </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
-        <v>432</v>
-      </c>
-      <c r="G102" t="s">
-        <v>433</v>
-      </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
-        <v>1.99</v>
-      </c>
-      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
STM32 (U5) renamed to U3.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -754,9 +754,6 @@
     <t>SST25VF010A-33-4I-SAE</t>
   </si>
   <si>
-    <t>U5</t>
-  </si>
-  <si>
     <t>MC34063SMD</t>
   </si>
   <si>
@@ -1364,6 +1361,9 @@
   </si>
   <si>
     <t>XS1-L02A-QF124-C4</t>
+  </si>
+  <si>
+    <t>U3</t>
   </si>
 </sst>
 </file>
@@ -2194,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,12 +2244,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2264,10 +2264,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G2" t="s">
         <v>318</v>
-      </c>
-      <c r="G2" t="s">
-        <v>319</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2301,10 +2301,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>319</v>
+      </c>
+      <c r="G3" t="s">
         <v>320</v>
-      </c>
-      <c r="G3" t="s">
-        <v>321</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2334,10 +2334,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G4" t="s">
         <v>322</v>
-      </c>
-      <c r="G4" t="s">
-        <v>323</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2391,10 +2391,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6" t="s">
         <v>327</v>
-      </c>
-      <c r="G6" t="s">
-        <v>328</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2451,10 +2451,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>328</v>
+      </c>
+      <c r="G8" t="s">
         <v>329</v>
-      </c>
-      <c r="G8" t="s">
-        <v>330</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2484,10 +2484,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>330</v>
+      </c>
+      <c r="G9" t="s">
         <v>331</v>
-      </c>
-      <c r="G9" t="s">
-        <v>332</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2517,10 +2517,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>342</v>
+      </c>
+      <c r="G10" t="s">
         <v>343</v>
-      </c>
-      <c r="G10" t="s">
-        <v>344</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2533,7 +2533,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,10 +2586,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>344</v>
+      </c>
+      <c r="G12" t="s">
         <v>345</v>
-      </c>
-      <c r="G12" t="s">
-        <v>346</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2619,10 +2619,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>342</v>
+      </c>
+      <c r="G13" t="s">
         <v>343</v>
-      </c>
-      <c r="G13" t="s">
-        <v>344</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2635,7 +2635,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2655,10 +2655,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>348</v>
+      </c>
+      <c r="G14" t="s">
         <v>349</v>
-      </c>
-      <c r="G14" t="s">
-        <v>350</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2671,7 +2671,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2715,10 +2715,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>332</v>
+      </c>
+      <c r="G16" t="s">
         <v>333</v>
-      </c>
-      <c r="G16" t="s">
-        <v>334</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2796,10 +2796,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>334</v>
+      </c>
+      <c r="G19" t="s">
         <v>335</v>
-      </c>
-      <c r="G19" t="s">
-        <v>336</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2812,7 +2812,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2832,10 +2832,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>337</v>
+      </c>
+      <c r="G20" t="s">
         <v>338</v>
-      </c>
-      <c r="G20" t="s">
-        <v>339</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2889,10 +2889,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>339</v>
+      </c>
+      <c r="G22" t="s">
         <v>340</v>
-      </c>
-      <c r="G22" t="s">
-        <v>341</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2907,10 +2907,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>366</v>
+      </c>
+      <c r="B23" t="s">
         <v>367</v>
-      </c>
-      <c r="B23" t="s">
-        <v>368</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2922,10 +2922,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>368</v>
+      </c>
+      <c r="G23" t="s">
         <v>369</v>
-      </c>
-      <c r="G23" t="s">
-        <v>370</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2940,10 +2940,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>407</v>
+      </c>
+      <c r="B24" t="s">
         <v>408</v>
-      </c>
-      <c r="B24" t="s">
-        <v>409</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2955,10 +2955,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>409</v>
+      </c>
+      <c r="G24" t="s">
         <v>410</v>
-      </c>
-      <c r="G24" t="s">
-        <v>411</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3021,10 +3021,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
+        <v>315</v>
+      </c>
+      <c r="G26" t="s">
         <v>316</v>
-      </c>
-      <c r="G26" t="s">
-        <v>317</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3054,10 +3054,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>357</v>
+      </c>
+      <c r="G27" t="s">
         <v>358</v>
-      </c>
-      <c r="G27" t="s">
-        <v>359</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3070,7 +3070,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3090,10 +3090,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
+        <v>350</v>
+      </c>
+      <c r="G28" t="s">
         <v>351</v>
-      </c>
-      <c r="G28" t="s">
-        <v>352</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3123,10 +3123,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>352</v>
+      </c>
+      <c r="G29" t="s">
         <v>353</v>
-      </c>
-      <c r="G29" t="s">
-        <v>354</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3156,10 +3156,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>354</v>
+      </c>
+      <c r="G30" t="s">
         <v>355</v>
-      </c>
-      <c r="G30" t="s">
-        <v>356</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3172,7 +3172,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3192,10 +3192,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>300</v>
+      </c>
+      <c r="G31" t="s">
         <v>301</v>
-      </c>
-      <c r="G31" t="s">
-        <v>302</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3210,25 +3210,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B32" t="s">
+        <v>391</v>
+      </c>
+      <c r="C32" t="s">
         <v>392</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>393</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>394</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>395</v>
-      </c>
-      <c r="G32" t="s">
-        <v>396</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -3243,25 +3243,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>428</v>
+      </c>
+      <c r="B33" t="s">
+        <v>431</v>
+      </c>
+      <c r="C33" t="s">
+        <v>431</v>
+      </c>
+      <c r="D33" t="s">
+        <v>432</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>429</v>
       </c>
-      <c r="B33" t="s">
-        <v>432</v>
-      </c>
-      <c r="C33" t="s">
-        <v>432</v>
-      </c>
-      <c r="D33" t="s">
-        <v>433</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>430</v>
-      </c>
-      <c r="G33" t="s">
-        <v>431</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3279,22 +3279,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
+        <v>364</v>
+      </c>
+      <c r="G34" t="s">
         <v>365</v>
-      </c>
-      <c r="G34" t="s">
-        <v>366</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3354,10 +3354,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F36" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3384,10 +3384,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F37" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3414,7 +3414,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3453,10 +3453,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
+        <v>313</v>
+      </c>
+      <c r="G39" t="s">
         <v>314</v>
-      </c>
-      <c r="G39" t="s">
-        <v>315</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -3502,12 +3502,12 @@
         <v>1.26</v>
       </c>
       <c r="L40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3573,7 +3573,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3588,10 +3588,10 @@
         <v>19</v>
       </c>
       <c r="F43" t="s">
+        <v>380</v>
+      </c>
+      <c r="G43" t="s">
         <v>381</v>
-      </c>
-      <c r="G43" t="s">
-        <v>382</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3606,22 +3606,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C44" t="s">
+        <v>376</v>
+      </c>
+      <c r="D44" t="s">
         <v>377</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>378</v>
       </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>379</v>
-      </c>
-      <c r="G44" t="s">
-        <v>380</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3636,22 +3636,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
+        <v>387</v>
+      </c>
+      <c r="G45" t="s">
         <v>388</v>
-      </c>
-      <c r="G45" t="s">
-        <v>389</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -3879,7 +3879,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B54" t="s">
         <v>146</v>
@@ -3960,10 +3960,10 @@
         <v>19</v>
       </c>
       <c r="F55" t="s">
+        <v>302</v>
+      </c>
+      <c r="G55" t="s">
         <v>303</v>
-      </c>
-      <c r="G55" t="s">
-        <v>304</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -4116,7 +4116,7 @@
         <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4125,10 +4125,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
+        <v>305</v>
+      </c>
+      <c r="G60" t="s">
         <v>306</v>
-      </c>
-      <c r="G60" t="s">
-        <v>307</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4149,7 +4149,7 @@
         <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D61" t="s">
         <v>116</v>
@@ -4158,10 +4158,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
+        <v>311</v>
+      </c>
+      <c r="G61" t="s">
         <v>312</v>
-      </c>
-      <c r="G61" t="s">
-        <v>313</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4224,10 +4224,10 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
+        <v>399</v>
+      </c>
+      <c r="G63" t="s">
         <v>400</v>
-      </c>
-      <c r="G63" t="s">
-        <v>401</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -4257,10 +4257,10 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
+        <v>403</v>
+      </c>
+      <c r="G64" t="s">
         <v>404</v>
-      </c>
-      <c r="G64" t="s">
-        <v>405</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4275,7 +4275,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -4704,7 +4704,7 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4713,10 +4713,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
+        <v>307</v>
+      </c>
+      <c r="G78" t="s">
         <v>308</v>
-      </c>
-      <c r="G78" t="s">
-        <v>309</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4737,7 +4737,7 @@
         <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D79" t="s">
         <v>116</v>
@@ -4746,10 +4746,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
+        <v>309</v>
+      </c>
+      <c r="G79" t="s">
         <v>310</v>
-      </c>
-      <c r="G79" t="s">
-        <v>311</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4830,25 +4830,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>446</v>
+      </c>
+      <c r="B82" t="s">
+        <v>444</v>
+      </c>
+      <c r="C82" t="s">
+        <v>444</v>
+      </c>
+      <c r="D82" t="s">
+        <v>445</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>447</v>
       </c>
-      <c r="B82" t="s">
-        <v>445</v>
-      </c>
-      <c r="C82" t="s">
-        <v>445</v>
-      </c>
-      <c r="D82" t="s">
-        <v>446</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>448</v>
-      </c>
-      <c r="G82" t="s">
-        <v>449</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4863,7 +4863,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>246</v>
+        <v>449</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B84" t="s">
         <v>241</v>
@@ -4929,16 +4929,16 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B85" t="s">
+        <v>267</v>
+      </c>
+      <c r="C85" t="s">
+        <v>267</v>
+      </c>
+      <c r="D85" t="s">
         <v>268</v>
-      </c>
-      <c r="C85" t="s">
-        <v>268</v>
-      </c>
-      <c r="D85" t="s">
-        <v>269</v>
       </c>
       <c r="G85" t="s">
         <v>14</v>
@@ -4951,30 +4951,30 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B86" t="s">
+        <v>271</v>
+      </c>
+      <c r="C86" t="s">
+        <v>271</v>
+      </c>
+      <c r="D86" t="s">
         <v>272</v>
       </c>
-      <c r="C86" t="s">
-        <v>272</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>273</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>274</v>
-      </c>
-      <c r="G86" t="s">
-        <v>275</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4989,25 +4989,25 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B87" t="s">
+        <v>246</v>
+      </c>
+      <c r="C87" t="s">
+        <v>246</v>
+      </c>
+      <c r="D87" t="s">
         <v>247</v>
       </c>
-      <c r="C87" t="s">
-        <v>247</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>248</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>249</v>
-      </c>
-      <c r="G87" t="s">
-        <v>250</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -5022,25 +5022,25 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B88" t="s">
+        <v>251</v>
+      </c>
+      <c r="C88" t="s">
+        <v>251</v>
+      </c>
+      <c r="D88" t="s">
         <v>252</v>
       </c>
-      <c r="C88" t="s">
-        <v>252</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>253</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>254</v>
-      </c>
-      <c r="G88" t="s">
-        <v>255</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -5055,25 +5055,25 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B89" t="s">
+        <v>256</v>
+      </c>
+      <c r="C89" t="s">
+        <v>256</v>
+      </c>
+      <c r="D89" t="s">
         <v>257</v>
       </c>
-      <c r="C89" t="s">
-        <v>257</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>258</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="G89" t="s">
         <v>259</v>
-      </c>
-      <c r="G89" t="s">
-        <v>260</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -5088,25 +5088,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B90" t="s">
+        <v>261</v>
+      </c>
+      <c r="C90" t="s">
+        <v>261</v>
+      </c>
+      <c r="D90" t="s">
         <v>262</v>
       </c>
-      <c r="C90" t="s">
-        <v>262</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>263</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>264</v>
-      </c>
-      <c r="G90" t="s">
-        <v>265</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5121,25 +5121,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B91" t="s">
+        <v>276</v>
+      </c>
+      <c r="C91" t="s">
+        <v>276</v>
+      </c>
+      <c r="D91" t="s">
         <v>277</v>
       </c>
-      <c r="C91" t="s">
-        <v>277</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>278</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>279</v>
-      </c>
-      <c r="G91" t="s">
-        <v>280</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5154,25 +5154,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B92" t="s">
+        <v>281</v>
+      </c>
+      <c r="C92" t="s">
+        <v>281</v>
+      </c>
+      <c r="D92" t="s">
         <v>282</v>
       </c>
-      <c r="C92" t="s">
-        <v>282</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>283</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>284</v>
-      </c>
-      <c r="G92" t="s">
-        <v>285</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5187,25 +5187,25 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B93" t="s">
+        <v>396</v>
+      </c>
+      <c r="C93" t="s">
+        <v>396</v>
+      </c>
+      <c r="D93" t="s">
+        <v>286</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>397</v>
       </c>
-      <c r="C93" t="s">
-        <v>397</v>
-      </c>
-      <c r="D93" t="s">
-        <v>287</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>398</v>
-      </c>
-      <c r="G93" t="s">
-        <v>399</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5220,25 +5220,25 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B94" t="s">
+        <v>372</v>
+      </c>
+      <c r="C94" t="s">
+        <v>372</v>
+      </c>
+      <c r="D94" t="s">
+        <v>374</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>373</v>
       </c>
-      <c r="C94" t="s">
-        <v>373</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="G94" t="s">
         <v>375</v>
-      </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>374</v>
-      </c>
-      <c r="G94" t="s">
-        <v>376</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5253,25 +5253,25 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>422</v>
+      </c>
+      <c r="B95" t="s">
         <v>423</v>
       </c>
-      <c r="B95" t="s">
-        <v>424</v>
-      </c>
       <c r="C95" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D95" t="s">
+        <v>433</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>434</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>435</v>
-      </c>
-      <c r="G95" t="s">
-        <v>436</v>
       </c>
       <c r="H95">
         <v>3</v>
@@ -5286,25 +5286,25 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B96" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C96" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D96" t="s">
+        <v>436</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>437</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>438</v>
-      </c>
-      <c r="G96" t="s">
-        <v>439</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -5319,25 +5319,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>439</v>
+      </c>
+      <c r="B97" t="s">
         <v>440</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
+        <v>440</v>
+      </c>
+      <c r="D97" t="s">
         <v>441</v>
       </c>
-      <c r="C97" t="s">
-        <v>441</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>442</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>443</v>
-      </c>
-      <c r="G97" t="s">
-        <v>444</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -5352,25 +5352,25 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>287</v>
+      </c>
+      <c r="B98" t="s">
         <v>288</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
+        <v>288</v>
+      </c>
+      <c r="D98" t="s">
         <v>289</v>
       </c>
-      <c r="C98" t="s">
-        <v>289</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>290</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
         <v>291</v>
       </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>292</v>
-      </c>
-      <c r="G98" t="s">
-        <v>293</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -5385,25 +5385,25 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>293</v>
+      </c>
+      <c r="B99" t="s">
         <v>294</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>294</v>
+      </c>
+      <c r="D99" t="s">
         <v>295</v>
       </c>
-      <c r="C99" t="s">
-        <v>295</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>296</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>297</v>
-      </c>
-      <c r="G99" t="s">
-        <v>298</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -5418,25 +5418,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>411</v>
+      </c>
+      <c r="B100" t="s">
         <v>412</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>413</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
+        <v>413</v>
+      </c>
+      <c r="E100" t="s">
+        <v>290</v>
+      </c>
+      <c r="F100" t="s">
         <v>414</v>
       </c>
-      <c r="D100" t="s">
-        <v>414</v>
-      </c>
-      <c r="E100" t="s">
-        <v>291</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
         <v>415</v>
-      </c>
-      <c r="G100" t="s">
-        <v>416</v>
       </c>
       <c r="H100">
         <v>2</v>
@@ -5451,25 +5451,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>298</v>
+      </c>
+      <c r="B101" t="s">
         <v>299</v>
       </c>
-      <c r="B101" t="s">
-        <v>300</v>
-      </c>
       <c r="C101" t="s">
+        <v>418</v>
+      </c>
+      <c r="D101" t="s">
         <v>419</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>420</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>421</v>
-      </c>
-      <c r="G101" t="s">
-        <v>422</v>
       </c>
       <c r="H101">
         <v>1</v>

</xml_diff>

<commit_message>
EEPROM (U6) renamed to U4.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -766,9 +766,6 @@
     <t>MC34063EBD-TR</t>
   </si>
   <si>
-    <t>U6</t>
-  </si>
-  <si>
     <t>TPS54620</t>
   </si>
   <si>
@@ -1364,6 +1361,9 @@
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
   </si>
 </sst>
 </file>
@@ -2195,7 +2195,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,12 +2244,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2264,10 +2264,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" t="s">
         <v>317</v>
-      </c>
-      <c r="G2" t="s">
-        <v>318</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2301,10 +2301,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G3" t="s">
         <v>319</v>
-      </c>
-      <c r="G3" t="s">
-        <v>320</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2334,10 +2334,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>320</v>
+      </c>
+      <c r="G4" t="s">
         <v>321</v>
-      </c>
-      <c r="G4" t="s">
-        <v>322</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2391,10 +2391,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>325</v>
+      </c>
+      <c r="G6" t="s">
         <v>326</v>
-      </c>
-      <c r="G6" t="s">
-        <v>327</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2451,10 +2451,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G8" t="s">
         <v>328</v>
-      </c>
-      <c r="G8" t="s">
-        <v>329</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2484,10 +2484,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>329</v>
+      </c>
+      <c r="G9" t="s">
         <v>330</v>
-      </c>
-      <c r="G9" t="s">
-        <v>331</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2517,10 +2517,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>341</v>
+      </c>
+      <c r="G10" t="s">
         <v>342</v>
-      </c>
-      <c r="G10" t="s">
-        <v>343</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2533,7 +2533,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,10 +2586,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G12" t="s">
         <v>344</v>
-      </c>
-      <c r="G12" t="s">
-        <v>345</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2619,10 +2619,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>341</v>
+      </c>
+      <c r="G13" t="s">
         <v>342</v>
-      </c>
-      <c r="G13" t="s">
-        <v>343</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2635,7 +2635,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2655,10 +2655,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>347</v>
+      </c>
+      <c r="G14" t="s">
         <v>348</v>
-      </c>
-      <c r="G14" t="s">
-        <v>349</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2671,7 +2671,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2715,10 +2715,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>331</v>
+      </c>
+      <c r="G16" t="s">
         <v>332</v>
-      </c>
-      <c r="G16" t="s">
-        <v>333</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2796,10 +2796,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>333</v>
+      </c>
+      <c r="G19" t="s">
         <v>334</v>
-      </c>
-      <c r="G19" t="s">
-        <v>335</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2812,7 +2812,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2832,10 +2832,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>336</v>
+      </c>
+      <c r="G20" t="s">
         <v>337</v>
-      </c>
-      <c r="G20" t="s">
-        <v>338</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2889,10 +2889,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>338</v>
+      </c>
+      <c r="G22" t="s">
         <v>339</v>
-      </c>
-      <c r="G22" t="s">
-        <v>340</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2907,10 +2907,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" t="s">
         <v>366</v>
-      </c>
-      <c r="B23" t="s">
-        <v>367</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2922,10 +2922,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>367</v>
+      </c>
+      <c r="G23" t="s">
         <v>368</v>
-      </c>
-      <c r="G23" t="s">
-        <v>369</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2940,10 +2940,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>406</v>
+      </c>
+      <c r="B24" t="s">
         <v>407</v>
-      </c>
-      <c r="B24" t="s">
-        <v>408</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2955,10 +2955,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>408</v>
+      </c>
+      <c r="G24" t="s">
         <v>409</v>
-      </c>
-      <c r="G24" t="s">
-        <v>410</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3021,10 +3021,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
+        <v>314</v>
+      </c>
+      <c r="G26" t="s">
         <v>315</v>
-      </c>
-      <c r="G26" t="s">
-        <v>316</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3054,10 +3054,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>356</v>
+      </c>
+      <c r="G27" t="s">
         <v>357</v>
-      </c>
-      <c r="G27" t="s">
-        <v>358</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3070,7 +3070,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3090,10 +3090,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
+        <v>349</v>
+      </c>
+      <c r="G28" t="s">
         <v>350</v>
-      </c>
-      <c r="G28" t="s">
-        <v>351</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3123,10 +3123,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>351</v>
+      </c>
+      <c r="G29" t="s">
         <v>352</v>
-      </c>
-      <c r="G29" t="s">
-        <v>353</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3156,10 +3156,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>353</v>
+      </c>
+      <c r="G30" t="s">
         <v>354</v>
-      </c>
-      <c r="G30" t="s">
-        <v>355</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3172,7 +3172,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3192,10 +3192,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>299</v>
+      </c>
+      <c r="G31" t="s">
         <v>300</v>
-      </c>
-      <c r="G31" t="s">
-        <v>301</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3210,25 +3210,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B32" t="s">
+        <v>390</v>
+      </c>
+      <c r="C32" t="s">
         <v>391</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>392</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>393</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>394</v>
-      </c>
-      <c r="G32" t="s">
-        <v>395</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -3243,25 +3243,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>427</v>
+      </c>
+      <c r="B33" t="s">
+        <v>430</v>
+      </c>
+      <c r="C33" t="s">
+        <v>430</v>
+      </c>
+      <c r="D33" t="s">
+        <v>431</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>428</v>
       </c>
-      <c r="B33" t="s">
-        <v>431</v>
-      </c>
-      <c r="C33" t="s">
-        <v>431</v>
-      </c>
-      <c r="D33" t="s">
-        <v>432</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>429</v>
-      </c>
-      <c r="G33" t="s">
-        <v>430</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3279,22 +3279,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
+        <v>363</v>
+      </c>
+      <c r="G34" t="s">
         <v>364</v>
-      </c>
-      <c r="G34" t="s">
-        <v>365</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3354,10 +3354,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3384,10 +3384,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3414,7 +3414,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3453,10 +3453,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
+        <v>312</v>
+      </c>
+      <c r="G39" t="s">
         <v>313</v>
-      </c>
-      <c r="G39" t="s">
-        <v>314</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -3502,12 +3502,12 @@
         <v>1.26</v>
       </c>
       <c r="L40" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3573,7 +3573,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3588,10 +3588,10 @@
         <v>19</v>
       </c>
       <c r="F43" t="s">
+        <v>379</v>
+      </c>
+      <c r="G43" t="s">
         <v>380</v>
-      </c>
-      <c r="G43" t="s">
-        <v>381</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3606,22 +3606,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C44" t="s">
+        <v>375</v>
+      </c>
+      <c r="D44" t="s">
         <v>376</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>377</v>
       </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>378</v>
-      </c>
-      <c r="G44" t="s">
-        <v>379</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3636,22 +3636,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
+        <v>386</v>
+      </c>
+      <c r="G45" t="s">
         <v>387</v>
-      </c>
-      <c r="G45" t="s">
-        <v>388</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -3879,7 +3879,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B54" t="s">
         <v>146</v>
@@ -3960,10 +3960,10 @@
         <v>19</v>
       </c>
       <c r="F55" t="s">
+        <v>301</v>
+      </c>
+      <c r="G55" t="s">
         <v>302</v>
-      </c>
-      <c r="G55" t="s">
-        <v>303</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -4116,7 +4116,7 @@
         <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4125,10 +4125,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
+        <v>304</v>
+      </c>
+      <c r="G60" t="s">
         <v>305</v>
-      </c>
-      <c r="G60" t="s">
-        <v>306</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4149,7 +4149,7 @@
         <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D61" t="s">
         <v>116</v>
@@ -4158,10 +4158,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G61" t="s">
         <v>311</v>
-      </c>
-      <c r="G61" t="s">
-        <v>312</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4224,10 +4224,10 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
+        <v>398</v>
+      </c>
+      <c r="G63" t="s">
         <v>399</v>
-      </c>
-      <c r="G63" t="s">
-        <v>400</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -4257,10 +4257,10 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
+        <v>402</v>
+      </c>
+      <c r="G64" t="s">
         <v>403</v>
-      </c>
-      <c r="G64" t="s">
-        <v>404</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4275,7 +4275,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -4704,7 +4704,7 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4713,10 +4713,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
+        <v>306</v>
+      </c>
+      <c r="G78" t="s">
         <v>307</v>
-      </c>
-      <c r="G78" t="s">
-        <v>308</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4737,7 +4737,7 @@
         <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D79" t="s">
         <v>116</v>
@@ -4746,10 +4746,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
+        <v>308</v>
+      </c>
+      <c r="G79" t="s">
         <v>309</v>
-      </c>
-      <c r="G79" t="s">
-        <v>310</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4830,25 +4830,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>445</v>
+      </c>
+      <c r="B82" t="s">
+        <v>443</v>
+      </c>
+      <c r="C82" t="s">
+        <v>443</v>
+      </c>
+      <c r="D82" t="s">
+        <v>444</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>446</v>
       </c>
-      <c r="B82" t="s">
-        <v>444</v>
-      </c>
-      <c r="C82" t="s">
-        <v>444</v>
-      </c>
-      <c r="D82" t="s">
-        <v>445</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>447</v>
-      </c>
-      <c r="G82" t="s">
-        <v>448</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4863,7 +4863,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>250</v>
+        <v>449</v>
       </c>
       <c r="B84" t="s">
         <v>241</v>
@@ -4929,16 +4929,16 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B85" t="s">
+        <v>266</v>
+      </c>
+      <c r="C85" t="s">
+        <v>266</v>
+      </c>
+      <c r="D85" t="s">
         <v>267</v>
-      </c>
-      <c r="C85" t="s">
-        <v>267</v>
-      </c>
-      <c r="D85" t="s">
-        <v>268</v>
       </c>
       <c r="G85" t="s">
         <v>14</v>
@@ -4951,30 +4951,30 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B86" t="s">
+        <v>270</v>
+      </c>
+      <c r="C86" t="s">
+        <v>270</v>
+      </c>
+      <c r="D86" t="s">
         <v>271</v>
       </c>
-      <c r="C86" t="s">
-        <v>271</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>272</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>273</v>
-      </c>
-      <c r="G86" t="s">
-        <v>274</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B87" t="s">
         <v>246</v>
@@ -5022,25 +5022,25 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B88" t="s">
+        <v>250</v>
+      </c>
+      <c r="C88" t="s">
+        <v>250</v>
+      </c>
+      <c r="D88" t="s">
         <v>251</v>
       </c>
-      <c r="C88" t="s">
-        <v>251</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>252</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>253</v>
-      </c>
-      <c r="G88" t="s">
-        <v>254</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -5055,25 +5055,25 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B89" t="s">
+        <v>255</v>
+      </c>
+      <c r="C89" t="s">
+        <v>255</v>
+      </c>
+      <c r="D89" t="s">
         <v>256</v>
       </c>
-      <c r="C89" t="s">
-        <v>256</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>257</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="G89" t="s">
         <v>258</v>
-      </c>
-      <c r="G89" t="s">
-        <v>259</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -5088,25 +5088,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B90" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" t="s">
+        <v>260</v>
+      </c>
+      <c r="D90" t="s">
         <v>261</v>
       </c>
-      <c r="C90" t="s">
-        <v>261</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>262</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>263</v>
-      </c>
-      <c r="G90" t="s">
-        <v>264</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5121,25 +5121,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B91" t="s">
+        <v>275</v>
+      </c>
+      <c r="C91" t="s">
+        <v>275</v>
+      </c>
+      <c r="D91" t="s">
         <v>276</v>
       </c>
-      <c r="C91" t="s">
-        <v>276</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>277</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>278</v>
-      </c>
-      <c r="G91" t="s">
-        <v>279</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5154,25 +5154,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B92" t="s">
+        <v>280</v>
+      </c>
+      <c r="C92" t="s">
+        <v>280</v>
+      </c>
+      <c r="D92" t="s">
         <v>281</v>
       </c>
-      <c r="C92" t="s">
-        <v>281</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>282</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>283</v>
-      </c>
-      <c r="G92" t="s">
-        <v>284</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5187,25 +5187,25 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B93" t="s">
+        <v>395</v>
+      </c>
+      <c r="C93" t="s">
+        <v>395</v>
+      </c>
+      <c r="D93" t="s">
+        <v>285</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>396</v>
       </c>
-      <c r="C93" t="s">
-        <v>396</v>
-      </c>
-      <c r="D93" t="s">
-        <v>286</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>397</v>
-      </c>
-      <c r="G93" t="s">
-        <v>398</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5220,25 +5220,25 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B94" t="s">
+        <v>371</v>
+      </c>
+      <c r="C94" t="s">
+        <v>371</v>
+      </c>
+      <c r="D94" t="s">
+        <v>373</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>372</v>
       </c>
-      <c r="C94" t="s">
-        <v>372</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="G94" t="s">
         <v>374</v>
-      </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>373</v>
-      </c>
-      <c r="G94" t="s">
-        <v>375</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5253,25 +5253,25 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>421</v>
+      </c>
+      <c r="B95" t="s">
         <v>422</v>
       </c>
-      <c r="B95" t="s">
-        <v>423</v>
-      </c>
       <c r="C95" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D95" t="s">
+        <v>432</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>433</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>434</v>
-      </c>
-      <c r="G95" t="s">
-        <v>435</v>
       </c>
       <c r="H95">
         <v>3</v>
@@ -5286,25 +5286,25 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B96" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C96" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D96" t="s">
+        <v>435</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>436</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>437</v>
-      </c>
-      <c r="G96" t="s">
-        <v>438</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -5319,25 +5319,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>438</v>
+      </c>
+      <c r="B97" t="s">
         <v>439</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
+        <v>439</v>
+      </c>
+      <c r="D97" t="s">
         <v>440</v>
       </c>
-      <c r="C97" t="s">
-        <v>440</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>441</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>442</v>
-      </c>
-      <c r="G97" t="s">
-        <v>443</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -5352,25 +5352,25 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>286</v>
+      </c>
+      <c r="B98" t="s">
         <v>287</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" t="s">
         <v>288</v>
       </c>
-      <c r="C98" t="s">
-        <v>288</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>289</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
         <v>290</v>
       </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>291</v>
-      </c>
-      <c r="G98" t="s">
-        <v>292</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -5385,25 +5385,25 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>292</v>
+      </c>
+      <c r="B99" t="s">
         <v>293</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>293</v>
+      </c>
+      <c r="D99" t="s">
         <v>294</v>
       </c>
-      <c r="C99" t="s">
-        <v>294</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>295</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>296</v>
-      </c>
-      <c r="G99" t="s">
-        <v>297</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -5418,25 +5418,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>410</v>
+      </c>
+      <c r="B100" t="s">
         <v>411</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>412</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
+        <v>412</v>
+      </c>
+      <c r="E100" t="s">
+        <v>289</v>
+      </c>
+      <c r="F100" t="s">
         <v>413</v>
       </c>
-      <c r="D100" t="s">
-        <v>413</v>
-      </c>
-      <c r="E100" t="s">
-        <v>290</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
         <v>414</v>
-      </c>
-      <c r="G100" t="s">
-        <v>415</v>
       </c>
       <c r="H100">
         <v>2</v>
@@ -5451,25 +5451,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>297</v>
+      </c>
+      <c r="B101" t="s">
         <v>298</v>
       </c>
-      <c r="B101" t="s">
-        <v>299</v>
-      </c>
       <c r="C101" t="s">
+        <v>417</v>
+      </c>
+      <c r="D101" t="s">
         <v>418</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>419</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>420</v>
-      </c>
-      <c r="G101" t="s">
-        <v>421</v>
       </c>
       <c r="H101">
         <v>1</v>

</xml_diff>

<commit_message>
Renamed U7->U5 and U8->U6.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -754,6 +754,9 @@
     <t>SST25VF010A-33-4I-SAE</t>
   </si>
   <si>
+    <t>U5</t>
+  </si>
+  <si>
     <t>MC34063SMD</t>
   </si>
   <si>
@@ -766,6 +769,9 @@
     <t>MC34063EBD-TR</t>
   </si>
   <si>
+    <t>U6</t>
+  </si>
+  <si>
     <t>TPS54620</t>
   </si>
   <si>
@@ -778,9 +784,6 @@
     <t>TPS54620RGYR</t>
   </si>
   <si>
-    <t>U7</t>
-  </si>
-  <si>
     <t>FAN2012</t>
   </si>
   <si>
@@ -791,9 +794,6 @@
   </si>
   <si>
     <t>FAN2012MPXCT</t>
-  </si>
-  <si>
-    <t>U8</t>
   </si>
   <si>
     <t>TPS5431</t>
@@ -2195,7 +2195,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4929,7 +4929,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B85" t="s">
         <v>266</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B86" t="s">
         <v>270</v>
@@ -4992,22 +4992,22 @@
         <v>264</v>
       </c>
       <c r="B87" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C87" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D87" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G87" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -5025,22 +5025,22 @@
         <v>265</v>
       </c>
       <c r="B88" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C88" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D88" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G88" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -5058,22 +5058,22 @@
         <v>269</v>
       </c>
       <c r="B89" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C89" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D89" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G89" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H89">
         <v>1</v>

</xml_diff>

<commit_message>
Added logic level translation for STM32 I2C2.
This is the I2C bus multiplexed on Arduino A4 and A5.
PC4 now controls both mux control pins, as well as the enable pin of a TXS0102 (U11).
The TXS0102 B-side (5V) connects to the B pins of the muxes, with the ADC still on A.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="455">
   <si>
     <t>Part</t>
   </si>
@@ -829,6 +829,9 @@
     <t>NON STOCK</t>
   </si>
   <si>
+    <t>U11</t>
+  </si>
+  <si>
     <t>NC7WZ07</t>
   </si>
   <si>
@@ -1364,6 +1367,18 @@
   </si>
   <si>
     <t>U4</t>
+  </si>
+  <si>
+    <t>DCT-R-PDSO-G8</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>595-TXS0102DCTR</t>
+  </si>
+  <si>
+    <t>TXS0102DCTR</t>
   </si>
 </sst>
 </file>
@@ -2192,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G85" sqref="E85:G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,12 +2259,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2264,10 +2279,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2280,8 +2295,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J109)</f>
-        <v>188.25300000000004</v>
+        <f>SUM(J2:J110)</f>
+        <v>189.48300000000003</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2301,10 +2316,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2319,7 +2334,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2334,10 +2349,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2391,10 +2406,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2407,7 +2422,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2451,10 +2466,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2484,10 +2499,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2517,10 +2532,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G10" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2533,7 +2548,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,10 +2601,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G12" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2619,10 +2634,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2635,7 +2650,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2655,10 +2670,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G14" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2671,7 +2686,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2715,10 +2730,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G16" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2796,10 +2811,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G19" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2812,7 +2827,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2832,10 +2847,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2889,10 +2904,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G22" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2907,10 +2922,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B23" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2922,10 +2937,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="G23" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2940,10 +2955,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B24" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2955,10 +2970,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G24" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3021,10 +3036,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G26" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3054,10 +3069,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G27" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3070,7 +3085,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3090,10 +3105,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G28" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3123,10 +3138,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G29" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3156,10 +3171,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G30" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3172,7 +3187,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3192,10 +3207,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G31" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3210,25 +3225,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B32" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C32" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D32" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G32" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -3243,25 +3258,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B33" t="s">
+        <v>431</v>
+      </c>
+      <c r="C33" t="s">
+        <v>431</v>
+      </c>
+      <c r="D33" t="s">
+        <v>432</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>429</v>
+      </c>
+      <c r="G33" t="s">
         <v>430</v>
-      </c>
-      <c r="C33" t="s">
-        <v>430</v>
-      </c>
-      <c r="D33" t="s">
-        <v>431</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
-        <v>428</v>
-      </c>
-      <c r="G33" t="s">
-        <v>429</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3279,22 +3294,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
+        <v>365</v>
+      </c>
+      <c r="C34" t="s">
+        <v>365</v>
+      </c>
+      <c r="D34" t="s">
+        <v>365</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
         <v>364</v>
       </c>
-      <c r="C34" t="s">
-        <v>364</v>
-      </c>
-      <c r="D34" t="s">
-        <v>364</v>
-      </c>
-      <c r="E34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" t="s">
-        <v>363</v>
-      </c>
       <c r="G34" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3342,7 +3357,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3354,10 +3369,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F36" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3372,7 +3387,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3384,10 +3399,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F37" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3414,7 +3429,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3438,7 +3453,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3453,10 +3468,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G39" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -3502,12 +3517,12 @@
         <v>1.26</v>
       </c>
       <c r="L40" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3573,7 +3588,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3588,10 +3603,10 @@
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G43" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3606,22 +3621,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C44" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D44" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G44" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3636,22 +3651,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G45" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3822,7 +3837,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -3879,7 +3894,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
@@ -3912,7 +3927,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B54" t="s">
         <v>146</v>
@@ -3960,10 +3975,10 @@
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G55" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4044,7 +4059,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -4116,7 +4131,7 @@
         <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4125,10 +4140,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G60" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4149,7 +4164,7 @@
         <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D61" t="s">
         <v>116</v>
@@ -4158,10 +4173,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G61" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4224,10 +4239,10 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G63" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4242,7 +4257,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -4257,10 +4272,10 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G64" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4275,7 +4290,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -4566,7 +4581,7 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
+        <f t="shared" ref="J73:J102" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
@@ -4704,7 +4719,7 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4713,10 +4728,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G78" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4737,7 +4752,7 @@
         <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D79" t="s">
         <v>116</v>
@@ -4746,10 +4761,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G79" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4830,25 +4845,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>446</v>
+      </c>
+      <c r="B82" t="s">
+        <v>444</v>
+      </c>
+      <c r="C82" t="s">
+        <v>444</v>
+      </c>
+      <c r="D82" t="s">
         <v>445</v>
       </c>
-      <c r="B82" t="s">
-        <v>443</v>
-      </c>
-      <c r="C82" t="s">
-        <v>443</v>
-      </c>
-      <c r="D82" t="s">
-        <v>444</v>
-      </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G82" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4863,7 +4878,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
@@ -4890,13 +4905,13 @@
         <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J90" si="2">H83*I83</f>
+        <f t="shared" ref="J83:J91" si="2">H83*I83</f>
         <v>6.6</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B84" t="s">
         <v>241</v>
@@ -4940,9 +4955,6 @@
       <c r="D85" t="s">
         <v>269</v>
       </c>
-      <c r="G85" t="s">
-        <v>14</v>
-      </c>
       <c r="H85">
         <v>1</v>
       </c>
@@ -4959,22 +4971,22 @@
         <v>251</v>
       </c>
       <c r="B86" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C86" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D86" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G86" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -5121,363 +5133,396 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>271</v>
+      </c>
+      <c r="B91" t="s">
+        <v>424</v>
+      </c>
+      <c r="C91" t="s">
+        <v>424</v>
+      </c>
+      <c r="D91" t="s">
+        <v>451</v>
+      </c>
+      <c r="E91" t="s">
+        <v>452</v>
+      </c>
+      <c r="F91" t="s">
+        <v>453</v>
+      </c>
+      <c r="G91" t="s">
+        <v>454</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>1.23</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="2"/>
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>280</v>
+      </c>
+      <c r="B92" t="s">
+        <v>276</v>
+      </c>
+      <c r="C92" t="s">
+        <v>276</v>
+      </c>
+      <c r="D92" t="s">
+        <v>277</v>
+      </c>
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
+        <v>278</v>
+      </c>
+      <c r="G92" t="s">
         <v>279</v>
       </c>
-      <c r="B91" t="s">
-        <v>275</v>
-      </c>
-      <c r="C91" t="s">
-        <v>275</v>
-      </c>
-      <c r="D91" t="s">
-        <v>276</v>
-      </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
-        <v>277</v>
-      </c>
-      <c r="G91" t="s">
-        <v>278</v>
-      </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>3.79</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>285</v>
+      </c>
+      <c r="B93" t="s">
+        <v>281</v>
+      </c>
+      <c r="C93" t="s">
+        <v>281</v>
+      </c>
+      <c r="D93" t="s">
+        <v>282</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
+        <v>283</v>
+      </c>
+      <c r="G93" t="s">
         <v>284</v>
       </c>
-      <c r="B92" t="s">
-        <v>280</v>
-      </c>
-      <c r="C92" t="s">
-        <v>280</v>
-      </c>
-      <c r="D92" t="s">
-        <v>281</v>
-      </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
-        <v>282</v>
-      </c>
-      <c r="G92" t="s">
-        <v>283</v>
-      </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>1.57</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>370</v>
-      </c>
-      <c r="B93" t="s">
-        <v>395</v>
-      </c>
-      <c r="C93" t="s">
-        <v>395</v>
-      </c>
-      <c r="D93" t="s">
-        <v>285</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>371</v>
+      </c>
+      <c r="B94" t="s">
         <v>396</v>
       </c>
-      <c r="G93" t="s">
+      <c r="C94" t="s">
+        <v>396</v>
+      </c>
+      <c r="D94" t="s">
+        <v>286</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>397</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="G94" t="s">
+        <v>398</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>8.48</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>415</v>
-      </c>
-      <c r="B94" t="s">
-        <v>371</v>
-      </c>
-      <c r="C94" t="s">
-        <v>371</v>
-      </c>
-      <c r="D94" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>416</v>
+      </c>
+      <c r="B95" t="s">
+        <v>372</v>
+      </c>
+      <c r="C95" t="s">
+        <v>372</v>
+      </c>
+      <c r="D95" t="s">
+        <v>374</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>373</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>372</v>
-      </c>
-      <c r="G94" t="s">
-        <v>374</v>
-      </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="G95" t="s">
+        <v>375</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>6.84</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>421</v>
-      </c>
-      <c r="B95" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>422</v>
       </c>
-      <c r="C95" t="s">
-        <v>422</v>
-      </c>
-      <c r="D95" t="s">
-        <v>432</v>
-      </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="B96" t="s">
+        <v>423</v>
+      </c>
+      <c r="C96" t="s">
+        <v>423</v>
+      </c>
+      <c r="D96" t="s">
         <v>433</v>
       </c>
-      <c r="G95" t="s">
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>434</v>
       </c>
-      <c r="H95">
+      <c r="G96" t="s">
+        <v>435</v>
+      </c>
+      <c r="H96">
         <v>3</v>
       </c>
-      <c r="I95">
+      <c r="I96">
         <v>2.8</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>8.3999999999999986</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>416</v>
-      </c>
-      <c r="B96" t="s">
-        <v>423</v>
-      </c>
-      <c r="C96" t="s">
-        <v>423</v>
-      </c>
-      <c r="D96" t="s">
-        <v>435</v>
-      </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>417</v>
+      </c>
+      <c r="B97" t="s">
+        <v>424</v>
+      </c>
+      <c r="C97" t="s">
+        <v>424</v>
+      </c>
+      <c r="D97" t="s">
         <v>436</v>
       </c>
-      <c r="G96" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>437</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="G97" t="s">
+        <v>438</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
         <v>1.33</v>
       </c>
-      <c r="J96">
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>1.33</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>438</v>
-      </c>
-      <c r="B97" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>439</v>
       </c>
-      <c r="C97" t="s">
-        <v>439</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="B98" t="s">
         <v>440</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="C98" t="s">
+        <v>440</v>
+      </c>
+      <c r="D98" t="s">
         <v>441</v>
       </c>
-      <c r="G97" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>442</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="G98" t="s">
+        <v>443</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>1.86</v>
       </c>
-      <c r="J97">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>286</v>
-      </c>
-      <c r="B98" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>287</v>
       </c>
-      <c r="C98" t="s">
-        <v>287</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="B99" t="s">
         <v>288</v>
       </c>
-      <c r="E98" t="s">
+      <c r="C99" t="s">
+        <v>288</v>
+      </c>
+      <c r="D99" t="s">
         <v>289</v>
       </c>
-      <c r="F98" t="s">
+      <c r="E99" t="s">
         <v>290</v>
       </c>
-      <c r="G98" t="s">
+      <c r="F99" t="s">
         <v>291</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="G99" t="s">
+        <v>292</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.5</v>
       </c>
-      <c r="J98">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>292</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>293</v>
       </c>
-      <c r="C99" t="s">
-        <v>293</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="B100" t="s">
         <v>294</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="C100" t="s">
+        <v>294</v>
+      </c>
+      <c r="D100" t="s">
         <v>295</v>
       </c>
-      <c r="G99" t="s">
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>296</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="G100" t="s">
+        <v>297</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>2.96</v>
       </c>
-      <c r="J99">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>410</v>
-      </c>
-      <c r="B100" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>411</v>
       </c>
-      <c r="C100" t="s">
+      <c r="B101" t="s">
         <v>412</v>
       </c>
-      <c r="D100" t="s">
-        <v>412</v>
-      </c>
-      <c r="E100" t="s">
-        <v>289</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="C101" t="s">
         <v>413</v>
       </c>
-      <c r="G100" t="s">
+      <c r="D101" t="s">
+        <v>413</v>
+      </c>
+      <c r="E101" t="s">
+        <v>290</v>
+      </c>
+      <c r="F101" t="s">
         <v>414</v>
       </c>
-      <c r="H100">
+      <c r="G101" t="s">
+        <v>415</v>
+      </c>
+      <c r="H101">
         <v>2</v>
       </c>
-      <c r="I100">
+      <c r="I101">
         <v>0.95</v>
       </c>
-      <c r="J100">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>297</v>
-      </c>
-      <c r="B101" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>298</v>
       </c>
-      <c r="C101" t="s">
-        <v>417</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="B102" t="s">
+        <v>299</v>
+      </c>
+      <c r="C102" t="s">
         <v>418</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="D102" t="s">
         <v>419</v>
       </c>
-      <c r="G101" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>420</v>
       </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+      <c r="G102" t="s">
+        <v>421</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>1.99</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Found U5 on Mouser, added product info to BOM.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="456">
   <si>
     <t>Part</t>
   </si>
@@ -826,9 +826,6 @@
     <t>SOT23-5</t>
   </si>
   <si>
-    <t>NON STOCK</t>
-  </si>
-  <si>
     <t>U11</t>
   </si>
   <si>
@@ -1379,6 +1376,12 @@
   </si>
   <si>
     <t>TXS0102DCTR</t>
+  </si>
+  <si>
+    <t>863-NCP303LSN09T1G</t>
+  </si>
+  <si>
+    <t>NCP303LSN09T1G</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2213,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G85" sqref="E85:G85"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,12 +2262,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2279,10 +2282,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" t="s">
         <v>317</v>
-      </c>
-      <c r="G2" t="s">
-        <v>318</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2296,7 +2299,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J110)</f>
-        <v>189.48300000000003</v>
+        <v>189.93300000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2316,10 +2319,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G3" t="s">
         <v>319</v>
-      </c>
-      <c r="G3" t="s">
-        <v>320</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2349,10 +2352,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>320</v>
+      </c>
+      <c r="G4" t="s">
         <v>321</v>
-      </c>
-      <c r="G4" t="s">
-        <v>322</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2406,10 +2409,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>325</v>
+      </c>
+      <c r="G6" t="s">
         <v>326</v>
-      </c>
-      <c r="G6" t="s">
-        <v>327</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2422,7 +2425,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2466,10 +2469,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G8" t="s">
         <v>328</v>
-      </c>
-      <c r="G8" t="s">
-        <v>329</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2499,10 +2502,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>329</v>
+      </c>
+      <c r="G9" t="s">
         <v>330</v>
-      </c>
-      <c r="G9" t="s">
-        <v>331</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2532,10 +2535,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>341</v>
+      </c>
+      <c r="G10" t="s">
         <v>342</v>
-      </c>
-      <c r="G10" t="s">
-        <v>343</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2548,7 +2551,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2601,10 +2604,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>343</v>
+      </c>
+      <c r="G12" t="s">
         <v>344</v>
-      </c>
-      <c r="G12" t="s">
-        <v>345</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2634,10 +2637,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>341</v>
+      </c>
+      <c r="G13" t="s">
         <v>342</v>
-      </c>
-      <c r="G13" t="s">
-        <v>343</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2650,7 +2653,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2670,10 +2673,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>347</v>
+      </c>
+      <c r="G14" t="s">
         <v>348</v>
-      </c>
-      <c r="G14" t="s">
-        <v>349</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2686,7 +2689,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2730,10 +2733,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>331</v>
+      </c>
+      <c r="G16" t="s">
         <v>332</v>
-      </c>
-      <c r="G16" t="s">
-        <v>333</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2811,10 +2814,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>333</v>
+      </c>
+      <c r="G19" t="s">
         <v>334</v>
-      </c>
-      <c r="G19" t="s">
-        <v>335</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2827,7 +2830,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2847,10 +2850,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>336</v>
+      </c>
+      <c r="G20" t="s">
         <v>337</v>
-      </c>
-      <c r="G20" t="s">
-        <v>338</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2904,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>338</v>
+      </c>
+      <c r="G22" t="s">
         <v>339</v>
-      </c>
-      <c r="G22" t="s">
-        <v>340</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2922,10 +2925,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" t="s">
         <v>366</v>
-      </c>
-      <c r="B23" t="s">
-        <v>367</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2937,10 +2940,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>367</v>
+      </c>
+      <c r="G23" t="s">
         <v>368</v>
-      </c>
-      <c r="G23" t="s">
-        <v>369</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2955,10 +2958,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>406</v>
+      </c>
+      <c r="B24" t="s">
         <v>407</v>
-      </c>
-      <c r="B24" t="s">
-        <v>408</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2970,10 +2973,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>408</v>
+      </c>
+      <c r="G24" t="s">
         <v>409</v>
-      </c>
-      <c r="G24" t="s">
-        <v>410</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3036,10 +3039,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
+        <v>314</v>
+      </c>
+      <c r="G26" t="s">
         <v>315</v>
-      </c>
-      <c r="G26" t="s">
-        <v>316</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3069,10 +3072,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>356</v>
+      </c>
+      <c r="G27" t="s">
         <v>357</v>
-      </c>
-      <c r="G27" t="s">
-        <v>358</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3085,7 +3088,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3105,10 +3108,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
+        <v>349</v>
+      </c>
+      <c r="G28" t="s">
         <v>350</v>
-      </c>
-      <c r="G28" t="s">
-        <v>351</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3138,10 +3141,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>351</v>
+      </c>
+      <c r="G29" t="s">
         <v>352</v>
-      </c>
-      <c r="G29" t="s">
-        <v>353</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3171,10 +3174,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>353</v>
+      </c>
+      <c r="G30" t="s">
         <v>354</v>
-      </c>
-      <c r="G30" t="s">
-        <v>355</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3187,7 +3190,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3207,10 +3210,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>299</v>
+      </c>
+      <c r="G31" t="s">
         <v>300</v>
-      </c>
-      <c r="G31" t="s">
-        <v>301</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3225,25 +3228,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B32" t="s">
+        <v>390</v>
+      </c>
+      <c r="C32" t="s">
         <v>391</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>392</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>393</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>394</v>
-      </c>
-      <c r="G32" t="s">
-        <v>395</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -3258,25 +3261,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>427</v>
+      </c>
+      <c r="B33" t="s">
+        <v>430</v>
+      </c>
+      <c r="C33" t="s">
+        <v>430</v>
+      </c>
+      <c r="D33" t="s">
+        <v>431</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>428</v>
       </c>
-      <c r="B33" t="s">
-        <v>431</v>
-      </c>
-      <c r="C33" t="s">
-        <v>431</v>
-      </c>
-      <c r="D33" t="s">
-        <v>432</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>429</v>
-      </c>
-      <c r="G33" t="s">
-        <v>430</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3294,22 +3297,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
+        <v>363</v>
+      </c>
+      <c r="G34" t="s">
         <v>364</v>
-      </c>
-      <c r="G34" t="s">
-        <v>365</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3357,7 +3360,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3369,10 +3372,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3387,7 +3390,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3399,10 +3402,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3429,7 +3432,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3453,7 +3456,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3468,10 +3471,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
+        <v>312</v>
+      </c>
+      <c r="G39" t="s">
         <v>313</v>
-      </c>
-      <c r="G39" t="s">
-        <v>314</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -3517,12 +3520,12 @@
         <v>1.26</v>
       </c>
       <c r="L40" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3588,7 +3591,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3603,10 +3606,10 @@
         <v>19</v>
       </c>
       <c r="F43" t="s">
+        <v>379</v>
+      </c>
+      <c r="G43" t="s">
         <v>380</v>
-      </c>
-      <c r="G43" t="s">
-        <v>381</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3621,22 +3624,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C44" t="s">
+        <v>375</v>
+      </c>
+      <c r="D44" t="s">
         <v>376</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>377</v>
       </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>378</v>
-      </c>
-      <c r="G44" t="s">
-        <v>379</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3651,22 +3654,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
+        <v>386</v>
+      </c>
+      <c r="G45" t="s">
         <v>387</v>
-      </c>
-      <c r="G45" t="s">
-        <v>388</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3837,7 +3840,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -3894,7 +3897,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
@@ -3927,7 +3930,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B54" t="s">
         <v>146</v>
@@ -3975,10 +3978,10 @@
         <v>19</v>
       </c>
       <c r="F55" t="s">
+        <v>301</v>
+      </c>
+      <c r="G55" t="s">
         <v>302</v>
-      </c>
-      <c r="G55" t="s">
-        <v>303</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4059,7 +4062,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -4131,7 +4134,7 @@
         <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4140,10 +4143,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
+        <v>304</v>
+      </c>
+      <c r="G60" t="s">
         <v>305</v>
-      </c>
-      <c r="G60" t="s">
-        <v>306</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4164,7 +4167,7 @@
         <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D61" t="s">
         <v>116</v>
@@ -4173,10 +4176,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G61" t="s">
         <v>311</v>
-      </c>
-      <c r="G61" t="s">
-        <v>312</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4239,10 +4242,10 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
+        <v>398</v>
+      </c>
+      <c r="G63" t="s">
         <v>399</v>
-      </c>
-      <c r="G63" t="s">
-        <v>400</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4257,7 +4260,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B64">
         <v>100</v>
@@ -4272,10 +4275,10 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
+        <v>402</v>
+      </c>
+      <c r="G64" t="s">
         <v>403</v>
-      </c>
-      <c r="G64" t="s">
-        <v>404</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4290,7 +4293,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -4719,7 +4722,7 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4728,10 +4731,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
+        <v>306</v>
+      </c>
+      <c r="G78" t="s">
         <v>307</v>
-      </c>
-      <c r="G78" t="s">
-        <v>308</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4752,7 +4755,7 @@
         <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D79" t="s">
         <v>116</v>
@@ -4761,10 +4764,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
+        <v>308</v>
+      </c>
+      <c r="G79" t="s">
         <v>309</v>
-      </c>
-      <c r="G79" t="s">
-        <v>310</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4810,7 +4813,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>233</v>
       </c>
@@ -4843,27 +4846,27 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>445</v>
+      </c>
+      <c r="B82" t="s">
+        <v>443</v>
+      </c>
+      <c r="C82" t="s">
+        <v>443</v>
+      </c>
+      <c r="D82" t="s">
+        <v>444</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>446</v>
       </c>
-      <c r="B82" t="s">
-        <v>444</v>
-      </c>
-      <c r="C82" t="s">
-        <v>444</v>
-      </c>
-      <c r="D82" t="s">
-        <v>445</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>447</v>
-      </c>
-      <c r="G82" t="s">
-        <v>448</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4876,9 +4879,9 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
@@ -4909,9 +4912,9 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B84" t="s">
         <v>241</v>
@@ -4942,7 +4945,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>246</v>
       </c>
@@ -4955,38 +4958,47 @@
       <c r="D85" t="s">
         <v>269</v>
       </c>
+      <c r="E85" t="s">
+        <v>451</v>
+      </c>
+      <c r="F85" t="s">
+        <v>454</v>
+      </c>
+      <c r="G85" t="s">
+        <v>455</v>
+      </c>
       <c r="H85">
         <v>1</v>
+      </c>
+      <c r="I85">
+        <v>0.45</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K85" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>251</v>
       </c>
       <c r="B86" t="s">
+        <v>271</v>
+      </c>
+      <c r="C86" t="s">
+        <v>271</v>
+      </c>
+      <c r="D86" t="s">
         <v>272</v>
       </c>
-      <c r="C86" t="s">
-        <v>272</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>273</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>274</v>
-      </c>
-      <c r="G86" t="s">
-        <v>275</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4999,7 +5011,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>256</v>
       </c>
@@ -5032,7 +5044,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>261</v>
       </c>
@@ -5065,7 +5077,7 @@
         <v>6.63</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>266</v>
       </c>
@@ -5098,7 +5110,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>267</v>
       </c>
@@ -5131,27 +5143,27 @@
         <v>5.88</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B91" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C91" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D91" t="s">
+        <v>450</v>
+      </c>
+      <c r="E91" t="s">
         <v>451</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>452</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>453</v>
-      </c>
-      <c r="G91" t="s">
-        <v>454</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5164,27 +5176,27 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B92" t="s">
+        <v>275</v>
+      </c>
+      <c r="C92" t="s">
+        <v>275</v>
+      </c>
+      <c r="D92" t="s">
         <v>276</v>
       </c>
-      <c r="C92" t="s">
-        <v>276</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>277</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>278</v>
-      </c>
-      <c r="G92" t="s">
-        <v>279</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5197,27 +5209,27 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B93" t="s">
+        <v>280</v>
+      </c>
+      <c r="C93" t="s">
+        <v>280</v>
+      </c>
+      <c r="D93" t="s">
         <v>281</v>
       </c>
-      <c r="C93" t="s">
-        <v>281</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>282</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>283</v>
-      </c>
-      <c r="G93" t="s">
-        <v>284</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5230,27 +5242,27 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B94" t="s">
+        <v>395</v>
+      </c>
+      <c r="C94" t="s">
+        <v>395</v>
+      </c>
+      <c r="D94" t="s">
+        <v>285</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>396</v>
       </c>
-      <c r="C94" t="s">
-        <v>396</v>
-      </c>
-      <c r="D94" t="s">
-        <v>286</v>
-      </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>397</v>
-      </c>
-      <c r="G94" t="s">
-        <v>398</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5263,27 +5275,27 @@
         <v>8.48</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B95" t="s">
+        <v>371</v>
+      </c>
+      <c r="C95" t="s">
+        <v>371</v>
+      </c>
+      <c r="D95" t="s">
+        <v>373</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>372</v>
       </c>
-      <c r="C95" t="s">
-        <v>372</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="G95" t="s">
         <v>374</v>
-      </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
-        <v>373</v>
-      </c>
-      <c r="G95" t="s">
-        <v>375</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -5296,27 +5308,27 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>421</v>
+      </c>
+      <c r="B96" t="s">
         <v>422</v>
       </c>
-      <c r="B96" t="s">
-        <v>423</v>
-      </c>
       <c r="C96" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D96" t="s">
+        <v>432</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>433</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>434</v>
-      </c>
-      <c r="G96" t="s">
-        <v>435</v>
       </c>
       <c r="H96">
         <v>3</v>
@@ -5331,25 +5343,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B97" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D97" t="s">
+        <v>435</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>436</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>437</v>
-      </c>
-      <c r="G97" t="s">
-        <v>438</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -5364,25 +5376,25 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>438</v>
+      </c>
+      <c r="B98" t="s">
         <v>439</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
+        <v>439</v>
+      </c>
+      <c r="D98" t="s">
         <v>440</v>
       </c>
-      <c r="C98" t="s">
-        <v>440</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>441</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>442</v>
-      </c>
-      <c r="G98" t="s">
-        <v>443</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -5397,25 +5409,25 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>286</v>
+      </c>
+      <c r="B99" t="s">
         <v>287</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>287</v>
+      </c>
+      <c r="D99" t="s">
         <v>288</v>
       </c>
-      <c r="C99" t="s">
-        <v>288</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>289</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>290</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>291</v>
-      </c>
-      <c r="G99" t="s">
-        <v>292</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -5430,25 +5442,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>292</v>
+      </c>
+      <c r="B100" t="s">
         <v>293</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
+        <v>293</v>
+      </c>
+      <c r="D100" t="s">
         <v>294</v>
       </c>
-      <c r="C100" t="s">
-        <v>294</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>295</v>
       </c>
-      <c r="E100" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
         <v>296</v>
-      </c>
-      <c r="G100" t="s">
-        <v>297</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -5463,25 +5475,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>410</v>
+      </c>
+      <c r="B101" t="s">
         <v>411</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>412</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
+        <v>412</v>
+      </c>
+      <c r="E101" t="s">
+        <v>289</v>
+      </c>
+      <c r="F101" t="s">
         <v>413</v>
       </c>
-      <c r="D101" t="s">
-        <v>413</v>
-      </c>
-      <c r="E101" t="s">
-        <v>290</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>414</v>
-      </c>
-      <c r="G101" t="s">
-        <v>415</v>
       </c>
       <c r="H101">
         <v>2</v>
@@ -5496,25 +5508,25 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>297</v>
+      </c>
+      <c r="B102" t="s">
         <v>298</v>
       </c>
-      <c r="B102" t="s">
-        <v>299</v>
-      </c>
       <c r="C102" t="s">
+        <v>417</v>
+      </c>
+      <c r="D102" t="s">
         <v>418</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>419</v>
       </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="G102" t="s">
         <v>420</v>
-      </c>
-      <c r="G102" t="s">
-        <v>421</v>
       </c>
       <c r="H102">
         <v>1</v>

</xml_diff>

<commit_message>
Replaced the H-bridge logic translators with the DQS variant.
-The TXB0108DQS is a smaller QFN without the heat slug.
-Sourced from Mouser.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="460">
   <si>
     <t>Part</t>
   </si>
@@ -1382,6 +1382,18 @@
   </si>
   <si>
     <t>NCP303LSN09T1G</t>
+  </si>
+  <si>
+    <t>DQS_R-PUSON-N20</t>
+  </si>
+  <si>
+    <t>U12, U19</t>
+  </si>
+  <si>
+    <t>595-TXB0108DQSR</t>
+  </si>
+  <si>
+    <t>TXB0108DQSR</t>
   </si>
 </sst>
 </file>
@@ -2210,10 +2222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,8 +2310,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J110)</f>
-        <v>189.93300000000002</v>
+        <f>SUM(J2:J111)</f>
+        <v>189.85300000000004</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4584,7 +4596,7 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J102" si="1">H73*I73</f>
+        <f t="shared" ref="J73:J103" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
@@ -4908,7 +4920,7 @@
         <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J91" si="2">H83*I83</f>
+        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
         <v>6.6</v>
       </c>
     </row>
@@ -5178,363 +5190,396 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>457</v>
+      </c>
+      <c r="B92" t="s">
+        <v>422</v>
+      </c>
+      <c r="C92" t="s">
+        <v>422</v>
+      </c>
+      <c r="D92" t="s">
+        <v>456</v>
+      </c>
+      <c r="E92" t="s">
+        <v>451</v>
+      </c>
+      <c r="F92" t="s">
+        <v>458</v>
+      </c>
+      <c r="G92" t="s">
+        <v>459</v>
+      </c>
+      <c r="H92">
+        <v>2</v>
+      </c>
+      <c r="I92">
+        <v>2.76</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="2"/>
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>279</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>275</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>275</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>276</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>277</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" t="s">
         <v>278</v>
       </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>3.79</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>284</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>280</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>280</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>281</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>282</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>283</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>1.57</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>370</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>395</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>395</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>285</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>396</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>397</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>8.48</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>415</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>371</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>371</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>373</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>372</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>374</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>6.84</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>421</v>
-      </c>
-      <c r="B96" t="s">
-        <v>422</v>
-      </c>
-      <c r="C96" t="s">
-        <v>422</v>
-      </c>
-      <c r="D96" t="s">
-        <v>432</v>
-      </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
-        <v>433</v>
-      </c>
-      <c r="G96" t="s">
-        <v>434</v>
-      </c>
-      <c r="H96">
-        <v>3</v>
-      </c>
-      <c r="I96">
-        <v>2.8</v>
-      </c>
-      <c r="J96">
-        <f t="shared" si="1"/>
-        <v>8.3999999999999986</v>
-      </c>
-    </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B97" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C97" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D97" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G97" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>1.33</v>
+        <v>2.8</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>1.33</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>438</v>
+        <v>416</v>
       </c>
       <c r="B98" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="C98" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="D98" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G98" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>1.86</v>
+        <v>1.33</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>438</v>
       </c>
       <c r="B99" t="s">
-        <v>287</v>
+        <v>439</v>
       </c>
       <c r="C99" t="s">
-        <v>287</v>
+        <v>439</v>
       </c>
       <c r="D99" t="s">
-        <v>288</v>
+        <v>440</v>
       </c>
       <c r="E99" t="s">
-        <v>289</v>
+        <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>290</v>
+        <v>441</v>
       </c>
       <c r="G99" t="s">
-        <v>291</v>
+        <v>442</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.5</v>
+        <v>1.86</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B100" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C100" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D100" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E100" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
       <c r="F100" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G100" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100">
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>410</v>
+        <v>292</v>
       </c>
       <c r="B101" t="s">
-        <v>411</v>
+        <v>293</v>
       </c>
       <c r="C101" t="s">
-        <v>412</v>
+        <v>293</v>
       </c>
       <c r="D101" t="s">
-        <v>412</v>
+        <v>294</v>
       </c>
       <c r="E101" t="s">
-        <v>289</v>
+        <v>19</v>
       </c>
       <c r="F101" t="s">
-        <v>413</v>
+        <v>295</v>
       </c>
       <c r="G101" t="s">
-        <v>414</v>
+        <v>296</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I101">
-        <v>0.95</v>
+        <v>2.96</v>
       </c>
       <c r="J101">
         <f t="shared" si="1"/>
-        <v>1.9</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>410</v>
+      </c>
+      <c r="B102" t="s">
+        <v>411</v>
+      </c>
+      <c r="C102" t="s">
+        <v>412</v>
+      </c>
+      <c r="D102" t="s">
+        <v>412</v>
+      </c>
+      <c r="E102" t="s">
+        <v>289</v>
+      </c>
+      <c r="F102" t="s">
+        <v>413</v>
+      </c>
+      <c r="G102" t="s">
+        <v>414</v>
+      </c>
+      <c r="H102">
+        <v>2</v>
+      </c>
+      <c r="I102">
+        <v>0.95</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>297</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>298</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>417</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>418</v>
       </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="E103" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" t="s">
         <v>419</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G103" t="s">
         <v>420</v>
       </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
         <v>1.99</v>
       </c>
-      <c r="J102">
+      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
New Arduino level translator circuit added to schematic.
-Clock buffer IC renamed: U21->U20.
-The new pair of TXB0108 chips are U21 and U22.
-The old translator circuit has NOT been removed yet.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1330,9 +1330,6 @@
     <t>TXS0102YZPR</t>
   </si>
   <si>
-    <t>U21</t>
-  </si>
-  <si>
     <t>NB3N551</t>
   </si>
   <si>
@@ -1387,13 +1384,16 @@
     <t>DQS_R-PUSON-N20</t>
   </si>
   <si>
-    <t>U12, U19</t>
-  </si>
-  <si>
     <t>595-TXB0108DQSR</t>
   </si>
   <si>
     <t>TXB0108DQSR</t>
+  </si>
+  <si>
+    <t>U20</t>
+  </si>
+  <si>
+    <t>U12, U19, U21, U22</t>
   </si>
 </sst>
 </file>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J111)</f>
-        <v>189.85300000000004</v>
+        <v>195.37300000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4860,25 +4860,25 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>444</v>
+      </c>
+      <c r="B82" t="s">
+        <v>442</v>
+      </c>
+      <c r="C82" t="s">
+        <v>442</v>
+      </c>
+      <c r="D82" t="s">
+        <v>443</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>445</v>
       </c>
-      <c r="B82" t="s">
-        <v>443</v>
-      </c>
-      <c r="C82" t="s">
-        <v>443</v>
-      </c>
-      <c r="D82" t="s">
-        <v>444</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>446</v>
-      </c>
-      <c r="G82" t="s">
-        <v>447</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B84" t="s">
         <v>241</v>
@@ -4971,13 +4971,13 @@
         <v>269</v>
       </c>
       <c r="E85" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F85" t="s">
+        <v>453</v>
+      </c>
+      <c r="G85" t="s">
         <v>454</v>
-      </c>
-      <c r="G85" t="s">
-        <v>455</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -5166,16 +5166,16 @@
         <v>423</v>
       </c>
       <c r="D91" t="s">
+        <v>449</v>
+      </c>
+      <c r="E91" t="s">
         <v>450</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>451</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>452</v>
-      </c>
-      <c r="G91" t="s">
-        <v>453</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5190,7 +5190,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B92" t="s">
         <v>422</v>
@@ -5199,26 +5199,26 @@
         <v>422</v>
       </c>
       <c r="D92" t="s">
+        <v>455</v>
+      </c>
+      <c r="E92" t="s">
+        <v>450</v>
+      </c>
+      <c r="F92" t="s">
         <v>456</v>
       </c>
-      <c r="E92" t="s">
-        <v>451</v>
-      </c>
-      <c r="F92" t="s">
-        <v>458</v>
-      </c>
       <c r="G92" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H92">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I92">
         <v>2.76</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>5.52</v>
+        <v>11.04</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -5421,25 +5421,25 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>458</v>
+      </c>
+      <c r="B99" t="s">
         <v>438</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D99" t="s">
         <v>439</v>
       </c>
-      <c r="C99" t="s">
-        <v>439</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>440</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>441</v>
-      </c>
-      <c r="G99" t="s">
-        <v>442</v>
       </c>
       <c r="H99">
         <v>1</v>

</xml_diff>

<commit_message>
Removed the old Arduino logic translation circuit.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="456">
   <si>
     <t>Part</t>
   </si>
@@ -418,21 +418,12 @@
     <t>CHIPLED_0603</t>
   </si>
   <si>
-    <t>DMG1012UW</t>
-  </si>
-  <si>
     <t>MOSFET-NCHANNELSMD</t>
   </si>
   <si>
     <t>SOT23-3</t>
   </si>
   <si>
-    <t>DMG1012UW-7DICT-ND</t>
-  </si>
-  <si>
-    <t>DMG1012UW-7</t>
-  </si>
-  <si>
     <t>Q17, Q25, Q30</t>
   </si>
   <si>
@@ -1286,9 +1277,6 @@
   </si>
   <si>
     <t>TXS0102</t>
-  </si>
-  <si>
-    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q24, Q26, Q27, Q28, Q29</t>
   </si>
   <si>
     <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
@@ -2222,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,12 +2262,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2294,10 +2282,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2310,8 +2298,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J111)</f>
-        <v>195.37300000000002</v>
+        <f>SUM(J2:J110)</f>
+        <v>188.85300000000007</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2331,10 +2319,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2343,13 +2331,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J71" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2364,10 +2352,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2421,10 +2409,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2437,7 +2425,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2481,10 +2469,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2514,10 +2502,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G9" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2547,10 +2535,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G10" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2563,7 +2551,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2616,10 +2604,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2649,10 +2637,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G13" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2665,7 +2653,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2685,10 +2673,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2701,7 +2689,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2745,10 +2733,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G16" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2826,10 +2814,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G19" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2842,7 +2830,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2862,10 +2850,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G20" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2919,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G22" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2937,10 +2925,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B23" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2952,10 +2940,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G23" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2970,10 +2958,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B24" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2985,10 +2973,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G24" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3051,10 +3039,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G26" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3084,10 +3072,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G27" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3100,7 +3088,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3120,10 +3108,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G28" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3153,10 +3141,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G29" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3186,10 +3174,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G30" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3202,7 +3190,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3222,10 +3210,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G31" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3240,25 +3228,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B32" t="s">
+        <v>387</v>
+      </c>
+      <c r="C32" t="s">
+        <v>388</v>
+      </c>
+      <c r="D32" t="s">
+        <v>389</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>390</v>
       </c>
-      <c r="C32" t="s">
+      <c r="G32" t="s">
         <v>391</v>
-      </c>
-      <c r="D32" t="s">
-        <v>392</v>
-      </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
-        <v>393</v>
-      </c>
-      <c r="G32" t="s">
-        <v>394</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -3273,25 +3261,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>423</v>
+      </c>
+      <c r="B33" t="s">
+        <v>426</v>
+      </c>
+      <c r="C33" t="s">
+        <v>426</v>
+      </c>
+      <c r="D33" t="s">
         <v>427</v>
       </c>
-      <c r="B33" t="s">
-        <v>430</v>
-      </c>
-      <c r="C33" t="s">
-        <v>430</v>
-      </c>
-      <c r="D33" t="s">
-        <v>431</v>
-      </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G33" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3309,22 +3297,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C34" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D34" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G34" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3372,7 +3360,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3384,10 +3372,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F36" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3402,7 +3390,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3414,10 +3402,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F37" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3444,7 +3432,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3468,7 +3456,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3483,10 +3471,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G39" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -3532,12 +3520,12 @@
         <v>1.26</v>
       </c>
       <c r="L40" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
@@ -3603,7 +3591,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
@@ -3618,10 +3606,10 @@
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G43" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -3636,22 +3624,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C44" t="s">
+        <v>372</v>
+      </c>
+      <c r="D44" t="s">
+        <v>373</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>374</v>
+      </c>
+      <c r="G44" t="s">
         <v>375</v>
-      </c>
-      <c r="D44" t="s">
-        <v>376</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>377</v>
-      </c>
-      <c r="G44" t="s">
-        <v>378</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3666,22 +3654,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
       <c r="D45" t="s">
+        <v>381</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>383</v>
+      </c>
+      <c r="G45" t="s">
         <v>384</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>386</v>
-      </c>
-      <c r="G45" t="s">
-        <v>387</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3852,172 +3840,172 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>424</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
-      </c>
-      <c r="E51" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G51" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="H51">
-        <v>18</v>
-      </c>
-      <c r="I51">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>5.3999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>385</v>
       </c>
       <c r="B52" t="s">
         <v>140</v>
       </c>
       <c r="C52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
         <v>141</v>
       </c>
-      <c r="D52" t="s">
+      <c r="G52" t="s">
         <v>142</v>
       </c>
-      <c r="G52" t="s">
-        <v>14</v>
-      </c>
       <c r="H52">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0.41</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
       </c>
       <c r="C53" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" t="s">
         <v>135</v>
       </c>
-      <c r="D53" t="s">
-        <v>136</v>
-      </c>
       <c r="E53" t="s">
         <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G53" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>389</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C54" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>148</v>
+        <v>298</v>
       </c>
       <c r="G54" t="s">
-        <v>149</v>
+        <v>299</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" t="s">
         <v>150</v>
       </c>
-      <c r="B55" t="s">
-        <v>151</v>
-      </c>
-      <c r="C55" t="s">
-        <v>152</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" t="s">
         <v>153</v>
       </c>
-      <c r="E55" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" t="s">
-        <v>301</v>
-      </c>
       <c r="G55" t="s">
-        <v>302</v>
+        <v>154</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>154</v>
-      </c>
-      <c r="B56" t="s">
         <v>155</v>
       </c>
+      <c r="B56">
+        <v>470</v>
+      </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E56" t="s">
         <v>19</v>
@@ -4041,16 +4029,16 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>421</v>
+      </c>
+      <c r="B57" t="s">
         <v>158</v>
       </c>
-      <c r="B57">
-        <v>470</v>
-      </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E57" t="s">
         <v>19</v>
@@ -4062,91 +4050,91 @@
         <v>160</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I57">
         <v>0.04</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>425</v>
+        <v>161</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G58" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H58">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>300</v>
       </c>
       <c r="D59" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>166</v>
+        <v>301</v>
       </c>
       <c r="G59" t="s">
-        <v>167</v>
+        <v>302</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I59">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>167</v>
+      </c>
+      <c r="B60" t="s">
         <v>168</v>
       </c>
-      <c r="B60" t="s">
-        <v>169</v>
-      </c>
       <c r="C60" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D60" t="s">
         <v>116</v>
@@ -4155,10 +4143,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G60" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4173,322 +4161,322 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" t="s">
         <v>170</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" t="s">
+        <v>150</v>
+      </c>
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" t="s">
         <v>171</v>
       </c>
-      <c r="C61" t="s">
-        <v>303</v>
-      </c>
-      <c r="D61" t="s">
-        <v>116</v>
-      </c>
-      <c r="E61" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" t="s">
-        <v>310</v>
-      </c>
       <c r="G61" t="s">
-        <v>311</v>
+        <v>172</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>172</v>
-      </c>
-      <c r="B62" t="s">
         <v>173</v>
       </c>
+      <c r="B62">
+        <v>200</v>
+      </c>
       <c r="C62" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="D62" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>174</v>
+        <v>395</v>
       </c>
       <c r="G62" t="s">
-        <v>175</v>
+        <v>396</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I62">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>176</v>
+        <v>397</v>
       </c>
       <c r="B63">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G63" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H63">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>204</v>
+        <v>149</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>402</v>
+        <v>174</v>
       </c>
       <c r="G64" t="s">
-        <v>403</v>
+        <v>175</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>401</v>
-      </c>
-      <c r="B65">
-        <v>100</v>
+        <v>176</v>
+      </c>
+      <c r="B65" t="s">
+        <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D65" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G65" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B66" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G66" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H66">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D67" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G67" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H67">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B68" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D68" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G68" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B69" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G69" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H69">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B70" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D70" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G70" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4503,91 +4491,91 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>199</v>
-      </c>
-      <c r="B71" t="s">
         <v>200</v>
       </c>
+      <c r="B71">
+        <v>0.3</v>
+      </c>
       <c r="C71" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G71" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H71">
         <v>1</v>
       </c>
       <c r="I71">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>203</v>
-      </c>
-      <c r="B72">
-        <v>0.3</v>
+        <v>205</v>
+      </c>
+      <c r="B72" t="s">
+        <v>206</v>
       </c>
       <c r="C72" t="s">
-        <v>204</v>
+        <v>149</v>
       </c>
       <c r="D72" t="s">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G72" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J72">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" ref="J72:J102" si="1">H72*I72</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B73" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G73" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4596,31 +4584,31 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J103" si="1">H73*I73</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B74" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C74" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D74" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G74" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4635,106 +4623,106 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B75" t="s">
-        <v>217</v>
+        <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D75" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
       </c>
-      <c r="F75" t="s">
-        <v>218</v>
-      </c>
       <c r="G75" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" t="s">
+        <v>149</v>
+      </c>
+      <c r="D76" t="s">
+        <v>150</v>
+      </c>
+      <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
         <v>220</v>
       </c>
-      <c r="B76" t="s">
-        <v>14</v>
-      </c>
-      <c r="C76" t="s">
-        <v>152</v>
-      </c>
-      <c r="D76" t="s">
-        <v>153</v>
-      </c>
-      <c r="E76" t="s">
-        <v>19</v>
-      </c>
       <c r="G76" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="H76">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0.04</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B77" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C77" t="s">
-        <v>152</v>
+        <v>300</v>
       </c>
       <c r="D77" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>223</v>
+        <v>303</v>
       </c>
       <c r="G77" t="s">
-        <v>224</v>
+        <v>304</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" t="s">
         <v>225</v>
       </c>
-      <c r="B78" t="s">
-        <v>226</v>
-      </c>
       <c r="C78" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D78" t="s">
         <v>116</v>
@@ -4743,10 +4731,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
+        <v>305</v>
+      </c>
+      <c r="G78" t="s">
         <v>306</v>
-      </c>
-      <c r="G78" t="s">
-        <v>307</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4761,58 +4749,58 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>226</v>
+      </c>
+      <c r="B79" t="s">
         <v>227</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" t="s">
+        <v>150</v>
+      </c>
+      <c r="E79" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s">
         <v>228</v>
       </c>
-      <c r="C79" t="s">
-        <v>303</v>
-      </c>
-      <c r="D79" t="s">
-        <v>116</v>
-      </c>
-      <c r="E79" t="s">
-        <v>19</v>
-      </c>
-      <c r="F79" t="s">
-        <v>308</v>
-      </c>
       <c r="G79" t="s">
-        <v>309</v>
+        <v>229</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B80" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D80" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G80" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4827,139 +4815,139 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>440</v>
       </c>
       <c r="B81" t="s">
-        <v>234</v>
+        <v>438</v>
       </c>
       <c r="C81" t="s">
-        <v>152</v>
+        <v>438</v>
       </c>
       <c r="D81" t="s">
-        <v>153</v>
+        <v>439</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>235</v>
+        <v>441</v>
       </c>
       <c r="G81" t="s">
-        <v>236</v>
+        <v>442</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B82" t="s">
-        <v>442</v>
+        <v>234</v>
       </c>
       <c r="C82" t="s">
-        <v>442</v>
+        <v>234</v>
       </c>
       <c r="D82" t="s">
-        <v>443</v>
+        <v>235</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>445</v>
+        <v>236</v>
       </c>
       <c r="G82" t="s">
-        <v>446</v>
+        <v>237</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J82">
-        <f t="shared" si="1"/>
-        <v>15.1</v>
+        <f t="shared" ref="J82:J91" si="2">H82*I82</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C83" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D83" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G83" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>448</v>
+        <v>243</v>
       </c>
       <c r="B84" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="C84" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
       <c r="D84" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="E84" t="s">
-        <v>19</v>
+        <v>446</v>
       </c>
       <c r="F84" t="s">
-        <v>244</v>
+        <v>449</v>
       </c>
       <c r="G84" t="s">
-        <v>245</v>
+        <v>450</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="J84">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B85" t="s">
         <v>268</v>
@@ -4971,155 +4959,155 @@
         <v>269</v>
       </c>
       <c r="E85" t="s">
-        <v>450</v>
+        <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>453</v>
+        <v>270</v>
       </c>
       <c r="G85" t="s">
-        <v>454</v>
+        <v>271</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B86" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="C86" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="D86" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="G86" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J86">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B87" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C87" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D87" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G87" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B88" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C88" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D88" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G88" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J88">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B89" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C89" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D89" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G89" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -5127,274 +5115,274 @@
         <v>267</v>
       </c>
       <c r="B90" t="s">
-        <v>262</v>
+        <v>420</v>
       </c>
       <c r="C90" t="s">
-        <v>262</v>
+        <v>420</v>
       </c>
       <c r="D90" t="s">
-        <v>263</v>
+        <v>445</v>
       </c>
       <c r="E90" t="s">
-        <v>19</v>
+        <v>446</v>
       </c>
       <c r="F90" t="s">
-        <v>264</v>
+        <v>447</v>
       </c>
       <c r="G90" t="s">
-        <v>265</v>
+        <v>448</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>455</v>
       </c>
       <c r="B91" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C91" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D91" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E91" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F91" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G91" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I91">
-        <v>1.23</v>
+        <v>2.76</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>11.04</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>459</v>
+        <v>276</v>
       </c>
       <c r="B92" t="s">
-        <v>422</v>
+        <v>272</v>
       </c>
       <c r="C92" t="s">
-        <v>422</v>
+        <v>272</v>
       </c>
       <c r="D92" t="s">
-        <v>455</v>
+        <v>273</v>
       </c>
       <c r="E92" t="s">
-        <v>450</v>
+        <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>456</v>
+        <v>274</v>
       </c>
       <c r="G92" t="s">
-        <v>457</v>
+        <v>275</v>
       </c>
       <c r="H92">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I92">
-        <v>2.76</v>
+        <v>3.79</v>
       </c>
       <c r="J92">
-        <f t="shared" si="2"/>
-        <v>11.04</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>281</v>
+      </c>
+      <c r="B93" t="s">
+        <v>277</v>
+      </c>
+      <c r="C93" t="s">
+        <v>277</v>
+      </c>
+      <c r="D93" t="s">
+        <v>278</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>279</v>
       </c>
-      <c r="B93" t="s">
-        <v>275</v>
-      </c>
-      <c r="C93" t="s">
-        <v>275</v>
-      </c>
-      <c r="D93" t="s">
-        <v>276</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
-        <v>277</v>
-      </c>
       <c r="G93" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>284</v>
+        <v>367</v>
       </c>
       <c r="B94" t="s">
-        <v>280</v>
+        <v>392</v>
       </c>
       <c r="C94" t="s">
-        <v>280</v>
+        <v>392</v>
       </c>
       <c r="D94" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>282</v>
+        <v>393</v>
       </c>
       <c r="G94" t="s">
-        <v>283</v>
+        <v>394</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>412</v>
+      </c>
+      <c r="B95" t="s">
+        <v>368</v>
+      </c>
+      <c r="C95" t="s">
+        <v>368</v>
+      </c>
+      <c r="D95" t="s">
         <v>370</v>
       </c>
-      <c r="B95" t="s">
-        <v>395</v>
-      </c>
-      <c r="C95" t="s">
-        <v>395</v>
-      </c>
-      <c r="D95" t="s">
-        <v>285</v>
-      </c>
       <c r="E95" t="s">
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="G95" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B96" t="s">
-        <v>371</v>
+        <v>419</v>
       </c>
       <c r="C96" t="s">
-        <v>371</v>
+        <v>419</v>
       </c>
       <c r="D96" t="s">
-        <v>373</v>
+        <v>428</v>
       </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>372</v>
+        <v>429</v>
       </c>
       <c r="G96" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="I96">
-        <v>6.84</v>
+        <v>2.8</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B97" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C97" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D97" t="s">
+        <v>431</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>432</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>433</v>
       </c>
-      <c r="G97" t="s">
-        <v>434</v>
-      </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>2.8</v>
+        <v>1.33</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>416</v>
+        <v>454</v>
       </c>
       <c r="B98" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="C98" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D98" t="s">
         <v>435</v>
@@ -5412,174 +5400,141 @@
         <v>1</v>
       </c>
       <c r="I98">
-        <v>1.33</v>
+        <v>1.86</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.33</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>458</v>
+        <v>283</v>
       </c>
       <c r="B99" t="s">
-        <v>438</v>
+        <v>284</v>
       </c>
       <c r="C99" t="s">
-        <v>438</v>
+        <v>284</v>
       </c>
       <c r="D99" t="s">
-        <v>439</v>
+        <v>285</v>
       </c>
       <c r="E99" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="F99" t="s">
-        <v>440</v>
+        <v>287</v>
       </c>
       <c r="G99" t="s">
-        <v>441</v>
+        <v>288</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.86</v>
+        <v>1.5</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D100" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E100" t="s">
-        <v>289</v>
+        <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G100" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100">
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>292</v>
+        <v>407</v>
       </c>
       <c r="B101" t="s">
-        <v>293</v>
+        <v>408</v>
       </c>
       <c r="C101" t="s">
-        <v>293</v>
+        <v>409</v>
       </c>
       <c r="D101" t="s">
-        <v>294</v>
+        <v>409</v>
       </c>
       <c r="E101" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="F101" t="s">
-        <v>295</v>
+        <v>410</v>
       </c>
       <c r="G101" t="s">
-        <v>296</v>
+        <v>411</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I101">
-        <v>2.96</v>
+        <v>0.95</v>
       </c>
       <c r="J101">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>410</v>
+        <v>294</v>
       </c>
       <c r="B102" t="s">
-        <v>411</v>
+        <v>295</v>
       </c>
       <c r="C102" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D102" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E102" t="s">
-        <v>289</v>
+        <v>19</v>
       </c>
       <c r="F102" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="G102" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="H102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I102">
-        <v>0.95</v>
+        <v>1.99</v>
       </c>
       <c r="J102">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>297</v>
-      </c>
-      <c r="B103" t="s">
-        <v>298</v>
-      </c>
-      <c r="C103" t="s">
-        <v>417</v>
-      </c>
-      <c r="D103" t="s">
-        <v>418</v>
-      </c>
-      <c r="E103" t="s">
-        <v>19</v>
-      </c>
-      <c r="F103" t="s">
-        <v>419</v>
-      </c>
-      <c r="G103" t="s">
-        <v>420</v>
-      </c>
-      <c r="H103">
-        <v>1</v>
-      </c>
-      <c r="I103">
-        <v>1.99</v>
-      </c>
-      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Added quadrature encoder headers to schematic.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="461">
   <si>
     <t>Part</t>
   </si>
@@ -1382,6 +1382,21 @@
   </si>
   <si>
     <t>U12, U19, U21, U22</t>
+  </si>
+  <si>
+    <t>JP26, JP27, JP28</t>
+  </si>
+  <si>
+    <t>M05PTH (M05)</t>
+  </si>
+  <si>
+    <t>1X05</t>
+  </si>
+  <si>
+    <t>609-4303-ND</t>
+  </si>
+  <si>
+    <t>68002-205HLF</t>
   </si>
 </sst>
 </file>
@@ -2210,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,8 +2313,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J110)</f>
-        <v>188.85300000000007</v>
+        <f>SUM(J2:J111)</f>
+        <v>190.35300000000004</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2331,7 +2346,7 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J71" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
@@ -3684,178 +3699,184 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46" t="s">
-        <v>108</v>
+        <v>456</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>457</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>458</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
+        <v>459</v>
       </c>
       <c r="G46" t="s">
-        <v>112</v>
+        <v>460</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I46">
-        <v>2.13</v>
+        <v>0.5</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G47" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G48" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G49" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="H50">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1.85</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
       </c>
       <c r="H51">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
@@ -3864,46 +3885,37 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>385</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G52" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
         <v>135</v>
@@ -3912,61 +3924,61 @@
         <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G53" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>386</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>298</v>
+        <v>145</v>
       </c>
       <c r="G54" t="s">
-        <v>299</v>
+        <v>146</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
         <v>149</v>
@@ -3978,28 +3990,28 @@
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="G55" t="s">
-        <v>154</v>
+        <v>299</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>155</v>
-      </c>
-      <c r="B56">
-        <v>470</v>
+        <v>151</v>
+      </c>
+      <c r="B56" t="s">
+        <v>152</v>
       </c>
       <c r="C56" t="s">
         <v>149</v>
@@ -4011,10 +4023,10 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G56" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -4029,10 +4041,10 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>421</v>
-      </c>
-      <c r="B57" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="B57">
+        <v>470</v>
       </c>
       <c r="C57" t="s">
         <v>149</v>
@@ -4044,28 +4056,28 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H57">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <v>0.04</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>421</v>
       </c>
       <c r="B58" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C58" t="s">
         <v>149</v>
@@ -4077,61 +4089,61 @@
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G58" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H58">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="D59" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>301</v>
+        <v>163</v>
       </c>
       <c r="G59" t="s">
-        <v>302</v>
+        <v>164</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I59">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B60" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C60" t="s">
         <v>300</v>
@@ -4143,10 +4155,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G60" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4161,76 +4173,76 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B61" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D61" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>171</v>
+        <v>307</v>
       </c>
       <c r="G61" t="s">
-        <v>172</v>
+        <v>308</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>173</v>
-      </c>
-      <c r="B62">
-        <v>200</v>
+        <v>169</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
       </c>
       <c r="C62" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>395</v>
+        <v>171</v>
       </c>
       <c r="G62" t="s">
-        <v>396</v>
+        <v>172</v>
       </c>
       <c r="H62">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>397</v>
+        <v>173</v>
       </c>
       <c r="B63">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C63" t="s">
         <v>201</v>
@@ -4242,61 +4254,61 @@
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G63" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="H63">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I63">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="D64" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>174</v>
+        <v>399</v>
       </c>
       <c r="G64" t="s">
-        <v>175</v>
+        <v>400</v>
       </c>
       <c r="H64">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>176</v>
-      </c>
-      <c r="B65" t="s">
-        <v>177</v>
+        <v>398</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
       </c>
       <c r="C65" t="s">
         <v>149</v>
@@ -4308,28 +4320,28 @@
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G65" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H65">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C66" t="s">
         <v>149</v>
@@ -4341,28 +4353,28 @@
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G66" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H66">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C67" t="s">
         <v>149</v>
@@ -4374,28 +4386,28 @@
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G67" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H67">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B68" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C68" t="s">
         <v>149</v>
@@ -4407,28 +4419,28 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G68" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C69" t="s">
         <v>149</v>
@@ -4440,28 +4452,28 @@
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G69" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B70" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
         <v>149</v>
@@ -4473,10 +4485,10 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G70" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4491,76 +4503,76 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>200</v>
-      </c>
-      <c r="B71">
-        <v>0.3</v>
+        <v>196</v>
+      </c>
+      <c r="B71" t="s">
+        <v>197</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G71" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H71">
         <v>1</v>
       </c>
       <c r="I71">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>205</v>
-      </c>
-      <c r="B72" t="s">
-        <v>206</v>
+        <v>200</v>
+      </c>
+      <c r="B72">
+        <v>0.3</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="D72" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G72" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72:J102" si="1">H72*I72</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
         <v>149</v>
@@ -4572,10 +4584,10 @@
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G73" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4584,16 +4596,16 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J73:J103" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
         <v>149</v>
@@ -4605,10 +4617,10 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G74" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4623,10 +4635,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="C75" t="s">
         <v>149</v>
@@ -4637,23 +4649,29 @@
       <c r="E75" t="s">
         <v>19</v>
       </c>
+      <c r="F75" t="s">
+        <v>215</v>
+      </c>
       <c r="G75" t="s">
-        <v>14</v>
+        <v>216</v>
       </c>
       <c r="H75">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>0.04</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B76" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s">
         <v>149</v>
@@ -4664,62 +4682,56 @@
       <c r="E76" t="s">
         <v>19</v>
       </c>
-      <c r="F76" t="s">
-        <v>220</v>
-      </c>
       <c r="G76" t="s">
-        <v>221</v>
+        <v>14</v>
       </c>
       <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C77" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="D77" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>303</v>
+        <v>220</v>
       </c>
       <c r="G77" t="s">
-        <v>304</v>
+        <v>221</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B78" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C78" t="s">
         <v>300</v>
@@ -4731,10 +4743,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G78" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4749,43 +4761,43 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B79" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D79" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="G79" t="s">
-        <v>229</v>
+        <v>306</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C80" t="s">
         <v>149</v>
@@ -4797,10 +4809,10 @@
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G80" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4815,726 +4827,759 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>440</v>
+        <v>230</v>
       </c>
       <c r="B81" t="s">
-        <v>438</v>
+        <v>231</v>
       </c>
       <c r="C81" t="s">
-        <v>438</v>
+        <v>149</v>
       </c>
       <c r="D81" t="s">
-        <v>439</v>
+        <v>150</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>441</v>
+        <v>232</v>
       </c>
       <c r="G81" t="s">
-        <v>442</v>
+        <v>233</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B82" t="s">
-        <v>234</v>
+        <v>438</v>
       </c>
       <c r="C82" t="s">
-        <v>234</v>
+        <v>438</v>
       </c>
       <c r="D82" t="s">
-        <v>235</v>
+        <v>439</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>236</v>
+        <v>441</v>
       </c>
       <c r="G82" t="s">
-        <v>237</v>
+        <v>442</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J82">
-        <f t="shared" ref="J82:J91" si="2">H82*I82</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>15.1</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>443</v>
+      </c>
+      <c r="B83" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" t="s">
+        <v>234</v>
+      </c>
+      <c r="D83" t="s">
+        <v>235</v>
+      </c>
+      <c r="E83" t="s">
+        <v>19</v>
+      </c>
+      <c r="F83" t="s">
+        <v>236</v>
+      </c>
+      <c r="G83" t="s">
+        <v>237</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>6.6</v>
+      </c>
+      <c r="J83">
+        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>444</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>238</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>239</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>240</v>
       </c>
-      <c r="E83" t="s">
-        <v>19</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
         <v>241</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G84" t="s">
         <v>242</v>
       </c>
-      <c r="H83">
-        <v>1</v>
-      </c>
-      <c r="I83">
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
         <v>0.79</v>
       </c>
-      <c r="J83">
+      <c r="J84">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>243</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>265</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>265</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>266</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" t="s">
         <v>446</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" t="s">
         <v>449</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>450</v>
       </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84">
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
         <v>0.45</v>
       </c>
-      <c r="J84">
+      <c r="J85">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>248</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>268</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>268</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>269</v>
       </c>
-      <c r="E85" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>270</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G86" t="s">
         <v>271</v>
       </c>
-      <c r="H85">
-        <v>1</v>
-      </c>
-      <c r="I85">
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
         <v>0.47</v>
       </c>
-      <c r="J85">
+      <c r="J86">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>253</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>244</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>244</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>245</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>246</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" t="s">
         <v>247</v>
       </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
         <v>0.67</v>
       </c>
-      <c r="J86">
+      <c r="J87">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>258</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>249</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>249</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>250</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>251</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" t="s">
         <v>252</v>
       </c>
-      <c r="H87">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
         <v>6.63</v>
       </c>
-      <c r="J87">
+      <c r="J88">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>263</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>254</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>254</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>255</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>256</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" t="s">
         <v>257</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>1.67</v>
       </c>
-      <c r="J88">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>264</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>259</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>259</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>260</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>261</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" t="s">
         <v>262</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>5.88</v>
       </c>
-      <c r="J89">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>267</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>420</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>420</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>445</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E91" t="s">
         <v>446</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F91" t="s">
         <v>447</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" t="s">
         <v>448</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>1.23</v>
       </c>
-      <c r="J90">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>455</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>419</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>419</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>451</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E92" t="s">
         <v>446</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F92" t="s">
         <v>452</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G92" t="s">
         <v>453</v>
       </c>
-      <c r="H91">
+      <c r="H92">
         <v>4</v>
       </c>
-      <c r="I91">
+      <c r="I92">
         <v>2.76</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>11.04</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>276</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>272</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>272</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>273</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>274</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" t="s">
         <v>275</v>
       </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>3.79</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>281</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>277</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>277</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>278</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>279</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>280</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>1.57</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>367</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>392</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>392</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>282</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>393</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>394</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>8.48</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>412</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>368</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>368</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>370</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>369</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>371</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>6.84</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>418</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>419</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>419</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>428</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>429</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G97" t="s">
         <v>430</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
         <v>2.8</v>
       </c>
-      <c r="J96">
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>413</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>420</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>420</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>431</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>432</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G98" t="s">
         <v>433</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>1.33</v>
       </c>
-      <c r="J97">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>1.33</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>454</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>434</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>434</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>435</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>436</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G99" t="s">
         <v>437</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.86</v>
       </c>
-      <c r="J98">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>283</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>284</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>284</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>285</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>286</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" t="s">
         <v>287</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G100" t="s">
         <v>288</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>1.5</v>
       </c>
-      <c r="J99">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>289</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>290</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>290</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>291</v>
       </c>
-      <c r="E100" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>292</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G101" t="s">
         <v>293</v>
       </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
         <v>2.96</v>
       </c>
-      <c r="J100">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>407</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>408</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>409</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>409</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E102" t="s">
         <v>286</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F102" t="s">
         <v>410</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" t="s">
         <v>411</v>
       </c>
-      <c r="H101">
+      <c r="H102">
         <v>2</v>
       </c>
-      <c r="I101">
+      <c r="I102">
         <v>0.95</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>294</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>295</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>414</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>415</v>
       </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="E103" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" t="s">
         <v>416</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G103" t="s">
         <v>417</v>
       </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
         <v>1.99</v>
       </c>
-      <c r="J102">
+      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Removed pins 12 and 16 of the XBee from JP25.
-Pin 12 is CTS, 16 is RTS. These will be connected to an XMOS.
-JP25 has been shortened from 2x6 pins to 2x5.
-The JP25 ends of the remaining 10 JP25 signals have been ripped up,
as it will be moved shortly to make use of extra space from the Arduino move.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="466">
   <si>
     <t>Part</t>
   </si>
@@ -1219,9 +1219,6 @@
     <t>ERJ-2GEJ101X</t>
   </si>
   <si>
-    <t>JP3, JP4, JP5, JP25</t>
-  </si>
-  <si>
     <t>C1, C68</t>
   </si>
   <si>
@@ -1397,6 +1394,24 @@
   </si>
   <si>
     <t>68002-205HLF</t>
+  </si>
+  <si>
+    <t>JP3, JP4, JP5</t>
+  </si>
+  <si>
+    <t>JP25</t>
+  </si>
+  <si>
+    <t>PINHD-2X5</t>
+  </si>
+  <si>
+    <t>2X05 Female</t>
+  </si>
+  <si>
+    <t>609-3573-ND</t>
+  </si>
+  <si>
+    <t>68683-305LF</t>
   </si>
 </sst>
 </file>
@@ -2225,9 +2240,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
@@ -2282,7 +2297,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2313,8 +2328,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J111)</f>
-        <v>190.35300000000004</v>
+        <f>SUM(J2:J112)</f>
+        <v>190.55300000000005</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2346,7 +2361,7 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J73" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
@@ -2973,10 +2988,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>402</v>
+      </c>
+      <c r="B24" t="s">
         <v>403</v>
-      </c>
-      <c r="B24" t="s">
-        <v>404</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2988,10 +3003,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>404</v>
+      </c>
+      <c r="G24" t="s">
         <v>405</v>
-      </c>
-      <c r="G24" t="s">
-        <v>406</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3243,7 +3258,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B32" t="s">
         <v>387</v>
@@ -3276,25 +3291,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>422</v>
+      </c>
+      <c r="B33" t="s">
+        <v>425</v>
+      </c>
+      <c r="C33" t="s">
+        <v>425</v>
+      </c>
+      <c r="D33" t="s">
+        <v>426</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>423</v>
       </c>
-      <c r="B33" t="s">
-        <v>426</v>
-      </c>
-      <c r="C33" t="s">
-        <v>426</v>
-      </c>
-      <c r="D33" t="s">
-        <v>427</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>424</v>
-      </c>
-      <c r="G33" t="s">
-        <v>425</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3471,7 +3486,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>401</v>
+        <v>460</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3492,14 +3507,14 @@
         <v>310</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I39">
         <v>1.47</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>5.88</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -3699,208 +3714,214 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="C46" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="D46" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="G46" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="H46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>0.5</v>
+        <v>1.67</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" t="s">
-        <v>108</v>
+        <v>455</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>456</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
+        <v>457</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>111</v>
+        <v>458</v>
       </c>
       <c r="G47" t="s">
-        <v>112</v>
+        <v>459</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I47">
-        <v>2.13</v>
+        <v>0.5</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G48" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G49" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
         <v>19</v>
       </c>
       <c r="F50" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G50" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>129</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="H51">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1.85</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -3909,46 +3930,37 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>385</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G53" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D54" t="s">
         <v>135</v>
@@ -3957,61 +3969,61 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G54" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>147</v>
+        <v>386</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D55" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>298</v>
+        <v>145</v>
       </c>
       <c r="G55" t="s">
-        <v>299</v>
+        <v>146</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C56" t="s">
         <v>149</v>
@@ -4023,28 +4035,28 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="G56" t="s">
-        <v>154</v>
+        <v>299</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>155</v>
-      </c>
-      <c r="B57">
-        <v>470</v>
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
+        <v>152</v>
       </c>
       <c r="C57" t="s">
         <v>149</v>
@@ -4056,10 +4068,10 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G57" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4074,10 +4086,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>421</v>
-      </c>
-      <c r="B58" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="B58">
+        <v>470</v>
       </c>
       <c r="C58" t="s">
         <v>149</v>
@@ -4089,28 +4101,28 @@
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H58">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>420</v>
       </c>
       <c r="B59" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C59" t="s">
         <v>149</v>
@@ -4122,61 +4134,61 @@
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G59" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="D60" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>301</v>
+        <v>163</v>
       </c>
       <c r="G60" t="s">
-        <v>302</v>
+        <v>164</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I60">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C61" t="s">
         <v>300</v>
@@ -4188,10 +4200,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G61" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4206,76 +4218,76 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D62" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>171</v>
+        <v>307</v>
       </c>
       <c r="G62" t="s">
-        <v>172</v>
+        <v>308</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>173</v>
-      </c>
-      <c r="B63">
-        <v>200</v>
+        <v>169</v>
+      </c>
+      <c r="B63" t="s">
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>395</v>
+        <v>171</v>
       </c>
       <c r="G63" t="s">
-        <v>396</v>
+        <v>172</v>
       </c>
       <c r="H63">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>397</v>
+        <v>173</v>
       </c>
       <c r="B64">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C64" t="s">
         <v>201</v>
@@ -4287,61 +4299,61 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G64" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I64">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="D65" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>174</v>
+        <v>399</v>
       </c>
       <c r="G65" t="s">
-        <v>175</v>
+        <v>400</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>176</v>
-      </c>
-      <c r="B66" t="s">
-        <v>177</v>
+        <v>398</v>
+      </c>
+      <c r="B66">
+        <v>100</v>
       </c>
       <c r="C66" t="s">
         <v>149</v>
@@ -4353,28 +4365,28 @@
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G66" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H66">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C67" t="s">
         <v>149</v>
@@ -4386,28 +4398,28 @@
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G67" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H67">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B68" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C68" t="s">
         <v>149</v>
@@ -4419,28 +4431,28 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G68" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H68">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C69" t="s">
         <v>149</v>
@@ -4452,28 +4464,28 @@
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G69" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B70" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C70" t="s">
         <v>149</v>
@@ -4485,28 +4497,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G70" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B71" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
         <v>149</v>
@@ -4518,10 +4530,10 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G71" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4536,76 +4548,76 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>200</v>
-      </c>
-      <c r="B72">
-        <v>0.3</v>
+        <v>196</v>
+      </c>
+      <c r="B72" t="s">
+        <v>197</v>
       </c>
       <c r="C72" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D72" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G72" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>205</v>
-      </c>
-      <c r="B73" t="s">
-        <v>206</v>
+        <v>200</v>
+      </c>
+      <c r="B73">
+        <v>0.3</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="D73" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G73" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J103" si="1">H73*I73</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C74" t="s">
         <v>149</v>
@@ -4617,10 +4629,10 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G74" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4629,16 +4641,16 @@
         <v>0.04</v>
       </c>
       <c r="J74">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J74:J104" si="1">H74*I74</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C75" t="s">
         <v>149</v>
@@ -4650,10 +4662,10 @@
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G75" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4668,10 +4680,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="C76" t="s">
         <v>149</v>
@@ -4682,23 +4694,29 @@
       <c r="E76" t="s">
         <v>19</v>
       </c>
+      <c r="F76" t="s">
+        <v>215</v>
+      </c>
       <c r="G76" t="s">
-        <v>14</v>
+        <v>216</v>
       </c>
       <c r="H76">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0.04</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
         <v>149</v>
@@ -4709,62 +4727,56 @@
       <c r="E77" t="s">
         <v>19</v>
       </c>
-      <c r="F77" t="s">
-        <v>220</v>
-      </c>
       <c r="G77" t="s">
-        <v>221</v>
+        <v>14</v>
       </c>
       <c r="H77">
-        <v>1</v>
-      </c>
-      <c r="I77">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B78" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C78" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="D78" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>303</v>
+        <v>220</v>
       </c>
       <c r="G78" t="s">
-        <v>304</v>
+        <v>221</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C79" t="s">
         <v>300</v>
@@ -4776,10 +4788,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G79" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4794,43 +4806,43 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C80" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D80" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="G80" t="s">
-        <v>229</v>
+        <v>306</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B81" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C81" t="s">
         <v>149</v>
@@ -4842,10 +4854,10 @@
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G81" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4860,726 +4872,759 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>440</v>
+        <v>230</v>
       </c>
       <c r="B82" t="s">
-        <v>438</v>
+        <v>231</v>
       </c>
       <c r="C82" t="s">
-        <v>438</v>
+        <v>149</v>
       </c>
       <c r="D82" t="s">
-        <v>439</v>
+        <v>150</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>441</v>
+        <v>232</v>
       </c>
       <c r="G82" t="s">
-        <v>442</v>
+        <v>233</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B83" t="s">
-        <v>234</v>
+        <v>437</v>
       </c>
       <c r="C83" t="s">
-        <v>234</v>
+        <v>437</v>
       </c>
       <c r="D83" t="s">
-        <v>235</v>
+        <v>438</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>236</v>
+        <v>440</v>
       </c>
       <c r="G83" t="s">
-        <v>237</v>
+        <v>441</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>15.1</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B84" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" t="s">
+        <v>235</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
+        <v>236</v>
+      </c>
+      <c r="G84" t="s">
+        <v>237</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>6.6</v>
+      </c>
+      <c r="J84">
+        <f t="shared" ref="J84:J93" si="2">H84*I84</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>443</v>
+      </c>
+      <c r="B85" t="s">
         <v>238</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>239</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>240</v>
       </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
         <v>241</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>242</v>
       </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84">
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
         <v>0.79</v>
       </c>
-      <c r="J84">
+      <c r="J85">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>243</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>265</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>265</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>266</v>
       </c>
-      <c r="E85" t="s">
-        <v>446</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E86" t="s">
+        <v>445</v>
+      </c>
+      <c r="F86" t="s">
+        <v>448</v>
+      </c>
+      <c r="G86" t="s">
         <v>449</v>
       </c>
-      <c r="G85" t="s">
-        <v>450</v>
-      </c>
-      <c r="H85">
-        <v>1</v>
-      </c>
-      <c r="I85">
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
         <v>0.45</v>
       </c>
-      <c r="J85">
+      <c r="J86">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>248</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>268</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>268</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>269</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>270</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" t="s">
         <v>271</v>
       </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
         <v>0.47</v>
       </c>
-      <c r="J86">
+      <c r="J87">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>253</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>244</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>244</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>245</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>246</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" t="s">
         <v>247</v>
       </c>
-      <c r="H87">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
         <v>0.67</v>
       </c>
-      <c r="J87">
+      <c r="J88">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>258</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>249</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>249</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>250</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>251</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" t="s">
         <v>252</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>6.63</v>
       </c>
-      <c r="J88">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>263</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>254</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>254</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>255</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>256</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" t="s">
         <v>257</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>1.67</v>
       </c>
-      <c r="J89">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>264</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>259</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>259</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>260</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>261</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" t="s">
         <v>262</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>5.88</v>
       </c>
-      <c r="J90">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>267</v>
       </c>
-      <c r="B91" t="s">
-        <v>420</v>
-      </c>
-      <c r="C91" t="s">
-        <v>420</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="B92" t="s">
+        <v>419</v>
+      </c>
+      <c r="C92" t="s">
+        <v>419</v>
+      </c>
+      <c r="D92" t="s">
+        <v>444</v>
+      </c>
+      <c r="E92" t="s">
         <v>445</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F92" t="s">
         <v>446</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G92" t="s">
         <v>447</v>
       </c>
-      <c r="G91" t="s">
-        <v>448</v>
-      </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>1.23</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>455</v>
-      </c>
-      <c r="B92" t="s">
-        <v>419</v>
-      </c>
-      <c r="C92" t="s">
-        <v>419</v>
-      </c>
-      <c r="D92" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>454</v>
+      </c>
+      <c r="B93" t="s">
+        <v>418</v>
+      </c>
+      <c r="C93" t="s">
+        <v>418</v>
+      </c>
+      <c r="D93" t="s">
+        <v>450</v>
+      </c>
+      <c r="E93" t="s">
+        <v>445</v>
+      </c>
+      <c r="F93" t="s">
         <v>451</v>
       </c>
-      <c r="E92" t="s">
-        <v>446</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G93" t="s">
         <v>452</v>
       </c>
-      <c r="G92" t="s">
-        <v>453</v>
-      </c>
-      <c r="H92">
+      <c r="H93">
         <v>4</v>
       </c>
-      <c r="I92">
+      <c r="I93">
         <v>2.76</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="2"/>
         <v>11.04</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>276</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>272</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>272</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>273</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>274</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>275</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>3.79</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>281</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>277</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>277</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>278</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>279</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>280</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>1.57</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>367</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>392</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>392</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>282</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>393</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>394</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>8.48</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>412</v>
-      </c>
-      <c r="B96" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>411</v>
+      </c>
+      <c r="B97" t="s">
         <v>368</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>368</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>370</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>369</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G97" t="s">
         <v>371</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
         <v>6.84</v>
       </c>
-      <c r="J96">
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>417</v>
+      </c>
+      <c r="B98" t="s">
         <v>418</v>
       </c>
-      <c r="B97" t="s">
-        <v>419</v>
-      </c>
-      <c r="C97" t="s">
-        <v>419</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C98" t="s">
+        <v>418</v>
+      </c>
+      <c r="D98" t="s">
+        <v>427</v>
+      </c>
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>428</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G98" t="s">
         <v>429</v>
       </c>
-      <c r="G97" t="s">
-        <v>430</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>2.8</v>
       </c>
-      <c r="J97">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>413</v>
-      </c>
-      <c r="B98" t="s">
-        <v>420</v>
-      </c>
-      <c r="C98" t="s">
-        <v>420</v>
-      </c>
-      <c r="D98" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>412</v>
+      </c>
+      <c r="B99" t="s">
+        <v>419</v>
+      </c>
+      <c r="C99" t="s">
+        <v>419</v>
+      </c>
+      <c r="D99" t="s">
+        <v>430</v>
+      </c>
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>431</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="G99" t="s">
         <v>432</v>
       </c>
-      <c r="G98" t="s">
-        <v>433</v>
-      </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.33</v>
       </c>
-      <c r="J98">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.33</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>454</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>453</v>
+      </c>
+      <c r="B100" t="s">
+        <v>433</v>
+      </c>
+      <c r="C100" t="s">
+        <v>433</v>
+      </c>
+      <c r="D100" t="s">
         <v>434</v>
       </c>
-      <c r="C99" t="s">
-        <v>434</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>435</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="G100" t="s">
         <v>436</v>
       </c>
-      <c r="G99" t="s">
-        <v>437</v>
-      </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>1.86</v>
       </c>
-      <c r="J99">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>283</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>284</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>284</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>285</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E101" t="s">
         <v>286</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F101" t="s">
         <v>287</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G101" t="s">
         <v>288</v>
       </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
         <v>1.5</v>
       </c>
-      <c r="J100">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>289</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>290</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>290</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>291</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>292</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" t="s">
         <v>293</v>
       </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>2.96</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>406</v>
+      </c>
+      <c r="B103" t="s">
         <v>407</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C103" t="s">
         <v>408</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D103" t="s">
+        <v>408</v>
+      </c>
+      <c r="E103" t="s">
+        <v>286</v>
+      </c>
+      <c r="F103" t="s">
         <v>409</v>
       </c>
-      <c r="D102" t="s">
-        <v>409</v>
-      </c>
-      <c r="E102" t="s">
-        <v>286</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="G103" t="s">
         <v>410</v>
       </c>
-      <c r="G102" t="s">
-        <v>411</v>
-      </c>
-      <c r="H102">
+      <c r="H103">
         <v>2</v>
       </c>
-      <c r="I102">
+      <c r="I103">
         <v>0.95</v>
       </c>
-      <c r="J102">
+      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>294</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>295</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
+        <v>413</v>
+      </c>
+      <c r="D104" t="s">
         <v>414</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E104" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" t="s">
         <v>415</v>
       </c>
-      <c r="E103" t="s">
-        <v>19</v>
-      </c>
-      <c r="F103" t="s">
+      <c r="G104" t="s">
         <v>416</v>
       </c>
-      <c r="G103" t="s">
-        <v>417</v>
-      </c>
-      <c r="H103">
-        <v>1</v>
-      </c>
-      <c r="I103">
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
         <v>1.99</v>
       </c>
-      <c r="J103">
+      <c r="J104">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
U20 (XMOS clock) renamed to U23.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1375,9 +1375,6 @@
     <t>TXB0108DQSR</t>
   </si>
   <si>
-    <t>U20</t>
-  </si>
-  <si>
     <t>U12, U19, U21, U22</t>
   </si>
   <si>
@@ -1412,6 +1409,9 @@
   </si>
   <si>
     <t>68683-305LF</t>
+  </si>
+  <si>
+    <t>U23</t>
   </si>
 </sst>
 </file>
@@ -2242,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3714,22 +3714,22 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>460</v>
+      </c>
+      <c r="C46" t="s">
         <v>461</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>462</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
         <v>463</v>
       </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>464</v>
-      </c>
-      <c r="G46" t="s">
-        <v>465</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -3744,22 +3744,22 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>454</v>
+      </c>
+      <c r="C47" t="s">
         <v>455</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>456</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
         <v>457</v>
       </c>
-      <c r="E47" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>458</v>
-      </c>
-      <c r="G47" t="s">
-        <v>459</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -5235,7 +5235,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B93" t="s">
         <v>418</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B100" t="s">
         <v>433</v>

</xml_diff>

<commit_message>
Added another TXB0108 to handle the encoders.
This will likely throw off the current U12 and U19 pin assignments.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1375,9 +1375,6 @@
     <t>TXB0108DQSR</t>
   </si>
   <si>
-    <t>U12, U19, U21, U22</t>
-  </si>
-  <si>
     <t>JP26, JP27, JP28</t>
   </si>
   <si>
@@ -1412,6 +1409,9 @@
   </si>
   <si>
     <t>U23</t>
+  </si>
+  <si>
+    <t>U12, U19, U20, U21, U22</t>
   </si>
 </sst>
 </file>
@@ -2243,7 +2243,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J112)</f>
-        <v>190.55300000000005</v>
+        <v>193.31300000000007</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3714,22 +3714,22 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>459</v>
+      </c>
+      <c r="C46" t="s">
         <v>460</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>461</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
         <v>462</v>
       </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>463</v>
-      </c>
-      <c r="G46" t="s">
-        <v>464</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -3744,22 +3744,22 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>453</v>
+      </c>
+      <c r="C47" t="s">
         <v>454</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>455</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
         <v>456</v>
       </c>
-      <c r="E47" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>457</v>
-      </c>
-      <c r="G47" t="s">
-        <v>458</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -5235,7 +5235,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B93" t="s">
         <v>418</v>
@@ -5256,14 +5256,14 @@
         <v>452</v>
       </c>
       <c r="H93">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I93">
         <v>2.76</v>
       </c>
       <c r="J93">
         <f t="shared" si="2"/>
-        <v>11.04</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -5466,7 +5466,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B100" t="s">
         <v>433</v>

</xml_diff>

<commit_message>
Fixed U1/U2 quantity, it was only listed as one.
That's a very important $15 difference to account for...

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -2242,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J112)</f>
-        <v>193.31300000000007</v>
+        <v>208.41300000000004</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4926,14 +4926,14 @@
         <v>441</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I83">
         <v>15.1</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>15.1</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revised the Gadgeteer level shifter circuit.
-U17 must always be enabled because the Gadgeteer spec calls for
two GPIO pins on a type-I socket. U17_OE tied to +3V3.
-The U17_OE inverter (IC8) has been deleted.
-Two more 74LVC1G3157 mux/demux chips (IC8 and IC9) added
to the B-side of the translator. This isolates the B-side I2C
signals (JP13_8 and JP13_9) between U17 and U18.
-Swapped U17 for the smaller QFN variant used on the rest of the board.
-This block might get one more pass to swap U18 for the QFN variant,
which has a different pinout. This may allow the I2C circuit to be
compacted further.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="457">
   <si>
     <t>Part</t>
   </si>
@@ -1267,9 +1267,6 @@
     <t>ASFL1-20.000MHZ-L-T</t>
   </si>
   <si>
-    <t>U17</t>
-  </si>
-  <si>
     <t>TXB0108</t>
   </si>
   <si>
@@ -1279,33 +1276,6 @@
     <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
   </si>
   <si>
-    <t>IC4, IC5, IC6, IC7</t>
-  </si>
-  <si>
-    <t>IC8</t>
-  </si>
-  <si>
-    <t>568-4822-1-ND</t>
-  </si>
-  <si>
-    <t>74AHC1G04GV,125</t>
-  </si>
-  <si>
-    <t>74AHC1G04DCK</t>
-  </si>
-  <si>
-    <t>SC70-5</t>
-  </si>
-  <si>
-    <t>QFN20_3,5X4,5</t>
-  </si>
-  <si>
-    <t>296-21528-1-ND</t>
-  </si>
-  <si>
-    <t>TXB0108RGYR</t>
-  </si>
-  <si>
     <t>YZP-R-XBGA-N8</t>
   </si>
   <si>
@@ -1411,7 +1381,10 @@
     <t>U23</t>
   </si>
   <si>
-    <t>U12, U19, U20, U21, U22</t>
+    <t>IC4, IC5, IC6, IC7, IC8, IC9</t>
+  </si>
+  <si>
+    <t>U12, U17, U19, U20, U21, U22</t>
   </si>
 </sst>
 </file>
@@ -2240,10 +2213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,8 +2301,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J112)</f>
-        <v>208.41300000000004</v>
+        <f>SUM(J2:J110)</f>
+        <v>208.87300000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2361,7 +2334,7 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J73" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
@@ -3258,7 +3231,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="B32" t="s">
         <v>387</v>
@@ -3279,118 +3252,115 @@
         <v>391</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I32">
         <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>422</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>425</v>
+        <v>361</v>
       </c>
       <c r="C33" t="s">
-        <v>425</v>
+        <v>361</v>
       </c>
       <c r="D33" t="s">
-        <v>426</v>
+        <v>361</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>423</v>
+        <v>360</v>
       </c>
       <c r="G33" t="s">
-        <v>424</v>
+        <v>361</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
-        <v>0.38</v>
+        <v>2.15</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.38</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>361</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>361</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>361</v>
+        <v>85</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>360</v>
+        <v>86</v>
       </c>
       <c r="G34" t="s">
-        <v>361</v>
+        <v>85</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>2.15</v>
+        <v>0.77</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>356</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>0.77</v>
+        <v>0.5</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3405,7 +3375,10 @@
         <v>286</v>
       </c>
       <c r="F36" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="G36" t="s">
+        <v>14</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3420,112 +3393,115 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>355</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>381</v>
       </c>
       <c r="E37" t="s">
-        <v>286</v>
+        <v>19</v>
       </c>
       <c r="F37" t="s">
-        <v>357</v>
+        <v>91</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="I37">
-        <v>0.5</v>
+        <v>0.93</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>448</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>381</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>91</v>
+        <v>309</v>
       </c>
       <c r="G38" t="s">
-        <v>92</v>
+        <v>310</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I38">
-        <v>0.93</v>
+        <v>1.47</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>458</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>309</v>
+        <v>99</v>
       </c>
       <c r="G39" t="s">
-        <v>310</v>
+        <v>100</v>
       </c>
       <c r="H39">
         <v>3</v>
       </c>
       <c r="I39">
-        <v>1.47</v>
+        <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>1.26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>380</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s">
         <v>97</v>
@@ -3540,388 +3516,376 @@
         <v>100</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I40">
         <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L40" t="s">
-        <v>320</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>380</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G41" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H41">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>0.42</v>
+        <v>3.65</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>379</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>103</v>
+        <v>376</v>
       </c>
       <c r="G42" t="s">
-        <v>104</v>
+        <v>377</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>3.65</v>
+        <v>0.13</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>379</v>
-      </c>
-      <c r="B43" t="s">
-        <v>14</v>
+        <v>378</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>372</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>373</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G43" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>0.13</v>
+        <v>0.71</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C44" t="s">
-        <v>372</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="G44" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>382</v>
+        <v>449</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>450</v>
       </c>
       <c r="D45" t="s">
-        <v>381</v>
+        <v>451</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>383</v>
+        <v>452</v>
       </c>
       <c r="G45" t="s">
-        <v>384</v>
+        <v>453</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>3.15</v>
+        <v>1.67</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="C46" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="D46" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="G46" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I46">
-        <v>1.67</v>
+        <v>0.5</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>453</v>
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>454</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>455</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>456</v>
+        <v>111</v>
       </c>
       <c r="G47" t="s">
-        <v>457</v>
+        <v>112</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47">
-        <v>0.5</v>
+        <v>2.13</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G48" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="G49" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
         <v>19</v>
       </c>
       <c r="F50" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>128</v>
-      </c>
-      <c r="E51" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G51" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
-        <v>1.85</v>
+        <v>8</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
       </c>
       <c r="H52">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -3930,37 +3894,46 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>385</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>135</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>141</v>
       </c>
       <c r="G53" t="s">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0.41</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
         <v>135</v>
@@ -3969,61 +3942,61 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G54" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>386</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>145</v>
+        <v>298</v>
       </c>
       <c r="G55" t="s">
-        <v>146</v>
+        <v>299</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C56" t="s">
         <v>149</v>
@@ -4035,28 +4008,28 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>298</v>
+        <v>153</v>
       </c>
       <c r="G56" t="s">
-        <v>299</v>
+        <v>154</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>151</v>
-      </c>
-      <c r="B57" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="B57">
+        <v>470</v>
       </c>
       <c r="C57" t="s">
         <v>149</v>
@@ -4068,10 +4041,10 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4086,10 +4059,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>155</v>
-      </c>
-      <c r="B58">
-        <v>470</v>
+        <v>419</v>
+      </c>
+      <c r="B58" t="s">
+        <v>158</v>
       </c>
       <c r="C58" t="s">
         <v>149</v>
@@ -4101,28 +4074,28 @@
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G58" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>420</v>
+        <v>161</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
         <v>149</v>
@@ -4134,61 +4107,61 @@
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G59" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H59">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B60" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C60" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D60" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>163</v>
+        <v>301</v>
       </c>
       <c r="G60" t="s">
-        <v>164</v>
+        <v>302</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I60">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B61" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
         <v>300</v>
@@ -4200,10 +4173,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="G61" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4218,76 +4191,76 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C62" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>307</v>
+        <v>171</v>
       </c>
       <c r="G62" t="s">
-        <v>308</v>
+        <v>172</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>169</v>
-      </c>
-      <c r="B63" t="s">
-        <v>170</v>
+        <v>173</v>
+      </c>
+      <c r="B63">
+        <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="D63" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>171</v>
+        <v>395</v>
       </c>
       <c r="G63" t="s">
-        <v>172</v>
+        <v>396</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I63">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>173</v>
+        <v>397</v>
       </c>
       <c r="B64">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
         <v>201</v>
@@ -4299,61 +4272,61 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="G64" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="H64">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I64">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D65" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>399</v>
+        <v>174</v>
       </c>
       <c r="G65" t="s">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>398</v>
-      </c>
-      <c r="B66">
-        <v>100</v>
+        <v>176</v>
+      </c>
+      <c r="B66" t="s">
+        <v>177</v>
       </c>
       <c r="C66" t="s">
         <v>149</v>
@@ -4365,28 +4338,28 @@
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G66" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H66">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C67" t="s">
         <v>149</v>
@@ -4398,28 +4371,28 @@
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="G67" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H67">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B68" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C68" t="s">
         <v>149</v>
@@ -4431,28 +4404,28 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G68" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B69" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C69" t="s">
         <v>149</v>
@@ -4464,28 +4437,28 @@
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G69" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B70" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
         <v>149</v>
@@ -4497,28 +4470,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G70" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B71" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C71" t="s">
         <v>149</v>
@@ -4530,10 +4503,10 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G71" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4548,76 +4521,76 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>196</v>
-      </c>
-      <c r="B72" t="s">
-        <v>197</v>
+        <v>200</v>
+      </c>
+      <c r="B72">
+        <v>0.3</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="D72" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="G72" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>200</v>
-      </c>
-      <c r="B73">
-        <v>0.3</v>
+        <v>205</v>
+      </c>
+      <c r="B73" t="s">
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G73" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" ref="J73:J102" si="1">H73*I73</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
         <v>149</v>
@@ -4629,10 +4602,10 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G74" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4641,16 +4614,16 @@
         <v>0.04</v>
       </c>
       <c r="J74">
-        <f t="shared" ref="J74:J104" si="1">H74*I74</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B75" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C75" t="s">
         <v>149</v>
@@ -4662,10 +4635,10 @@
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="G75" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4680,10 +4653,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B76" t="s">
-        <v>214</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s">
         <v>149</v>
@@ -4694,29 +4667,23 @@
       <c r="E76" t="s">
         <v>19</v>
       </c>
-      <c r="F76" t="s">
-        <v>215</v>
-      </c>
       <c r="G76" t="s">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>219</v>
       </c>
       <c r="C77" t="s">
         <v>149</v>
@@ -4727,56 +4694,62 @@
       <c r="E77" t="s">
         <v>19</v>
       </c>
+      <c r="F77" t="s">
+        <v>220</v>
+      </c>
       <c r="G77" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="H77">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>0.04</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="D78" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>220</v>
+        <v>303</v>
       </c>
       <c r="G78" t="s">
-        <v>221</v>
+        <v>304</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B79" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C79" t="s">
         <v>300</v>
@@ -4788,10 +4761,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="G79" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4806,43 +4779,43 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C80" t="s">
-        <v>300</v>
+        <v>149</v>
       </c>
       <c r="D80" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>305</v>
+        <v>228</v>
       </c>
       <c r="G80" t="s">
-        <v>306</v>
+        <v>229</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C81" t="s">
         <v>149</v>
@@ -4854,10 +4827,10 @@
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G81" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4872,759 +4845,693 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>230</v>
+        <v>429</v>
       </c>
       <c r="B82" t="s">
-        <v>231</v>
+        <v>427</v>
       </c>
       <c r="C82" t="s">
-        <v>149</v>
+        <v>427</v>
       </c>
       <c r="D82" t="s">
-        <v>150</v>
+        <v>428</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>232</v>
+        <v>430</v>
       </c>
       <c r="G82" t="s">
-        <v>233</v>
+        <v>431</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82">
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B83" t="s">
-        <v>437</v>
+        <v>234</v>
       </c>
       <c r="C83" t="s">
-        <v>437</v>
+        <v>234</v>
       </c>
       <c r="D83" t="s">
-        <v>438</v>
+        <v>235</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>440</v>
+        <v>236</v>
       </c>
       <c r="G83" t="s">
-        <v>441</v>
+        <v>237</v>
       </c>
       <c r="H83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I83">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
-        <v>30.2</v>
+        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="B84" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C84" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D84" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="G84" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J84">
-        <f t="shared" ref="J84:J93" si="2">H84*I84</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>443</v>
+        <v>243</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="C85" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="D85" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="E85" t="s">
-        <v>19</v>
+        <v>435</v>
       </c>
       <c r="F85" t="s">
-        <v>241</v>
+        <v>438</v>
       </c>
       <c r="G85" t="s">
-        <v>242</v>
+        <v>439</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B86" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C86" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D86" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E86" t="s">
-        <v>445</v>
+        <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>448</v>
+        <v>270</v>
       </c>
       <c r="G86" t="s">
-        <v>449</v>
+        <v>271</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="J86">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B87" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="C87" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D87" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="G87" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C88" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D88" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G88" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J88">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B89" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C89" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="D89" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G89" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B90" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="D90" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G90" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B91" t="s">
-        <v>259</v>
+        <v>418</v>
       </c>
       <c r="C91" t="s">
-        <v>259</v>
+        <v>418</v>
       </c>
       <c r="D91" t="s">
-        <v>260</v>
+        <v>434</v>
       </c>
       <c r="E91" t="s">
-        <v>19</v>
+        <v>435</v>
       </c>
       <c r="F91" t="s">
-        <v>261</v>
+        <v>436</v>
       </c>
       <c r="G91" t="s">
-        <v>262</v>
+        <v>437</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>456</v>
       </c>
       <c r="B92" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C92" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D92" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E92" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="F92" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G92" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I92">
-        <v>1.23</v>
+        <v>2.76</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>16.559999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>465</v>
+        <v>276</v>
       </c>
       <c r="B93" t="s">
-        <v>418</v>
+        <v>272</v>
       </c>
       <c r="C93" t="s">
-        <v>418</v>
+        <v>272</v>
       </c>
       <c r="D93" t="s">
-        <v>450</v>
+        <v>273</v>
       </c>
       <c r="E93" t="s">
-        <v>445</v>
+        <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>451</v>
+        <v>274</v>
       </c>
       <c r="G93" t="s">
-        <v>452</v>
+        <v>275</v>
       </c>
       <c r="H93">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I93">
-        <v>2.76</v>
+        <v>3.79</v>
       </c>
       <c r="J93">
-        <f t="shared" si="2"/>
-        <v>13.799999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B94" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C94" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D94" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G94" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>281</v>
+        <v>367</v>
       </c>
       <c r="B95" t="s">
-        <v>277</v>
+        <v>392</v>
       </c>
       <c r="C95" t="s">
-        <v>277</v>
+        <v>392</v>
       </c>
       <c r="D95" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>279</v>
+        <v>393</v>
       </c>
       <c r="G95" t="s">
-        <v>280</v>
+        <v>394</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
       <c r="B96" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="C96" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="D96" t="s">
-        <v>282</v>
+        <v>370</v>
       </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="G96" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="I96">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B97" t="s">
-        <v>368</v>
+        <v>418</v>
       </c>
       <c r="C97" t="s">
-        <v>368</v>
+        <v>418</v>
       </c>
       <c r="D97" t="s">
-        <v>370</v>
+        <v>420</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="G97" t="s">
-        <v>371</v>
+        <v>422</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>6.84</v>
+        <v>1.33</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>417</v>
+        <v>454</v>
       </c>
       <c r="B98" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="C98" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D98" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G98" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>2.8</v>
+        <v>1.86</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>412</v>
+        <v>283</v>
       </c>
       <c r="B99" t="s">
-        <v>419</v>
+        <v>284</v>
       </c>
       <c r="C99" t="s">
-        <v>419</v>
+        <v>284</v>
       </c>
       <c r="D99" t="s">
-        <v>430</v>
+        <v>285</v>
       </c>
       <c r="E99" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="F99" t="s">
-        <v>431</v>
+        <v>287</v>
       </c>
       <c r="G99" t="s">
-        <v>432</v>
+        <v>288</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.33</v>
+        <v>1.5</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.33</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>464</v>
+        <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>433</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>433</v>
+        <v>290</v>
       </c>
       <c r="D100" t="s">
-        <v>434</v>
+        <v>291</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>435</v>
+        <v>292</v>
       </c>
       <c r="G100" t="s">
-        <v>436</v>
+        <v>293</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100">
-        <v>1.86</v>
+        <v>2.96</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>283</v>
+        <v>406</v>
       </c>
       <c r="B101" t="s">
-        <v>284</v>
+        <v>407</v>
       </c>
       <c r="C101" t="s">
-        <v>284</v>
+        <v>408</v>
       </c>
       <c r="D101" t="s">
-        <v>285</v>
+        <v>408</v>
       </c>
       <c r="E101" t="s">
         <v>286</v>
       </c>
       <c r="F101" t="s">
-        <v>287</v>
+        <v>409</v>
       </c>
       <c r="G101" t="s">
-        <v>288</v>
+        <v>410</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I101">
-        <v>1.5</v>
+        <v>0.95</v>
       </c>
       <c r="J101">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B102" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C102" t="s">
-        <v>290</v>
+        <v>413</v>
       </c>
       <c r="D102" t="s">
-        <v>291</v>
+        <v>414</v>
       </c>
       <c r="E102" t="s">
         <v>19</v>
       </c>
       <c r="F102" t="s">
-        <v>292</v>
+        <v>415</v>
       </c>
       <c r="G102" t="s">
-        <v>293</v>
+        <v>416</v>
       </c>
       <c r="H102">
         <v>1</v>
       </c>
       <c r="I102">
-        <v>2.96</v>
+        <v>1.99</v>
       </c>
       <c r="J102">
-        <f t="shared" si="1"/>
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>406</v>
-      </c>
-      <c r="B103" t="s">
-        <v>407</v>
-      </c>
-      <c r="C103" t="s">
-        <v>408</v>
-      </c>
-      <c r="D103" t="s">
-        <v>408</v>
-      </c>
-      <c r="E103" t="s">
-        <v>286</v>
-      </c>
-      <c r="F103" t="s">
-        <v>409</v>
-      </c>
-      <c r="G103" t="s">
-        <v>410</v>
-      </c>
-      <c r="H103">
-        <v>2</v>
-      </c>
-      <c r="I103">
-        <v>0.95</v>
-      </c>
-      <c r="J103">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>294</v>
-      </c>
-      <c r="B104" t="s">
-        <v>295</v>
-      </c>
-      <c r="C104" t="s">
-        <v>413</v>
-      </c>
-      <c r="D104" t="s">
-        <v>414</v>
-      </c>
-      <c r="E104" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" t="s">
-        <v>415</v>
-      </c>
-      <c r="G104" t="s">
-        <v>416</v>
-      </c>
-      <c r="H104">
-        <v>1</v>
-      </c>
-      <c r="I104">
-        <v>1.99</v>
-      </c>
-      <c r="J104">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Revised the Gadgeteer circuit for further space savings.
Now using the DQE package variant of the TXS0102 for U18.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1276,15 +1276,6 @@
     <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
   </si>
   <si>
-    <t>YZP-R-XBGA-N8</t>
-  </si>
-  <si>
-    <t>296-21932-1-ND</t>
-  </si>
-  <si>
-    <t>TXS0102YZPR</t>
-  </si>
-  <si>
     <t>NB3N551</t>
   </si>
   <si>
@@ -1385,6 +1376,15 @@
   </si>
   <si>
     <t>U12, U17, U19, U20, U21, U22</t>
+  </si>
+  <si>
+    <t>DQE-R-PX2SON-N8</t>
+  </si>
+  <si>
+    <t>296-28368-1-ND</t>
+  </si>
+  <si>
+    <t>TXS0102DQER</t>
   </si>
 </sst>
 </file>
@@ -2216,7 +2216,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J110)</f>
-        <v>208.87300000000002</v>
+        <v>208.79300000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B32" t="s">
         <v>387</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -3654,22 +3654,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>446</v>
+      </c>
+      <c r="C45" t="s">
+        <v>447</v>
+      </c>
+      <c r="D45" t="s">
+        <v>448</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
         <v>449</v>
       </c>
-      <c r="C45" t="s">
+      <c r="G45" t="s">
         <v>450</v>
-      </c>
-      <c r="D45" t="s">
-        <v>451</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>452</v>
-      </c>
-      <c r="G45" t="s">
-        <v>453</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3684,22 +3684,22 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>440</v>
+      </c>
+      <c r="C46" t="s">
+        <v>441</v>
+      </c>
+      <c r="D46" t="s">
+        <v>442</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
         <v>443</v>
       </c>
-      <c r="C46" t="s">
+      <c r="G46" t="s">
         <v>444</v>
-      </c>
-      <c r="D46" t="s">
-        <v>445</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>446</v>
-      </c>
-      <c r="G46" t="s">
-        <v>447</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -4845,25 +4845,25 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B82" t="s">
+        <v>424</v>
+      </c>
+      <c r="C82" t="s">
+        <v>424</v>
+      </c>
+      <c r="D82" t="s">
+        <v>425</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
         <v>427</v>
       </c>
-      <c r="C82" t="s">
-        <v>427</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="G82" t="s">
         <v>428</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
-        <v>430</v>
-      </c>
-      <c r="G82" t="s">
-        <v>431</v>
       </c>
       <c r="H82">
         <v>2</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B83" t="s">
         <v>234</v>
@@ -4911,7 +4911,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B84" t="s">
         <v>238</v>
@@ -4956,13 +4956,13 @@
         <v>266</v>
       </c>
       <c r="E85" t="s">
+        <v>432</v>
+      </c>
+      <c r="F85" t="s">
         <v>435</v>
       </c>
-      <c r="F85" t="s">
-        <v>438</v>
-      </c>
       <c r="G85" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -5151,16 +5151,16 @@
         <v>418</v>
       </c>
       <c r="D91" t="s">
+        <v>431</v>
+      </c>
+      <c r="E91" t="s">
+        <v>432</v>
+      </c>
+      <c r="F91" t="s">
+        <v>433</v>
+      </c>
+      <c r="G91" t="s">
         <v>434</v>
-      </c>
-      <c r="E91" t="s">
-        <v>435</v>
-      </c>
-      <c r="F91" t="s">
-        <v>436</v>
-      </c>
-      <c r="G91" t="s">
-        <v>437</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5175,7 +5175,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B92" t="s">
         <v>417</v>
@@ -5184,16 +5184,16 @@
         <v>417</v>
       </c>
       <c r="D92" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E92" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F92" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G92" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H92">
         <v>6</v>
@@ -5349,49 +5349,49 @@
         <v>418</v>
       </c>
       <c r="D97" t="s">
-        <v>420</v>
+        <v>454</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="G97" t="s">
-        <v>422</v>
+        <v>456</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>1.33</v>
+        <v>1.25</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>1.33</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B98" t="s">
+        <v>420</v>
+      </c>
+      <c r="C98" t="s">
+        <v>420</v>
+      </c>
+      <c r="D98" t="s">
+        <v>421</v>
+      </c>
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
+        <v>422</v>
+      </c>
+      <c r="G98" t="s">
         <v>423</v>
-      </c>
-      <c r="C98" t="s">
-        <v>423</v>
-      </c>
-      <c r="D98" t="s">
-        <v>424</v>
-      </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
-        <v>425</v>
-      </c>
-      <c r="G98" t="s">
-        <v>426</v>
       </c>
       <c r="H98">
         <v>1</v>

</xml_diff>

<commit_message>
Gadgeteer I2C mode is now controlled by a SPDT switch, S1.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="461">
   <si>
     <t>Part</t>
   </si>
@@ -1385,6 +1385,18 @@
   </si>
   <si>
     <t>TXS0102DQER</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SWITCH-SPDT</t>
+  </si>
+  <si>
+    <t>679-1854-ND</t>
+  </si>
+  <si>
+    <t>MMS1208</t>
   </si>
 </sst>
 </file>
@@ -2213,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,8 +2313,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J110)</f>
-        <v>208.79300000000001</v>
+        <f>SUM(J2:J111)</f>
+        <v>209.81299999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4581,7 +4593,7 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J102" si="1">H73*I73</f>
+        <f t="shared" ref="J73:J103" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
@@ -4845,693 +4857,723 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>426</v>
-      </c>
-      <c r="B82" t="s">
-        <v>424</v>
+        <v>457</v>
       </c>
       <c r="C82" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="D82" t="s">
-        <v>425</v>
+        <v>458</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c r="G82" t="s">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I82">
-        <v>15.1</v>
+        <v>1.02</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>30.2</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B83" t="s">
-        <v>234</v>
+        <v>424</v>
       </c>
       <c r="C83" t="s">
-        <v>234</v>
+        <v>424</v>
       </c>
       <c r="D83" t="s">
-        <v>235</v>
+        <v>425</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>236</v>
+        <v>427</v>
       </c>
       <c r="G83" t="s">
-        <v>237</v>
+        <v>428</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I83">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>30.2</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>429</v>
+      </c>
+      <c r="B84" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" t="s">
+        <v>235</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
+        <v>236</v>
+      </c>
+      <c r="G84" t="s">
+        <v>237</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>6.6</v>
+      </c>
+      <c r="J84">
+        <f t="shared" ref="J84:J93" si="2">H84*I84</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>430</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>238</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>239</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>240</v>
       </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
         <v>241</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>242</v>
       </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84">
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
         <v>0.79</v>
       </c>
-      <c r="J84">
+      <c r="J85">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>243</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>265</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>265</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>266</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E86" t="s">
         <v>432</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F86" t="s">
         <v>435</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G86" t="s">
         <v>436</v>
       </c>
-      <c r="H85">
-        <v>1</v>
-      </c>
-      <c r="I85">
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
         <v>0.45</v>
       </c>
-      <c r="J85">
+      <c r="J86">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>248</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>268</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>268</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>269</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>270</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" t="s">
         <v>271</v>
       </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
         <v>0.47</v>
       </c>
-      <c r="J86">
+      <c r="J87">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>253</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>244</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>244</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>245</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>246</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" t="s">
         <v>247</v>
       </c>
-      <c r="H87">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
         <v>0.67</v>
       </c>
-      <c r="J87">
+      <c r="J88">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>258</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>249</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>249</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>250</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>251</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" t="s">
         <v>252</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>6.63</v>
       </c>
-      <c r="J88">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>263</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>254</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>254</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>255</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>256</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" t="s">
         <v>257</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>1.67</v>
       </c>
-      <c r="J89">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>264</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>259</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>259</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>260</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>261</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" t="s">
         <v>262</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>5.88</v>
       </c>
-      <c r="J90">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>267</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>418</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>418</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>431</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E92" t="s">
         <v>432</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F92" t="s">
         <v>433</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G92" t="s">
         <v>434</v>
       </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>1.23</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>453</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>417</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>417</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>437</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" t="s">
         <v>432</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F93" t="s">
         <v>438</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" t="s">
         <v>439</v>
       </c>
-      <c r="H92">
+      <c r="H93">
         <v>6</v>
       </c>
-      <c r="I92">
+      <c r="I93">
         <v>2.76</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="2"/>
         <v>16.559999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>276</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>272</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>272</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>273</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>274</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>275</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>3.79</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>281</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>277</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>277</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>278</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>279</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>280</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>1.57</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>367</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>392</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>392</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>282</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>393</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>394</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>8.48</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>411</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>368</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>368</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>370</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>369</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G97" t="s">
         <v>371</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
         <v>6.84</v>
       </c>
-      <c r="J96">
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>412</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>418</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>418</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>454</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>455</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G98" t="s">
         <v>456</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>1.25</v>
       </c>
-      <c r="J97">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>451</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>420</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>420</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>421</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>422</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G99" t="s">
         <v>423</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.86</v>
       </c>
-      <c r="J98">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>283</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>284</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>284</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>285</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>286</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" t="s">
         <v>287</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G100" t="s">
         <v>288</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>1.5</v>
       </c>
-      <c r="J99">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>289</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>290</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>290</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>291</v>
       </c>
-      <c r="E100" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>292</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G101" t="s">
         <v>293</v>
       </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
         <v>2.96</v>
       </c>
-      <c r="J100">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>406</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>407</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>408</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>408</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E102" t="s">
         <v>286</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F102" t="s">
         <v>409</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" t="s">
         <v>410</v>
       </c>
-      <c r="H101">
+      <c r="H102">
         <v>2</v>
       </c>
-      <c r="I101">
+      <c r="I102">
         <v>0.95</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>294</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>295</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>413</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>414</v>
       </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="E103" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" t="s">
         <v>415</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G103" t="s">
         <v>416</v>
       </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
         <v>1.99</v>
       </c>
-      <c r="J102">
+      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Replaced the Gadgeteer block with an Olimex UEXT connector.
The Gadgeteer specification calls for 3.3V-level I/O. However,
all of the I/O pins must be 3.6V tolerant minimum. Thus, the logic
level translation scheme implemented would not have worked correctly.
By contrast, the UEXT is a pure-3.3V specification with no second 5V supply.

-The I2C and UART pins of the UEXT will be their own serial busses, independent
of the I2C bus used for the IMU and the STM32/XBee UARTs.
-The UEXT SPI bus will connect to the existing XMOS SPI bus, only adding another
slave select line.
-Only 5 1-bit ports are required to the Gadgeteer's 7.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="453">
   <si>
     <t>Part</t>
   </si>
@@ -322,15 +322,6 @@
     <t>JP13</t>
   </si>
   <si>
-    <t>SHF-105-01-L-D-SM</t>
-  </si>
-  <si>
-    <t>HF-105-01-L-D-SM-LC-ND</t>
-  </si>
-  <si>
-    <t>HF-105-01-L-D-SM-LC</t>
-  </si>
-  <si>
     <t>M02PTH</t>
   </si>
   <si>
@@ -1252,9 +1243,6 @@
     <t>U16</t>
   </si>
   <si>
-    <t>U18</t>
-  </si>
-  <si>
     <t>ASFL1</t>
   </si>
   <si>
@@ -1372,31 +1360,19 @@
     <t>U23</t>
   </si>
   <si>
-    <t>IC4, IC5, IC6, IC7, IC8, IC9</t>
-  </si>
-  <si>
-    <t>U12, U17, U19, U20, U21, U22</t>
-  </si>
-  <si>
-    <t>DQE-R-PX2SON-N8</t>
-  </si>
-  <si>
-    <t>296-28368-1-ND</t>
-  </si>
-  <si>
-    <t>TXS0102DQER</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>SWITCH-SPDT</t>
-  </si>
-  <si>
-    <t>679-1854-ND</t>
-  </si>
-  <si>
-    <t>MMS1208</t>
+    <t>U12, U19, U20, U21, U22</t>
+  </si>
+  <si>
+    <t>IC4, IC5</t>
+  </si>
+  <si>
+    <t>M05X2SHD</t>
+  </si>
+  <si>
+    <t>2X5-SHROUDED</t>
+  </si>
+  <si>
+    <t>WM3478-ND</t>
   </si>
 </sst>
 </file>
@@ -2225,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,12 +2253,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2297,10 +2273,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2313,8 +2289,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J111)</f>
-        <v>209.81299999999999</v>
+        <f>SUM(J2:J109)</f>
+        <v>201.01300000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2334,10 +2310,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2352,7 +2328,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2367,10 +2343,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G4" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H4">
         <v>33</v>
@@ -2424,10 +2400,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2440,7 +2416,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2484,10 +2460,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2517,10 +2493,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G9" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2550,10 +2526,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G10" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2566,7 +2542,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2619,10 +2595,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G12" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2652,10 +2628,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G13" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2668,7 +2644,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2688,10 +2664,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G14" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2704,7 +2680,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2748,10 +2724,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G16" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2829,10 +2805,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2845,7 +2821,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2865,10 +2841,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G20" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2922,10 +2898,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G22" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2940,10 +2916,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B23" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2955,10 +2931,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2973,10 +2949,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -2988,10 +2964,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G24" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3054,10 +3030,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G26" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3087,10 +3063,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G27" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -3103,7 +3079,7 @@
         <v>0.4</v>
       </c>
       <c r="L27" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3123,10 +3099,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G28" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3156,10 +3132,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G29" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3189,10 +3165,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G30" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3205,7 +3181,7 @@
         <v>2.7</v>
       </c>
       <c r="L30" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3225,10 +3201,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G31" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3243,35 +3219,35 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B32" t="s">
+        <v>384</v>
+      </c>
+      <c r="C32" t="s">
+        <v>385</v>
+      </c>
+      <c r="D32" t="s">
+        <v>386</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>387</v>
       </c>
-      <c r="C32" t="s">
+      <c r="G32" t="s">
         <v>388</v>
       </c>
-      <c r="D32" t="s">
-        <v>389</v>
-      </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
-        <v>390</v>
-      </c>
-      <c r="G32" t="s">
-        <v>391</v>
-      </c>
       <c r="H32">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I32">
         <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>2.64</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3279,22 +3255,22 @@
         <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C33" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D33" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G33" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3342,7 +3318,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B35" t="s">
         <v>87</v>
@@ -3354,10 +3330,10 @@
         <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F35" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -3372,7 +3348,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3384,10 +3360,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F36" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
@@ -3414,7 +3390,7 @@
         <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -3438,7 +3414,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -3453,10 +3429,10 @@
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G38" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -3502,12 +3478,12 @@
         <v>1.26</v>
       </c>
       <c r="L39" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3542,56 +3518,53 @@
       <c r="A41" t="s">
         <v>101</v>
       </c>
-      <c r="B41" t="s">
-        <v>102</v>
-      </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>450</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>451</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>103</v>
-      </c>
-      <c r="G41" t="s">
-        <v>104</v>
+        <v>452</v>
+      </c>
+      <c r="G41">
+        <v>702461004</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41">
-        <v>3.65</v>
+        <v>1.64</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G42" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H42">
         <v>3</v>
@@ -3606,22 +3579,22 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C43" t="s">
+        <v>369</v>
+      </c>
+      <c r="D43" t="s">
+        <v>370</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>371</v>
+      </c>
+      <c r="G43" t="s">
         <v>372</v>
-      </c>
-      <c r="D43" t="s">
-        <v>373</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>374</v>
-      </c>
-      <c r="G43" t="s">
-        <v>375</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3636,22 +3609,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
       </c>
       <c r="D44" t="s">
+        <v>378</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>380</v>
+      </c>
+      <c r="G44" t="s">
         <v>381</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>383</v>
-      </c>
-      <c r="G44" t="s">
-        <v>384</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3666,22 +3639,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>442</v>
+      </c>
+      <c r="C45" t="s">
+        <v>443</v>
+      </c>
+      <c r="D45" t="s">
+        <v>444</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>445</v>
+      </c>
+      <c r="G45" t="s">
         <v>446</v>
-      </c>
-      <c r="C45" t="s">
-        <v>447</v>
-      </c>
-      <c r="D45" t="s">
-        <v>448</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>449</v>
-      </c>
-      <c r="G45" t="s">
-        <v>450</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3696,22 +3669,22 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>436</v>
+      </c>
+      <c r="C46" t="s">
+        <v>437</v>
+      </c>
+      <c r="D46" t="s">
+        <v>438</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>439</v>
+      </c>
+      <c r="G46" t="s">
         <v>440</v>
-      </c>
-      <c r="C46" t="s">
-        <v>441</v>
-      </c>
-      <c r="D46" t="s">
-        <v>442</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>443</v>
-      </c>
-      <c r="G46" t="s">
-        <v>444</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -3726,25 +3699,25 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" t="s">
         <v>107</v>
       </c>
-      <c r="B47" t="s">
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
         <v>108</v>
       </c>
-      <c r="C47" t="s">
+      <c r="G47" t="s">
         <v>109</v>
-      </c>
-      <c r="D47" t="s">
-        <v>110</v>
-      </c>
-      <c r="E47" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" t="s">
-        <v>111</v>
-      </c>
-      <c r="G47" t="s">
-        <v>112</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -3759,25 +3732,25 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" t="s">
         <v>113</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
         <v>114</v>
       </c>
-      <c r="C48" t="s">
+      <c r="G48" t="s">
         <v>115</v>
-      </c>
-      <c r="D48" t="s">
-        <v>116</v>
-      </c>
-      <c r="E48" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" t="s">
-        <v>117</v>
-      </c>
-      <c r="G48" t="s">
-        <v>118</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -3792,25 +3765,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" t="s">
         <v>119</v>
       </c>
-      <c r="B49" t="s">
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
         <v>120</v>
       </c>
-      <c r="C49" t="s">
+      <c r="G49" t="s">
         <v>121</v>
-      </c>
-      <c r="D49" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" t="s">
-        <v>123</v>
-      </c>
-      <c r="G49" t="s">
-        <v>124</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -3825,25 +3798,25 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" t="s">
+        <v>124</v>
+      </c>
+      <c r="D50" t="s">
         <v>125</v>
       </c>
-      <c r="B50" t="s">
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
         <v>126</v>
       </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
         <v>127</v>
-      </c>
-      <c r="D50" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" t="s">
-        <v>130</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -3858,16 +3831,16 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
@@ -3882,16 +3855,16 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" t="s">
         <v>136</v>
-      </c>
-      <c r="B52" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" t="s">
-        <v>139</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
@@ -3906,25 +3879,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E53" t="s">
         <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G53" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3939,25 +3912,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
+        <v>132</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" t="s">
         <v>143</v>
-      </c>
-      <c r="C54" t="s">
-        <v>144</v>
-      </c>
-      <c r="D54" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
-        <v>145</v>
-      </c>
-      <c r="G54" t="s">
-        <v>146</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3972,25 +3945,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" t="s">
         <v>147</v>
       </c>
-      <c r="B55" t="s">
-        <v>148</v>
-      </c>
-      <c r="C55" t="s">
-        <v>149</v>
-      </c>
-      <c r="D55" t="s">
-        <v>150</v>
-      </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G55" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4005,25 +3978,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" t="s">
+        <v>146</v>
+      </c>
+      <c r="D56" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>150</v>
+      </c>
+      <c r="G56" t="s">
         <v>151</v>
-      </c>
-      <c r="B56" t="s">
-        <v>152</v>
-      </c>
-      <c r="C56" t="s">
-        <v>149</v>
-      </c>
-      <c r="D56" t="s">
-        <v>150</v>
-      </c>
-      <c r="E56" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" t="s">
-        <v>153</v>
-      </c>
-      <c r="G56" t="s">
-        <v>154</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -4038,25 +4011,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B57">
         <v>470</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G57" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4071,25 +4044,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H58">
         <v>16</v>
@@ -4104,25 +4077,25 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" t="s">
+        <v>147</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G59" t="s">
         <v>161</v>
-      </c>
-      <c r="B59" t="s">
-        <v>162</v>
-      </c>
-      <c r="C59" t="s">
-        <v>149</v>
-      </c>
-      <c r="D59" t="s">
-        <v>150</v>
-      </c>
-      <c r="E59" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" t="s">
-        <v>163</v>
-      </c>
-      <c r="G59" t="s">
-        <v>164</v>
       </c>
       <c r="H59">
         <v>4</v>
@@ -4137,25 +4110,25 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C60" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D60" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G60" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4170,25 +4143,25 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C61" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D61" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G61" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4203,25 +4176,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" t="s">
+        <v>167</v>
+      </c>
+      <c r="C62" t="s">
+        <v>146</v>
+      </c>
+      <c r="D62" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
+        <v>168</v>
+      </c>
+      <c r="G62" t="s">
         <v>169</v>
-      </c>
-      <c r="B62" t="s">
-        <v>170</v>
-      </c>
-      <c r="C62" t="s">
-        <v>149</v>
-      </c>
-      <c r="D62" t="s">
-        <v>150</v>
-      </c>
-      <c r="E62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
-        <v>171</v>
-      </c>
-      <c r="G62" t="s">
-        <v>172</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -4236,25 +4209,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B63">
         <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G63" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4269,25 +4242,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D64" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G64" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4302,25 +4275,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D65" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G65" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H65">
         <v>6</v>
@@ -4335,25 +4308,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" t="s">
+        <v>147</v>
+      </c>
+      <c r="E66" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" t="s">
         <v>176</v>
-      </c>
-      <c r="B66" t="s">
-        <v>177</v>
-      </c>
-      <c r="C66" t="s">
-        <v>149</v>
-      </c>
-      <c r="D66" t="s">
-        <v>150</v>
-      </c>
-      <c r="E66" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" t="s">
-        <v>178</v>
-      </c>
-      <c r="G66" t="s">
-        <v>179</v>
       </c>
       <c r="H66">
         <v>15</v>
@@ -4368,25 +4341,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>177</v>
+      </c>
+      <c r="B67" t="s">
+        <v>178</v>
+      </c>
+      <c r="C67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" t="s">
+        <v>179</v>
+      </c>
+      <c r="G67" t="s">
         <v>180</v>
-      </c>
-      <c r="B67" t="s">
-        <v>181</v>
-      </c>
-      <c r="C67" t="s">
-        <v>149</v>
-      </c>
-      <c r="D67" t="s">
-        <v>150</v>
-      </c>
-      <c r="E67" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" t="s">
-        <v>182</v>
-      </c>
-      <c r="G67" t="s">
-        <v>183</v>
       </c>
       <c r="H67">
         <v>6</v>
@@ -4401,25 +4374,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" t="s">
+        <v>147</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" t="s">
+        <v>183</v>
+      </c>
+      <c r="G68" t="s">
         <v>184</v>
-      </c>
-      <c r="B68" t="s">
-        <v>185</v>
-      </c>
-      <c r="C68" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" t="s">
-        <v>150</v>
-      </c>
-      <c r="E68" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" t="s">
-        <v>186</v>
-      </c>
-      <c r="G68" t="s">
-        <v>187</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -4434,25 +4407,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>185</v>
+      </c>
+      <c r="B69" t="s">
+        <v>186</v>
+      </c>
+      <c r="C69" t="s">
+        <v>146</v>
+      </c>
+      <c r="D69" t="s">
+        <v>147</v>
+      </c>
+      <c r="E69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" t="s">
+        <v>187</v>
+      </c>
+      <c r="G69" t="s">
         <v>188</v>
-      </c>
-      <c r="B69" t="s">
-        <v>189</v>
-      </c>
-      <c r="C69" t="s">
-        <v>149</v>
-      </c>
-      <c r="D69" t="s">
-        <v>150</v>
-      </c>
-      <c r="E69" t="s">
-        <v>19</v>
-      </c>
-      <c r="F69" t="s">
-        <v>190</v>
-      </c>
-      <c r="G69" t="s">
-        <v>191</v>
       </c>
       <c r="H69">
         <v>4</v>
@@ -4467,25 +4440,25 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" t="s">
+        <v>146</v>
+      </c>
+      <c r="D70" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" t="s">
+        <v>191</v>
+      </c>
+      <c r="G70" t="s">
         <v>192</v>
-      </c>
-      <c r="B70" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" t="s">
-        <v>149</v>
-      </c>
-      <c r="D70" t="s">
-        <v>150</v>
-      </c>
-      <c r="E70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F70" t="s">
-        <v>194</v>
-      </c>
-      <c r="G70" t="s">
-        <v>195</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4500,25 +4473,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>193</v>
+      </c>
+      <c r="B71" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" t="s">
+        <v>146</v>
+      </c>
+      <c r="D71" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" t="s">
+        <v>195</v>
+      </c>
+      <c r="G71" t="s">
         <v>196</v>
-      </c>
-      <c r="B71" t="s">
-        <v>197</v>
-      </c>
-      <c r="C71" t="s">
-        <v>149</v>
-      </c>
-      <c r="D71" t="s">
-        <v>150</v>
-      </c>
-      <c r="E71" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" t="s">
-        <v>198</v>
-      </c>
-      <c r="G71" t="s">
-        <v>199</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4533,25 +4506,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B72">
         <v>0.3</v>
       </c>
       <c r="C72" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" t="s">
+        <v>199</v>
+      </c>
+      <c r="E72" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" t="s">
+        <v>200</v>
+      </c>
+      <c r="G72" t="s">
         <v>201</v>
-      </c>
-      <c r="D72" t="s">
-        <v>202</v>
-      </c>
-      <c r="E72" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" t="s">
-        <v>203</v>
-      </c>
-      <c r="G72" t="s">
-        <v>204</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4566,25 +4539,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>202</v>
+      </c>
+      <c r="B73" t="s">
+        <v>203</v>
+      </c>
+      <c r="C73" t="s">
+        <v>146</v>
+      </c>
+      <c r="D73" t="s">
+        <v>147</v>
+      </c>
+      <c r="E73" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" t="s">
+        <v>204</v>
+      </c>
+      <c r="G73" t="s">
         <v>205</v>
-      </c>
-      <c r="B73" t="s">
-        <v>206</v>
-      </c>
-      <c r="C73" t="s">
-        <v>149</v>
-      </c>
-      <c r="D73" t="s">
-        <v>150</v>
-      </c>
-      <c r="E73" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" t="s">
-        <v>207</v>
-      </c>
-      <c r="G73" t="s">
-        <v>208</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4593,31 +4566,31 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J103" si="1">H73*I73</f>
+        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" t="s">
+        <v>147</v>
+      </c>
+      <c r="E74" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
+        <v>208</v>
+      </c>
+      <c r="G74" t="s">
         <v>209</v>
-      </c>
-      <c r="B74" t="s">
-        <v>210</v>
-      </c>
-      <c r="C74" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" t="s">
-        <v>150</v>
-      </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" t="s">
-        <v>211</v>
-      </c>
-      <c r="G74" t="s">
-        <v>212</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4632,25 +4605,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" t="s">
+        <v>147</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
+        <v>212</v>
+      </c>
+      <c r="G75" t="s">
         <v>213</v>
-      </c>
-      <c r="B75" t="s">
-        <v>214</v>
-      </c>
-      <c r="C75" t="s">
-        <v>149</v>
-      </c>
-      <c r="D75" t="s">
-        <v>150</v>
-      </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" t="s">
-        <v>215</v>
-      </c>
-      <c r="G75" t="s">
-        <v>216</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4665,16 +4638,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D76" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
@@ -4692,25 +4665,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>215</v>
+      </c>
+      <c r="B77" t="s">
+        <v>216</v>
+      </c>
+      <c r="C77" t="s">
+        <v>146</v>
+      </c>
+      <c r="D77" t="s">
+        <v>147</v>
+      </c>
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s">
+        <v>217</v>
+      </c>
+      <c r="G77" t="s">
         <v>218</v>
-      </c>
-      <c r="B77" t="s">
-        <v>219</v>
-      </c>
-      <c r="C77" t="s">
-        <v>149</v>
-      </c>
-      <c r="D77" t="s">
-        <v>150</v>
-      </c>
-      <c r="E77" t="s">
-        <v>19</v>
-      </c>
-      <c r="F77" t="s">
-        <v>220</v>
-      </c>
-      <c r="G77" t="s">
-        <v>221</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4725,25 +4698,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B78" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C78" t="s">
+        <v>297</v>
+      </c>
+      <c r="D78" t="s">
+        <v>113</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" t="s">
         <v>300</v>
       </c>
-      <c r="D78" t="s">
-        <v>116</v>
-      </c>
-      <c r="E78" t="s">
-        <v>19</v>
-      </c>
-      <c r="F78" t="s">
-        <v>303</v>
-      </c>
       <c r="G78" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4758,25 +4731,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C79" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D79" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G79" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4791,25 +4764,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" t="s">
+        <v>146</v>
+      </c>
+      <c r="D80" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" t="s">
+        <v>225</v>
+      </c>
+      <c r="G80" t="s">
         <v>226</v>
-      </c>
-      <c r="B80" t="s">
-        <v>227</v>
-      </c>
-      <c r="C80" t="s">
-        <v>149</v>
-      </c>
-      <c r="D80" t="s">
-        <v>150</v>
-      </c>
-      <c r="E80" t="s">
-        <v>19</v>
-      </c>
-      <c r="F80" t="s">
-        <v>228</v>
-      </c>
-      <c r="G80" t="s">
-        <v>229</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4824,25 +4797,25 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>227</v>
+      </c>
+      <c r="B81" t="s">
+        <v>228</v>
+      </c>
+      <c r="C81" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" t="s">
+        <v>147</v>
+      </c>
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s">
+        <v>229</v>
+      </c>
+      <c r="G81" t="s">
         <v>230</v>
-      </c>
-      <c r="B81" t="s">
-        <v>231</v>
-      </c>
-      <c r="C81" t="s">
-        <v>149</v>
-      </c>
-      <c r="D81" t="s">
-        <v>150</v>
-      </c>
-      <c r="E81" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81" t="s">
-        <v>232</v>
-      </c>
-      <c r="G81" t="s">
-        <v>233</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4857,136 +4830,139 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>457</v>
+        <v>422</v>
+      </c>
+      <c r="B82" t="s">
+        <v>420</v>
       </c>
       <c r="C82" t="s">
-        <v>458</v>
+        <v>420</v>
       </c>
       <c r="D82" t="s">
-        <v>458</v>
+        <v>421</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>459</v>
+        <v>423</v>
       </c>
       <c r="G82" t="s">
-        <v>460</v>
+        <v>424</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82">
-        <v>1.02</v>
+        <v>15.1</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>1.02</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B83" t="s">
-        <v>424</v>
+        <v>231</v>
       </c>
       <c r="C83" t="s">
-        <v>424</v>
+        <v>231</v>
       </c>
       <c r="D83" t="s">
-        <v>425</v>
+        <v>232</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>427</v>
+        <v>233</v>
       </c>
       <c r="G83" t="s">
-        <v>428</v>
+        <v>234</v>
       </c>
       <c r="H83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I83">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
-        <v>30.2</v>
+        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B84" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C84" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D84" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G84" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J84">
-        <f t="shared" ref="J84:J93" si="2">H84*I84</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>430</v>
+        <v>240</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="C85" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="D85" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
       <c r="E85" t="s">
-        <v>19</v>
+        <v>428</v>
       </c>
       <c r="F85" t="s">
-        <v>241</v>
+        <v>431</v>
       </c>
       <c r="G85" t="s">
-        <v>242</v>
+        <v>432</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B86" t="s">
         <v>265</v>
@@ -4998,155 +4974,155 @@
         <v>266</v>
       </c>
       <c r="E86" t="s">
-        <v>432</v>
+        <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>435</v>
+        <v>267</v>
       </c>
       <c r="G86" t="s">
-        <v>436</v>
+        <v>268</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="J86">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B87" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C87" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="D87" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="G87" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C88" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D88" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G88" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J88">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B89" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C89" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D89" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G89" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B90" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D90" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G90" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -5154,426 +5130,360 @@
         <v>264</v>
       </c>
       <c r="B91" t="s">
-        <v>259</v>
+        <v>414</v>
       </c>
       <c r="C91" t="s">
-        <v>259</v>
+        <v>414</v>
       </c>
       <c r="D91" t="s">
-        <v>260</v>
+        <v>427</v>
       </c>
       <c r="E91" t="s">
-        <v>19</v>
+        <v>428</v>
       </c>
       <c r="F91" t="s">
-        <v>261</v>
+        <v>429</v>
       </c>
       <c r="G91" t="s">
-        <v>262</v>
+        <v>430</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>448</v>
       </c>
       <c r="B92" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C92" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D92" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="E92" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F92" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G92" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I92">
-        <v>1.23</v>
+        <v>2.76</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>453</v>
+        <v>273</v>
       </c>
       <c r="B93" t="s">
-        <v>417</v>
+        <v>269</v>
       </c>
       <c r="C93" t="s">
-        <v>417</v>
+        <v>269</v>
       </c>
       <c r="D93" t="s">
-        <v>437</v>
+        <v>270</v>
       </c>
       <c r="E93" t="s">
-        <v>432</v>
+        <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>438</v>
+        <v>271</v>
       </c>
       <c r="G93" t="s">
-        <v>439</v>
+        <v>272</v>
       </c>
       <c r="H93">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I93">
-        <v>2.76</v>
+        <v>3.79</v>
       </c>
       <c r="J93">
-        <f t="shared" si="2"/>
-        <v>16.559999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>278</v>
+      </c>
+      <c r="B94" t="s">
+        <v>274</v>
+      </c>
+      <c r="C94" t="s">
+        <v>274</v>
+      </c>
+      <c r="D94" t="s">
+        <v>275</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>276</v>
       </c>
-      <c r="B94" t="s">
-        <v>272</v>
-      </c>
-      <c r="C94" t="s">
-        <v>272</v>
-      </c>
-      <c r="D94" t="s">
-        <v>273</v>
-      </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>274</v>
-      </c>
       <c r="G94" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>281</v>
+        <v>364</v>
       </c>
       <c r="B95" t="s">
-        <v>277</v>
+        <v>389</v>
       </c>
       <c r="C95" t="s">
-        <v>277</v>
+        <v>389</v>
       </c>
       <c r="D95" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>279</v>
+        <v>390</v>
       </c>
       <c r="G95" t="s">
-        <v>280</v>
+        <v>391</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>408</v>
+      </c>
+      <c r="B96" t="s">
+        <v>365</v>
+      </c>
+      <c r="C96" t="s">
+        <v>365</v>
+      </c>
+      <c r="D96" t="s">
         <v>367</v>
       </c>
-      <c r="B96" t="s">
-        <v>392</v>
-      </c>
-      <c r="C96" t="s">
-        <v>392</v>
-      </c>
-      <c r="D96" t="s">
-        <v>282</v>
-      </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
       <c r="G96" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="I96">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>411</v>
+        <v>447</v>
       </c>
       <c r="B97" t="s">
-        <v>368</v>
+        <v>416</v>
       </c>
       <c r="C97" t="s">
-        <v>368</v>
+        <v>416</v>
       </c>
       <c r="D97" t="s">
-        <v>370</v>
+        <v>417</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>369</v>
+        <v>418</v>
       </c>
       <c r="G97" t="s">
-        <v>371</v>
+        <v>419</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>6.84</v>
+        <v>1.86</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>412</v>
+        <v>280</v>
       </c>
       <c r="B98" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="C98" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="D98" t="s">
-        <v>454</v>
+        <v>282</v>
       </c>
       <c r="E98" t="s">
-        <v>19</v>
+        <v>283</v>
       </c>
       <c r="F98" t="s">
-        <v>455</v>
+        <v>284</v>
       </c>
       <c r="G98" t="s">
-        <v>456</v>
+        <v>285</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>451</v>
+        <v>286</v>
       </c>
       <c r="B99" t="s">
-        <v>420</v>
+        <v>287</v>
       </c>
       <c r="C99" t="s">
-        <v>420</v>
+        <v>287</v>
       </c>
       <c r="D99" t="s">
-        <v>421</v>
+        <v>288</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>422</v>
+        <v>289</v>
       </c>
       <c r="G99" t="s">
-        <v>423</v>
+        <v>290</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.86</v>
+        <v>2.96</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>403</v>
+      </c>
+      <c r="B100" t="s">
+        <v>404</v>
+      </c>
+      <c r="C100" t="s">
+        <v>405</v>
+      </c>
+      <c r="D100" t="s">
+        <v>405</v>
+      </c>
+      <c r="E100" t="s">
         <v>283</v>
       </c>
-      <c r="B100" t="s">
-        <v>284</v>
-      </c>
-      <c r="C100" t="s">
-        <v>284</v>
-      </c>
-      <c r="D100" t="s">
-        <v>285</v>
-      </c>
-      <c r="E100" t="s">
-        <v>286</v>
-      </c>
       <c r="F100" t="s">
-        <v>287</v>
+        <v>406</v>
       </c>
       <c r="G100" t="s">
-        <v>288</v>
+        <v>407</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100">
-        <v>1.5</v>
+        <v>0.95</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B101" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C101" t="s">
-        <v>290</v>
+        <v>409</v>
       </c>
       <c r="D101" t="s">
-        <v>291</v>
+        <v>410</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
       </c>
       <c r="F101" t="s">
-        <v>292</v>
+        <v>411</v>
       </c>
       <c r="G101" t="s">
-        <v>293</v>
+        <v>412</v>
       </c>
       <c r="H101">
         <v>1</v>
       </c>
       <c r="I101">
-        <v>2.96</v>
+        <v>1.99</v>
       </c>
       <c r="J101">
-        <f t="shared" si="1"/>
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>406</v>
-      </c>
-      <c r="B102" t="s">
-        <v>407</v>
-      </c>
-      <c r="C102" t="s">
-        <v>408</v>
-      </c>
-      <c r="D102" t="s">
-        <v>408</v>
-      </c>
-      <c r="E102" t="s">
-        <v>286</v>
-      </c>
-      <c r="F102" t="s">
-        <v>409</v>
-      </c>
-      <c r="G102" t="s">
-        <v>410</v>
-      </c>
-      <c r="H102">
-        <v>2</v>
-      </c>
-      <c r="I102">
-        <v>0.95</v>
-      </c>
-      <c r="J102">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>294</v>
-      </c>
-      <c r="B103" t="s">
-        <v>295</v>
-      </c>
-      <c r="C103" t="s">
-        <v>413</v>
-      </c>
-      <c r="D103" t="s">
-        <v>414</v>
-      </c>
-      <c r="E103" t="s">
-        <v>19</v>
-      </c>
-      <c r="F103" t="s">
-        <v>415</v>
-      </c>
-      <c r="G103" t="s">
-        <v>416</v>
-      </c>
-      <c r="H103">
-        <v>1</v>
-      </c>
-      <c r="I103">
-        <v>1.99</v>
-      </c>
-      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
JP23 output capacitors moved to top of board.
-All U16 block capacitors (C57 to C67) changed to a 0402 package.
-The polarity on JP23 was reversed to make this change possible
with cleaner routing of outputs from U16.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="458">
   <si>
     <t>Part</t>
   </si>
@@ -1105,9 +1105,6 @@
     <t>C1608X7R1H472K</t>
   </si>
   <si>
-    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C58, C59, C60, C61, C62, C63, C64, C65, C66, C67</t>
-  </si>
-  <si>
     <t>U15</t>
   </si>
   <si>
@@ -1373,6 +1370,24 @@
   </si>
   <si>
     <t>WM3478-ND</t>
+  </si>
+  <si>
+    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56</t>
+  </si>
+  <si>
+    <t>C58, C59, C60, C61, C62, C63, C64, C65, C66, C67</t>
+  </si>
+  <si>
+    <t>C-US0402</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>445-7384-1-ND</t>
+  </si>
+  <si>
+    <t>C1005X5R1V104K</t>
   </si>
 </sst>
 </file>
@@ -2201,10 +2216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,7 +2273,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2289,8 +2304,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J109)</f>
-        <v>201.01300000000001</v>
+        <f>SUM(J2:J110)</f>
+        <v>203.25400000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2322,13 +2337,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J73" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>363</v>
+        <v>452</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2349,14 +2364,14 @@
         <v>315</v>
       </c>
       <c r="H4">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.69300000000000006</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2949,79 +2964,79 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>399</v>
+        <v>453</v>
       </c>
       <c r="B24" t="s">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>454</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>455</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>401</v>
+        <v>456</v>
       </c>
       <c r="G24" t="s">
-        <v>402</v>
+        <v>457</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I24">
-        <v>0.12</v>
+        <v>0.27</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>398</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>399</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
+        <v>400</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>401</v>
       </c>
       <c r="H25">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>0.315</v>
+        <v>0.12</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>8.19</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
         <v>66</v>
@@ -3030,64 +3045,61 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>308</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>309</v>
+        <v>65</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="I26">
-        <v>0.35</v>
+        <v>0.315</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="G27" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L27" t="s">
-        <v>356</v>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>72</v>
@@ -3099,28 +3111,31 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="G28" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0.68</v>
+        <v>0.4</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
         <v>72</v>
@@ -3132,28 +3147,28 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G29" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>72</v>
@@ -3165,190 +3180,193 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>0.9</v>
+        <v>0.42</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="L30" t="s">
-        <v>349</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>293</v>
+        <v>347</v>
       </c>
       <c r="G31" t="s">
-        <v>294</v>
+        <v>348</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="I31">
-        <v>11.91</v>
+        <v>0.9</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>2.7</v>
+      </c>
+      <c r="L31" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>449</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>384</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>385</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>386</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>387</v>
+        <v>293</v>
       </c>
       <c r="G32" t="s">
-        <v>388</v>
+        <v>294</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>0.44</v>
+        <v>11.91</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>448</v>
       </c>
       <c r="B33" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="C33" t="s">
-        <v>358</v>
+        <v>384</v>
       </c>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>385</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>357</v>
+        <v>386</v>
       </c>
       <c r="G33" t="s">
-        <v>358</v>
+        <v>387</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33">
-        <v>2.15</v>
+        <v>0.44</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>86</v>
+        <v>357</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>0.77</v>
+        <v>2.15</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>353</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>355</v>
+        <v>86</v>
+      </c>
+      <c r="G35" t="s">
+        <v>85</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3363,10 +3381,7 @@
         <v>283</v>
       </c>
       <c r="F36" t="s">
-        <v>354</v>
-      </c>
-      <c r="G36" t="s">
-        <v>14</v>
+        <v>355</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3381,115 +3396,112 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>352</v>
       </c>
       <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" t="s">
+        <v>283</v>
+      </c>
+      <c r="F37" t="s">
+        <v>354</v>
+      </c>
+      <c r="G37" t="s">
         <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" t="s">
-        <v>378</v>
-      </c>
-      <c r="E37" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" t="s">
-        <v>92</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="I37">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>441</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>377</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>306</v>
+        <v>91</v>
       </c>
       <c r="G38" t="s">
-        <v>307</v>
+        <v>92</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I38">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>440</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>99</v>
+        <v>306</v>
       </c>
       <c r="G39" t="s">
-        <v>100</v>
+        <v>307</v>
       </c>
       <c r="H39">
         <v>3</v>
       </c>
       <c r="I39">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L39" t="s">
-        <v>317</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>377</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
         <v>97</v>
@@ -3504,373 +3516,385 @@
         <v>100</v>
       </c>
       <c r="H40">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I40">
         <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>1.26</v>
+      </c>
+      <c r="L40" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>376</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>450</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>451</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>452</v>
-      </c>
-      <c r="G41">
-        <v>702461004</v>
+        <v>99</v>
+      </c>
+      <c r="G41" t="s">
+        <v>100</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I41">
-        <v>1.64</v>
+        <v>0.42</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>1.64</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>376</v>
-      </c>
-      <c r="B42" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>449</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>450</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>373</v>
-      </c>
-      <c r="G42" t="s">
-        <v>374</v>
+        <v>451</v>
+      </c>
+      <c r="G42">
+        <v>702461004</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0.13</v>
+        <v>1.64</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>375</v>
       </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
       <c r="C43" t="s">
-        <v>369</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>370</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G43" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I43">
-        <v>0.71</v>
+        <v>0.13</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>368</v>
       </c>
       <c r="D44" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="G44" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>442</v>
+        <v>378</v>
       </c>
       <c r="C45" t="s">
-        <v>443</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>444</v>
+        <v>377</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="G45" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>1.67</v>
+        <v>3.15</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="C46" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D46" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="G46" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="H46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>0.5</v>
+        <v>1.67</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" t="s">
-        <v>105</v>
+        <v>435</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>436</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>437</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>108</v>
+        <v>438</v>
       </c>
       <c r="G47" t="s">
-        <v>109</v>
+        <v>439</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I47">
-        <v>2.13</v>
+        <v>0.5</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G48" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D49" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G49" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E50" t="s">
         <v>19</v>
       </c>
       <c r="F50" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G50" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>130</v>
+        <v>125</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>126</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="H51">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1.85</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B52" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -3879,46 +3903,37 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>382</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G53" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
         <v>132</v>
@@ -3927,61 +3942,61 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G54" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>382</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>295</v>
+        <v>142</v>
       </c>
       <c r="G55" t="s">
-        <v>296</v>
+        <v>143</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C56" t="s">
         <v>146</v>
@@ -3993,28 +4008,28 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>150</v>
+        <v>295</v>
       </c>
       <c r="G56" t="s">
-        <v>151</v>
+        <v>296</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>152</v>
-      </c>
-      <c r="B57">
-        <v>470</v>
+        <v>148</v>
+      </c>
+      <c r="B57" t="s">
+        <v>149</v>
       </c>
       <c r="C57" t="s">
         <v>146</v>
@@ -4026,10 +4041,10 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G57" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4044,10 +4059,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>415</v>
-      </c>
-      <c r="B58" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+      <c r="B58">
+        <v>470</v>
       </c>
       <c r="C58" t="s">
         <v>146</v>
@@ -4059,28 +4074,28 @@
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G58" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H58">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>414</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C59" t="s">
         <v>146</v>
@@ -4092,61 +4107,61 @@
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G59" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>297</v>
+        <v>146</v>
       </c>
       <c r="D60" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>298</v>
+        <v>160</v>
       </c>
       <c r="G60" t="s">
-        <v>299</v>
+        <v>161</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I60">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C61" t="s">
         <v>297</v>
@@ -4158,10 +4173,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G61" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4176,76 +4191,76 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B62" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C62" t="s">
-        <v>146</v>
+        <v>297</v>
       </c>
       <c r="D62" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>168</v>
+        <v>304</v>
       </c>
       <c r="G62" t="s">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>170</v>
-      </c>
-      <c r="B63">
-        <v>200</v>
+        <v>166</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
       </c>
       <c r="C63" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="D63" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>392</v>
+        <v>168</v>
       </c>
       <c r="G63" t="s">
-        <v>393</v>
+        <v>169</v>
       </c>
       <c r="H63">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>394</v>
+        <v>170</v>
       </c>
       <c r="B64">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C64" t="s">
         <v>198</v>
@@ -4257,61 +4272,61 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G64" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I64">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="D65" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>171</v>
+        <v>395</v>
       </c>
       <c r="G65" t="s">
-        <v>172</v>
+        <v>396</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>173</v>
-      </c>
-      <c r="B66" t="s">
-        <v>174</v>
+        <v>394</v>
+      </c>
+      <c r="B66">
+        <v>100</v>
       </c>
       <c r="C66" t="s">
         <v>146</v>
@@ -4323,28 +4338,28 @@
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G66" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H66">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C67" t="s">
         <v>146</v>
@@ -4356,28 +4371,28 @@
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G67" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H67">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C68" t="s">
         <v>146</v>
@@ -4389,28 +4404,28 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G68" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H68">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C69" t="s">
         <v>146</v>
@@ -4422,28 +4437,28 @@
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G69" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B70" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C70" t="s">
         <v>146</v>
@@ -4455,28 +4470,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G70" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B71" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C71" t="s">
         <v>146</v>
@@ -4488,10 +4503,10 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G71" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4506,76 +4521,76 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>197</v>
-      </c>
-      <c r="B72">
-        <v>0.3</v>
+        <v>193</v>
+      </c>
+      <c r="B72" t="s">
+        <v>194</v>
       </c>
       <c r="C72" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="D72" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G72" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>202</v>
-      </c>
-      <c r="B73" t="s">
-        <v>203</v>
+        <v>197</v>
+      </c>
+      <c r="B73">
+        <v>0.3</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="D73" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G73" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B74" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C74" t="s">
         <v>146</v>
@@ -4587,10 +4602,10 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G74" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4599,16 +4614,16 @@
         <v>0.04</v>
       </c>
       <c r="J74">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J74:J102" si="1">H74*I74</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C75" t="s">
         <v>146</v>
@@ -4620,10 +4635,10 @@
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G75" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4638,10 +4653,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="C76" t="s">
         <v>146</v>
@@ -4652,23 +4667,29 @@
       <c r="E76" t="s">
         <v>19</v>
       </c>
+      <c r="F76" t="s">
+        <v>212</v>
+      </c>
       <c r="G76" t="s">
-        <v>14</v>
+        <v>213</v>
       </c>
       <c r="H76">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0.04</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B77" t="s">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
         <v>146</v>
@@ -4679,62 +4700,56 @@
       <c r="E77" t="s">
         <v>19</v>
       </c>
-      <c r="F77" t="s">
-        <v>217</v>
-      </c>
       <c r="G77" t="s">
-        <v>218</v>
+        <v>14</v>
       </c>
       <c r="H77">
-        <v>1</v>
-      </c>
-      <c r="I77">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>297</v>
+        <v>146</v>
       </c>
       <c r="D78" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>300</v>
+        <v>217</v>
       </c>
       <c r="G78" t="s">
-        <v>301</v>
+        <v>218</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C79" t="s">
         <v>297</v>
@@ -4746,10 +4761,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G79" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4764,43 +4779,43 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C80" t="s">
-        <v>146</v>
+        <v>297</v>
       </c>
       <c r="D80" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>225</v>
+        <v>302</v>
       </c>
       <c r="G80" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B81" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C81" t="s">
         <v>146</v>
@@ -4812,10 +4827,10 @@
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G81" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4830,660 +4845,693 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>422</v>
+        <v>227</v>
       </c>
       <c r="B82" t="s">
-        <v>420</v>
+        <v>228</v>
       </c>
       <c r="C82" t="s">
-        <v>420</v>
+        <v>146</v>
       </c>
       <c r="D82" t="s">
-        <v>421</v>
+        <v>147</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>423</v>
+        <v>229</v>
       </c>
       <c r="G82" t="s">
-        <v>424</v>
+        <v>230</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I82">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>30.2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B83" t="s">
-        <v>231</v>
+        <v>419</v>
       </c>
       <c r="C83" t="s">
-        <v>231</v>
+        <v>419</v>
       </c>
       <c r="D83" t="s">
-        <v>232</v>
+        <v>420</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>233</v>
+        <v>422</v>
       </c>
       <c r="G83" t="s">
-        <v>234</v>
+        <v>423</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I83">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>30.2</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D84" t="s">
+        <v>232</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
+        <v>233</v>
+      </c>
+      <c r="G84" t="s">
+        <v>234</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>6.6</v>
+      </c>
+      <c r="J84">
+        <f t="shared" ref="J84:J93" si="2">H84*I84</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>425</v>
+      </c>
+      <c r="B85" t="s">
         <v>235</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>236</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>237</v>
       </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
         <v>238</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>239</v>
       </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84">
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
         <v>0.79</v>
       </c>
-      <c r="J84">
+      <c r="J85">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>240</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>262</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>262</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>263</v>
       </c>
-      <c r="E85" t="s">
-        <v>428</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E86" t="s">
+        <v>427</v>
+      </c>
+      <c r="F86" t="s">
+        <v>430</v>
+      </c>
+      <c r="G86" t="s">
         <v>431</v>
       </c>
-      <c r="G85" t="s">
-        <v>432</v>
-      </c>
-      <c r="H85">
-        <v>1</v>
-      </c>
-      <c r="I85">
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
         <v>0.45</v>
       </c>
-      <c r="J85">
+      <c r="J86">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>245</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>265</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>265</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>266</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>267</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" t="s">
         <v>268</v>
       </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
         <v>0.47</v>
       </c>
-      <c r="J86">
+      <c r="J87">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>250</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>241</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>241</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>242</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>243</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" t="s">
         <v>244</v>
       </c>
-      <c r="H87">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
         <v>0.67</v>
       </c>
-      <c r="J87">
+      <c r="J88">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>255</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>246</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>246</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>247</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>248</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" t="s">
         <v>249</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>6.63</v>
       </c>
-      <c r="J88">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>260</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>251</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>251</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>252</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>253</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" t="s">
         <v>254</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>1.67</v>
       </c>
-      <c r="J89">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>261</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>256</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>256</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>257</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>258</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" t="s">
         <v>259</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>5.88</v>
       </c>
-      <c r="J90">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>264</v>
       </c>
-      <c r="B91" t="s">
-        <v>414</v>
-      </c>
-      <c r="C91" t="s">
-        <v>414</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="B92" t="s">
+        <v>413</v>
+      </c>
+      <c r="C92" t="s">
+        <v>413</v>
+      </c>
+      <c r="D92" t="s">
+        <v>426</v>
+      </c>
+      <c r="E92" t="s">
         <v>427</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F92" t="s">
         <v>428</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G92" t="s">
         <v>429</v>
       </c>
-      <c r="G91" t="s">
-        <v>430</v>
-      </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>1.23</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>448</v>
-      </c>
-      <c r="B92" t="s">
-        <v>413</v>
-      </c>
-      <c r="C92" t="s">
-        <v>413</v>
-      </c>
-      <c r="D92" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>447</v>
+      </c>
+      <c r="B93" t="s">
+        <v>412</v>
+      </c>
+      <c r="C93" t="s">
+        <v>412</v>
+      </c>
+      <c r="D93" t="s">
+        <v>432</v>
+      </c>
+      <c r="E93" t="s">
+        <v>427</v>
+      </c>
+      <c r="F93" t="s">
         <v>433</v>
       </c>
-      <c r="E92" t="s">
-        <v>428</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G93" t="s">
         <v>434</v>
       </c>
-      <c r="G92" t="s">
-        <v>435</v>
-      </c>
-      <c r="H92">
+      <c r="H93">
         <v>5</v>
       </c>
-      <c r="I92">
+      <c r="I93">
         <v>2.76</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="2"/>
         <v>13.799999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>273</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>269</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>269</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>270</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>271</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>272</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>3.79</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>278</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>274</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>274</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>275</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>276</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>277</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>1.57</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>364</v>
-      </c>
-      <c r="B95" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>363</v>
+      </c>
+      <c r="B96" t="s">
+        <v>388</v>
+      </c>
+      <c r="C96" t="s">
+        <v>388</v>
+      </c>
+      <c r="D96" t="s">
+        <v>279</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>389</v>
       </c>
-      <c r="C95" t="s">
-        <v>389</v>
-      </c>
-      <c r="D95" t="s">
-        <v>279</v>
-      </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="G96" t="s">
         <v>390</v>
       </c>
-      <c r="G95" t="s">
-        <v>391</v>
-      </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>8.48</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>408</v>
-      </c>
-      <c r="B96" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>407</v>
+      </c>
+      <c r="B97" t="s">
+        <v>364</v>
+      </c>
+      <c r="C97" t="s">
+        <v>364</v>
+      </c>
+      <c r="D97" t="s">
+        <v>366</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>365</v>
       </c>
-      <c r="C96" t="s">
-        <v>365</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="G97" t="s">
         <v>367</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
-        <v>366</v>
-      </c>
-      <c r="G96" t="s">
-        <v>368</v>
-      </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
         <v>6.84</v>
       </c>
-      <c r="J96">
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>447</v>
-      </c>
-      <c r="B97" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>446</v>
+      </c>
+      <c r="B98" t="s">
+        <v>415</v>
+      </c>
+      <c r="C98" t="s">
+        <v>415</v>
+      </c>
+      <c r="D98" t="s">
         <v>416</v>
       </c>
-      <c r="C97" t="s">
-        <v>416</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>417</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G98" t="s">
         <v>418</v>
       </c>
-      <c r="G97" t="s">
-        <v>419</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>1.86</v>
       </c>
-      <c r="J97">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>280</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>281</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>281</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>282</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E99" t="s">
         <v>283</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F99" t="s">
         <v>284</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G99" t="s">
         <v>285</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.5</v>
       </c>
-      <c r="J98">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>286</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>287</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>287</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>288</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>289</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G100" t="s">
         <v>290</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>2.96</v>
       </c>
-      <c r="J99">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>402</v>
+      </c>
+      <c r="B101" t="s">
         <v>403</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C101" t="s">
         <v>404</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D101" t="s">
+        <v>404</v>
+      </c>
+      <c r="E101" t="s">
+        <v>283</v>
+      </c>
+      <c r="F101" t="s">
         <v>405</v>
       </c>
-      <c r="D100" t="s">
-        <v>405</v>
-      </c>
-      <c r="E100" t="s">
-        <v>283</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="G101" t="s">
         <v>406</v>
       </c>
-      <c r="G100" t="s">
-        <v>407</v>
-      </c>
-      <c r="H100">
+      <c r="H101">
         <v>2</v>
       </c>
-      <c r="I100">
+      <c r="I101">
         <v>0.95</v>
       </c>
-      <c r="J100">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>291</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>292</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
+        <v>408</v>
+      </c>
+      <c r="D102" t="s">
         <v>409</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>410</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="G102" t="s">
         <v>411</v>
       </c>
-      <c r="G101" t="s">
-        <v>412</v>
-      </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>1.99</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Moved the Pmod header diodes to the top side of the board.
In order to make this fit, JP6-JP8 were finally replaced with the
SparkFun.lbr component with non-long pads. The BOM line items have
been consolidated.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="455">
   <si>
     <t>Part</t>
   </si>
@@ -301,12 +301,6 @@
     <t>2X06</t>
   </si>
   <si>
-    <t>JP6, JP7, JP8</t>
-  </si>
-  <si>
-    <t>PINHD-1X3</t>
-  </si>
-  <si>
     <t>1X03</t>
   </si>
   <si>
@@ -967,9 +961,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Redudndant line item</t>
-  </si>
-  <si>
     <t>Real part value is 300pF</t>
   </si>
   <si>
@@ -1144,9 +1135,6 @@
     <t>JP20, JP21, JP22</t>
   </si>
   <si>
-    <t>JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19</t>
-  </si>
-  <si>
     <t>2X10 Right angle</t>
   </si>
   <si>
@@ -1388,6 +1376,9 @@
   </si>
   <si>
     <t>C1005X5R1V104K</t>
+  </si>
+  <si>
+    <t>JP6, JP7, JP8, JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19</t>
   </si>
 </sst>
 </file>
@@ -2216,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,12 +2259,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2288,10 +2279,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2304,8 +2295,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J110)</f>
-        <v>203.25400000000002</v>
+        <f>SUM(J2:J109)</f>
+        <v>203.25399999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2325,10 +2316,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2337,13 +2328,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J73" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2358,10 +2349,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H4">
         <v>24</v>
@@ -2415,10 +2406,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2431,7 +2422,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2475,10 +2466,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2508,10 +2499,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G9" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2541,10 +2532,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G10" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2557,7 +2548,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2610,10 +2601,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2643,10 +2634,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G13" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2659,7 +2650,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2679,10 +2670,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G14" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2695,7 +2686,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2739,10 +2730,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G16" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2820,10 +2811,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G19" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2836,7 +2827,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2856,10 +2847,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G20" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2913,10 +2904,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G22" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2931,10 +2922,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B23" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2946,10 +2937,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G23" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2964,25 +2955,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D24" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G24" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -2997,10 +2988,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B25" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3012,10 +3003,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G25" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3078,10 +3069,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -3111,10 +3102,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3127,7 +3118,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3147,10 +3138,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G29" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3180,10 +3171,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3213,10 +3204,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G31" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3229,7 +3220,7 @@
         <v>2.7</v>
       </c>
       <c r="L31" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3249,10 +3240,10 @@
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -3265,27 +3256,27 @@
         <v>35.730000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B33" t="s">
+        <v>379</v>
+      </c>
+      <c r="C33" t="s">
+        <v>380</v>
+      </c>
+      <c r="D33" t="s">
+        <v>381</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>382</v>
+      </c>
+      <c r="G33" t="s">
         <v>383</v>
-      </c>
-      <c r="C33" t="s">
-        <v>384</v>
-      </c>
-      <c r="D33" t="s">
-        <v>385</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
-        <v>386</v>
-      </c>
-      <c r="G33" t="s">
-        <v>387</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -3298,27 +3289,27 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C34" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D34" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G34" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3331,7 +3322,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -3364,9 +3355,9 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3378,10 +3369,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F36" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3394,9 +3385,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3408,10 +3399,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F37" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3427,7 +3418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -3438,7 +3429,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3460,9 +3451,9 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3477,10 +3468,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G39" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H39">
         <v>3</v>
@@ -3493,9 +3484,9 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>454</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3504,397 +3495,385 @@
         <v>96</v>
       </c>
       <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
         <v>97</v>
       </c>
-      <c r="E40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>99</v>
-      </c>
       <c r="G40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I40">
         <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="L40" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>376</v>
-      </c>
-      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
+        <v>445</v>
+      </c>
+      <c r="D41" t="s">
+        <v>446</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>447</v>
+      </c>
+      <c r="G41">
+        <v>702461004</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1.64</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>372</v>
+      </c>
+      <c r="B42" t="s">
         <v>14</v>
       </c>
-      <c r="C41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
-        <v>99</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="C42" t="s">
         <v>100</v>
       </c>
-      <c r="H41">
-        <v>10</v>
-      </c>
-      <c r="I41">
-        <v>0.42</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="0"/>
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D42" t="s">
         <v>101</v>
       </c>
-      <c r="C42" t="s">
-        <v>449</v>
-      </c>
-      <c r="D42" t="s">
-        <v>450</v>
-      </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>451</v>
-      </c>
-      <c r="G42">
-        <v>702461004</v>
+        <v>369</v>
+      </c>
+      <c r="G42" t="s">
+        <v>370</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>1.64</v>
+        <v>0.13</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>375</v>
-      </c>
-      <c r="B43" t="s">
-        <v>14</v>
+        <v>371</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>365</v>
       </c>
       <c r="D43" t="s">
-        <v>103</v>
+        <v>366</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="G43" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="H43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>0.13</v>
+        <v>0.71</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>374</v>
       </c>
       <c r="C44" t="s">
-        <v>368</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="G44" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>378</v>
+        <v>437</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>438</v>
       </c>
       <c r="D45" t="s">
-        <v>377</v>
+        <v>439</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>379</v>
+        <v>440</v>
       </c>
       <c r="G45" t="s">
-        <v>380</v>
+        <v>441</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <v>3.15</v>
+        <v>1.67</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C46" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="D46" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="G46" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I46">
-        <v>1.67</v>
+        <v>0.5</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>435</v>
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>436</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>437</v>
+        <v>105</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>438</v>
+        <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>439</v>
+        <v>107</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47">
-        <v>0.5</v>
+        <v>2.13</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D48" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G48" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D49" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G49" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E50" t="s">
         <v>19</v>
       </c>
       <c r="F50" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G50" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
-      </c>
-      <c r="E51" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G51" t="s">
-        <v>127</v>
+        <v>14</v>
       </c>
       <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
-        <v>1.85</v>
+        <v>8</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
       </c>
       <c r="H52">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -3903,148 +3882,157 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>377</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D53" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
         <v>136</v>
       </c>
       <c r="G53" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0.41</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G54" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>382</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>142</v>
+        <v>293</v>
       </c>
       <c r="G55" t="s">
-        <v>143</v>
+        <v>294</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" t="s">
         <v>144</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>145</v>
       </c>
-      <c r="C56" t="s">
-        <v>146</v>
-      </c>
-      <c r="D56" t="s">
-        <v>147</v>
-      </c>
       <c r="E56" t="s">
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>295</v>
+        <v>148</v>
       </c>
       <c r="G56" t="s">
-        <v>296</v>
+        <v>149</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>148</v>
-      </c>
-      <c r="B57" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+      <c r="B57">
+        <v>470</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G57" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4059,101 +4047,101 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>152</v>
-      </c>
-      <c r="B58">
-        <v>470</v>
+        <v>410</v>
+      </c>
+      <c r="B58" t="s">
+        <v>153</v>
       </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D58" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>414</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C59" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G59" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H59">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>295</v>
       </c>
       <c r="D60" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>296</v>
       </c>
       <c r="G60" t="s">
-        <v>161</v>
+        <v>297</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I60">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -4164,19 +4152,19 @@
         <v>163</v>
       </c>
       <c r="C61" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="G61" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4197,76 +4185,76 @@
         <v>165</v>
       </c>
       <c r="C62" t="s">
-        <v>297</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>304</v>
+        <v>166</v>
       </c>
       <c r="G62" t="s">
-        <v>305</v>
+        <v>167</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>166</v>
-      </c>
-      <c r="B63" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="B63">
+        <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>146</v>
+        <v>196</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>197</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>168</v>
+        <v>387</v>
       </c>
       <c r="G63" t="s">
-        <v>169</v>
+        <v>388</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I63">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>389</v>
       </c>
       <c r="B64">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
@@ -4278,235 +4266,235 @@
         <v>392</v>
       </c>
       <c r="H64">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I64">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>395</v>
+        <v>169</v>
       </c>
       <c r="G65" t="s">
-        <v>396</v>
+        <v>170</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>394</v>
-      </c>
-      <c r="B66">
-        <v>100</v>
+        <v>171</v>
+      </c>
+      <c r="B66" t="s">
+        <v>172</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G66" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H66">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I66">
         <v>0.04</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B67" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G67" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H67">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I67">
         <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B68" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G68" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C69" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G69" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B70" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G70" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B71" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D71" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G71" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4521,91 +4509,91 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>193</v>
-      </c>
-      <c r="B72" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="B72">
+        <v>0.3</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>196</v>
       </c>
       <c r="D72" t="s">
-        <v>147</v>
+        <v>197</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G72" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>197</v>
-      </c>
-      <c r="B73">
-        <v>0.3</v>
+        <v>200</v>
+      </c>
+      <c r="B73" t="s">
+        <v>201</v>
       </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
       <c r="D73" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G73" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B74" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G74" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4614,31 +4602,31 @@
         <v>0.04</v>
       </c>
       <c r="J74">
-        <f t="shared" ref="J74:J102" si="1">H74*I74</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B75" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D75" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G75" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4653,95 +4641,95 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D76" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
       </c>
-      <c r="F76" t="s">
-        <v>212</v>
-      </c>
       <c r="G76" t="s">
-        <v>213</v>
+        <v>14</v>
       </c>
       <c r="H76">
-        <v>1</v>
-      </c>
-      <c r="I76">
-        <v>0.04</v>
+        <v>8</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>213</v>
+      </c>
+      <c r="B77" t="s">
         <v>214</v>
       </c>
-      <c r="B77" t="s">
-        <v>14</v>
-      </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D77" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
+      <c r="F77" t="s">
+        <v>215</v>
+      </c>
       <c r="G77" t="s">
-        <v>14</v>
+        <v>216</v>
       </c>
       <c r="H77">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>0.04</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C78" t="s">
-        <v>146</v>
+        <v>295</v>
       </c>
       <c r="D78" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>217</v>
+        <v>298</v>
       </c>
       <c r="G78" t="s">
-        <v>218</v>
+        <v>299</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -4752,10 +4740,10 @@
         <v>220</v>
       </c>
       <c r="C79" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D79" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
@@ -4785,52 +4773,52 @@
         <v>222</v>
       </c>
       <c r="C80" t="s">
-        <v>297</v>
+        <v>144</v>
       </c>
       <c r="D80" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>302</v>
+        <v>223</v>
       </c>
       <c r="G80" t="s">
-        <v>303</v>
+        <v>224</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D81" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G81" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4845,693 +4833,660 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>227</v>
+        <v>417</v>
       </c>
       <c r="B82" t="s">
-        <v>228</v>
+        <v>415</v>
       </c>
       <c r="C82" t="s">
-        <v>146</v>
+        <v>415</v>
       </c>
       <c r="D82" t="s">
-        <v>147</v>
+        <v>416</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>229</v>
+        <v>418</v>
       </c>
       <c r="G82" t="s">
-        <v>230</v>
+        <v>419</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82">
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B83" t="s">
-        <v>419</v>
+        <v>229</v>
       </c>
       <c r="C83" t="s">
-        <v>419</v>
+        <v>229</v>
       </c>
       <c r="D83" t="s">
-        <v>420</v>
+        <v>230</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>422</v>
+        <v>231</v>
       </c>
       <c r="G83" t="s">
-        <v>423</v>
+        <v>232</v>
       </c>
       <c r="H83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I83">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
-        <v>30.2</v>
+        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D84" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G84" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J84">
-        <f t="shared" ref="J84:J93" si="2">H84*I84</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>425</v>
+        <v>238</v>
       </c>
       <c r="B85" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C85" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="D85" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="E85" t="s">
-        <v>19</v>
+        <v>423</v>
       </c>
       <c r="F85" t="s">
-        <v>238</v>
+        <v>426</v>
       </c>
       <c r="G85" t="s">
-        <v>239</v>
+        <v>427</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C86" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D86" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E86" t="s">
-        <v>427</v>
+        <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>430</v>
+        <v>265</v>
       </c>
       <c r="G86" t="s">
-        <v>431</v>
+        <v>266</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="J86">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B87" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="D87" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="G87" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B88" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C88" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D88" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G88" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J88">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B89" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C89" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D89" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G89" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B90" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C90" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D90" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="G90" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B91" t="s">
-        <v>256</v>
+        <v>409</v>
       </c>
       <c r="C91" t="s">
-        <v>256</v>
+        <v>409</v>
       </c>
       <c r="D91" t="s">
-        <v>257</v>
+        <v>422</v>
       </c>
       <c r="E91" t="s">
-        <v>19</v>
+        <v>423</v>
       </c>
       <c r="F91" t="s">
-        <v>258</v>
+        <v>424</v>
       </c>
       <c r="G91" t="s">
-        <v>259</v>
+        <v>425</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>264</v>
+        <v>443</v>
       </c>
       <c r="B92" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C92" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D92" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="E92" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F92" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G92" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I92">
-        <v>1.23</v>
+        <v>2.76</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>447</v>
+        <v>271</v>
       </c>
       <c r="B93" t="s">
-        <v>412</v>
+        <v>267</v>
       </c>
       <c r="C93" t="s">
-        <v>412</v>
+        <v>267</v>
       </c>
       <c r="D93" t="s">
-        <v>432</v>
+        <v>268</v>
       </c>
       <c r="E93" t="s">
-        <v>427</v>
+        <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>433</v>
+        <v>269</v>
       </c>
       <c r="G93" t="s">
-        <v>434</v>
+        <v>270</v>
       </c>
       <c r="H93">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I93">
-        <v>2.76</v>
+        <v>3.79</v>
       </c>
       <c r="J93">
-        <f t="shared" si="2"/>
-        <v>13.799999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>276</v>
+      </c>
+      <c r="B94" t="s">
+        <v>272</v>
+      </c>
+      <c r="C94" t="s">
+        <v>272</v>
+      </c>
+      <c r="D94" t="s">
         <v>273</v>
       </c>
-      <c r="B94" t="s">
-        <v>269</v>
-      </c>
-      <c r="C94" t="s">
-        <v>269</v>
-      </c>
-      <c r="D94" t="s">
-        <v>270</v>
-      </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G94" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>278</v>
+        <v>360</v>
       </c>
       <c r="B95" t="s">
-        <v>274</v>
+        <v>384</v>
       </c>
       <c r="C95" t="s">
-        <v>274</v>
+        <v>384</v>
       </c>
       <c r="D95" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>276</v>
+        <v>385</v>
       </c>
       <c r="G95" t="s">
-        <v>277</v>
+        <v>386</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J95">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>403</v>
+      </c>
+      <c r="B96" t="s">
+        <v>361</v>
+      </c>
+      <c r="C96" t="s">
+        <v>361</v>
+      </c>
+      <c r="D96" t="s">
         <v>363</v>
       </c>
-      <c r="B96" t="s">
-        <v>388</v>
-      </c>
-      <c r="C96" t="s">
-        <v>388</v>
-      </c>
-      <c r="D96" t="s">
-        <v>279</v>
-      </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>389</v>
+        <v>362</v>
       </c>
       <c r="G96" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="H96">
         <v>1</v>
       </c>
       <c r="I96">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J96">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>407</v>
+        <v>442</v>
       </c>
       <c r="B97" t="s">
-        <v>364</v>
+        <v>411</v>
       </c>
       <c r="C97" t="s">
-        <v>364</v>
+        <v>411</v>
       </c>
       <c r="D97" t="s">
-        <v>366</v>
+        <v>412</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
       <c r="G97" t="s">
-        <v>367</v>
+        <v>414</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>6.84</v>
+        <v>1.86</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>446</v>
+        <v>278</v>
       </c>
       <c r="B98" t="s">
-        <v>415</v>
+        <v>279</v>
       </c>
       <c r="C98" t="s">
-        <v>415</v>
+        <v>279</v>
       </c>
       <c r="D98" t="s">
-        <v>416</v>
+        <v>280</v>
       </c>
       <c r="E98" t="s">
-        <v>19</v>
+        <v>281</v>
       </c>
       <c r="F98" t="s">
-        <v>417</v>
+        <v>282</v>
       </c>
       <c r="G98" t="s">
-        <v>418</v>
+        <v>283</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>1.86</v>
+        <v>1.5</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B99" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C99" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D99" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E99" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G99" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>286</v>
+        <v>398</v>
       </c>
       <c r="B100" t="s">
-        <v>287</v>
+        <v>399</v>
       </c>
       <c r="C100" t="s">
-        <v>287</v>
+        <v>400</v>
       </c>
       <c r="D100" t="s">
-        <v>288</v>
+        <v>400</v>
       </c>
       <c r="E100" t="s">
-        <v>19</v>
+        <v>281</v>
       </c>
       <c r="F100" t="s">
-        <v>289</v>
+        <v>401</v>
       </c>
       <c r="G100" t="s">
-        <v>290</v>
+        <v>402</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100">
-        <v>2.96</v>
+        <v>0.95</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>402</v>
+        <v>289</v>
       </c>
       <c r="B101" t="s">
-        <v>403</v>
+        <v>290</v>
       </c>
       <c r="C101" t="s">
         <v>404</v>
       </c>
       <c r="D101" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E101" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
       <c r="F101" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G101" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I101">
-        <v>0.95</v>
+        <v>1.99</v>
       </c>
       <c r="J101">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>291</v>
-      </c>
-      <c r="B102" t="s">
-        <v>292</v>
-      </c>
-      <c r="C102" t="s">
-        <v>408</v>
-      </c>
-      <c r="D102" t="s">
-        <v>409</v>
-      </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
-        <v>410</v>
-      </c>
-      <c r="G102" t="s">
-        <v>411</v>
-      </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
-        <v>1.99</v>
-      </c>
-      <c r="J102">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Tied H-bridges directly to the 12V plane.
-With properly sized vias and the internal/external 12V planes,
it is no longer necessary to limit the drivers to less than their
maximum rated current.

-The output traces have been replaced with a pair of polygons (top and bottom).
-IC3 output net names have been corrected.
-Fuses and LEDs for all three drivers have been removed.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -394,9 +394,6 @@
     <t>IHLP3232DZER150M11</t>
   </si>
   <si>
-    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8</t>
-  </si>
-  <si>
     <t>LEDCHIPLED_0603</t>
   </si>
   <si>
@@ -652,9 +649,6 @@
     <t>ERJ-3EKF3241V</t>
   </si>
   <si>
-    <t>R136, R137, R138, R139, R140, R141, R142, R143</t>
-  </si>
-  <si>
     <t>R144</t>
   </si>
   <si>
@@ -1379,6 +1373,12 @@
   </si>
   <si>
     <t>JP6, JP7, JP8, JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19</t>
+  </si>
+  <si>
+    <t>R139, R140, R141, R142, R143</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5</t>
   </si>
 </sst>
 </file>
@@ -2209,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,12 +2259,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2279,10 +2279,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2316,10 +2316,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2349,10 +2349,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H4">
         <v>24</v>
@@ -2406,10 +2406,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2422,7 +2422,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2466,10 +2466,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2499,10 +2499,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2532,10 +2532,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2548,7 +2548,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2601,10 +2601,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2634,10 +2634,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2650,7 +2650,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2670,10 +2670,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2686,7 +2686,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2730,10 +2730,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2811,10 +2811,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2827,7 +2827,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2847,10 +2847,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G20" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2904,10 +2904,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2922,10 +2922,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B23" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2937,10 +2937,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G23" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2955,25 +2955,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
+        <v>448</v>
+      </c>
+      <c r="D24" t="s">
+        <v>449</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
         <v>450</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>451</v>
-      </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>452</v>
-      </c>
-      <c r="G24" t="s">
-        <v>453</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -2988,10 +2988,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3003,10 +3003,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G25" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3069,10 +3069,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -3102,10 +3102,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3118,7 +3118,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3138,10 +3138,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G29" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3171,10 +3171,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3204,10 +3204,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3220,7 +3220,7 @@
         <v>2.7</v>
       </c>
       <c r="L31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3240,10 +3240,10 @@
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G32" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -3258,25 +3258,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B33" t="s">
+        <v>377</v>
+      </c>
+      <c r="C33" t="s">
+        <v>378</v>
+      </c>
+      <c r="D33" t="s">
         <v>379</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>380</v>
       </c>
-      <c r="D33" t="s">
+      <c r="G33" t="s">
         <v>381</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
-        <v>382</v>
-      </c>
-      <c r="G33" t="s">
-        <v>383</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -3294,22 +3294,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C34" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D34" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G34" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3369,10 +3369,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F36" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3399,10 +3399,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F37" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3429,7 +3429,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3468,10 +3468,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G39" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H39">
         <v>3</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3522,16 +3522,16 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
+        <v>443</v>
+      </c>
+      <c r="D41" t="s">
+        <v>444</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
         <v>445</v>
-      </c>
-      <c r="D41" t="s">
-        <v>446</v>
-      </c>
-      <c r="E41" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
-        <v>447</v>
       </c>
       <c r="G41">
         <v>702461004</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
@@ -3564,10 +3564,10 @@
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G42" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H42">
         <v>3</v>
@@ -3582,22 +3582,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C43" t="s">
+        <v>363</v>
+      </c>
+      <c r="D43" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
         <v>365</v>
       </c>
-      <c r="D43" t="s">
+      <c r="G43" t="s">
         <v>366</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>367</v>
-      </c>
-      <c r="G43" t="s">
-        <v>368</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3612,22 +3612,22 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
       </c>
       <c r="D44" t="s">
+        <v>371</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>373</v>
       </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>375</v>
-      </c>
       <c r="G44" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3642,22 +3642,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>435</v>
+      </c>
+      <c r="C45" t="s">
+        <v>436</v>
+      </c>
+      <c r="D45" t="s">
         <v>437</v>
       </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
         <v>438</v>
       </c>
-      <c r="D45" t="s">
+      <c r="G45" t="s">
         <v>439</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>440</v>
-      </c>
-      <c r="G45" t="s">
-        <v>441</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3672,22 +3672,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>429</v>
+      </c>
+      <c r="C46" t="s">
+        <v>430</v>
+      </c>
+      <c r="D46" t="s">
         <v>431</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
         <v>432</v>
       </c>
-      <c r="D46" t="s">
+      <c r="G46" t="s">
         <v>433</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>434</v>
-      </c>
-      <c r="G46" t="s">
-        <v>435</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -3834,22 +3834,22 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>454</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
       </c>
       <c r="C51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" t="s">
         <v>127</v>
-      </c>
-      <c r="D51" t="s">
-        <v>128</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
       </c>
       <c r="H51">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
@@ -3858,16 +3858,16 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" t="s">
         <v>131</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>132</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>133</v>
-      </c>
-      <c r="D52" t="s">
-        <v>134</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
@@ -3882,25 +3882,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
         <v>135</v>
       </c>
-      <c r="C53" t="s">
-        <v>129</v>
-      </c>
-      <c r="D53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>136</v>
-      </c>
-      <c r="G53" t="s">
-        <v>137</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3915,25 +3915,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" t="s">
         <v>138</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
         <v>139</v>
       </c>
-      <c r="D54" t="s">
-        <v>130</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>140</v>
-      </c>
-      <c r="G54" t="s">
-        <v>141</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3948,25 +3948,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" t="s">
         <v>142</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>143</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>144</v>
       </c>
-      <c r="D55" t="s">
-        <v>145</v>
-      </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G55" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3981,25 +3981,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" t="s">
         <v>146</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
         <v>147</v>
       </c>
-      <c r="C56" t="s">
-        <v>144</v>
-      </c>
-      <c r="D56" t="s">
-        <v>145</v>
-      </c>
-      <c r="E56" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>148</v>
-      </c>
-      <c r="G56" t="s">
-        <v>149</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -4014,25 +4014,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B57">
         <v>470</v>
       </c>
       <c r="C57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" t="s">
         <v>144</v>
       </c>
-      <c r="D57" t="s">
-        <v>145</v>
-      </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
+        <v>150</v>
+      </c>
+      <c r="G57" t="s">
         <v>151</v>
-      </c>
-      <c r="G57" t="s">
-        <v>152</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4047,25 +4047,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58" t="s">
+        <v>144</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" t="s">
         <v>153</v>
       </c>
-      <c r="C58" t="s">
-        <v>144</v>
-      </c>
-      <c r="D58" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>154</v>
-      </c>
-      <c r="G58" t="s">
-        <v>155</v>
       </c>
       <c r="H58">
         <v>16</v>
@@ -4080,25 +4080,25 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" t="s">
         <v>156</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" t="s">
+        <v>144</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
         <v>157</v>
       </c>
-      <c r="C59" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" t="s">
-        <v>145</v>
-      </c>
-      <c r="E59" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>158</v>
-      </c>
-      <c r="G59" t="s">
-        <v>159</v>
       </c>
       <c r="H59">
         <v>4</v>
@@ -4113,13 +4113,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" t="s">
         <v>160</v>
       </c>
-      <c r="B60" t="s">
-        <v>161</v>
-      </c>
       <c r="C60" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D60" t="s">
         <v>111</v>
@@ -4128,10 +4128,10 @@
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G60" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4146,13 +4146,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>161</v>
+      </c>
+      <c r="B61" t="s">
         <v>162</v>
       </c>
-      <c r="B61" t="s">
-        <v>163</v>
-      </c>
       <c r="C61" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D61" t="s">
         <v>111</v>
@@ -4161,10 +4161,10 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4179,25 +4179,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" t="s">
         <v>164</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
         <v>165</v>
       </c>
-      <c r="C62" t="s">
-        <v>144</v>
-      </c>
-      <c r="D62" t="s">
-        <v>145</v>
-      </c>
-      <c r="E62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>166</v>
-      </c>
-      <c r="G62" t="s">
-        <v>167</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -4212,25 +4212,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B63">
         <v>200</v>
       </c>
       <c r="C63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" t="s">
         <v>196</v>
       </c>
-      <c r="D63" t="s">
-        <v>197</v>
-      </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G63" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H63">
         <v>24</v>
@@ -4245,25 +4245,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" t="s">
         <v>196</v>
       </c>
-      <c r="D64" t="s">
-        <v>197</v>
-      </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G64" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H64">
         <v>4</v>
@@ -4278,25 +4278,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" t="s">
+        <v>143</v>
+      </c>
+      <c r="D65" t="s">
         <v>144</v>
       </c>
-      <c r="D65" t="s">
-        <v>145</v>
-      </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
+        <v>168</v>
+      </c>
+      <c r="G65" t="s">
         <v>169</v>
-      </c>
-      <c r="G65" t="s">
-        <v>170</v>
       </c>
       <c r="H65">
         <v>6</v>
@@ -4311,25 +4311,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" t="s">
         <v>171</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>143</v>
+      </c>
+      <c r="D66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E66" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" t="s">
         <v>172</v>
       </c>
-      <c r="C66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" t="s">
-        <v>145</v>
-      </c>
-      <c r="E66" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>173</v>
-      </c>
-      <c r="G66" t="s">
-        <v>174</v>
       </c>
       <c r="H66">
         <v>15</v>
@@ -4344,25 +4344,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>174</v>
+      </c>
+      <c r="B67" t="s">
         <v>175</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>143</v>
+      </c>
+      <c r="D67" t="s">
+        <v>144</v>
+      </c>
+      <c r="E67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" t="s">
         <v>176</v>
       </c>
-      <c r="C67" t="s">
-        <v>144</v>
-      </c>
-      <c r="D67" t="s">
-        <v>145</v>
-      </c>
-      <c r="E67" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>177</v>
-      </c>
-      <c r="G67" t="s">
-        <v>178</v>
       </c>
       <c r="H67">
         <v>6</v>
@@ -4377,25 +4377,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" t="s">
         <v>179</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" t="s">
         <v>180</v>
       </c>
-      <c r="C68" t="s">
-        <v>144</v>
-      </c>
-      <c r="D68" t="s">
-        <v>145</v>
-      </c>
-      <c r="E68" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>181</v>
-      </c>
-      <c r="G68" t="s">
-        <v>182</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -4410,25 +4410,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" t="s">
         <v>183</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>143</v>
+      </c>
+      <c r="D69" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" t="s">
         <v>184</v>
       </c>
-      <c r="C69" t="s">
-        <v>144</v>
-      </c>
-      <c r="D69" t="s">
-        <v>145</v>
-      </c>
-      <c r="E69" t="s">
-        <v>19</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>185</v>
-      </c>
-      <c r="G69" t="s">
-        <v>186</v>
       </c>
       <c r="H69">
         <v>4</v>
@@ -4443,25 +4443,25 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>186</v>
+      </c>
+      <c r="B70" t="s">
         <v>187</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>143</v>
+      </c>
+      <c r="D70" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" t="s">
         <v>188</v>
       </c>
-      <c r="C70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D70" t="s">
-        <v>145</v>
-      </c>
-      <c r="E70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>189</v>
-      </c>
-      <c r="G70" t="s">
-        <v>190</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -4476,25 +4476,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>190</v>
+      </c>
+      <c r="B71" t="s">
         <v>191</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>143</v>
+      </c>
+      <c r="D71" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" t="s">
         <v>192</v>
       </c>
-      <c r="C71" t="s">
-        <v>144</v>
-      </c>
-      <c r="D71" t="s">
-        <v>145</v>
-      </c>
-      <c r="E71" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>193</v>
-      </c>
-      <c r="G71" t="s">
-        <v>194</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -4509,25 +4509,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B72">
         <v>0.3</v>
       </c>
       <c r="C72" t="s">
+        <v>195</v>
+      </c>
+      <c r="D72" t="s">
         <v>196</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" t="s">
         <v>197</v>
       </c>
-      <c r="E72" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>198</v>
-      </c>
-      <c r="G72" t="s">
-        <v>199</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -4542,25 +4542,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>199</v>
+      </c>
+      <c r="B73" t="s">
         <v>200</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>143</v>
+      </c>
+      <c r="D73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" t="s">
         <v>201</v>
       </c>
-      <c r="C73" t="s">
-        <v>144</v>
-      </c>
-      <c r="D73" t="s">
-        <v>145</v>
-      </c>
-      <c r="E73" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>202</v>
-      </c>
-      <c r="G73" t="s">
-        <v>203</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4575,25 +4575,25 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" t="s">
         <v>204</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
+        <v>143</v>
+      </c>
+      <c r="D74" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
         <v>205</v>
       </c>
-      <c r="C74" t="s">
-        <v>144</v>
-      </c>
-      <c r="D74" t="s">
-        <v>145</v>
-      </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>206</v>
-      </c>
-      <c r="G74" t="s">
-        <v>207</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4608,25 +4608,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" t="s">
         <v>208</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
         <v>209</v>
       </c>
-      <c r="C75" t="s">
-        <v>144</v>
-      </c>
-      <c r="D75" t="s">
-        <v>145</v>
-      </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>210</v>
-      </c>
-      <c r="G75" t="s">
-        <v>211</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4641,16 +4641,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>453</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
       </c>
       <c r="C76" t="s">
+        <v>143</v>
+      </c>
+      <c r="D76" t="s">
         <v>144</v>
-      </c>
-      <c r="D76" t="s">
-        <v>145</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
@@ -4659,7 +4659,7 @@
         <v>14</v>
       </c>
       <c r="H76">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
@@ -4668,25 +4668,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>211</v>
+      </c>
+      <c r="B77" t="s">
+        <v>212</v>
+      </c>
+      <c r="C77" t="s">
+        <v>143</v>
+      </c>
+      <c r="D77" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s">
         <v>213</v>
       </c>
-      <c r="B77" t="s">
+      <c r="G77" t="s">
         <v>214</v>
-      </c>
-      <c r="C77" t="s">
-        <v>144</v>
-      </c>
-      <c r="D77" t="s">
-        <v>145</v>
-      </c>
-      <c r="E77" t="s">
-        <v>19</v>
-      </c>
-      <c r="F77" t="s">
-        <v>215</v>
-      </c>
-      <c r="G77" t="s">
-        <v>216</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4701,13 +4701,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B78" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D78" t="s">
         <v>111</v>
@@ -4716,10 +4716,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G78" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4734,13 +4734,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B79" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C79" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D79" t="s">
         <v>111</v>
@@ -4749,10 +4749,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G79" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4767,25 +4767,25 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" t="s">
+        <v>220</v>
+      </c>
+      <c r="C80" t="s">
+        <v>143</v>
+      </c>
+      <c r="D80" t="s">
+        <v>144</v>
+      </c>
+      <c r="E80" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" t="s">
         <v>221</v>
       </c>
-      <c r="B80" t="s">
+      <c r="G80" t="s">
         <v>222</v>
-      </c>
-      <c r="C80" t="s">
-        <v>144</v>
-      </c>
-      <c r="D80" t="s">
-        <v>145</v>
-      </c>
-      <c r="E80" t="s">
-        <v>19</v>
-      </c>
-      <c r="F80" t="s">
-        <v>223</v>
-      </c>
-      <c r="G80" t="s">
-        <v>224</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -4800,25 +4800,25 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>223</v>
+      </c>
+      <c r="B81" t="s">
+        <v>224</v>
+      </c>
+      <c r="C81" t="s">
+        <v>143</v>
+      </c>
+      <c r="D81" t="s">
+        <v>144</v>
+      </c>
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s">
         <v>225</v>
       </c>
-      <c r="B81" t="s">
+      <c r="G81" t="s">
         <v>226</v>
-      </c>
-      <c r="C81" t="s">
-        <v>144</v>
-      </c>
-      <c r="D81" t="s">
-        <v>145</v>
-      </c>
-      <c r="E81" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81" t="s">
-        <v>227</v>
-      </c>
-      <c r="G81" t="s">
-        <v>228</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4833,25 +4833,25 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>415</v>
+      </c>
+      <c r="B82" t="s">
+        <v>413</v>
+      </c>
+      <c r="C82" t="s">
+        <v>413</v>
+      </c>
+      <c r="D82" t="s">
+        <v>414</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
+        <v>416</v>
+      </c>
+      <c r="G82" t="s">
         <v>417</v>
-      </c>
-      <c r="B82" t="s">
-        <v>415</v>
-      </c>
-      <c r="C82" t="s">
-        <v>415</v>
-      </c>
-      <c r="D82" t="s">
-        <v>416</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
-        <v>418</v>
-      </c>
-      <c r="G82" t="s">
-        <v>419</v>
       </c>
       <c r="H82">
         <v>2</v>
@@ -4866,25 +4866,25 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B83" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" t="s">
+        <v>227</v>
+      </c>
+      <c r="D83" t="s">
+        <v>228</v>
+      </c>
+      <c r="E83" t="s">
+        <v>19</v>
+      </c>
+      <c r="F83" t="s">
         <v>229</v>
       </c>
-      <c r="C83" t="s">
-        <v>229</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="G83" t="s">
         <v>230</v>
-      </c>
-      <c r="E83" t="s">
-        <v>19</v>
-      </c>
-      <c r="F83" t="s">
-        <v>231</v>
-      </c>
-      <c r="G83" t="s">
-        <v>232</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4899,25 +4899,25 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" t="s">
+        <v>232</v>
+      </c>
+      <c r="D84" t="s">
         <v>233</v>
       </c>
-      <c r="C84" t="s">
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
         <v>234</v>
       </c>
-      <c r="D84" t="s">
+      <c r="G84" t="s">
         <v>235</v>
-      </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" t="s">
-        <v>236</v>
-      </c>
-      <c r="G84" t="s">
-        <v>237</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4932,25 +4932,25 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B85" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C85" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D85" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E85" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F85" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G85" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4965,25 +4965,25 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B86" t="s">
+        <v>261</v>
+      </c>
+      <c r="C86" t="s">
+        <v>261</v>
+      </c>
+      <c r="D86" t="s">
+        <v>262</v>
+      </c>
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>263</v>
       </c>
-      <c r="C86" t="s">
-        <v>263</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
         <v>264</v>
-      </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
-        <v>265</v>
-      </c>
-      <c r="G86" t="s">
-        <v>266</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4998,25 +4998,25 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B87" t="s">
+        <v>237</v>
+      </c>
+      <c r="C87" t="s">
+        <v>237</v>
+      </c>
+      <c r="D87" t="s">
+        <v>238</v>
+      </c>
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>239</v>
       </c>
-      <c r="C87" t="s">
-        <v>239</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>240</v>
-      </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
-        <v>241</v>
-      </c>
-      <c r="G87" t="s">
-        <v>242</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -5031,25 +5031,25 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B88" t="s">
+        <v>242</v>
+      </c>
+      <c r="C88" t="s">
+        <v>242</v>
+      </c>
+      <c r="D88" t="s">
+        <v>243</v>
+      </c>
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>244</v>
       </c>
-      <c r="C88" t="s">
-        <v>244</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="G88" t="s">
         <v>245</v>
-      </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
-        <v>246</v>
-      </c>
-      <c r="G88" t="s">
-        <v>247</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -5064,25 +5064,25 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B89" t="s">
+        <v>247</v>
+      </c>
+      <c r="C89" t="s">
+        <v>247</v>
+      </c>
+      <c r="D89" t="s">
+        <v>248</v>
+      </c>
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>249</v>
       </c>
-      <c r="C89" t="s">
-        <v>249</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="G89" t="s">
         <v>250</v>
-      </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
-        <v>251</v>
-      </c>
-      <c r="G89" t="s">
-        <v>252</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -5097,25 +5097,25 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B90" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" t="s">
+        <v>252</v>
+      </c>
+      <c r="D90" t="s">
+        <v>253</v>
+      </c>
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>254</v>
       </c>
-      <c r="C90" t="s">
-        <v>254</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="G90" t="s">
         <v>255</v>
-      </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
-        <v>256</v>
-      </c>
-      <c r="G90" t="s">
-        <v>257</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5130,25 +5130,25 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B91" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C91" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D91" t="s">
+        <v>420</v>
+      </c>
+      <c r="E91" t="s">
+        <v>421</v>
+      </c>
+      <c r="F91" t="s">
         <v>422</v>
       </c>
-      <c r="E91" t="s">
+      <c r="G91" t="s">
         <v>423</v>
-      </c>
-      <c r="F91" t="s">
-        <v>424</v>
-      </c>
-      <c r="G91" t="s">
-        <v>425</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5163,25 +5163,25 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B92" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C92" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D92" t="s">
+        <v>426</v>
+      </c>
+      <c r="E92" t="s">
+        <v>421</v>
+      </c>
+      <c r="F92" t="s">
+        <v>427</v>
+      </c>
+      <c r="G92" t="s">
         <v>428</v>
-      </c>
-      <c r="E92" t="s">
-        <v>423</v>
-      </c>
-      <c r="F92" t="s">
-        <v>429</v>
-      </c>
-      <c r="G92" t="s">
-        <v>430</v>
       </c>
       <c r="H92">
         <v>5</v>
@@ -5196,25 +5196,25 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B93" t="s">
+        <v>265</v>
+      </c>
+      <c r="C93" t="s">
+        <v>265</v>
+      </c>
+      <c r="D93" t="s">
+        <v>266</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>267</v>
       </c>
-      <c r="C93" t="s">
-        <v>267</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="G93" t="s">
         <v>268</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
-        <v>269</v>
-      </c>
-      <c r="G93" t="s">
-        <v>270</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5229,25 +5229,25 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B94" t="s">
+        <v>270</v>
+      </c>
+      <c r="C94" t="s">
+        <v>270</v>
+      </c>
+      <c r="D94" t="s">
+        <v>271</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>272</v>
       </c>
-      <c r="C94" t="s">
-        <v>272</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="G94" t="s">
         <v>273</v>
-      </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>274</v>
-      </c>
-      <c r="G94" t="s">
-        <v>275</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5262,25 +5262,25 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B95" t="s">
+        <v>382</v>
+      </c>
+      <c r="C95" t="s">
+        <v>382</v>
+      </c>
+      <c r="D95" t="s">
+        <v>275</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
+        <v>383</v>
+      </c>
+      <c r="G95" t="s">
         <v>384</v>
-      </c>
-      <c r="C95" t="s">
-        <v>384</v>
-      </c>
-      <c r="D95" t="s">
-        <v>277</v>
-      </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
-        <v>385</v>
-      </c>
-      <c r="G95" t="s">
-        <v>386</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -5295,25 +5295,25 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B96" t="s">
+        <v>359</v>
+      </c>
+      <c r="C96" t="s">
+        <v>359</v>
+      </c>
+      <c r="D96" t="s">
         <v>361</v>
       </c>
-      <c r="C96" t="s">
-        <v>361</v>
-      </c>
-      <c r="D96" t="s">
-        <v>363</v>
-      </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
+        <v>360</v>
+      </c>
+      <c r="G96" t="s">
         <v>362</v>
-      </c>
-      <c r="G96" t="s">
-        <v>364</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -5328,25 +5328,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B97" t="s">
+        <v>409</v>
+      </c>
+      <c r="C97" t="s">
+        <v>409</v>
+      </c>
+      <c r="D97" t="s">
+        <v>410</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>411</v>
       </c>
-      <c r="C97" t="s">
-        <v>411</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="G97" t="s">
         <v>412</v>
-      </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
-        <v>413</v>
-      </c>
-      <c r="G97" t="s">
-        <v>414</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -5361,25 +5361,25 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" t="s">
+        <v>277</v>
+      </c>
+      <c r="C98" t="s">
+        <v>277</v>
+      </c>
+      <c r="D98" t="s">
         <v>278</v>
       </c>
-      <c r="B98" t="s">
+      <c r="E98" t="s">
         <v>279</v>
       </c>
-      <c r="C98" t="s">
-        <v>279</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="F98" t="s">
         <v>280</v>
       </c>
-      <c r="E98" t="s">
+      <c r="G98" t="s">
         <v>281</v>
-      </c>
-      <c r="F98" t="s">
-        <v>282</v>
-      </c>
-      <c r="G98" t="s">
-        <v>283</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -5394,25 +5394,25 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>282</v>
+      </c>
+      <c r="B99" t="s">
+        <v>283</v>
+      </c>
+      <c r="C99" t="s">
+        <v>283</v>
+      </c>
+      <c r="D99" t="s">
         <v>284</v>
       </c>
-      <c r="B99" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>285</v>
       </c>
-      <c r="C99" t="s">
-        <v>285</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="G99" t="s">
         <v>286</v>
-      </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
-        <v>287</v>
-      </c>
-      <c r="G99" t="s">
-        <v>288</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -5427,25 +5427,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>396</v>
+      </c>
+      <c r="B100" t="s">
+        <v>397</v>
+      </c>
+      <c r="C100" t="s">
         <v>398</v>
       </c>
-      <c r="B100" t="s">
+      <c r="D100" t="s">
+        <v>398</v>
+      </c>
+      <c r="E100" t="s">
+        <v>279</v>
+      </c>
+      <c r="F100" t="s">
         <v>399</v>
       </c>
-      <c r="C100" t="s">
+      <c r="G100" t="s">
         <v>400</v>
-      </c>
-      <c r="D100" t="s">
-        <v>400</v>
-      </c>
-      <c r="E100" t="s">
-        <v>281</v>
-      </c>
-      <c r="F100" t="s">
-        <v>401</v>
-      </c>
-      <c r="G100" t="s">
-        <v>402</v>
       </c>
       <c r="H100">
         <v>2</v>
@@ -5460,25 +5460,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B101" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C101" t="s">
+        <v>402</v>
+      </c>
+      <c r="D101" t="s">
+        <v>403</v>
+      </c>
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>404</v>
       </c>
-      <c r="D101" t="s">
+      <c r="G101" t="s">
         <v>405</v>
-      </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
-        <v>406</v>
-      </c>
-      <c r="G101" t="s">
-        <v>407</v>
       </c>
       <c r="H101">
         <v>1</v>

</xml_diff>

<commit_message>
Replaced clock fanout buffer with a 1:2 input:output model.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1243,18 +1243,6 @@
     <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
   </si>
   <si>
-    <t>NB3N551</t>
-  </si>
-  <si>
-    <t>SOIC8</t>
-  </si>
-  <si>
-    <t>NB3N551DGOS-ND</t>
-  </si>
-  <si>
-    <t>NB3N551DG</t>
-  </si>
-  <si>
     <t>XS2-L2-124QFN</t>
   </si>
   <si>
@@ -1336,9 +1324,6 @@
     <t>68683-305LF</t>
   </si>
   <si>
-    <t>U23</t>
-  </si>
-  <si>
     <t>U12, U19, U20, U21, U22</t>
   </si>
   <si>
@@ -1379,6 +1364,21 @@
   </si>
   <si>
     <t>LED1, LED2, LED3, LED4, LED5</t>
+  </si>
+  <si>
+    <t>296-27610-1-ND</t>
+  </si>
+  <si>
+    <t>CDCLVC1102PWR</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>CDCLVC1102</t>
+  </si>
+  <si>
+    <t>PW_R-PDSO-G08</t>
   </si>
 </sst>
 </file>
@@ -2209,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J109)</f>
-        <v>203.25399999999999</v>
+        <v>204.54399999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2955,25 +2955,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D24" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="G24" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -3258,7 +3258,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B33" t="s">
         <v>377</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3522,16 +3522,16 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D41" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G41">
         <v>702461004</v>
@@ -3642,22 +3642,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>431</v>
+      </c>
+      <c r="C45" t="s">
+        <v>432</v>
+      </c>
+      <c r="D45" t="s">
+        <v>433</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>434</v>
+      </c>
+      <c r="G45" t="s">
         <v>435</v>
-      </c>
-      <c r="C45" t="s">
-        <v>436</v>
-      </c>
-      <c r="D45" t="s">
-        <v>437</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>438</v>
-      </c>
-      <c r="G45" t="s">
-        <v>439</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3672,22 +3672,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>425</v>
+      </c>
+      <c r="C46" t="s">
+        <v>426</v>
+      </c>
+      <c r="D46" t="s">
+        <v>427</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>428</v>
+      </c>
+      <c r="G46" t="s">
         <v>429</v>
-      </c>
-      <c r="C46" t="s">
-        <v>430</v>
-      </c>
-      <c r="D46" t="s">
-        <v>431</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>432</v>
-      </c>
-      <c r="G46" t="s">
-        <v>433</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
@@ -4833,25 +4833,25 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B82" t="s">
+        <v>409</v>
+      </c>
+      <c r="C82" t="s">
+        <v>409</v>
+      </c>
+      <c r="D82" t="s">
+        <v>410</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
+        <v>412</v>
+      </c>
+      <c r="G82" t="s">
         <v>413</v>
-      </c>
-      <c r="C82" t="s">
-        <v>413</v>
-      </c>
-      <c r="D82" t="s">
-        <v>414</v>
-      </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" t="s">
-        <v>416</v>
-      </c>
-      <c r="G82" t="s">
-        <v>417</v>
       </c>
       <c r="H82">
         <v>2</v>
@@ -4866,7 +4866,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B83" t="s">
         <v>227</v>
@@ -4899,7 +4899,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B84" t="s">
         <v>231</v>
@@ -4944,13 +4944,13 @@
         <v>259</v>
       </c>
       <c r="E85" t="s">
+        <v>417</v>
+      </c>
+      <c r="F85" t="s">
+        <v>420</v>
+      </c>
+      <c r="G85" t="s">
         <v>421</v>
-      </c>
-      <c r="F85" t="s">
-        <v>424</v>
-      </c>
-      <c r="G85" t="s">
-        <v>425</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -5139,16 +5139,16 @@
         <v>407</v>
       </c>
       <c r="D91" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E91" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F91" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G91" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5163,7 +5163,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B92" t="s">
         <v>406</v>
@@ -5172,16 +5172,16 @@
         <v>406</v>
       </c>
       <c r="D92" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E92" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F92" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G92" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H92">
         <v>5</v>
@@ -5328,35 +5328,35 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B97" t="s">
-        <v>409</v>
+        <v>453</v>
       </c>
       <c r="C97" t="s">
-        <v>409</v>
+        <v>453</v>
       </c>
       <c r="D97" t="s">
-        <v>410</v>
+        <v>454</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>411</v>
+        <v>450</v>
       </c>
       <c r="G97" t="s">
-        <v>412</v>
+        <v>451</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <v>1.86</v>
+        <v>3.15</v>
       </c>
       <c r="J97">
         <f t="shared" si="1"/>
-        <v>1.86</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Upgraded U17 to the 1:3 input:output model.
The third output will be used for an ethernet PHY.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -1366,19 +1366,19 @@
     <t>LED1, LED2, LED3, LED4, LED5</t>
   </si>
   <si>
-    <t>296-27610-1-ND</t>
-  </si>
-  <si>
-    <t>CDCLVC1102PWR</t>
-  </si>
-  <si>
     <t>U17</t>
   </si>
   <si>
-    <t>CDCLVC1102</t>
-  </si>
-  <si>
     <t>PW_R-PDSO-G08</t>
+  </si>
+  <si>
+    <t>CDCLVC1103</t>
+  </si>
+  <si>
+    <t>296-27587-1-ND</t>
+  </si>
+  <si>
+    <t>CDCLVC1103PWR</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2210,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5328,25 +5328,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>450</v>
+      </c>
+      <c r="B97" t="s">
         <v>452</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
+        <v>452</v>
+      </c>
+      <c r="D97" t="s">
+        <v>451</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>453</v>
       </c>
-      <c r="C97" t="s">
-        <v>453</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="G97" t="s">
         <v>454</v>
-      </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
-        <v>450</v>
-      </c>
-      <c r="G97" t="s">
-        <v>451</v>
       </c>
       <c r="H97">
         <v>1</v>

</xml_diff>

<commit_message>
Added parts to board for the onboard ST-LINK/v2 debugger.
-Deleted JP22 as the U3 USB port will never be connected to power.
-Deleted JP2 (STM32 JTAG).
-Deleted old R5-R7 (old JP2 resistors).
-Cleaned up a bunch of outdated entries for passives in the BOM.
-Updated mini-USB port source to ME (it's also on DK) instead of SFE.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="463">
   <si>
     <t>Part</t>
   </si>
@@ -481,9 +481,6 @@
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
-    <t>R36, R78, R119, R135</t>
-  </si>
-  <si>
     <t>100K</t>
   </si>
   <si>
@@ -844,9 +841,6 @@
     <t>LGA16-4X4</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
     <t>MINI-USB-UX60-MB-5S8</t>
   </si>
   <si>
@@ -856,9 +850,6 @@
     <t>SFE</t>
   </si>
   <si>
-    <t>PRT-00587</t>
-  </si>
-  <si>
     <t>MUSB-05-X-D-SM-A</t>
   </si>
   <si>
@@ -1177,9 +1168,6 @@
     <t>ERJ-2GEJ201X</t>
   </si>
   <si>
-    <t>R65, R66, R67, R68</t>
-  </si>
-  <si>
     <t>R100, R101, R102, R103, R104, R105</t>
   </si>
   <si>
@@ -1240,9 +1228,6 @@
     <t>TXS0102</t>
   </si>
   <si>
-    <t>R2, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
-  </si>
-  <si>
     <t>XS2-L2-124QFN</t>
   </si>
   <si>
@@ -1339,9 +1324,6 @@
     <t>WM3478-ND</t>
   </si>
   <si>
-    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56</t>
-  </si>
-  <si>
     <t>C58, C59, C60, C61, C62, C63, C64, C65, C66, C67</t>
   </si>
   <si>
@@ -1360,12 +1342,6 @@
     <t>JP6, JP7, JP8, JP9, JP10, JP11, JP12, JP14, JP15, JP16, JP17, JP18, JP19</t>
   </si>
   <si>
-    <t>R139, R140, R141, R142, R143</t>
-  </si>
-  <si>
-    <t>LED1, LED2, LED3, LED4, LED5</t>
-  </si>
-  <si>
     <t>U17</t>
   </si>
   <si>
@@ -1379,6 +1355,54 @@
   </si>
   <si>
     <t>CDCLVC1103PWR</t>
+  </si>
+  <si>
+    <t>X1, X4</t>
+  </si>
+  <si>
+    <t>U23</t>
+  </si>
+  <si>
+    <t>STM32F103C8T6</t>
+  </si>
+  <si>
+    <t>TQFP48</t>
+  </si>
+  <si>
+    <t>511-STM32F103C8T6</t>
+  </si>
+  <si>
+    <t>AO3416</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>785-1011-1-ND</t>
+  </si>
+  <si>
+    <t>R10, R139, R140, R141, R142, R143</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6</t>
+  </si>
+  <si>
+    <t>R11, R12</t>
+  </si>
+  <si>
+    <t>R13, R14, R36, R78, R119, R135</t>
+  </si>
+  <si>
+    <t>R15, R65, R66, R67, R68</t>
+  </si>
+  <si>
+    <t>R2, R8, R9, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
+  </si>
+  <si>
+    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C86, C87, C88, C89</t>
+  </si>
+  <si>
+    <t>798-UX60-MB-5S8</t>
   </si>
 </sst>
 </file>
@@ -2207,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,12 +2283,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2279,10 +2303,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2295,8 +2319,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J109)</f>
-        <v>204.54399999999998</v>
+        <f>SUM(J2:J130)</f>
+        <v>211.66800000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2316,10 +2340,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G3" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2328,13 +2352,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J72" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J74" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>441</v>
+        <v>461</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2349,20 +2373,20 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H4">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.504</v>
+        <v>0.58800000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2406,10 +2430,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2422,7 +2446,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2466,10 +2490,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2499,10 +2523,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G9" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2532,10 +2556,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G10" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2548,7 +2572,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2601,10 +2625,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2634,10 +2658,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G13" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2650,7 +2674,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2670,10 +2694,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2686,7 +2710,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2730,10 +2754,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G16" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2811,10 +2835,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2827,7 +2851,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2847,10 +2871,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G20" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2904,10 +2928,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G22" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2922,10 +2946,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B23" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2937,10 +2961,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G23" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2955,25 +2979,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D24" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="G24" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -2988,10 +3012,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B25" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3003,10 +3027,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3069,10 +3093,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G27" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -3102,10 +3126,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G28" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3118,7 +3142,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3138,10 +3162,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G29" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3171,10 +3195,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G30" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3204,10 +3228,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G31" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3220,7 +3244,7 @@
         <v>2.7</v>
       </c>
       <c r="L31" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3240,10 +3264,10 @@
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G32" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -3258,25 +3282,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B33" t="s">
+        <v>374</v>
+      </c>
+      <c r="C33" t="s">
+        <v>375</v>
+      </c>
+      <c r="D33" t="s">
+        <v>376</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>377</v>
       </c>
-      <c r="C33" t="s">
+      <c r="G33" t="s">
         <v>378</v>
-      </c>
-      <c r="D33" t="s">
-        <v>379</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
-        <v>380</v>
-      </c>
-      <c r="G33" t="s">
-        <v>381</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -3294,22 +3318,22 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3357,7 +3381,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
@@ -3369,10 +3393,10 @@
         <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F36" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3387,7 +3411,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -3399,10 +3423,10 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F37" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3429,7 +3453,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3453,7 +3477,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3468,10 +3492,10 @@
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G39" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H39">
         <v>3</v>
@@ -3486,7 +3510,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3522,16 +3546,16 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D41" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="G41">
         <v>702461004</v>
@@ -3549,7 +3573,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
@@ -3564,10 +3588,10 @@
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G42" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H42">
         <v>3</v>
@@ -3582,22 +3606,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C43" t="s">
+        <v>360</v>
+      </c>
+      <c r="D43" t="s">
+        <v>361</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>362</v>
+      </c>
+      <c r="G43" t="s">
         <v>363</v>
-      </c>
-      <c r="D43" t="s">
-        <v>364</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>365</v>
-      </c>
-      <c r="G43" t="s">
-        <v>366</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3612,22 +3636,22 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
       </c>
       <c r="D44" t="s">
+        <v>368</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>370</v>
+      </c>
+      <c r="G44" t="s">
         <v>371</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>373</v>
-      </c>
-      <c r="G44" t="s">
-        <v>374</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3642,22 +3666,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C45" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D45" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G45" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3672,22 +3696,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C46" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G46" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -3834,7 +3858,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -3849,7 +3873,7 @@
         <v>14</v>
       </c>
       <c r="H51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
@@ -3858,70 +3882,70 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>453</v>
       </c>
       <c r="B52" t="s">
         <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>133</v>
+        <v>129</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>454</v>
       </c>
       <c r="G52" t="s">
-        <v>14</v>
+        <v>452</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0.55000000000000004</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>375</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G53" t="s">
-        <v>136</v>
+        <v>14</v>
       </c>
       <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D54" t="s">
         <v>129</v>
@@ -3930,61 +3954,61 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G54" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>141</v>
+        <v>373</v>
       </c>
       <c r="B55" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C55" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>291</v>
+        <v>139</v>
       </c>
       <c r="G55" t="s">
-        <v>292</v>
+        <v>140</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
         <v>143</v>
@@ -3996,28 +4020,28 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>147</v>
+        <v>288</v>
       </c>
       <c r="G56" t="s">
-        <v>148</v>
+        <v>289</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="B57">
-        <v>470</v>
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>146</v>
       </c>
       <c r="C57" t="s">
         <v>143</v>
@@ -4029,10 +4053,10 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4047,10 +4071,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>408</v>
-      </c>
-      <c r="B58" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="B58">
+        <v>470</v>
       </c>
       <c r="C58" t="s">
         <v>143</v>
@@ -4062,28 +4086,28 @@
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G58" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H58">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>460</v>
       </c>
       <c r="B59" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
         <v>143</v>
@@ -4095,193 +4119,181 @@
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G59" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>457</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C60" t="s">
-        <v>293</v>
+        <v>194</v>
       </c>
       <c r="D60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" t="s">
-        <v>294</v>
-      </c>
-      <c r="G60" t="s">
-        <v>295</v>
+        <v>195</v>
       </c>
       <c r="H60">
-        <v>1</v>
-      </c>
-      <c r="I60">
-        <v>0.15</v>
+        <v>2</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>458</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>293</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>300</v>
+        <v>156</v>
       </c>
       <c r="G61" t="s">
-        <v>301</v>
+        <v>157</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I61">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>163</v>
-      </c>
-      <c r="B62" t="s">
-        <v>164</v>
+        <v>459</v>
+      </c>
+      <c r="B62">
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D62" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>165</v>
+        <v>385</v>
       </c>
       <c r="G62" t="s">
-        <v>166</v>
+        <v>386</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
       <c r="J62">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>H62*I62</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>167</v>
-      </c>
-      <c r="B63">
-        <v>200</v>
+        <v>158</v>
+      </c>
+      <c r="B63" t="s">
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>290</v>
       </c>
       <c r="D63" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>385</v>
+        <v>291</v>
       </c>
       <c r="G63" t="s">
-        <v>386</v>
+        <v>292</v>
       </c>
       <c r="H63">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>387</v>
-      </c>
-      <c r="B64">
-        <v>100</v>
+        <v>160</v>
+      </c>
+      <c r="B64" t="s">
+        <v>161</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>290</v>
       </c>
       <c r="D64" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>389</v>
+        <v>297</v>
       </c>
       <c r="G64" t="s">
-        <v>390</v>
+        <v>298</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I64">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>388</v>
-      </c>
-      <c r="B65">
-        <v>100</v>
+        <v>162</v>
+      </c>
+      <c r="B65" t="s">
+        <v>163</v>
       </c>
       <c r="C65" t="s">
         <v>143</v>
@@ -4293,61 +4305,61 @@
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G65" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>170</v>
-      </c>
-      <c r="B66" t="s">
-        <v>171</v>
+        <v>166</v>
+      </c>
+      <c r="B66">
+        <v>200</v>
       </c>
       <c r="C66" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D66" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>172</v>
+        <v>382</v>
       </c>
       <c r="G66" t="s">
-        <v>173</v>
+        <v>383</v>
       </c>
       <c r="H66">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I66">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>174</v>
-      </c>
-      <c r="B67" t="s">
-        <v>175</v>
+        <v>384</v>
+      </c>
+      <c r="B67">
+        <v>100</v>
       </c>
       <c r="C67" t="s">
         <v>143</v>
@@ -4359,10 +4371,10 @@
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G67" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H67">
         <v>6</v>
@@ -4377,10 +4389,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C68" t="s">
         <v>143</v>
@@ -4392,28 +4404,28 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="G68" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H68">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B69" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C69" t="s">
         <v>143</v>
@@ -4425,28 +4437,28 @@
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G69" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H69">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I69">
         <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C70" t="s">
         <v>143</v>
@@ -4458,28 +4470,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="G70" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B71" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C71" t="s">
         <v>143</v>
@@ -4491,61 +4503,61 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G71" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I71">
         <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>194</v>
-      </c>
-      <c r="B72">
-        <v>0.3</v>
+        <v>185</v>
+      </c>
+      <c r="B72" t="s">
+        <v>186</v>
       </c>
       <c r="C72" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="D72" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="G72" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B73" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C73" t="s">
         <v>143</v>
@@ -4557,10 +4569,10 @@
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="G73" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -4569,109 +4581,115 @@
         <v>0.04</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J101" si="1">H73*I73</f>
+        <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>193</v>
+      </c>
+      <c r="B74">
+        <v>0.3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>194</v>
+      </c>
+      <c r="D74" t="s">
+        <v>195</v>
+      </c>
+      <c r="E74" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
+        <v>196</v>
+      </c>
+      <c r="G74" t="s">
+        <v>197</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>0.59</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>198</v>
+      </c>
+      <c r="B75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
+        <v>200</v>
+      </c>
+      <c r="G75" t="s">
+        <v>201</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>0.04</v>
+      </c>
+      <c r="J75">
+        <f t="shared" ref="J75:J104" si="1">H75*I75</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>202</v>
+      </c>
+      <c r="B76" t="s">
         <v>203</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C76" t="s">
+        <v>143</v>
+      </c>
+      <c r="D76" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
         <v>204</v>
       </c>
-      <c r="C74" t="s">
-        <v>143</v>
-      </c>
-      <c r="D74" t="s">
-        <v>144</v>
-      </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="G76" t="s">
         <v>205</v>
       </c>
-      <c r="G74" t="s">
-        <v>206</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74">
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
         <v>0.04</v>
       </c>
-      <c r="J74">
+      <c r="J76">
         <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>207</v>
-      </c>
-      <c r="B75" t="s">
-        <v>208</v>
-      </c>
-      <c r="C75" t="s">
-        <v>143</v>
-      </c>
-      <c r="D75" t="s">
-        <v>144</v>
-      </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" t="s">
-        <v>209</v>
-      </c>
-      <c r="G75" t="s">
-        <v>210</v>
-      </c>
-      <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75">
-        <v>0.04</v>
-      </c>
-      <c r="J75">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>448</v>
-      </c>
-      <c r="B76" t="s">
-        <v>14</v>
-      </c>
-      <c r="C76" t="s">
-        <v>143</v>
-      </c>
-      <c r="D76" t="s">
-        <v>144</v>
-      </c>
-      <c r="E76" t="s">
-        <v>19</v>
-      </c>
-      <c r="G76" t="s">
-        <v>14</v>
-      </c>
-      <c r="H76">
-        <v>5</v>
-      </c>
-      <c r="J76">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C77" t="s">
         <v>143</v>
@@ -4683,10 +4701,10 @@
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G77" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4701,792 +4719,885 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>215</v>
+        <v>455</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>293</v>
+        <v>143</v>
       </c>
       <c r="D78" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
-      <c r="F78" t="s">
-        <v>296</v>
-      </c>
       <c r="G78" t="s">
-        <v>297</v>
+        <v>14</v>
       </c>
       <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78">
-        <v>0.15</v>
+        <v>6</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B79" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C79" t="s">
-        <v>293</v>
+        <v>143</v>
       </c>
       <c r="D79" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>298</v>
+        <v>212</v>
       </c>
       <c r="G79" t="s">
-        <v>299</v>
+        <v>213</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B80" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C80" t="s">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="D80" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>221</v>
+        <v>293</v>
       </c>
       <c r="G80" t="s">
-        <v>222</v>
+        <v>294</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="D81" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81" t="s">
-        <v>225</v>
+        <v>295</v>
       </c>
       <c r="G81" t="s">
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>411</v>
+        <v>218</v>
       </c>
       <c r="B82" t="s">
-        <v>409</v>
+        <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>409</v>
+        <v>143</v>
       </c>
       <c r="D82" t="s">
-        <v>410</v>
+        <v>144</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>412</v>
+        <v>220</v>
       </c>
       <c r="G82" t="s">
-        <v>413</v>
+        <v>221</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I82">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>30.2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>414</v>
+        <v>222</v>
       </c>
       <c r="B83" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C83" t="s">
-        <v>227</v>
+        <v>143</v>
       </c>
       <c r="D83" t="s">
-        <v>228</v>
+        <v>144</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G83" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>6.6</v>
+        <v>0.04</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J92" si="2">H83*I83</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>0.04</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="B84" t="s">
+        <v>404</v>
+      </c>
+      <c r="C84" t="s">
+        <v>404</v>
+      </c>
+      <c r="D84" t="s">
+        <v>405</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
+        <v>407</v>
+      </c>
+      <c r="G84" t="s">
+        <v>408</v>
+      </c>
+      <c r="H84">
+        <v>2</v>
+      </c>
+      <c r="I84">
+        <v>15.1</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="1"/>
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>409</v>
+      </c>
+      <c r="B85" t="s">
+        <v>226</v>
+      </c>
+      <c r="C85" t="s">
+        <v>226</v>
+      </c>
+      <c r="D85" t="s">
+        <v>227</v>
+      </c>
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G85" t="s">
+        <v>229</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>6.6</v>
+      </c>
+      <c r="J85">
+        <f t="shared" ref="J85:J94" si="2">H85*I85</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>410</v>
+      </c>
+      <c r="B86" t="s">
+        <v>230</v>
+      </c>
+      <c r="C86" t="s">
         <v>231</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D86" t="s">
         <v>232</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>233</v>
       </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="G86" t="s">
         <v>234</v>
       </c>
-      <c r="G84" t="s">
-        <v>235</v>
-      </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84">
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
         <v>0.79</v>
       </c>
-      <c r="J84">
+      <c r="J86">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>236</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>235</v>
+      </c>
+      <c r="B87" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" t="s">
+        <v>257</v>
+      </c>
+      <c r="D87" t="s">
         <v>258</v>
       </c>
-      <c r="C85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D85" t="s">
-        <v>259</v>
-      </c>
-      <c r="E85" t="s">
-        <v>417</v>
-      </c>
-      <c r="F85" t="s">
-        <v>420</v>
-      </c>
-      <c r="G85" t="s">
-        <v>421</v>
-      </c>
-      <c r="H85">
-        <v>1</v>
-      </c>
-      <c r="I85">
+      <c r="E87" t="s">
+        <v>412</v>
+      </c>
+      <c r="F87" t="s">
+        <v>415</v>
+      </c>
+      <c r="G87" t="s">
+        <v>416</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
         <v>0.45</v>
       </c>
-      <c r="J85">
+      <c r="J87">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>241</v>
-      </c>
-      <c r="B86" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" t="s">
+        <v>260</v>
+      </c>
+      <c r="C88" t="s">
+        <v>260</v>
+      </c>
+      <c r="D88" t="s">
         <v>261</v>
       </c>
-      <c r="C86" t="s">
-        <v>261</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>262</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="G88" t="s">
         <v>263</v>
       </c>
-      <c r="G86" t="s">
-        <v>264</v>
-      </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
         <v>0.47</v>
       </c>
-      <c r="J86">
+      <c r="J88">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>246</v>
-      </c>
-      <c r="B87" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>245</v>
+      </c>
+      <c r="B89" t="s">
+        <v>236</v>
+      </c>
+      <c r="C89" t="s">
+        <v>236</v>
+      </c>
+      <c r="D89" t="s">
         <v>237</v>
       </c>
-      <c r="C87" t="s">
-        <v>237</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>238</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="G89" t="s">
         <v>239</v>
       </c>
-      <c r="G87" t="s">
-        <v>240</v>
-      </c>
-      <c r="H87">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>0.67</v>
       </c>
-      <c r="J87">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>251</v>
-      </c>
-      <c r="B88" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>250</v>
+      </c>
+      <c r="B90" t="s">
+        <v>241</v>
+      </c>
+      <c r="C90" t="s">
+        <v>241</v>
+      </c>
+      <c r="D90" t="s">
         <v>242</v>
       </c>
-      <c r="C88" t="s">
-        <v>242</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>243</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="G90" t="s">
         <v>244</v>
       </c>
-      <c r="G88" t="s">
-        <v>245</v>
-      </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>6.63</v>
       </c>
-      <c r="J88">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>256</v>
-      </c>
-      <c r="B89" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>255</v>
+      </c>
+      <c r="B91" t="s">
+        <v>246</v>
+      </c>
+      <c r="C91" t="s">
+        <v>246</v>
+      </c>
+      <c r="D91" t="s">
         <v>247</v>
       </c>
-      <c r="C89" t="s">
-        <v>247</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>248</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="G91" t="s">
         <v>249</v>
       </c>
-      <c r="G89" t="s">
-        <v>250</v>
-      </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>1.67</v>
       </c>
-      <c r="J89">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>257</v>
-      </c>
-      <c r="B90" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>256</v>
+      </c>
+      <c r="B92" t="s">
+        <v>251</v>
+      </c>
+      <c r="C92" t="s">
+        <v>251</v>
+      </c>
+      <c r="D92" t="s">
         <v>252</v>
       </c>
-      <c r="C90" t="s">
-        <v>252</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>253</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="G92" t="s">
         <v>254</v>
       </c>
-      <c r="G90" t="s">
-        <v>255</v>
-      </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>5.88</v>
       </c>
-      <c r="J90">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>260</v>
-      </c>
-      <c r="B91" t="s">
-        <v>407</v>
-      </c>
-      <c r="C91" t="s">
-        <v>407</v>
-      </c>
-      <c r="D91" t="s">
-        <v>416</v>
-      </c>
-      <c r="E91" t="s">
-        <v>417</v>
-      </c>
-      <c r="F91" t="s">
-        <v>418</v>
-      </c>
-      <c r="G91" t="s">
-        <v>419</v>
-      </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>259</v>
+      </c>
+      <c r="B93" t="s">
+        <v>403</v>
+      </c>
+      <c r="C93" t="s">
+        <v>403</v>
+      </c>
+      <c r="D93" t="s">
+        <v>411</v>
+      </c>
+      <c r="E93" t="s">
+        <v>412</v>
+      </c>
+      <c r="F93" t="s">
+        <v>413</v>
+      </c>
+      <c r="G93" t="s">
+        <v>414</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>1.23</v>
       </c>
-      <c r="J91">
+      <c r="J93">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>436</v>
-      </c>
-      <c r="B92" t="s">
-        <v>406</v>
-      </c>
-      <c r="C92" t="s">
-        <v>406</v>
-      </c>
-      <c r="D92" t="s">
-        <v>422</v>
-      </c>
-      <c r="E92" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>431</v>
+      </c>
+      <c r="B94" t="s">
+        <v>402</v>
+      </c>
+      <c r="C94" t="s">
+        <v>402</v>
+      </c>
+      <c r="D94" t="s">
         <v>417</v>
       </c>
-      <c r="F92" t="s">
-        <v>423</v>
-      </c>
-      <c r="G92" t="s">
-        <v>424</v>
-      </c>
-      <c r="H92">
+      <c r="E94" t="s">
+        <v>412</v>
+      </c>
+      <c r="F94" t="s">
+        <v>418</v>
+      </c>
+      <c r="G94" t="s">
+        <v>419</v>
+      </c>
+      <c r="H94">
         <v>5</v>
       </c>
-      <c r="I92">
+      <c r="I94">
         <v>2.76</v>
       </c>
-      <c r="J92">
+      <c r="J94">
         <f t="shared" si="2"/>
         <v>13.799999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>269</v>
-      </c>
-      <c r="B93" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>268</v>
+      </c>
+      <c r="B95" t="s">
+        <v>264</v>
+      </c>
+      <c r="C95" t="s">
+        <v>264</v>
+      </c>
+      <c r="D95" t="s">
         <v>265</v>
       </c>
-      <c r="C93" t="s">
-        <v>265</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>266</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G95" t="s">
         <v>267</v>
       </c>
-      <c r="G93" t="s">
-        <v>268</v>
-      </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>3.79</v>
       </c>
-      <c r="J93">
+      <c r="J95">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>274</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>273</v>
+      </c>
+      <c r="B96" t="s">
+        <v>269</v>
+      </c>
+      <c r="C96" t="s">
+        <v>269</v>
+      </c>
+      <c r="D96" t="s">
         <v>270</v>
       </c>
-      <c r="C94" t="s">
-        <v>270</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
         <v>271</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="G96" t="s">
         <v>272</v>
       </c>
-      <c r="G94" t="s">
-        <v>273</v>
-      </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>1.57</v>
       </c>
-      <c r="J94">
+      <c r="J96">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>358</v>
-      </c>
-      <c r="B95" t="s">
-        <v>382</v>
-      </c>
-      <c r="C95" t="s">
-        <v>382</v>
-      </c>
-      <c r="D95" t="s">
-        <v>275</v>
-      </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
-        <v>383</v>
-      </c>
-      <c r="G95" t="s">
-        <v>384</v>
-      </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>355</v>
+      </c>
+      <c r="B97" t="s">
+        <v>379</v>
+      </c>
+      <c r="C97" t="s">
+        <v>379</v>
+      </c>
+      <c r="D97" t="s">
+        <v>274</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
+        <v>380</v>
+      </c>
+      <c r="G97" t="s">
+        <v>381</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
         <v>8.48</v>
       </c>
-      <c r="J95">
+      <c r="J97">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>401</v>
-      </c>
-      <c r="B96" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>397</v>
+      </c>
+      <c r="B98" t="s">
+        <v>356</v>
+      </c>
+      <c r="C98" t="s">
+        <v>356</v>
+      </c>
+      <c r="D98" t="s">
+        <v>358</v>
+      </c>
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
+        <v>357</v>
+      </c>
+      <c r="G98" t="s">
         <v>359</v>
       </c>
-      <c r="C96" t="s">
-        <v>359</v>
-      </c>
-      <c r="D96" t="s">
-        <v>361</v>
-      </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
-        <v>360</v>
-      </c>
-      <c r="G96" t="s">
-        <v>362</v>
-      </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>6.84</v>
       </c>
-      <c r="J96">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>450</v>
-      </c>
-      <c r="B97" t="s">
-        <v>452</v>
-      </c>
-      <c r="C97" t="s">
-        <v>452</v>
-      </c>
-      <c r="D97" t="s">
-        <v>451</v>
-      </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
-        <v>453</v>
-      </c>
-      <c r="G97" t="s">
-        <v>454</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>442</v>
+      </c>
+      <c r="B99" t="s">
+        <v>444</v>
+      </c>
+      <c r="C99" t="s">
+        <v>444</v>
+      </c>
+      <c r="D99" t="s">
+        <v>443</v>
+      </c>
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
+        <v>445</v>
+      </c>
+      <c r="G99" t="s">
+        <v>446</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>3.15</v>
       </c>
-      <c r="J97">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>3.15</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>448</v>
+      </c>
+      <c r="B100" t="s">
+        <v>449</v>
+      </c>
+      <c r="C100" t="s">
+        <v>449</v>
+      </c>
+      <c r="D100" t="s">
+        <v>450</v>
+      </c>
+      <c r="E100" t="s">
+        <v>412</v>
+      </c>
+      <c r="F100" t="s">
+        <v>451</v>
+      </c>
+      <c r="G100" t="s">
+        <v>449</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
+        <v>5.71</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="1"/>
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>447</v>
+      </c>
+      <c r="B101" t="s">
+        <v>275</v>
+      </c>
+      <c r="C101" t="s">
+        <v>275</v>
+      </c>
+      <c r="D101" t="s">
         <v>276</v>
       </c>
-      <c r="B98" t="s">
-        <v>277</v>
-      </c>
-      <c r="C98" t="s">
-        <v>277</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E101" t="s">
+        <v>412</v>
+      </c>
+      <c r="F101" t="s">
+        <v>462</v>
+      </c>
+      <c r="G101" t="s">
         <v>278</v>
       </c>
-      <c r="E98" t="s">
+      <c r="H101">
+        <v>2</v>
+      </c>
+      <c r="I101">
+        <v>1.26</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="1"/>
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>279</v>
       </c>
-      <c r="F98" t="s">
+      <c r="B102" t="s">
         <v>280</v>
       </c>
-      <c r="G98" t="s">
+      <c r="C102" t="s">
+        <v>280</v>
+      </c>
+      <c r="D102" t="s">
         <v>281</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
-        <v>1.5</v>
-      </c>
-      <c r="J98">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>282</v>
       </c>
-      <c r="B99" t="s">
+      <c r="G102" t="s">
         <v>283</v>
       </c>
-      <c r="C99" t="s">
-        <v>283</v>
-      </c>
-      <c r="D99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
-        <v>285</v>
-      </c>
-      <c r="G99" t="s">
-        <v>286</v>
-      </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>2.96</v>
       </c>
-      <c r="J99">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>392</v>
+      </c>
+      <c r="B103" t="s">
+        <v>393</v>
+      </c>
+      <c r="C103" t="s">
+        <v>394</v>
+      </c>
+      <c r="D103" t="s">
+        <v>394</v>
+      </c>
+      <c r="E103" t="s">
+        <v>277</v>
+      </c>
+      <c r="F103" t="s">
+        <v>395</v>
+      </c>
+      <c r="G103" t="s">
         <v>396</v>
       </c>
-      <c r="B100" t="s">
-        <v>397</v>
-      </c>
-      <c r="C100" t="s">
-        <v>398</v>
-      </c>
-      <c r="D100" t="s">
-        <v>398</v>
-      </c>
-      <c r="E100" t="s">
-        <v>279</v>
-      </c>
-      <c r="F100" t="s">
-        <v>399</v>
-      </c>
-      <c r="G100" t="s">
-        <v>400</v>
-      </c>
-      <c r="H100">
+      <c r="H103">
         <v>2</v>
       </c>
-      <c r="I100">
+      <c r="I103">
         <v>0.95</v>
       </c>
-      <c r="J100">
+      <c r="J103">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>287</v>
-      </c>
-      <c r="B101" t="s">
-        <v>288</v>
-      </c>
-      <c r="C101" t="s">
-        <v>402</v>
-      </c>
-      <c r="D101" t="s">
-        <v>403</v>
-      </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
-        <v>404</v>
-      </c>
-      <c r="G101" t="s">
-        <v>405</v>
-      </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>284</v>
+      </c>
+      <c r="B104" t="s">
+        <v>285</v>
+      </c>
+      <c r="C104" t="s">
+        <v>398</v>
+      </c>
+      <c r="D104" t="s">
+        <v>399</v>
+      </c>
+      <c r="E104" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" t="s">
+        <v>400</v>
+      </c>
+      <c r="G104" t="s">
+        <v>401</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
         <v>1.99</v>
       </c>
-      <c r="J101">
+      <c r="J104">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Added resistors to X1 matching the STLINK/v2 USB resistors.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="466">
   <si>
     <t>Part</t>
   </si>
@@ -1396,13 +1396,22 @@
     <t>R15, R65, R66, R67, R68</t>
   </si>
   <si>
-    <t>R2, R8, R9, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
-  </si>
-  <si>
     <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C86, C87, C88, C89</t>
   </si>
   <si>
     <t>798-UX60-MB-5S8</t>
+  </si>
+  <si>
+    <t>R6, R7, R17, R18</t>
+  </si>
+  <si>
+    <t>R2, R8, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
+  </si>
+  <si>
+    <t>R9, R19</t>
+  </si>
+  <si>
+    <t>R5, R16</t>
   </si>
 </sst>
 </file>
@@ -2231,10 +2240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="J101" sqref="J101"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,8 +2328,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J130)</f>
-        <v>211.66800000000001</v>
+        <f>SUM(J2:J133)</f>
+        <v>211.58799999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2352,13 +2361,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J74" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J77" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -4104,97 +4113,77 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" t="s">
-        <v>153</v>
-      </c>
-      <c r="G59" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
       <c r="H59">
-        <v>7</v>
-      </c>
-      <c r="I59">
-        <v>0.04</v>
-      </c>
-      <c r="J59">
-        <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C60" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="D60" t="s">
-        <v>195</v>
+        <v>144</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" t="s">
+        <v>154</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <v>0.04</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>458</v>
-      </c>
-      <c r="B61" t="s">
-        <v>155</v>
+        <v>462</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D61" t="s">
-        <v>144</v>
-      </c>
-      <c r="E61" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" t="s">
-        <v>156</v>
-      </c>
-      <c r="G61" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="H61">
-        <v>6</v>
-      </c>
-      <c r="I61">
-        <v>0.04</v>
-      </c>
-      <c r="J61">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>459</v>
-      </c>
-      <c r="B62">
-        <v>100</v>
+        <v>464</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
       </c>
       <c r="C62" t="s">
         <v>194</v>
@@ -4202,197 +4191,169 @@
       <c r="D62" t="s">
         <v>195</v>
       </c>
-      <c r="E62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
-        <v>385</v>
-      </c>
-      <c r="G62" t="s">
-        <v>386</v>
-      </c>
       <c r="H62">
-        <v>5</v>
-      </c>
-      <c r="I62">
-        <v>0.04</v>
-      </c>
-      <c r="J62">
-        <f>H62*I62</f>
-        <v>0.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>457</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="D63" t="s">
-        <v>111</v>
-      </c>
-      <c r="E63" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" t="s">
-        <v>291</v>
-      </c>
-      <c r="G63" t="s">
-        <v>292</v>
+        <v>195</v>
       </c>
       <c r="H63">
-        <v>1</v>
-      </c>
-      <c r="I63">
-        <v>0.15</v>
+        <v>2</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>160</v>
+        <v>458</v>
       </c>
       <c r="B64" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>290</v>
+        <v>143</v>
       </c>
       <c r="D64" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>297</v>
+        <v>156</v>
       </c>
       <c r="G64" t="s">
-        <v>298</v>
+        <v>157</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I64">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>162</v>
-      </c>
-      <c r="B65" t="s">
-        <v>163</v>
+        <v>459</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D65" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>164</v>
+        <v>385</v>
       </c>
       <c r="G65" t="s">
-        <v>165</v>
+        <v>386</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I65">
         <v>0.04</v>
       </c>
       <c r="J65">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>H65*I65</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>166</v>
-      </c>
-      <c r="B66">
-        <v>200</v>
+        <v>158</v>
+      </c>
+      <c r="B66" t="s">
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="D66" t="s">
-        <v>195</v>
+        <v>111</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>382</v>
+        <v>291</v>
       </c>
       <c r="G66" t="s">
-        <v>383</v>
+        <v>292</v>
       </c>
       <c r="H66">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>384</v>
-      </c>
-      <c r="B67">
-        <v>100</v>
+        <v>160</v>
+      </c>
+      <c r="B67" t="s">
+        <v>161</v>
       </c>
       <c r="C67" t="s">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>167</v>
+        <v>297</v>
       </c>
       <c r="G67" t="s">
-        <v>168</v>
+        <v>298</v>
       </c>
       <c r="H67">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B68" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C68" t="s">
         <v>143</v>
@@ -4404,61 +4365,61 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G68" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H68">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I68">
         <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>173</v>
-      </c>
-      <c r="B69" t="s">
-        <v>174</v>
+        <v>166</v>
+      </c>
+      <c r="B69">
+        <v>200</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D69" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="G69" t="s">
-        <v>176</v>
+        <v>383</v>
       </c>
       <c r="H69">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="I69">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>177</v>
-      </c>
-      <c r="B70" t="s">
-        <v>178</v>
+        <v>384</v>
+      </c>
+      <c r="B70">
+        <v>100</v>
       </c>
       <c r="C70" t="s">
         <v>143</v>
@@ -4470,28 +4431,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="G70" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="H70">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C71" t="s">
         <v>143</v>
@@ -4503,28 +4464,28 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G71" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="H71">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I71">
         <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B72" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C72" t="s">
         <v>143</v>
@@ -4536,28 +4497,28 @@
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="G72" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I72">
         <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C73" t="s">
         <v>143</v>
@@ -4569,61 +4530,61 @@
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G73" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I73">
         <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>193</v>
-      </c>
-      <c r="B74">
-        <v>0.3</v>
+        <v>181</v>
+      </c>
+      <c r="B74" t="s">
+        <v>182</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="D74" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G74" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C75" t="s">
         <v>143</v>
@@ -4635,10 +4596,10 @@
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G75" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4647,16 +4608,16 @@
         <v>0.04</v>
       </c>
       <c r="J75">
-        <f t="shared" ref="J75:J104" si="1">H75*I75</f>
+        <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B76" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C76" t="s">
         <v>143</v>
@@ -4668,10 +4629,10 @@
         <v>19</v>
       </c>
       <c r="F76" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G76" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4680,49 +4641,49 @@
         <v>0.04</v>
       </c>
       <c r="J76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>206</v>
-      </c>
-      <c r="B77" t="s">
-        <v>207</v>
+        <v>193</v>
+      </c>
+      <c r="B77">
+        <v>0.3</v>
       </c>
       <c r="C77" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D77" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G77" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J77">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>455</v>
+        <v>198</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>199</v>
       </c>
       <c r="C78" t="s">
         <v>143</v>
@@ -4733,23 +4694,29 @@
       <c r="E78" t="s">
         <v>19</v>
       </c>
+      <c r="F78" t="s">
+        <v>200</v>
+      </c>
       <c r="G78" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="H78">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>0.04</v>
       </c>
       <c r="J78">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="J78:J107" si="1">H78*I78</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B79" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C79" t="s">
         <v>143</v>
@@ -4761,10 +4728,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G79" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4779,76 +4746,70 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C80" t="s">
-        <v>290</v>
+        <v>143</v>
       </c>
       <c r="D80" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>293</v>
+        <v>208</v>
       </c>
       <c r="G80" t="s">
-        <v>294</v>
+        <v>209</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>216</v>
+        <v>455</v>
       </c>
       <c r="B81" t="s">
-        <v>217</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>290</v>
+        <v>143</v>
       </c>
       <c r="D81" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
-      <c r="F81" t="s">
-        <v>295</v>
-      </c>
       <c r="G81" t="s">
-        <v>296</v>
+        <v>14</v>
       </c>
       <c r="H81">
-        <v>1</v>
-      </c>
-      <c r="I81">
-        <v>0.15</v>
+        <v>6</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B82" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C82" t="s">
         <v>143</v>
@@ -4860,10 +4821,10 @@
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="G82" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4878,726 +4839,825 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B83" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C83" t="s">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="D83" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>224</v>
+        <v>293</v>
       </c>
       <c r="G83" t="s">
-        <v>225</v>
+        <v>294</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>406</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>404</v>
+        <v>217</v>
       </c>
       <c r="C84" t="s">
-        <v>404</v>
+        <v>290</v>
       </c>
       <c r="D84" t="s">
-        <v>405</v>
+        <v>111</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>407</v>
+        <v>295</v>
       </c>
       <c r="G84" t="s">
-        <v>408</v>
+        <v>296</v>
       </c>
       <c r="H84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I84">
-        <v>15.1</v>
+        <v>0.15</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>30.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>409</v>
+        <v>218</v>
       </c>
       <c r="B85" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C85" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
       <c r="D85" t="s">
-        <v>227</v>
+        <v>144</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="G85" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <v>6.6</v>
+        <v>0.04</v>
       </c>
       <c r="J85">
-        <f t="shared" ref="J85:J94" si="2">H85*I85</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>0.04</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>222</v>
+      </c>
+      <c r="B86" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" t="s">
+        <v>143</v>
+      </c>
+      <c r="D86" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
+        <v>224</v>
+      </c>
+      <c r="G86" t="s">
+        <v>225</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>0.04</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>406</v>
+      </c>
+      <c r="B87" t="s">
+        <v>404</v>
+      </c>
+      <c r="C87" t="s">
+        <v>404</v>
+      </c>
+      <c r="D87" t="s">
+        <v>405</v>
+      </c>
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
+        <v>407</v>
+      </c>
+      <c r="G87" t="s">
+        <v>408</v>
+      </c>
+      <c r="H87">
+        <v>2</v>
+      </c>
+      <c r="I87">
+        <v>15.1</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="1"/>
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>409</v>
+      </c>
+      <c r="B88" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" t="s">
+        <v>226</v>
+      </c>
+      <c r="D88" t="s">
+        <v>227</v>
+      </c>
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
+        <v>228</v>
+      </c>
+      <c r="G88" t="s">
+        <v>229</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>6.6</v>
+      </c>
+      <c r="J88">
+        <f t="shared" ref="J88:J97" si="2">H88*I88</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>410</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" t="s">
         <v>230</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C89" t="s">
         <v>231</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D89" t="s">
         <v>232</v>
       </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>233</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G89" t="s">
         <v>234</v>
       </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>0.79</v>
       </c>
-      <c r="J86">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>235</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B90" t="s">
         <v>257</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C90" t="s">
         <v>257</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D90" t="s">
         <v>258</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E90" t="s">
         <v>412</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F90" t="s">
         <v>415</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G90" t="s">
         <v>416</v>
       </c>
-      <c r="H87">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>0.45</v>
       </c>
-      <c r="J87">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>240</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B91" t="s">
         <v>260</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C91" t="s">
         <v>260</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D91" t="s">
         <v>261</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>262</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G91" t="s">
         <v>263</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>0.47</v>
       </c>
-      <c r="J88">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>245</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B92" t="s">
         <v>236</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C92" t="s">
         <v>236</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D92" t="s">
         <v>237</v>
       </c>
-      <c r="E89" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>238</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G92" t="s">
         <v>239</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>0.67</v>
       </c>
-      <c r="J89">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>250</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B93" t="s">
         <v>241</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C93" t="s">
         <v>241</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D93" t="s">
         <v>242</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>243</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G93" t="s">
         <v>244</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>6.63</v>
       </c>
-      <c r="J90">
+      <c r="J93">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>255</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B94" t="s">
         <v>246</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C94" t="s">
         <v>246</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D94" t="s">
         <v>247</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>248</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G94" t="s">
         <v>249</v>
       </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>1.67</v>
       </c>
-      <c r="J91">
+      <c r="J94">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>256</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B95" t="s">
         <v>251</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C95" t="s">
         <v>251</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D95" t="s">
         <v>252</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>253</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G95" t="s">
         <v>254</v>
       </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>5.88</v>
       </c>
-      <c r="J92">
+      <c r="J95">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>259</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
         <v>403</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C96" t="s">
         <v>403</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D96" t="s">
         <v>411</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E96" t="s">
         <v>412</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F96" t="s">
         <v>413</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G96" t="s">
         <v>414</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>1.23</v>
       </c>
-      <c r="J93">
+      <c r="J96">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>431</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B97" t="s">
         <v>402</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C97" t="s">
         <v>402</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D97" t="s">
         <v>417</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E97" t="s">
         <v>412</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F97" t="s">
         <v>418</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G97" t="s">
         <v>419</v>
       </c>
-      <c r="H94">
+      <c r="H97">
         <v>5</v>
       </c>
-      <c r="I94">
+      <c r="I97">
         <v>2.76</v>
       </c>
-      <c r="J94">
+      <c r="J97">
         <f t="shared" si="2"/>
         <v>13.799999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>268</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B98" t="s">
         <v>264</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C98" t="s">
         <v>264</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D98" t="s">
         <v>265</v>
       </c>
-      <c r="E95" t="s">
-        <v>19</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>266</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G98" t="s">
         <v>267</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>3.79</v>
       </c>
-      <c r="J95">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>273</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B99" t="s">
         <v>269</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C99" t="s">
         <v>269</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D99" t="s">
         <v>270</v>
       </c>
-      <c r="E96" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>271</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G99" t="s">
         <v>272</v>
       </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.57</v>
       </c>
-      <c r="J96">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>355</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B100" t="s">
         <v>379</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C100" t="s">
         <v>379</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D100" t="s">
         <v>274</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>380</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G100" t="s">
         <v>381</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>8.48</v>
       </c>
-      <c r="J97">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>397</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B101" t="s">
         <v>356</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C101" t="s">
         <v>356</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D101" t="s">
         <v>358</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>357</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G101" t="s">
         <v>359</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
         <v>6.84</v>
       </c>
-      <c r="J98">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>442</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B102" t="s">
         <v>444</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C102" t="s">
         <v>444</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D102" t="s">
         <v>443</v>
       </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>445</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G102" t="s">
         <v>446</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>3.15</v>
       </c>
-      <c r="J99">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>3.15</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>448</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B103" t="s">
         <v>449</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C103" t="s">
         <v>449</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D103" t="s">
         <v>450</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E103" t="s">
         <v>412</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F103" t="s">
         <v>451</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G103" t="s">
         <v>449</v>
       </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
         <v>5.71</v>
       </c>
-      <c r="J100">
+      <c r="J103">
         <f t="shared" si="1"/>
         <v>5.71</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>447</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B104" t="s">
         <v>275</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C104" t="s">
         <v>275</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D104" t="s">
         <v>276</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E104" t="s">
         <v>412</v>
       </c>
-      <c r="F101" t="s">
-        <v>462</v>
-      </c>
-      <c r="G101" t="s">
+      <c r="F104" t="s">
+        <v>461</v>
+      </c>
+      <c r="G104" t="s">
         <v>278</v>
       </c>
-      <c r="H101">
+      <c r="H104">
         <v>2</v>
       </c>
-      <c r="I101">
+      <c r="I104">
         <v>1.26</v>
       </c>
-      <c r="J101">
+      <c r="J104">
         <f t="shared" si="1"/>
         <v>2.52</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>279</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B105" t="s">
         <v>280</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C105" t="s">
         <v>280</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D105" t="s">
         <v>281</v>
       </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="E105" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" t="s">
         <v>282</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G105" t="s">
         <v>283</v>
       </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="I105">
         <v>2.96</v>
       </c>
-      <c r="J102">
+      <c r="J105">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>392</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B106" t="s">
         <v>393</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C106" t="s">
         <v>394</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D106" t="s">
         <v>394</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E106" t="s">
         <v>277</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F106" t="s">
         <v>395</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G106" t="s">
         <v>396</v>
       </c>
-      <c r="H103">
+      <c r="H106">
         <v>2</v>
       </c>
-      <c r="I103">
+      <c r="I106">
         <v>0.95</v>
       </c>
-      <c r="J103">
+      <c r="J106">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>284</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B107" t="s">
         <v>285</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C107" t="s">
         <v>398</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D107" t="s">
         <v>399</v>
       </c>
-      <c r="E104" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="E107" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" t="s">
         <v>400</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G107" t="s">
         <v>401</v>
       </c>
-      <c r="H104">
-        <v>1</v>
-      </c>
-      <c r="I104">
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
         <v>1.99</v>
       </c>
-      <c r="J104">
+      <c r="J107">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Changed R13 and R14 to 0402 packages.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="461">
   <si>
     <t>Part</t>
   </si>
@@ -250,12 +250,6 @@
     <t>3A</t>
   </si>
   <si>
-    <t>F4, F5, F6</t>
-  </si>
-  <si>
-    <t>12A</t>
-  </si>
-  <si>
     <t>IC1, IC2, IC3</t>
   </si>
   <si>
@@ -481,6 +475,9 @@
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
+    <t>R36, R78, R119, R135</t>
+  </si>
+  <si>
     <t>100K</t>
   </si>
   <si>
@@ -1033,15 +1030,6 @@
     <t>RUEF300</t>
   </si>
   <si>
-    <t>MF-R900-ND</t>
-  </si>
-  <si>
-    <t>MF-R900</t>
-  </si>
-  <si>
-    <t>9A hold 18A trip</t>
-  </si>
-  <si>
     <t>RUEF160-ND</t>
   </si>
   <si>
@@ -1390,9 +1378,6 @@
     <t>R11, R12</t>
   </si>
   <si>
-    <t>R13, R14, R36, R78, R119, R135</t>
-  </si>
-  <si>
     <t>R15, R65, R66, R67, R68</t>
   </si>
   <si>
@@ -1408,10 +1393,10 @@
     <t>R2, R8, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R76, R106, R108, R109, R118, R122, R123, R124, R125, R134, R147, R150</t>
   </si>
   <si>
-    <t>R9, R19</t>
-  </si>
-  <si>
     <t>R5, R16</t>
+  </si>
+  <si>
+    <t>R9, R13, R14, R19</t>
   </si>
 </sst>
 </file>
@@ -2240,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,12 +2277,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2312,10 +2297,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" t="s">
         <v>303</v>
-      </c>
-      <c r="G2" t="s">
-        <v>304</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2328,8 +2313,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J133)</f>
-        <v>211.58799999999999</v>
+        <f>SUM(J2:J132)</f>
+        <v>208.80799999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2349,10 +2334,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>304</v>
+      </c>
+      <c r="G3" t="s">
         <v>305</v>
-      </c>
-      <c r="G3" t="s">
-        <v>306</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2361,13 +2346,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J77" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J76" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2382,10 +2367,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>306</v>
+      </c>
+      <c r="G4" t="s">
         <v>307</v>
-      </c>
-      <c r="G4" t="s">
-        <v>308</v>
       </c>
       <c r="H4">
         <v>28</v>
@@ -2439,10 +2424,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>310</v>
+      </c>
+      <c r="G6" t="s">
         <v>311</v>
-      </c>
-      <c r="G6" t="s">
-        <v>312</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2455,7 +2440,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2499,10 +2484,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>312</v>
+      </c>
+      <c r="G8" t="s">
         <v>313</v>
-      </c>
-      <c r="G8" t="s">
-        <v>314</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2532,10 +2517,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>314</v>
+      </c>
+      <c r="G9" t="s">
         <v>315</v>
-      </c>
-      <c r="G9" t="s">
-        <v>316</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2565,10 +2550,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>326</v>
+      </c>
+      <c r="G10" t="s">
         <v>327</v>
-      </c>
-      <c r="G10" t="s">
-        <v>328</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2581,7 +2566,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2634,10 +2619,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>328</v>
+      </c>
+      <c r="G12" t="s">
         <v>329</v>
-      </c>
-      <c r="G12" t="s">
-        <v>330</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2667,10 +2652,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>326</v>
+      </c>
+      <c r="G13" t="s">
         <v>327</v>
-      </c>
-      <c r="G13" t="s">
-        <v>328</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2683,7 +2668,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2703,10 +2688,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>332</v>
+      </c>
+      <c r="G14" t="s">
         <v>333</v>
-      </c>
-      <c r="G14" t="s">
-        <v>334</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2719,7 +2704,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2763,10 +2748,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>316</v>
+      </c>
+      <c r="G16" t="s">
         <v>317</v>
-      </c>
-      <c r="G16" t="s">
-        <v>318</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2844,10 +2829,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>318</v>
+      </c>
+      <c r="G19" t="s">
         <v>319</v>
-      </c>
-      <c r="G19" t="s">
-        <v>320</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2860,7 +2845,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2880,10 +2865,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>321</v>
+      </c>
+      <c r="G20" t="s">
         <v>322</v>
-      </c>
-      <c r="G20" t="s">
-        <v>323</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2937,10 +2922,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>323</v>
+      </c>
+      <c r="G22" t="s">
         <v>324</v>
-      </c>
-      <c r="G22" t="s">
-        <v>325</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2955,10 +2940,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B23" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2970,10 +2955,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G23" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2988,25 +2973,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D24" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G24" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -3021,10 +3006,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B25" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3036,10 +3021,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G25" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3102,10 +3087,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>300</v>
+      </c>
+      <c r="G27" t="s">
         <v>301</v>
-      </c>
-      <c r="G27" t="s">
-        <v>302</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -3135,10 +3120,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G28" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3151,7 +3136,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3171,10 +3156,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>334</v>
+      </c>
+      <c r="G29" t="s">
         <v>335</v>
-      </c>
-      <c r="G29" t="s">
-        <v>336</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3204,10 +3189,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>336</v>
+      </c>
+      <c r="G30" t="s">
         <v>337</v>
-      </c>
-      <c r="G30" t="s">
-        <v>338</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3228,136 +3213,133 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>339</v>
+        <v>285</v>
       </c>
       <c r="G31" t="s">
-        <v>340</v>
+        <v>286</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="I31">
-        <v>0.9</v>
+        <v>11.91</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="L31" t="s">
-        <v>341</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>428</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>370</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>371</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>372</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>286</v>
+        <v>373</v>
       </c>
       <c r="G32" t="s">
-        <v>287</v>
+        <v>374</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>11.91</v>
+        <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>432</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
       <c r="C33" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="D33" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>377</v>
+        <v>345</v>
       </c>
       <c r="G33" t="s">
-        <v>378</v>
+        <v>346</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>0.44</v>
+        <v>2.15</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="B34" t="s">
-        <v>350</v>
-      </c>
       <c r="C34" t="s">
-        <v>350</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>350</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>349</v>
+        <v>84</v>
       </c>
       <c r="G34" t="s">
-        <v>350</v>
+        <v>83</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>2.15</v>
+        <v>0.77</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>341</v>
       </c>
       <c r="B35" t="s">
         <v>85</v>
@@ -3366,46 +3348,46 @@
         <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>276</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" t="s">
-        <v>85</v>
+        <v>343</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>0.77</v>
+        <v>0.5</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F36" t="s">
-        <v>347</v>
+        <v>342</v>
+      </c>
+      <c r="G36" t="s">
+        <v>14</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3420,457 +3402,448 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>344</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>364</v>
       </c>
       <c r="E37" t="s">
-        <v>277</v>
+        <v>19</v>
       </c>
       <c r="F37" t="s">
-        <v>346</v>
+        <v>89</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="I37">
-        <v>0.5</v>
+        <v>0.93</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>421</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>368</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>91</v>
+        <v>298</v>
       </c>
       <c r="G38" t="s">
-        <v>92</v>
+        <v>299</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I38">
-        <v>0.93</v>
+        <v>1.47</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" t="s">
         <v>93</v>
       </c>
-      <c r="D39" t="s">
-        <v>94</v>
-      </c>
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>299</v>
+        <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>300</v>
+        <v>96</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I39">
-        <v>1.47</v>
+        <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>441</v>
-      </c>
-      <c r="B40" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>429</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>430</v>
       </c>
       <c r="E40" t="s">
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>97</v>
-      </c>
-      <c r="G40" t="s">
-        <v>98</v>
+        <v>431</v>
+      </c>
+      <c r="G40">
+        <v>702461004</v>
       </c>
       <c r="H40">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>0.42</v>
+        <v>1.64</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>5.46</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>363</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
         <v>99</v>
       </c>
-      <c r="C41" t="s">
-        <v>433</v>
-      </c>
-      <c r="D41" t="s">
-        <v>434</v>
-      </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>435</v>
-      </c>
-      <c r="G41">
-        <v>702461004</v>
+        <v>360</v>
+      </c>
+      <c r="G41" t="s">
+        <v>361</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <v>1.64</v>
+        <v>0.13</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>1.64</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>367</v>
-      </c>
-      <c r="B42" t="s">
-        <v>14</v>
+        <v>362</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>356</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>357</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G42" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0.13</v>
+        <v>0.71</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>365</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
         <v>366</v>
       </c>
-      <c r="C43" t="s">
-        <v>360</v>
-      </c>
-      <c r="D43" t="s">
-        <v>361</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>362</v>
-      </c>
       <c r="G43" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>369</v>
+        <v>422</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>423</v>
       </c>
       <c r="D44" t="s">
-        <v>368</v>
+        <v>424</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>370</v>
+        <v>425</v>
       </c>
       <c r="G44" t="s">
-        <v>371</v>
+        <v>426</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>3.15</v>
+        <v>1.67</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="C45" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="D45" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="G45" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I45">
-        <v>1.67</v>
+        <v>0.5</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>420</v>
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>421</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
-        <v>422</v>
+        <v>103</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>423</v>
+        <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>424</v>
+        <v>105</v>
       </c>
       <c r="H46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>0.5</v>
+        <v>2.13</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G47" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D48" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G48" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>452</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D50" t="s">
-        <v>123</v>
-      </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G50" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50">
-        <v>1.85</v>
+        <v>6</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
         <v>126</v>
@@ -3878,194 +3851,203 @@
       <c r="D51" t="s">
         <v>127</v>
       </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>450</v>
+      </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>448</v>
       </c>
       <c r="H51">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0.55000000000000004</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>453</v>
+        <v>128</v>
       </c>
       <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" t="s">
         <v>131</v>
       </c>
-      <c r="C52" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>454</v>
-      </c>
       <c r="G52" t="s">
-        <v>452</v>
+        <v>14</v>
       </c>
       <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>0.55000000000000004</v>
+        <v>3</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>368</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
         <v>133</v>
       </c>
       <c r="G53" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0.41</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G54" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>373</v>
+        <v>139</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>139</v>
+        <v>287</v>
       </c>
       <c r="G55" t="s">
-        <v>140</v>
+        <v>288</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" t="s">
         <v>141</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>142</v>
       </c>
-      <c r="C56" t="s">
-        <v>143</v>
-      </c>
-      <c r="D56" t="s">
-        <v>144</v>
-      </c>
       <c r="E56" t="s">
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>288</v>
+        <v>145</v>
       </c>
       <c r="G56" t="s">
-        <v>289</v>
+        <v>146</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>145</v>
-      </c>
-      <c r="B57" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="B57">
+        <v>470</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G57" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4080,99 +4062,83 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>149</v>
-      </c>
-      <c r="B58">
-        <v>470</v>
+        <v>459</v>
+      </c>
+      <c r="B58" t="s">
+        <v>177</v>
       </c>
       <c r="C58" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" t="s">
-        <v>150</v>
-      </c>
-      <c r="G58" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="H58">
-        <v>1</v>
-      </c>
-      <c r="I58">
-        <v>0.04</v>
-      </c>
-      <c r="J58">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>142</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
+        <v>151</v>
+      </c>
+      <c r="G59" t="s">
+        <v>152</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <v>0.04</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>463</v>
-      </c>
-      <c r="B60" t="s">
-        <v>152</v>
+        <v>457</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" t="s">
-        <v>153</v>
-      </c>
-      <c r="G60" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="H60">
-        <v>5</v>
-      </c>
-      <c r="I60">
-        <v>0.04</v>
-      </c>
-      <c r="J60">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>462</v>
-      </c>
-      <c r="B61">
-        <v>10</v>
+        <v>460</v>
+      </c>
+      <c r="B61" t="s">
+        <v>154</v>
       </c>
       <c r="C61" t="s">
+        <v>193</v>
+      </c>
+      <c r="D61" t="s">
         <v>194</v>
-      </c>
-      <c r="D61" t="s">
-        <v>195</v>
       </c>
       <c r="H61">
         <v>4</v>
@@ -4180,129 +4146,145 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" t="s">
         <v>194</v>
-      </c>
-      <c r="D62" t="s">
-        <v>195</v>
       </c>
       <c r="H62">
         <v>2</v>
       </c>
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>457</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="D63" t="s">
-        <v>195</v>
+        <v>142</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>155</v>
+      </c>
+      <c r="G63" t="s">
+        <v>156</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I63">
+        <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>458</v>
-      </c>
-      <c r="B64" t="s">
-        <v>155</v>
+        <v>454</v>
+      </c>
+      <c r="B64">
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>194</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>156</v>
+        <v>381</v>
       </c>
       <c r="G64" t="s">
-        <v>157</v>
+        <v>382</v>
       </c>
       <c r="H64">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
+        <f>H64*I64</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>459</v>
-      </c>
-      <c r="B65">
-        <v>100</v>
+        <v>157</v>
+      </c>
+      <c r="B65" t="s">
+        <v>158</v>
       </c>
       <c r="C65" t="s">
-        <v>194</v>
+        <v>289</v>
       </c>
       <c r="D65" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>385</v>
+        <v>290</v>
       </c>
       <c r="G65" t="s">
-        <v>386</v>
+        <v>291</v>
       </c>
       <c r="H65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I65">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J65">
-        <f>H65*I65</f>
-        <v>0.2</v>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C66" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="G66" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4317,289 +4299,289 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C67" t="s">
-        <v>290</v>
+        <v>141</v>
       </c>
       <c r="D67" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>297</v>
+        <v>163</v>
       </c>
       <c r="G67" t="s">
-        <v>298</v>
+        <v>164</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B68" t="s">
-        <v>163</v>
+        <v>165</v>
+      </c>
+      <c r="B68">
+        <v>200</v>
       </c>
       <c r="C68" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="D68" t="s">
-        <v>144</v>
+        <v>194</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>164</v>
+        <v>378</v>
       </c>
       <c r="G68" t="s">
-        <v>165</v>
+        <v>379</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I68">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>380</v>
+      </c>
+      <c r="B69">
+        <v>100</v>
+      </c>
+      <c r="C69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" t="s">
+        <v>142</v>
+      </c>
+      <c r="E69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" t="s">
         <v>166</v>
       </c>
-      <c r="B69">
-        <v>200</v>
-      </c>
-      <c r="C69" t="s">
-        <v>194</v>
-      </c>
-      <c r="D69" t="s">
-        <v>195</v>
-      </c>
-      <c r="E69" t="s">
-        <v>19</v>
-      </c>
-      <c r="F69" t="s">
-        <v>382</v>
-      </c>
       <c r="G69" t="s">
-        <v>383</v>
+        <v>167</v>
       </c>
       <c r="H69">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>384</v>
-      </c>
-      <c r="B70">
-        <v>100</v>
+        <v>168</v>
+      </c>
+      <c r="B70" t="s">
+        <v>169</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D70" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G70" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H70">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B71" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G71" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H71">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I71">
         <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G72" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H72">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I72">
         <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G73" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I73">
         <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B74" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C74" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D74" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G74" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H74">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I74">
         <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D75" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G75" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4614,91 +4596,91 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>189</v>
-      </c>
-      <c r="B76" t="s">
-        <v>190</v>
+        <v>192</v>
+      </c>
+      <c r="B76">
+        <v>0.3</v>
       </c>
       <c r="C76" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="D76" t="s">
-        <v>144</v>
+        <v>194</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
       </c>
       <c r="F76" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G76" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J76">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>193</v>
-      </c>
-      <c r="B77">
-        <v>0.3</v>
+        <v>197</v>
+      </c>
+      <c r="B77" t="s">
+        <v>198</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="D77" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G77" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J77">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" ref="J77:J106" si="1">H77*I77</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B78" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G78" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4707,31 +4689,31 @@
         <v>0.04</v>
       </c>
       <c r="J78">
-        <f t="shared" ref="J78:J107" si="1">H78*I78</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G79" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4746,118 +4728,118 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>206</v>
+        <v>451</v>
       </c>
       <c r="B80" t="s">
-        <v>207</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
-      <c r="F80" t="s">
-        <v>208</v>
-      </c>
       <c r="G80" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="H80">
-        <v>1</v>
-      </c>
-      <c r="I80">
-        <v>0.04</v>
+        <v>6</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>455</v>
+        <v>209</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D81" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
+      <c r="F81" t="s">
+        <v>211</v>
+      </c>
       <c r="G81" t="s">
-        <v>14</v>
+        <v>212</v>
       </c>
       <c r="H81">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>0.04</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B82" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C82" t="s">
-        <v>143</v>
+        <v>289</v>
       </c>
       <c r="D82" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>212</v>
+        <v>292</v>
       </c>
       <c r="G82" t="s">
-        <v>213</v>
+        <v>293</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B83" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C83" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D83" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G83" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4872,58 +4854,58 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C84" t="s">
-        <v>290</v>
+        <v>141</v>
       </c>
       <c r="D84" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>295</v>
+        <v>219</v>
       </c>
       <c r="G84" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B85" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D85" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G85" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4938,266 +4920,266 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>402</v>
       </c>
       <c r="B86" t="s">
-        <v>223</v>
+        <v>400</v>
       </c>
       <c r="C86" t="s">
-        <v>143</v>
+        <v>400</v>
       </c>
       <c r="D86" t="s">
-        <v>144</v>
+        <v>401</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>224</v>
+        <v>403</v>
       </c>
       <c r="G86" t="s">
-        <v>225</v>
+        <v>404</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I86">
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B87" t="s">
-        <v>404</v>
+        <v>225</v>
       </c>
       <c r="C87" t="s">
-        <v>404</v>
+        <v>225</v>
       </c>
       <c r="D87" t="s">
-        <v>405</v>
+        <v>226</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>407</v>
+        <v>227</v>
       </c>
       <c r="G87" t="s">
-        <v>408</v>
+        <v>228</v>
       </c>
       <c r="H87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I87">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J87">
-        <f t="shared" si="1"/>
-        <v>30.2</v>
+        <f t="shared" ref="J87:J96" si="2">H87*I87</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B88" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C88" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D88" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G88" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J88">
-        <f t="shared" ref="J88:J97" si="2">H88*I88</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>410</v>
+        <v>234</v>
       </c>
       <c r="B89" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="C89" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="D89" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="E89" t="s">
-        <v>19</v>
+        <v>408</v>
       </c>
       <c r="F89" t="s">
-        <v>233</v>
+        <v>411</v>
       </c>
       <c r="G89" t="s">
-        <v>234</v>
+        <v>412</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B90" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C90" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D90" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E90" t="s">
-        <v>412</v>
+        <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>415</v>
+        <v>261</v>
       </c>
       <c r="G90" t="s">
-        <v>416</v>
+        <v>262</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B91" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="C91" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="D91" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
       </c>
       <c r="F91" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="G91" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B92" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D92" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G92" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C93" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D93" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="G93" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J93">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -5205,459 +5187,426 @@
         <v>255</v>
       </c>
       <c r="B94" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C94" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D94" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="G94" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J94">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B95" t="s">
-        <v>251</v>
+        <v>399</v>
       </c>
       <c r="C95" t="s">
-        <v>251</v>
+        <v>399</v>
       </c>
       <c r="D95" t="s">
-        <v>252</v>
+        <v>407</v>
       </c>
       <c r="E95" t="s">
-        <v>19</v>
+        <v>408</v>
       </c>
       <c r="F95" t="s">
-        <v>253</v>
+        <v>409</v>
       </c>
       <c r="G95" t="s">
-        <v>254</v>
+        <v>410</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
       <c r="J95">
         <f t="shared" si="2"/>
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>259</v>
+        <v>427</v>
       </c>
       <c r="B96" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C96" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D96" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E96" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F96" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G96" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I96">
-        <v>1.23</v>
+        <v>2.76</v>
       </c>
       <c r="J96">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>431</v>
+        <v>267</v>
       </c>
       <c r="B97" t="s">
-        <v>402</v>
+        <v>263</v>
       </c>
       <c r="C97" t="s">
-        <v>402</v>
+        <v>263</v>
       </c>
       <c r="D97" t="s">
-        <v>417</v>
+        <v>264</v>
       </c>
       <c r="E97" t="s">
-        <v>412</v>
+        <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>418</v>
+        <v>265</v>
       </c>
       <c r="G97" t="s">
-        <v>419</v>
+        <v>266</v>
       </c>
       <c r="H97">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>2.76</v>
+        <v>3.79</v>
       </c>
       <c r="J97">
-        <f t="shared" si="2"/>
-        <v>13.799999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>272</v>
+      </c>
+      <c r="B98" t="s">
         <v>268</v>
       </c>
-      <c r="B98" t="s">
-        <v>264</v>
-      </c>
       <c r="C98" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D98" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G98" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>351</v>
+      </c>
+      <c r="B99" t="s">
+        <v>375</v>
+      </c>
+      <c r="C99" t="s">
+        <v>375</v>
+      </c>
+      <c r="D99" t="s">
         <v>273</v>
       </c>
-      <c r="B99" t="s">
-        <v>269</v>
-      </c>
-      <c r="C99" t="s">
-        <v>269</v>
-      </c>
-      <c r="D99" t="s">
-        <v>270</v>
-      </c>
       <c r="E99" t="s">
         <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>271</v>
+        <v>376</v>
       </c>
       <c r="G99" t="s">
-        <v>272</v>
+        <v>377</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>393</v>
+      </c>
+      <c r="B100" t="s">
+        <v>352</v>
+      </c>
+      <c r="C100" t="s">
+        <v>352</v>
+      </c>
+      <c r="D100" t="s">
+        <v>354</v>
+      </c>
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
+        <v>353</v>
+      </c>
+      <c r="G100" t="s">
         <v>355</v>
       </c>
-      <c r="B100" t="s">
-        <v>379</v>
-      </c>
-      <c r="C100" t="s">
-        <v>379</v>
-      </c>
-      <c r="D100" t="s">
-        <v>274</v>
-      </c>
-      <c r="E100" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" t="s">
-        <v>380</v>
-      </c>
-      <c r="G100" t="s">
-        <v>381</v>
-      </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
       <c r="B101" t="s">
-        <v>356</v>
+        <v>440</v>
       </c>
       <c r="C101" t="s">
-        <v>356</v>
+        <v>440</v>
       </c>
       <c r="D101" t="s">
-        <v>358</v>
+        <v>439</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
       </c>
       <c r="F101" t="s">
-        <v>357</v>
+        <v>441</v>
       </c>
       <c r="G101" t="s">
-        <v>359</v>
+        <v>442</v>
       </c>
       <c r="H101">
         <v>1</v>
       </c>
       <c r="I101">
-        <v>6.84</v>
+        <v>3.15</v>
       </c>
       <c r="J101">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B102" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C102" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D102" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="E102" t="s">
-        <v>19</v>
+        <v>408</v>
       </c>
       <c r="F102" t="s">
+        <v>447</v>
+      </c>
+      <c r="G102" t="s">
         <v>445</v>
       </c>
-      <c r="G102" t="s">
-        <v>446</v>
-      </c>
       <c r="H102">
         <v>1</v>
       </c>
       <c r="I102">
-        <v>3.15</v>
+        <v>5.71</v>
       </c>
       <c r="J102">
         <f t="shared" si="1"/>
-        <v>3.15</v>
+        <v>5.71</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B103" t="s">
-        <v>449</v>
+        <v>274</v>
       </c>
       <c r="C103" t="s">
-        <v>449</v>
+        <v>274</v>
       </c>
       <c r="D103" t="s">
-        <v>450</v>
+        <v>275</v>
       </c>
       <c r="E103" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F103" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="G103" t="s">
-        <v>449</v>
+        <v>277</v>
       </c>
       <c r="H103">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I103">
-        <v>5.71</v>
+        <v>1.26</v>
       </c>
       <c r="J103">
         <f t="shared" si="1"/>
-        <v>5.71</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>447</v>
+        <v>278</v>
       </c>
       <c r="B104" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C104" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D104" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E104" t="s">
-        <v>412</v>
+        <v>19</v>
       </c>
       <c r="F104" t="s">
-        <v>461</v>
+        <v>281</v>
       </c>
       <c r="G104" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="H104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I104">
-        <v>1.26</v>
+        <v>2.96</v>
       </c>
       <c r="J104">
         <f t="shared" si="1"/>
-        <v>2.52</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>279</v>
+        <v>388</v>
       </c>
       <c r="B105" t="s">
-        <v>280</v>
+        <v>389</v>
       </c>
       <c r="C105" t="s">
-        <v>280</v>
+        <v>390</v>
       </c>
       <c r="D105" t="s">
-        <v>281</v>
+        <v>390</v>
       </c>
       <c r="E105" t="s">
-        <v>19</v>
+        <v>276</v>
       </c>
       <c r="F105" t="s">
-        <v>282</v>
+        <v>391</v>
       </c>
       <c r="G105" t="s">
-        <v>283</v>
+        <v>392</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I105">
-        <v>2.96</v>
+        <v>0.95</v>
       </c>
       <c r="J105">
         <f t="shared" si="1"/>
-        <v>2.96</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>392</v>
+        <v>283</v>
       </c>
       <c r="B106" t="s">
-        <v>393</v>
+        <v>284</v>
       </c>
       <c r="C106" t="s">
         <v>394</v>
       </c>
       <c r="D106" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E106" t="s">
-        <v>277</v>
+        <v>19</v>
       </c>
       <c r="F106" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G106" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I106">
-        <v>0.95</v>
+        <v>1.99</v>
       </c>
       <c r="J106">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>284</v>
-      </c>
-      <c r="B107" t="s">
-        <v>285</v>
-      </c>
-      <c r="C107" t="s">
-        <v>398</v>
-      </c>
-      <c r="D107" t="s">
-        <v>399</v>
-      </c>
-      <c r="E107" t="s">
-        <v>19</v>
-      </c>
-      <c r="F107" t="s">
-        <v>400</v>
-      </c>
-      <c r="G107" t="s">
-        <v>401</v>
-      </c>
-      <c r="H107">
-        <v>1</v>
-      </c>
-      <c r="I107">
-        <v>1.99</v>
-      </c>
-      <c r="J107">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
JP24 changed from a 2x10 to 2x11 and moved right 400 mils.
The extra pins are connected to the STM32 UART2 TX/RX lines (PD5 and PD6).
Also removed the old JP2 JTAG header from the BOM.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="463">
   <si>
     <t>Part</t>
   </si>
@@ -277,9 +277,6 @@
     <t>DUEMILANOVE_VIAS</t>
   </si>
   <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
     <t>PINHD-2X10</t>
   </si>
   <si>
@@ -1114,12 +1111,6 @@
     <t>JP24</t>
   </si>
   <si>
-    <t>A26460-ND</t>
-  </si>
-  <si>
-    <t>1-534206-0</t>
-  </si>
-  <si>
     <t>Q15</t>
   </si>
   <si>
@@ -1397,6 +1388,21 @@
   </si>
   <si>
     <t>R9, R13, R14, R19</t>
+  </si>
+  <si>
+    <t>PINHD-2X11</t>
+  </si>
+  <si>
+    <t>2X11 Female</t>
+  </si>
+  <si>
+    <t>PPTC112LFBN-RC</t>
+  </si>
+  <si>
+    <t>S7079-ND</t>
+  </si>
+  <si>
+    <t>JP1</t>
   </si>
 </sst>
 </file>
@@ -2227,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,12 +2283,12 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2297,10 +2303,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" t="s">
         <v>302</v>
-      </c>
-      <c r="G2" t="s">
-        <v>303</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2314,7 +2320,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J132)</f>
-        <v>208.80799999999999</v>
+        <v>206.30799999999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2334,10 +2340,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G3" t="s">
         <v>304</v>
-      </c>
-      <c r="G3" t="s">
-        <v>305</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2352,7 +2358,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2367,10 +2373,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>305</v>
+      </c>
+      <c r="G4" t="s">
         <v>306</v>
-      </c>
-      <c r="G4" t="s">
-        <v>307</v>
       </c>
       <c r="H4">
         <v>28</v>
@@ -2424,10 +2430,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G6" t="s">
         <v>310</v>
-      </c>
-      <c r="G6" t="s">
-        <v>311</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2440,7 +2446,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2484,10 +2490,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
+        <v>311</v>
+      </c>
+      <c r="G8" t="s">
         <v>312</v>
-      </c>
-      <c r="G8" t="s">
-        <v>313</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2517,10 +2523,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G9" t="s">
         <v>314</v>
-      </c>
-      <c r="G9" t="s">
-        <v>315</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2550,10 +2556,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
+        <v>325</v>
+      </c>
+      <c r="G10" t="s">
         <v>326</v>
-      </c>
-      <c r="G10" t="s">
-        <v>327</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2566,7 +2572,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2619,10 +2625,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
+        <v>327</v>
+      </c>
+      <c r="G12" t="s">
         <v>328</v>
-      </c>
-      <c r="G12" t="s">
-        <v>329</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2652,10 +2658,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
+        <v>325</v>
+      </c>
+      <c r="G13" t="s">
         <v>326</v>
-      </c>
-      <c r="G13" t="s">
-        <v>327</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2668,7 +2674,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2688,10 +2694,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
+        <v>331</v>
+      </c>
+      <c r="G14" t="s">
         <v>332</v>
-      </c>
-      <c r="G14" t="s">
-        <v>333</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2704,7 +2710,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2748,10 +2754,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
+        <v>315</v>
+      </c>
+      <c r="G16" t="s">
         <v>316</v>
-      </c>
-      <c r="G16" t="s">
-        <v>317</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2829,10 +2835,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
+        <v>317</v>
+      </c>
+      <c r="G19" t="s">
         <v>318</v>
-      </c>
-      <c r="G19" t="s">
-        <v>319</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2845,7 +2851,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2865,10 +2871,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
+        <v>320</v>
+      </c>
+      <c r="G20" t="s">
         <v>321</v>
-      </c>
-      <c r="G20" t="s">
-        <v>322</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2922,10 +2928,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
+        <v>322</v>
+      </c>
+      <c r="G22" t="s">
         <v>323</v>
-      </c>
-      <c r="G22" t="s">
-        <v>324</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2940,10 +2946,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" t="s">
         <v>347</v>
-      </c>
-      <c r="B23" t="s">
-        <v>348</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2955,10 +2961,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>348</v>
+      </c>
+      <c r="G23" t="s">
         <v>349</v>
-      </c>
-      <c r="G23" t="s">
-        <v>350</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2973,25 +2979,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" t="s">
+        <v>431</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>432</v>
+      </c>
+      <c r="G24" t="s">
         <v>433</v>
-      </c>
-      <c r="D24" t="s">
-        <v>434</v>
-      </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>435</v>
-      </c>
-      <c r="G24" t="s">
-        <v>436</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -3006,10 +3012,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B25" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3021,10 +3027,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G25" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3087,10 +3093,10 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
+        <v>299</v>
+      </c>
+      <c r="G27" t="s">
         <v>300</v>
-      </c>
-      <c r="G27" t="s">
-        <v>301</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -3120,10 +3126,10 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
+        <v>337</v>
+      </c>
+      <c r="G28" t="s">
         <v>338</v>
-      </c>
-      <c r="G28" t="s">
-        <v>339</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -3136,7 +3142,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3156,10 +3162,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
+        <v>333</v>
+      </c>
+      <c r="G29" t="s">
         <v>334</v>
-      </c>
-      <c r="G29" t="s">
-        <v>335</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3189,10 +3195,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
+        <v>335</v>
+      </c>
+      <c r="G30" t="s">
         <v>336</v>
-      </c>
-      <c r="G30" t="s">
-        <v>337</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3222,10 +3228,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
+        <v>284</v>
+      </c>
+      <c r="G31" t="s">
         <v>285</v>
-      </c>
-      <c r="G31" t="s">
-        <v>286</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -3240,25 +3246,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B32" t="s">
+        <v>367</v>
+      </c>
+      <c r="C32" t="s">
+        <v>368</v>
+      </c>
+      <c r="D32" t="s">
+        <v>369</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
         <v>370</v>
       </c>
-      <c r="C32" t="s">
+      <c r="G32" t="s">
         <v>371</v>
-      </c>
-      <c r="D32" t="s">
-        <v>372</v>
-      </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
-        <v>373</v>
-      </c>
-      <c r="G32" t="s">
-        <v>374</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -3276,22 +3282,22 @@
         <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
+        <v>344</v>
+      </c>
+      <c r="G33" t="s">
         <v>345</v>
-      </c>
-      <c r="G33" t="s">
-        <v>346</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3339,7 +3345,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B35" t="s">
         <v>85</v>
@@ -3351,10 +3357,10 @@
         <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -3369,7 +3375,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B36" t="s">
         <v>85</v>
@@ -3381,10 +3387,10 @@
         <v>86</v>
       </c>
       <c r="E36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
@@ -3402,58 +3408,58 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>462</v>
       </c>
       <c r="B37" t="s">
         <v>14</v>
       </c>
       <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>363</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
         <v>88</v>
       </c>
-      <c r="D37" t="s">
-        <v>364</v>
-      </c>
-      <c r="E37" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>89</v>
       </c>
-      <c r="G37" t="s">
-        <v>90</v>
-      </c>
       <c r="H37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0.93</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" t="s">
         <v>91</v>
       </c>
-      <c r="D38" t="s">
-        <v>92</v>
-      </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
+        <v>297</v>
+      </c>
+      <c r="G38" t="s">
         <v>298</v>
-      </c>
-      <c r="G38" t="s">
-        <v>299</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -3468,25 +3474,25 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
         <v>94</v>
       </c>
-      <c r="D39" t="s">
-        <v>93</v>
-      </c>
-      <c r="E39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>95</v>
-      </c>
-      <c r="G39" t="s">
-        <v>96</v>
       </c>
       <c r="H39">
         <v>13</v>
@@ -3501,19 +3507,19 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D40" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E40" t="s">
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="G40">
         <v>702461004</v>
@@ -3531,25 +3537,25 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" t="s">
         <v>98</v>
       </c>
-      <c r="D41" t="s">
-        <v>99</v>
-      </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
+        <v>359</v>
+      </c>
+      <c r="G41" t="s">
         <v>360</v>
-      </c>
-      <c r="G41" t="s">
-        <v>361</v>
       </c>
       <c r="H41">
         <v>3</v>
@@ -3564,22 +3570,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C42" t="s">
+        <v>355</v>
+      </c>
+      <c r="D42" t="s">
         <v>356</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
         <v>357</v>
       </c>
-      <c r="E42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>358</v>
-      </c>
-      <c r="G42" t="s">
-        <v>359</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3594,52 +3600,52 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>458</v>
       </c>
       <c r="D43" t="s">
-        <v>364</v>
+        <v>459</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>366</v>
+        <v>461</v>
       </c>
       <c r="G43" t="s">
-        <v>367</v>
+        <v>460</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>3.15</v>
+        <v>1.58</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>3.15</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>419</v>
+      </c>
+      <c r="C44" t="s">
+        <v>420</v>
+      </c>
+      <c r="D44" t="s">
+        <v>421</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>422</v>
       </c>
-      <c r="C44" t="s">
+      <c r="G44" t="s">
         <v>423</v>
-      </c>
-      <c r="D44" t="s">
-        <v>424</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>425</v>
-      </c>
-      <c r="G44" t="s">
-        <v>426</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3654,22 +3660,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>413</v>
+      </c>
+      <c r="C45" t="s">
+        <v>414</v>
+      </c>
+      <c r="D45" t="s">
+        <v>415</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
         <v>416</v>
       </c>
-      <c r="C45" t="s">
+      <c r="G45" t="s">
         <v>417</v>
-      </c>
-      <c r="D45" t="s">
-        <v>418</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>419</v>
-      </c>
-      <c r="G45" t="s">
-        <v>420</v>
       </c>
       <c r="H45">
         <v>3</v>
@@ -3684,25 +3690,25 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
         <v>100</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>101</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>102</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
         <v>103</v>
       </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>104</v>
-      </c>
-      <c r="G46" t="s">
-        <v>105</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -3717,25 +3723,25 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" t="s">
         <v>106</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>107</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>108</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
         <v>109</v>
       </c>
-      <c r="E47" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>110</v>
-      </c>
-      <c r="G47" t="s">
-        <v>111</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -3750,25 +3756,25 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" t="s">
         <v>112</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>113</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>114</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
         <v>115</v>
       </c>
-      <c r="E48" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>116</v>
-      </c>
-      <c r="G48" t="s">
-        <v>117</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -3783,25 +3789,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
         <v>118</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>119</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>120</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
         <v>121</v>
       </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>122</v>
-      </c>
-      <c r="G49" t="s">
-        <v>123</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -3816,16 +3822,16 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B50" t="s">
         <v>14</v>
       </c>
       <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" t="s">
         <v>124</v>
-      </c>
-      <c r="D50" t="s">
-        <v>125</v>
       </c>
       <c r="G50" t="s">
         <v>14</v>
@@ -3840,25 +3846,25 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" t="s">
         <v>126</v>
       </c>
-      <c r="D51" t="s">
-        <v>127</v>
-      </c>
       <c r="E51" t="s">
         <v>19</v>
       </c>
       <c r="F51" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G51" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -3873,16 +3879,16 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" t="s">
         <v>128</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>129</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>130</v>
-      </c>
-      <c r="D52" t="s">
-        <v>131</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
@@ -3897,25 +3903,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
         <v>132</v>
       </c>
-      <c r="C53" t="s">
-        <v>126</v>
-      </c>
-      <c r="D53" t="s">
-        <v>127</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>133</v>
-      </c>
-      <c r="G53" t="s">
-        <v>134</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3930,25 +3936,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B54" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" t="s">
         <v>135</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
         <v>136</v>
       </c>
-      <c r="D54" t="s">
-        <v>127</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>137</v>
-      </c>
-      <c r="G54" t="s">
-        <v>138</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3963,25 +3969,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" t="s">
         <v>139</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>140</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>141</v>
       </c>
-      <c r="D55" t="s">
-        <v>142</v>
-      </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
+        <v>286</v>
+      </c>
+      <c r="G55" t="s">
         <v>287</v>
-      </c>
-      <c r="G55" t="s">
-        <v>288</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3996,25 +4002,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" t="s">
         <v>143</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
         <v>144</v>
       </c>
-      <c r="C56" t="s">
-        <v>141</v>
-      </c>
-      <c r="D56" t="s">
-        <v>142</v>
-      </c>
-      <c r="E56" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>145</v>
-      </c>
-      <c r="G56" t="s">
-        <v>146</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -4029,25 +4035,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57">
         <v>470</v>
       </c>
       <c r="C57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" t="s">
         <v>141</v>
       </c>
-      <c r="D57" t="s">
-        <v>142</v>
-      </c>
       <c r="E57" t="s">
         <v>19</v>
       </c>
       <c r="F57" t="s">
+        <v>147</v>
+      </c>
+      <c r="G57" t="s">
         <v>148</v>
-      </c>
-      <c r="G57" t="s">
-        <v>149</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4062,16 +4068,16 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C58" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" t="s">
         <v>193</v>
-      </c>
-      <c r="D58" t="s">
-        <v>194</v>
       </c>
       <c r="H58">
         <v>2</v>
@@ -4079,25 +4085,25 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B59" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" t="s">
+        <v>140</v>
+      </c>
+      <c r="D59" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
         <v>150</v>
       </c>
-      <c r="C59" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" t="s">
-        <v>142</v>
-      </c>
-      <c r="E59" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>151</v>
-      </c>
-      <c r="G59" t="s">
-        <v>152</v>
       </c>
       <c r="H59">
         <v>5</v>
@@ -4112,16 +4118,16 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B60">
         <v>10</v>
       </c>
       <c r="C60" t="s">
+        <v>192</v>
+      </c>
+      <c r="D60" t="s">
         <v>193</v>
-      </c>
-      <c r="D60" t="s">
-        <v>194</v>
       </c>
       <c r="H60">
         <v>4</v>
@@ -4129,16 +4135,16 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C61" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" t="s">
         <v>193</v>
-      </c>
-      <c r="D61" t="s">
-        <v>194</v>
       </c>
       <c r="H61">
         <v>4</v>
@@ -4146,16 +4152,16 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C62" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" t="s">
         <v>193</v>
-      </c>
-      <c r="D62" t="s">
-        <v>194</v>
       </c>
       <c r="H62">
         <v>2</v>
@@ -4167,25 +4173,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" t="s">
         <v>153</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63" t="s">
+        <v>141</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
         <v>154</v>
       </c>
-      <c r="C63" t="s">
-        <v>141</v>
-      </c>
-      <c r="D63" t="s">
-        <v>142</v>
-      </c>
-      <c r="E63" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>155</v>
-      </c>
-      <c r="G63" t="s">
-        <v>156</v>
       </c>
       <c r="H63">
         <v>4</v>
@@ -4200,25 +4206,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64" t="s">
+        <v>192</v>
+      </c>
+      <c r="D64" t="s">
         <v>193</v>
       </c>
-      <c r="D64" t="s">
-        <v>194</v>
-      </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G64" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H64">
         <v>5</v>
@@ -4233,25 +4239,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" t="s">
         <v>157</v>
       </c>
-      <c r="B65" t="s">
-        <v>158</v>
-      </c>
       <c r="C65" t="s">
+        <v>288</v>
+      </c>
+      <c r="D65" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" t="s">
         <v>289</v>
       </c>
-      <c r="D65" t="s">
-        <v>109</v>
-      </c>
-      <c r="E65" t="s">
-        <v>19</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>290</v>
-      </c>
-      <c r="G65" t="s">
-        <v>291</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -4266,25 +4272,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" t="s">
         <v>159</v>
       </c>
-      <c r="B66" t="s">
-        <v>160</v>
-      </c>
       <c r="C66" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
       </c>
       <c r="F66" t="s">
+        <v>295</v>
+      </c>
+      <c r="G66" t="s">
         <v>296</v>
-      </c>
-      <c r="G66" t="s">
-        <v>297</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4299,25 +4305,25 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" t="s">
         <v>161</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" t="s">
+        <v>141</v>
+      </c>
+      <c r="E67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" t="s">
         <v>162</v>
       </c>
-      <c r="C67" t="s">
-        <v>141</v>
-      </c>
-      <c r="D67" t="s">
-        <v>142</v>
-      </c>
-      <c r="E67" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>163</v>
-      </c>
-      <c r="G67" t="s">
-        <v>164</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -4332,25 +4338,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B68">
         <v>200</v>
       </c>
       <c r="C68" t="s">
+        <v>192</v>
+      </c>
+      <c r="D68" t="s">
         <v>193</v>
       </c>
-      <c r="D68" t="s">
-        <v>194</v>
-      </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G68" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H68">
         <v>24</v>
@@ -4365,25 +4371,25 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B69">
         <v>100</v>
       </c>
       <c r="C69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" t="s">
         <v>141</v>
       </c>
-      <c r="D69" t="s">
-        <v>142</v>
-      </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
+        <v>165</v>
+      </c>
+      <c r="G69" t="s">
         <v>166</v>
-      </c>
-      <c r="G69" t="s">
-        <v>167</v>
       </c>
       <c r="H69">
         <v>6</v>
@@ -4398,25 +4404,25 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" t="s">
         <v>168</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" t="s">
+        <v>141</v>
+      </c>
+      <c r="E70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" t="s">
         <v>169</v>
       </c>
-      <c r="C70" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" t="s">
-        <v>142</v>
-      </c>
-      <c r="E70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>170</v>
-      </c>
-      <c r="G70" t="s">
-        <v>171</v>
       </c>
       <c r="H70">
         <v>15</v>
@@ -4431,25 +4437,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71" t="s">
         <v>172</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D71" t="s">
+        <v>141</v>
+      </c>
+      <c r="E71" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" t="s">
         <v>173</v>
       </c>
-      <c r="C71" t="s">
-        <v>141</v>
-      </c>
-      <c r="D71" t="s">
-        <v>142</v>
-      </c>
-      <c r="E71" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>174</v>
-      </c>
-      <c r="G71" t="s">
-        <v>175</v>
       </c>
       <c r="H71">
         <v>6</v>
@@ -4464,25 +4470,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>175</v>
+      </c>
+      <c r="B72" t="s">
         <v>176</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>140</v>
+      </c>
+      <c r="D72" t="s">
+        <v>141</v>
+      </c>
+      <c r="E72" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" t="s">
         <v>177</v>
       </c>
-      <c r="C72" t="s">
-        <v>141</v>
-      </c>
-      <c r="D72" t="s">
-        <v>142</v>
-      </c>
-      <c r="E72" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>178</v>
-      </c>
-      <c r="G72" t="s">
-        <v>179</v>
       </c>
       <c r="H72">
         <v>3</v>
@@ -4497,25 +4503,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" t="s">
         <v>180</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" t="s">
         <v>181</v>
       </c>
-      <c r="C73" t="s">
-        <v>141</v>
-      </c>
-      <c r="D73" t="s">
-        <v>142</v>
-      </c>
-      <c r="E73" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>182</v>
-      </c>
-      <c r="G73" t="s">
-        <v>183</v>
       </c>
       <c r="H73">
         <v>4</v>
@@ -4530,25 +4536,25 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" t="s">
         <v>184</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
         <v>185</v>
       </c>
-      <c r="C74" t="s">
-        <v>141</v>
-      </c>
-      <c r="D74" t="s">
-        <v>142</v>
-      </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>186</v>
-      </c>
-      <c r="G74" t="s">
-        <v>187</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -4563,25 +4569,25 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>187</v>
+      </c>
+      <c r="B75" t="s">
         <v>188</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" t="s">
+        <v>141</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
         <v>189</v>
       </c>
-      <c r="C75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D75" t="s">
-        <v>142</v>
-      </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>190</v>
-      </c>
-      <c r="G75" t="s">
-        <v>191</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4596,25 +4602,25 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B76">
         <v>0.3</v>
       </c>
       <c r="C76" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" t="s">
         <v>193</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
         <v>194</v>
       </c>
-      <c r="E76" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>195</v>
-      </c>
-      <c r="G76" t="s">
-        <v>196</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -4629,25 +4635,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>196</v>
+      </c>
+      <c r="B77" t="s">
         <v>197</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
+        <v>140</v>
+      </c>
+      <c r="D77" t="s">
+        <v>141</v>
+      </c>
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s">
         <v>198</v>
       </c>
-      <c r="C77" t="s">
-        <v>141</v>
-      </c>
-      <c r="D77" t="s">
-        <v>142</v>
-      </c>
-      <c r="E77" t="s">
-        <v>19</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>199</v>
-      </c>
-      <c r="G77" t="s">
-        <v>200</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -4662,25 +4668,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>200</v>
+      </c>
+      <c r="B78" t="s">
         <v>201</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
+        <v>140</v>
+      </c>
+      <c r="D78" t="s">
+        <v>141</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" t="s">
         <v>202</v>
       </c>
-      <c r="C78" t="s">
-        <v>141</v>
-      </c>
-      <c r="D78" t="s">
-        <v>142</v>
-      </c>
-      <c r="E78" t="s">
-        <v>19</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>203</v>
-      </c>
-      <c r="G78" t="s">
-        <v>204</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4695,25 +4701,25 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>204</v>
+      </c>
+      <c r="B79" t="s">
         <v>205</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
+        <v>140</v>
+      </c>
+      <c r="D79" t="s">
+        <v>141</v>
+      </c>
+      <c r="E79" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s">
         <v>206</v>
       </c>
-      <c r="C79" t="s">
-        <v>141</v>
-      </c>
-      <c r="D79" t="s">
-        <v>142</v>
-      </c>
-      <c r="E79" t="s">
-        <v>19</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>207</v>
-      </c>
-      <c r="G79" t="s">
-        <v>208</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4728,16 +4734,16 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B80" t="s">
         <v>14</v>
       </c>
       <c r="C80" t="s">
+        <v>140</v>
+      </c>
+      <c r="D80" t="s">
         <v>141</v>
-      </c>
-      <c r="D80" t="s">
-        <v>142</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
@@ -4755,25 +4761,25 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>208</v>
+      </c>
+      <c r="B81" t="s">
         <v>209</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
+        <v>140</v>
+      </c>
+      <c r="D81" t="s">
+        <v>141</v>
+      </c>
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s">
         <v>210</v>
       </c>
-      <c r="C81" t="s">
-        <v>141</v>
-      </c>
-      <c r="D81" t="s">
-        <v>142</v>
-      </c>
-      <c r="E81" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>211</v>
-      </c>
-      <c r="G81" t="s">
-        <v>212</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -4788,25 +4794,25 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>212</v>
+      </c>
+      <c r="B82" t="s">
         <v>213</v>
       </c>
-      <c r="B82" t="s">
-        <v>214</v>
-      </c>
       <c r="C82" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
+        <v>291</v>
+      </c>
+      <c r="G82" t="s">
         <v>292</v>
-      </c>
-      <c r="G82" t="s">
-        <v>293</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4821,25 +4827,25 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>214</v>
+      </c>
+      <c r="B83" t="s">
         <v>215</v>
       </c>
-      <c r="B83" t="s">
-        <v>216</v>
-      </c>
       <c r="C83" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
       </c>
       <c r="F83" t="s">
+        <v>293</v>
+      </c>
+      <c r="G83" t="s">
         <v>294</v>
-      </c>
-      <c r="G83" t="s">
-        <v>295</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4854,25 +4860,25 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>216</v>
+      </c>
+      <c r="B84" t="s">
         <v>217</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>140</v>
+      </c>
+      <c r="D84" t="s">
+        <v>141</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
         <v>218</v>
       </c>
-      <c r="C84" t="s">
-        <v>141</v>
-      </c>
-      <c r="D84" t="s">
-        <v>142</v>
-      </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="G84" t="s">
         <v>219</v>
-      </c>
-      <c r="G84" t="s">
-        <v>220</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -4887,25 +4893,25 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>220</v>
+      </c>
+      <c r="B85" t="s">
         <v>221</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
+        <v>140</v>
+      </c>
+      <c r="D85" t="s">
+        <v>141</v>
+      </c>
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
         <v>222</v>
       </c>
-      <c r="C85" t="s">
-        <v>141</v>
-      </c>
-      <c r="D85" t="s">
-        <v>142</v>
-      </c>
-      <c r="E85" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>223</v>
-      </c>
-      <c r="G85" t="s">
-        <v>224</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4920,25 +4926,25 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B86" t="s">
+        <v>397</v>
+      </c>
+      <c r="C86" t="s">
+        <v>397</v>
+      </c>
+      <c r="D86" t="s">
+        <v>398</v>
+      </c>
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
         <v>400</v>
       </c>
-      <c r="C86" t="s">
-        <v>400</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
         <v>401</v>
-      </c>
-      <c r="E86" t="s">
-        <v>19</v>
-      </c>
-      <c r="F86" t="s">
-        <v>403</v>
-      </c>
-      <c r="G86" t="s">
-        <v>404</v>
       </c>
       <c r="H86">
         <v>2</v>
@@ -4953,25 +4959,25 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B87" t="s">
+        <v>224</v>
+      </c>
+      <c r="C87" t="s">
+        <v>224</v>
+      </c>
+      <c r="D87" t="s">
         <v>225</v>
       </c>
-      <c r="C87" t="s">
-        <v>225</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>226</v>
       </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>227</v>
-      </c>
-      <c r="G87" t="s">
-        <v>228</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -4986,25 +4992,25 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B88" t="s">
+        <v>228</v>
+      </c>
+      <c r="C88" t="s">
         <v>229</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>230</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
         <v>231</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>232</v>
-      </c>
-      <c r="G88" t="s">
-        <v>233</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -5019,25 +5025,25 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B89" t="s">
+        <v>255</v>
+      </c>
+      <c r="C89" t="s">
+        <v>255</v>
+      </c>
+      <c r="D89" t="s">
         <v>256</v>
       </c>
-      <c r="C89" t="s">
-        <v>256</v>
-      </c>
-      <c r="D89" t="s">
-        <v>257</v>
-      </c>
       <c r="E89" t="s">
+        <v>405</v>
+      </c>
+      <c r="F89" t="s">
         <v>408</v>
       </c>
-      <c r="F89" t="s">
-        <v>411</v>
-      </c>
       <c r="G89" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -5052,25 +5058,25 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B90" t="s">
+        <v>258</v>
+      </c>
+      <c r="C90" t="s">
+        <v>258</v>
+      </c>
+      <c r="D90" t="s">
         <v>259</v>
       </c>
-      <c r="C90" t="s">
-        <v>259</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
         <v>260</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>261</v>
-      </c>
-      <c r="G90" t="s">
-        <v>262</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5085,25 +5091,25 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B91" t="s">
+        <v>234</v>
+      </c>
+      <c r="C91" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" t="s">
         <v>235</v>
       </c>
-      <c r="C91" t="s">
-        <v>235</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>236</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>237</v>
-      </c>
-      <c r="G91" t="s">
-        <v>238</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -5118,25 +5124,25 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B92" t="s">
+        <v>239</v>
+      </c>
+      <c r="C92" t="s">
+        <v>239</v>
+      </c>
+      <c r="D92" t="s">
         <v>240</v>
       </c>
-      <c r="C92" t="s">
-        <v>240</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>241</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>242</v>
-      </c>
-      <c r="G92" t="s">
-        <v>243</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -5151,25 +5157,25 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B93" t="s">
+        <v>244</v>
+      </c>
+      <c r="C93" t="s">
+        <v>244</v>
+      </c>
+      <c r="D93" t="s">
         <v>245</v>
       </c>
-      <c r="C93" t="s">
-        <v>245</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>246</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>247</v>
-      </c>
-      <c r="G93" t="s">
-        <v>248</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -5184,25 +5190,25 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C94" t="s">
+        <v>249</v>
+      </c>
+      <c r="D94" t="s">
         <v>250</v>
       </c>
-      <c r="C94" t="s">
-        <v>250</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>251</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>252</v>
-      </c>
-      <c r="G94" t="s">
-        <v>253</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -5217,25 +5223,25 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B95" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C95" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D95" t="s">
+        <v>404</v>
+      </c>
+      <c r="E95" t="s">
+        <v>405</v>
+      </c>
+      <c r="F95" t="s">
+        <v>406</v>
+      </c>
+      <c r="G95" t="s">
         <v>407</v>
-      </c>
-      <c r="E95" t="s">
-        <v>408</v>
-      </c>
-      <c r="F95" t="s">
-        <v>409</v>
-      </c>
-      <c r="G95" t="s">
-        <v>410</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -5250,25 +5256,25 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B96" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C96" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D96" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E96" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F96" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G96" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H96">
         <v>5</v>
@@ -5283,25 +5289,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B97" t="s">
+        <v>262</v>
+      </c>
+      <c r="C97" t="s">
+        <v>262</v>
+      </c>
+      <c r="D97" t="s">
         <v>263</v>
       </c>
-      <c r="C97" t="s">
-        <v>263</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
         <v>264</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>265</v>
-      </c>
-      <c r="G97" t="s">
-        <v>266</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -5316,25 +5322,25 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B98" t="s">
+        <v>267</v>
+      </c>
+      <c r="C98" t="s">
+        <v>267</v>
+      </c>
+      <c r="D98" t="s">
         <v>268</v>
       </c>
-      <c r="C98" t="s">
-        <v>268</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>269</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>270</v>
-      </c>
-      <c r="G98" t="s">
-        <v>271</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -5349,25 +5355,25 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B99" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C99" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D99" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G99" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -5382,25 +5388,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B100" t="s">
+        <v>351</v>
+      </c>
+      <c r="C100" t="s">
+        <v>351</v>
+      </c>
+      <c r="D100" t="s">
+        <v>353</v>
+      </c>
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>352</v>
       </c>
-      <c r="C100" t="s">
-        <v>352</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="G100" t="s">
         <v>354</v>
-      </c>
-      <c r="E100" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" t="s">
-        <v>353</v>
-      </c>
-      <c r="G100" t="s">
-        <v>355</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -5415,25 +5421,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>435</v>
+      </c>
+      <c r="B101" t="s">
+        <v>437</v>
+      </c>
+      <c r="C101" t="s">
+        <v>437</v>
+      </c>
+      <c r="D101" t="s">
+        <v>436</v>
+      </c>
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>438</v>
       </c>
-      <c r="B101" t="s">
-        <v>440</v>
-      </c>
-      <c r="C101" t="s">
-        <v>440</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="G101" t="s">
         <v>439</v>
-      </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
-        <v>441</v>
-      </c>
-      <c r="G101" t="s">
-        <v>442</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -5448,25 +5454,25 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>441</v>
+      </c>
+      <c r="B102" t="s">
+        <v>442</v>
+      </c>
+      <c r="C102" t="s">
+        <v>442</v>
+      </c>
+      <c r="D102" t="s">
+        <v>443</v>
+      </c>
+      <c r="E102" t="s">
+        <v>405</v>
+      </c>
+      <c r="F102" t="s">
         <v>444</v>
       </c>
-      <c r="B102" t="s">
-        <v>445</v>
-      </c>
-      <c r="C102" t="s">
-        <v>445</v>
-      </c>
-      <c r="D102" t="s">
-        <v>446</v>
-      </c>
-      <c r="E102" t="s">
-        <v>408</v>
-      </c>
-      <c r="F102" t="s">
-        <v>447</v>
-      </c>
       <c r="G102" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -5481,25 +5487,25 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B103" t="s">
+        <v>273</v>
+      </c>
+      <c r="C103" t="s">
+        <v>273</v>
+      </c>
+      <c r="D103" t="s">
         <v>274</v>
       </c>
-      <c r="C103" t="s">
-        <v>274</v>
-      </c>
-      <c r="D103" t="s">
-        <v>275</v>
-      </c>
       <c r="E103" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F103" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G103" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H103">
         <v>2</v>
@@ -5514,25 +5520,25 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>277</v>
+      </c>
+      <c r="B104" t="s">
         <v>278</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
+        <v>278</v>
+      </c>
+      <c r="D104" t="s">
         <v>279</v>
       </c>
-      <c r="C104" t="s">
-        <v>279</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" t="s">
         <v>280</v>
       </c>
-      <c r="E104" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="G104" t="s">
         <v>281</v>
-      </c>
-      <c r="G104" t="s">
-        <v>282</v>
       </c>
       <c r="H104">
         <v>1</v>
@@ -5547,25 +5553,25 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>385</v>
+      </c>
+      <c r="B105" t="s">
+        <v>386</v>
+      </c>
+      <c r="C105" t="s">
+        <v>387</v>
+      </c>
+      <c r="D105" t="s">
+        <v>387</v>
+      </c>
+      <c r="E105" t="s">
+        <v>275</v>
+      </c>
+      <c r="F105" t="s">
         <v>388</v>
       </c>
-      <c r="B105" t="s">
+      <c r="G105" t="s">
         <v>389</v>
-      </c>
-      <c r="C105" t="s">
-        <v>390</v>
-      </c>
-      <c r="D105" t="s">
-        <v>390</v>
-      </c>
-      <c r="E105" t="s">
-        <v>276</v>
-      </c>
-      <c r="F105" t="s">
-        <v>391</v>
-      </c>
-      <c r="G105" t="s">
-        <v>392</v>
       </c>
       <c r="H105">
         <v>2</v>
@@ -5580,25 +5586,25 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>282</v>
+      </c>
+      <c r="B106" t="s">
         <v>283</v>
       </c>
-      <c r="B106" t="s">
-        <v>284</v>
-      </c>
       <c r="C106" t="s">
+        <v>391</v>
+      </c>
+      <c r="D106" t="s">
+        <v>392</v>
+      </c>
+      <c r="E106" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" t="s">
+        <v>393</v>
+      </c>
+      <c r="G106" t="s">
         <v>394</v>
-      </c>
-      <c r="D106" t="s">
-        <v>395</v>
-      </c>
-      <c r="E106" t="s">
-        <v>19</v>
-      </c>
-      <c r="F106" t="s">
-        <v>396</v>
-      </c>
-      <c r="G106" t="s">
-        <v>397</v>
       </c>
       <c r="H106">
         <v>1</v>

</xml_diff>

<commit_message>
Added 1.8V regulator used by the XTAG-2.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="471">
   <si>
     <t>Part</t>
   </si>
@@ -1102,9 +1102,6 @@
     <t>JP23</t>
   </si>
   <si>
-    <t>JP20, JP21, JP22</t>
-  </si>
-  <si>
     <t>2X10 Right angle</t>
   </si>
   <si>
@@ -1360,21 +1357,12 @@
     <t>785-1011-1-ND</t>
   </si>
   <si>
-    <t>R10, R139, R140, R141, R142, R143</t>
-  </si>
-  <si>
-    <t>LED1, LED2, LED3, LED4, LED5, LED6</t>
-  </si>
-  <si>
     <t>R11, R12</t>
   </si>
   <si>
     <t>R15, R65, R66, R67, R68</t>
   </si>
   <si>
-    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C86, C87, C88, C89</t>
-  </si>
-  <si>
     <t>798-UX60-MB-5S8</t>
   </si>
   <si>
@@ -1403,6 +1391,42 @@
   </si>
   <si>
     <t>JP1</t>
+  </si>
+  <si>
+    <t>JP20, JP21</t>
+  </si>
+  <si>
+    <t>NCP699</t>
+  </si>
+  <si>
+    <t>NCP699SN18T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>NCP699SN18T1G</t>
+  </si>
+  <si>
+    <t>C91</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>445-3451-1-ND</t>
+  </si>
+  <si>
+    <t>C1608Y5V1C225Z</t>
+  </si>
+  <si>
+    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C86, C87, C88, C89, C90</t>
+  </si>
+  <si>
+    <t>R10, R20, R139, R140, R141, R142, R143</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7</t>
+  </si>
+  <si>
+    <t>U18</t>
   </si>
 </sst>
 </file>
@@ -2231,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2267,7 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="12" max="12" width="32.85546875" customWidth="1"/>
   </cols>
@@ -2288,7 +2312,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2319,8 +2343,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J132)</f>
-        <v>206.30799999999999</v>
+        <f>SUM(J2:J134)</f>
+        <v>207.05900000000003</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2352,13 +2376,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J76" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J77" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>452</v>
+        <v>467</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2379,14 +2403,14 @@
         <v>306</v>
       </c>
       <c r="H4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.58800000000000008</v>
+        <v>0.60899999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2979,25 +3003,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
+        <v>429</v>
+      </c>
+      <c r="D24" t="s">
         <v>430</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
         <v>431</v>
       </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>432</v>
-      </c>
-      <c r="G24" t="s">
-        <v>433</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -3012,10 +3036,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>380</v>
+      </c>
+      <c r="B25" t="s">
         <v>381</v>
-      </c>
-      <c r="B25" t="s">
-        <v>382</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3027,10 +3051,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
+        <v>382</v>
+      </c>
+      <c r="G25" t="s">
         <v>383</v>
-      </c>
-      <c r="G25" t="s">
-        <v>384</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3045,46 +3069,46 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>463</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>464</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>465</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>466</v>
       </c>
       <c r="H26">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>0.315</v>
+        <v>0.24</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>8.19</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
         <v>66</v>
@@ -3093,64 +3117,61 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>299</v>
+        <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>300</v>
+        <v>65</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="I27">
-        <v>0.35</v>
+        <v>0.315</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="G28" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L28" t="s">
-        <v>343</v>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>72</v>
@@ -3162,28 +3183,31 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="G29" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0.68</v>
+        <v>0.4</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.4</v>
+      </c>
+      <c r="L29" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
         <v>72</v>
@@ -3195,187 +3219,190 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G30" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="G31" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>11.91</v>
+        <v>0.42</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>425</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>367</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>368</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>369</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>370</v>
+        <v>284</v>
       </c>
       <c r="G32" t="s">
-        <v>371</v>
+        <v>285</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>0.44</v>
+        <v>11.91</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>424</v>
       </c>
       <c r="B33" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="C33" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="D33" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="G33" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33">
-        <v>2.15</v>
+        <v>0.44</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>345</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>345</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>345</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>344</v>
       </c>
       <c r="G34" t="s">
-        <v>83</v>
+        <v>345</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>0.77</v>
+        <v>2.15</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>340</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>275</v>
+        <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>342</v>
+        <v>84</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B36" t="s">
         <v>85</v>
@@ -3390,10 +3417,7 @@
         <v>275</v>
       </c>
       <c r="F36" t="s">
-        <v>341</v>
-      </c>
-      <c r="G36" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3408,541 +3432,541 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>462</v>
+        <v>339</v>
       </c>
       <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F37" t="s">
+        <v>341</v>
+      </c>
+      <c r="G37" t="s">
         <v>14</v>
       </c>
-      <c r="C37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" t="s">
-        <v>363</v>
-      </c>
-      <c r="E37" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" t="s">
-        <v>88</v>
-      </c>
-      <c r="G37" t="s">
-        <v>89</v>
-      </c>
       <c r="H37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>0.93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>418</v>
+        <v>458</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>362</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>297</v>
+        <v>88</v>
       </c>
       <c r="G38" t="s">
-        <v>298</v>
+        <v>89</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>1.47</v>
+        <v>0.93</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>297</v>
       </c>
       <c r="G39" t="s">
-        <v>95</v>
+        <v>298</v>
       </c>
       <c r="H39">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I39">
-        <v>0.42</v>
+        <v>1.47</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>5.46</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>433</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>426</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>427</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>428</v>
-      </c>
-      <c r="G40">
-        <v>702461004</v>
+        <v>94</v>
+      </c>
+      <c r="G40" t="s">
+        <v>95</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I40">
-        <v>1.64</v>
+        <v>0.42</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>1.64</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>362</v>
-      </c>
-      <c r="B41" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>425</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>426</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>359</v>
-      </c>
-      <c r="G41" t="s">
-        <v>360</v>
+        <v>427</v>
+      </c>
+      <c r="G41">
+        <v>702461004</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>0.13</v>
+        <v>1.64</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>361</v>
+        <v>459</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>355</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>356</v>
+        <v>98</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G42" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42">
-        <v>0.71</v>
+        <v>0.13</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C43" t="s">
-        <v>458</v>
+        <v>355</v>
       </c>
       <c r="D43" t="s">
-        <v>459</v>
+        <v>356</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>461</v>
+        <v>357</v>
       </c>
       <c r="G43" t="s">
-        <v>460</v>
+        <v>358</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1.58</v>
+        <v>0.71</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>1.58</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>419</v>
+        <v>363</v>
       </c>
       <c r="C44" t="s">
-        <v>420</v>
+        <v>454</v>
       </c>
       <c r="D44" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="G44" t="s">
-        <v>423</v>
+        <v>456</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>1.67</v>
+        <v>1.58</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="C45" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D45" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G45" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="H45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I45">
-        <v>0.5</v>
+        <v>1.67</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" t="s">
-        <v>100</v>
+        <v>412</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>413</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>414</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>103</v>
+        <v>415</v>
       </c>
       <c r="G46" t="s">
-        <v>104</v>
+        <v>416</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I46">
-        <v>2.13</v>
+        <v>0.5</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G47" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G49" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>449</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
       </c>
       <c r="G50" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="H50">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1.85</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D51" t="s">
-        <v>126</v>
-      </c>
-      <c r="E51" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" t="s">
-        <v>447</v>
+        <v>124</v>
       </c>
       <c r="G51" t="s">
-        <v>445</v>
+        <v>14</v>
       </c>
       <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
-        <v>0.55000000000000004</v>
+        <v>7</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>445</v>
       </c>
       <c r="B52" t="s">
         <v>128</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D52" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>446</v>
       </c>
       <c r="G52" t="s">
-        <v>14</v>
+        <v>444</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0.55000000000000004</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>365</v>
+        <v>127</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D53" t="s">
-        <v>126</v>
-      </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G53" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53">
-        <v>0.41</v>
+        <v>3</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C54" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D54" t="s">
         <v>126</v>
@@ -3951,61 +3975,61 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G54" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>365</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>286</v>
+        <v>136</v>
       </c>
       <c r="G55" t="s">
-        <v>287</v>
+        <v>137</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
         <v>140</v>
@@ -4017,28 +4041,28 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>144</v>
+        <v>286</v>
       </c>
       <c r="G56" t="s">
-        <v>145</v>
+        <v>287</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>146</v>
-      </c>
-      <c r="B57">
-        <v>470</v>
+        <v>142</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
       </c>
       <c r="C57" t="s">
         <v>140</v>
@@ -4050,10 +4074,10 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G57" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4068,77 +4092,93 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>456</v>
-      </c>
-      <c r="B58" t="s">
-        <v>176</v>
+        <v>146</v>
+      </c>
+      <c r="B58">
+        <v>470</v>
       </c>
       <c r="C58" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>193</v>
+        <v>141</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" t="s">
+        <v>147</v>
+      </c>
+      <c r="G58" t="s">
+        <v>148</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>0.04</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B59" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" t="s">
-        <v>150</v>
-      </c>
-      <c r="G59" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="H59">
-        <v>5</v>
-      </c>
-      <c r="I59">
-        <v>0.04</v>
-      </c>
-      <c r="J59">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>454</v>
-      </c>
-      <c r="B60">
-        <v>10</v>
+        <v>451</v>
+      </c>
+      <c r="B60" t="s">
+        <v>149</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>141</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" t="s">
+        <v>150</v>
+      </c>
+      <c r="G60" t="s">
+        <v>151</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <v>0.04</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>457</v>
-      </c>
-      <c r="B61" t="s">
-        <v>153</v>
+        <v>450</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
       </c>
       <c r="C61" t="s">
         <v>192</v>
@@ -4152,10 +4192,10 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B62" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
         <v>192</v>
@@ -4164,118 +4204,102 @@
         <v>193</v>
       </c>
       <c r="H62">
-        <v>2</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>447</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>141</v>
-      </c>
-      <c r="E63" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" t="s">
-        <v>154</v>
-      </c>
-      <c r="G63" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="H63">
-        <v>4</v>
-      </c>
-      <c r="I63">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>451</v>
-      </c>
-      <c r="B64">
-        <v>100</v>
+        <v>152</v>
+      </c>
+      <c r="B64" t="s">
+        <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>378</v>
+        <v>154</v>
       </c>
       <c r="G64" t="s">
-        <v>379</v>
+        <v>155</v>
       </c>
       <c r="H64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
-        <f>H64*I64</f>
-        <v>0.2</v>
+        <f t="shared" si="0"/>
+        <v>0.16</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" t="s">
-        <v>157</v>
+        <v>448</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>288</v>
+        <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>289</v>
+        <v>377</v>
       </c>
       <c r="G65" t="s">
-        <v>290</v>
+        <v>378</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I65">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J65">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
+        <f>H65*I65</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C66" t="s">
         <v>288</v>
@@ -4287,10 +4311,10 @@
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G66" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4305,109 +4329,109 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
-        <v>140</v>
+        <v>288</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>162</v>
+        <v>295</v>
       </c>
       <c r="G67" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68">
-        <v>200</v>
+        <v>160</v>
+      </c>
+      <c r="B68" t="s">
+        <v>161</v>
       </c>
       <c r="C68" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>375</v>
+        <v>162</v>
       </c>
       <c r="G68" t="s">
-        <v>376</v>
+        <v>163</v>
       </c>
       <c r="H68">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>377</v>
+        <v>164</v>
       </c>
       <c r="B69">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D69" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>165</v>
+        <v>374</v>
       </c>
       <c r="G69" t="s">
-        <v>166</v>
+        <v>375</v>
       </c>
       <c r="H69">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="I69">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
-      </c>
-      <c r="B70" t="s">
-        <v>168</v>
+        <v>376</v>
+      </c>
+      <c r="B70">
+        <v>100</v>
       </c>
       <c r="C70" t="s">
         <v>140</v>
@@ -4419,28 +4443,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G70" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H70">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B71" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C71" t="s">
         <v>140</v>
@@ -4452,28 +4476,28 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G71" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H71">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I71">
         <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B72" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C72" t="s">
         <v>140</v>
@@ -4485,28 +4509,28 @@
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G72" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H72">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I72">
         <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B73" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C73" t="s">
         <v>140</v>
@@ -4518,28 +4542,28 @@
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G73" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I73">
         <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B74" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C74" t="s">
         <v>140</v>
@@ -4551,28 +4575,28 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G74" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I74">
         <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C75" t="s">
         <v>140</v>
@@ -4584,10 +4608,10 @@
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G75" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4602,76 +4626,76 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>191</v>
-      </c>
-      <c r="B76">
-        <v>0.3</v>
+        <v>187</v>
+      </c>
+      <c r="B76" t="s">
+        <v>188</v>
       </c>
       <c r="C76" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D76" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
       </c>
       <c r="F76" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G76" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J76">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>196</v>
-      </c>
-      <c r="B77" t="s">
-        <v>197</v>
+        <v>191</v>
+      </c>
+      <c r="B77">
+        <v>0.3</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D77" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G77" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J77">
-        <f t="shared" ref="J77:J106" si="1">H77*I77</f>
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B78" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C78" t="s">
         <v>140</v>
@@ -4683,10 +4707,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G78" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4695,16 +4719,16 @@
         <v>0.04</v>
       </c>
       <c r="J78">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J78:J108" si="1">H78*I78</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B79" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C79" t="s">
         <v>140</v>
@@ -4716,10 +4740,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G79" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4734,10 +4758,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>448</v>
+        <v>204</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>205</v>
       </c>
       <c r="C80" t="s">
         <v>140</v>
@@ -4748,23 +4772,29 @@
       <c r="E80" t="s">
         <v>19</v>
       </c>
+      <c r="F80" t="s">
+        <v>206</v>
+      </c>
       <c r="G80" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="H80">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>0.04</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>208</v>
+        <v>468</v>
       </c>
       <c r="B81" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
         <v>140</v>
@@ -4775,62 +4805,56 @@
       <c r="E81" t="s">
         <v>19</v>
       </c>
-      <c r="F81" t="s">
-        <v>210</v>
-      </c>
       <c r="G81" t="s">
-        <v>211</v>
+        <v>14</v>
       </c>
       <c r="H81">
-        <v>1</v>
-      </c>
-      <c r="I81">
-        <v>0.04</v>
+        <v>7</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B82" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C82" t="s">
-        <v>288</v>
+        <v>140</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>291</v>
+        <v>210</v>
       </c>
       <c r="G82" t="s">
-        <v>292</v>
+        <v>211</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B83" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C83" t="s">
         <v>288</v>
@@ -4842,10 +4866,10 @@
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G83" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4860,43 +4884,43 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C84" t="s">
-        <v>140</v>
+        <v>288</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>218</v>
+        <v>293</v>
       </c>
       <c r="G84" t="s">
-        <v>219</v>
+        <v>294</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B85" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C85" t="s">
         <v>140</v>
@@ -4908,10 +4932,10 @@
         <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G85" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4926,693 +4950,759 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>399</v>
+        <v>220</v>
       </c>
       <c r="B86" t="s">
-        <v>397</v>
+        <v>221</v>
       </c>
       <c r="C86" t="s">
-        <v>397</v>
+        <v>140</v>
       </c>
       <c r="D86" t="s">
-        <v>398</v>
+        <v>141</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>400</v>
+        <v>222</v>
       </c>
       <c r="G86" t="s">
-        <v>401</v>
+        <v>223</v>
       </c>
       <c r="H86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I86">
-        <v>15.1</v>
+        <v>0.04</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>30.2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B87" t="s">
-        <v>224</v>
+        <v>396</v>
       </c>
       <c r="C87" t="s">
-        <v>224</v>
+        <v>396</v>
       </c>
       <c r="D87" t="s">
-        <v>225</v>
+        <v>397</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>226</v>
+        <v>399</v>
       </c>
       <c r="G87" t="s">
-        <v>227</v>
+        <v>400</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I87">
-        <v>6.6</v>
+        <v>15.1</v>
       </c>
       <c r="J87">
-        <f t="shared" ref="J87:J96" si="2">H87*I87</f>
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>30.2</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B88" t="s">
+        <v>224</v>
+      </c>
+      <c r="C88" t="s">
+        <v>224</v>
+      </c>
+      <c r="D88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
+        <v>226</v>
+      </c>
+      <c r="G88" t="s">
+        <v>227</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>6.6</v>
+      </c>
+      <c r="J88">
+        <f t="shared" ref="J88:J97" si="2">H88*I88</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>402</v>
+      </c>
+      <c r="B89" t="s">
         <v>228</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>229</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>230</v>
       </c>
-      <c r="E88" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
         <v>231</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" t="s">
         <v>232</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
         <v>0.79</v>
       </c>
-      <c r="J88">
+      <c r="J89">
         <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>233</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>255</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>255</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>256</v>
       </c>
-      <c r="E89" t="s">
-        <v>405</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E90" t="s">
+        <v>404</v>
+      </c>
+      <c r="F90" t="s">
+        <v>407</v>
+      </c>
+      <c r="G90" t="s">
         <v>408</v>
       </c>
-      <c r="G89" t="s">
-        <v>409</v>
-      </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
         <v>0.45</v>
       </c>
-      <c r="J89">
+      <c r="J90">
         <f t="shared" si="2"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>238</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>258</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>258</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>259</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
         <v>260</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" t="s">
         <v>261</v>
       </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>0.47</v>
       </c>
-      <c r="J90">
+      <c r="J91">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>243</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>234</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>234</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>235</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
         <v>236</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G92" t="s">
         <v>237</v>
       </c>
-      <c r="H91">
-        <v>1</v>
-      </c>
-      <c r="I91">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
         <v>0.67</v>
       </c>
-      <c r="J91">
+      <c r="J92">
         <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>248</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>239</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>239</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>240</v>
       </c>
-      <c r="E92" t="s">
-        <v>19</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
         <v>241</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" t="s">
         <v>242</v>
       </c>
-      <c r="H92">
-        <v>1</v>
-      </c>
-      <c r="I92">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
         <v>6.63</v>
       </c>
-      <c r="J92">
+      <c r="J93">
         <f t="shared" si="2"/>
         <v>6.63</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>253</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>244</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>244</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>245</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
         <v>246</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>247</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
-      <c r="I93">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
         <v>1.67</v>
       </c>
-      <c r="J93">
+      <c r="J94">
         <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>254</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>249</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>249</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" t="s">
         <v>250</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
         <v>251</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>252</v>
       </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
         <v>5.88</v>
       </c>
-      <c r="J94">
+      <c r="J95">
         <f t="shared" si="2"/>
         <v>5.88</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>257</v>
       </c>
-      <c r="B95" t="s">
-        <v>396</v>
-      </c>
-      <c r="C95" t="s">
-        <v>396</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="B96" t="s">
+        <v>395</v>
+      </c>
+      <c r="C96" t="s">
+        <v>395</v>
+      </c>
+      <c r="D96" t="s">
+        <v>403</v>
+      </c>
+      <c r="E96" t="s">
         <v>404</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F96" t="s">
         <v>405</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G96" t="s">
         <v>406</v>
       </c>
-      <c r="G95" t="s">
-        <v>407</v>
-      </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
         <v>1.23</v>
       </c>
-      <c r="J95">
+      <c r="J96">
         <f t="shared" si="2"/>
         <v>1.23</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>424</v>
-      </c>
-      <c r="B96" t="s">
-        <v>395</v>
-      </c>
-      <c r="C96" t="s">
-        <v>395</v>
-      </c>
-      <c r="D96" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>423</v>
+      </c>
+      <c r="B97" t="s">
+        <v>394</v>
+      </c>
+      <c r="C97" t="s">
+        <v>394</v>
+      </c>
+      <c r="D97" t="s">
+        <v>409</v>
+      </c>
+      <c r="E97" t="s">
+        <v>404</v>
+      </c>
+      <c r="F97" t="s">
         <v>410</v>
       </c>
-      <c r="E96" t="s">
-        <v>405</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="G97" t="s">
         <v>411</v>
       </c>
-      <c r="G96" t="s">
-        <v>412</v>
-      </c>
-      <c r="H96">
+      <c r="H97">
         <v>5</v>
       </c>
-      <c r="I96">
+      <c r="I97">
         <v>2.76</v>
       </c>
-      <c r="J96">
+      <c r="J97">
         <f t="shared" si="2"/>
         <v>13.799999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>266</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>262</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>262</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>263</v>
       </c>
-      <c r="E97" t="s">
-        <v>19</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
         <v>264</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G98" t="s">
         <v>265</v>
       </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
         <v>3.79</v>
       </c>
-      <c r="J97">
+      <c r="J98">
         <f t="shared" si="1"/>
         <v>3.79</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>271</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>267</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>267</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>268</v>
       </c>
-      <c r="E98" t="s">
-        <v>19</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
         <v>269</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G99" t="s">
         <v>270</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
         <v>1.57</v>
       </c>
-      <c r="J98">
+      <c r="J99">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>350</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
+        <v>371</v>
+      </c>
+      <c r="C100" t="s">
+        <v>371</v>
+      </c>
+      <c r="D100" t="s">
+        <v>272</v>
+      </c>
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
         <v>372</v>
       </c>
-      <c r="C99" t="s">
-        <v>372</v>
-      </c>
-      <c r="D99" t="s">
-        <v>272</v>
-      </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="G100" t="s">
         <v>373</v>
       </c>
-      <c r="G99" t="s">
-        <v>374</v>
-      </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99">
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
         <v>8.48</v>
       </c>
-      <c r="J99">
+      <c r="J100">
         <f t="shared" si="1"/>
         <v>8.48</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>390</v>
-      </c>
-      <c r="B100" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>389</v>
+      </c>
+      <c r="B101" t="s">
         <v>351</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>351</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>353</v>
       </c>
-      <c r="E100" t="s">
-        <v>19</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>352</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G101" t="s">
         <v>354</v>
       </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
         <v>6.84</v>
       </c>
-      <c r="J100">
+      <c r="J101">
         <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>434</v>
+      </c>
+      <c r="B102" t="s">
+        <v>436</v>
+      </c>
+      <c r="C102" t="s">
+        <v>436</v>
+      </c>
+      <c r="D102" t="s">
         <v>435</v>
       </c>
-      <c r="B101" t="s">
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>437</v>
       </c>
-      <c r="C101" t="s">
-        <v>437</v>
-      </c>
-      <c r="D101" t="s">
-        <v>436</v>
-      </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="G102" t="s">
         <v>438</v>
       </c>
-      <c r="G101" t="s">
-        <v>439</v>
-      </c>
-      <c r="H101">
-        <v>1</v>
-      </c>
-      <c r="I101">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
         <v>3.15</v>
       </c>
-      <c r="J101">
+      <c r="J102">
         <f t="shared" si="1"/>
         <v>3.15</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>470</v>
+      </c>
+      <c r="B103" t="s">
+        <v>460</v>
+      </c>
+      <c r="C103" t="s">
+        <v>460</v>
+      </c>
+      <c r="D103" t="s">
+        <v>256</v>
+      </c>
+      <c r="E103" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" t="s">
+        <v>461</v>
+      </c>
+      <c r="G103" t="s">
+        <v>462</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>0.62</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="1"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>440</v>
+      </c>
+      <c r="B104" t="s">
         <v>441</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C104" t="s">
+        <v>441</v>
+      </c>
+      <c r="D104" t="s">
         <v>442</v>
       </c>
-      <c r="C102" t="s">
-        <v>442</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="E104" t="s">
+        <v>404</v>
+      </c>
+      <c r="F104" t="s">
         <v>443</v>
       </c>
-      <c r="E102" t="s">
-        <v>405</v>
-      </c>
-      <c r="F102" t="s">
-        <v>444</v>
-      </c>
-      <c r="G102" t="s">
-        <v>442</v>
-      </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="G104" t="s">
+        <v>441</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
         <v>5.71</v>
       </c>
-      <c r="J102">
+      <c r="J104">
         <f t="shared" si="1"/>
         <v>5.71</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>440</v>
-      </c>
-      <c r="B103" t="s">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>439</v>
+      </c>
+      <c r="B105" t="s">
         <v>273</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C105" t="s">
         <v>273</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D105" t="s">
         <v>274</v>
       </c>
-      <c r="E103" t="s">
-        <v>405</v>
-      </c>
-      <c r="F103" t="s">
-        <v>453</v>
-      </c>
-      <c r="G103" t="s">
+      <c r="E105" t="s">
+        <v>404</v>
+      </c>
+      <c r="F105" t="s">
+        <v>449</v>
+      </c>
+      <c r="G105" t="s">
         <v>276</v>
       </c>
-      <c r="H103">
+      <c r="H105">
         <v>2</v>
       </c>
-      <c r="I103">
+      <c r="I105">
         <v>1.26</v>
       </c>
-      <c r="J103">
+      <c r="J105">
         <f t="shared" si="1"/>
         <v>2.52</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>277</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>278</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C106" t="s">
         <v>278</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D106" t="s">
         <v>279</v>
       </c>
-      <c r="E104" t="s">
-        <v>19</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="E106" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" t="s">
         <v>280</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G106" t="s">
         <v>281</v>
       </c>
-      <c r="H104">
-        <v>1</v>
-      </c>
-      <c r="I104">
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="I106">
         <v>2.96</v>
       </c>
-      <c r="J104">
+      <c r="J106">
         <f t="shared" si="1"/>
         <v>2.96</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>384</v>
+      </c>
+      <c r="B107" t="s">
         <v>385</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C107" t="s">
         <v>386</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D107" t="s">
+        <v>386</v>
+      </c>
+      <c r="E107" t="s">
+        <v>275</v>
+      </c>
+      <c r="F107" t="s">
         <v>387</v>
       </c>
-      <c r="D105" t="s">
-        <v>387</v>
-      </c>
-      <c r="E105" t="s">
-        <v>275</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="G107" t="s">
         <v>388</v>
       </c>
-      <c r="G105" t="s">
-        <v>389</v>
-      </c>
-      <c r="H105">
+      <c r="H107">
         <v>2</v>
       </c>
-      <c r="I105">
+      <c r="I107">
         <v>0.95</v>
       </c>
-      <c r="J105">
+      <c r="J107">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>282</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B108" t="s">
         <v>283</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C108" t="s">
+        <v>390</v>
+      </c>
+      <c r="D108" t="s">
         <v>391</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E108" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" t="s">
         <v>392</v>
       </c>
-      <c r="E106" t="s">
-        <v>19</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="G108" t="s">
         <v>393</v>
       </c>
-      <c r="G106" t="s">
-        <v>394</v>
-      </c>
-      <c r="H106">
-        <v>1</v>
-      </c>
-      <c r="I106">
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="I108">
         <v>1.99</v>
       </c>
-      <c r="J106">
+      <c r="J108">
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>

</xml_diff>

<commit_message>
Filled in sources for unsourced 0402 resistors in BOM.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-byvalue" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="480">
   <si>
     <t>Part</t>
   </si>
@@ -919,12 +919,6 @@
     <t>CDSU400B</t>
   </si>
   <si>
-    <t>445-5146-1-ND</t>
-  </si>
-  <si>
-    <t>C1608X5R1E105K</t>
-  </si>
-  <si>
     <t>490-5523-1-ND</t>
   </si>
   <si>
@@ -1153,9 +1147,6 @@
     <t>ERJ-2GEJ101X</t>
   </si>
   <si>
-    <t>C1, C68</t>
-  </si>
-  <si>
     <t>C69</t>
   </si>
   <si>
@@ -1427,6 +1418,42 @@
   </si>
   <si>
     <t>U18</t>
+  </si>
+  <si>
+    <t>445-4979-1-ND</t>
+  </si>
+  <si>
+    <t>C1005X5R1C105M</t>
+  </si>
+  <si>
+    <t>C1, C76</t>
+  </si>
+  <si>
+    <t>TODO: Make this a 1206</t>
+  </si>
+  <si>
+    <t>RMCF0402FT1K50CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT1K50</t>
+  </si>
+  <si>
+    <t>P10.0LCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF10R0X</t>
+  </si>
+  <si>
+    <t>P100KJCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ104X</t>
+  </si>
+  <si>
+    <t>P4.7KJCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ472X</t>
   </si>
 </sst>
 </file>
@@ -2257,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,30 +2334,30 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>379</v>
+        <v>470</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>426</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>427</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>301</v>
+        <v>468</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>469</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2344,7 +2371,7 @@
       </c>
       <c r="K2">
         <f>SUM(J2:J134)</f>
-        <v>207.05900000000003</v>
+        <v>207.679</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2364,10 +2391,10 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -2382,7 +2409,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2397,10 +2424,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H4">
         <v>29</v>
@@ -2454,10 +2481,10 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2470,7 +2497,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2496,6 +2523,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L7" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2514,10 +2544,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -2547,10 +2577,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2580,10 +2610,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2596,7 +2626,7 @@
         <v>0.06</v>
       </c>
       <c r="L10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2649,10 +2679,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2682,10 +2712,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2698,7 +2728,7 @@
         <v>0.06</v>
       </c>
       <c r="L13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2718,10 +2748,10 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -2734,7 +2764,7 @@
         <v>0.48</v>
       </c>
       <c r="L14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2778,10 +2808,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2859,10 +2889,10 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2875,7 +2905,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2895,10 +2925,10 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G20" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2952,10 +2982,10 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2970,10 +3000,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B23" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -2985,10 +3015,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G23" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -3003,25 +3033,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
+        <v>426</v>
+      </c>
+      <c r="D24" t="s">
+        <v>427</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>428</v>
+      </c>
+      <c r="G24" t="s">
         <v>429</v>
-      </c>
-      <c r="D24" t="s">
-        <v>430</v>
-      </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>431</v>
-      </c>
-      <c r="G24" t="s">
-        <v>432</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -3036,10 +3066,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B25" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -3051,10 +3081,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G25" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3069,10 +3099,10 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B26" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -3084,10 +3114,10 @@
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G26" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -3183,10 +3213,10 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G29" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3199,7 +3229,7 @@
         <v>0.4</v>
       </c>
       <c r="L29" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3219,10 +3249,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G30" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3252,10 +3282,10 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G31" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -3303,25 +3333,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B33" t="s">
+        <v>364</v>
+      </c>
+      <c r="C33" t="s">
+        <v>365</v>
+      </c>
+      <c r="D33" t="s">
         <v>366</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>367</v>
       </c>
-      <c r="D33" t="s">
+      <c r="G33" t="s">
         <v>368</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" t="s">
-        <v>369</v>
-      </c>
-      <c r="G33" t="s">
-        <v>370</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -3339,22 +3369,22 @@
         <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C34" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D34" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G34" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3402,7 +3432,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B36" t="s">
         <v>85</v>
@@ -3417,7 +3447,7 @@
         <v>275</v>
       </c>
       <c r="F36" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3432,7 +3462,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B37" t="s">
         <v>85</v>
@@ -3447,7 +3477,7 @@
         <v>275</v>
       </c>
       <c r="F37" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
@@ -3465,7 +3495,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
@@ -3474,7 +3504,7 @@
         <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -3498,7 +3528,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -3531,7 +3561,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
@@ -3567,16 +3597,16 @@
         <v>96</v>
       </c>
       <c r="C41" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D41" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G41">
         <v>702461004</v>
@@ -3594,7 +3624,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
@@ -3609,10 +3639,10 @@
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G42" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H42">
         <v>2</v>
@@ -3627,22 +3657,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C43" t="s">
+        <v>353</v>
+      </c>
+      <c r="D43" t="s">
+        <v>354</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
         <v>355</v>
       </c>
-      <c r="D43" t="s">
+      <c r="G43" t="s">
         <v>356</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>357</v>
-      </c>
-      <c r="G43" t="s">
-        <v>358</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3657,22 +3687,22 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C44" t="s">
+        <v>451</v>
+      </c>
+      <c r="D44" t="s">
+        <v>452</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
         <v>454</v>
       </c>
-      <c r="D44" t="s">
-        <v>455</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>457</v>
-      </c>
       <c r="G44" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3687,22 +3717,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>415</v>
+      </c>
+      <c r="C45" t="s">
+        <v>416</v>
+      </c>
+      <c r="D45" t="s">
+        <v>417</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
         <v>418</v>
       </c>
-      <c r="C45" t="s">
+      <c r="G45" t="s">
         <v>419</v>
-      </c>
-      <c r="D45" t="s">
-        <v>420</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>421</v>
-      </c>
-      <c r="G45" t="s">
-        <v>422</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -3717,22 +3747,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>409</v>
+      </c>
+      <c r="C46" t="s">
+        <v>410</v>
+      </c>
+      <c r="D46" t="s">
+        <v>411</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
         <v>412</v>
       </c>
-      <c r="C46" t="s">
+      <c r="G46" t="s">
         <v>413</v>
-      </c>
-      <c r="D46" t="s">
-        <v>414</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>415</v>
-      </c>
-      <c r="G46" t="s">
-        <v>416</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -3879,7 +3909,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -3903,7 +3933,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B52" t="s">
         <v>128</v>
@@ -3918,10 +3948,10 @@
         <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="G52" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3960,7 +3990,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B54" t="s">
         <v>131</v>
@@ -3993,7 +4023,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B55" t="s">
         <v>134</v>
@@ -4125,7 +4155,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B59" t="s">
         <v>176</v>
@@ -4136,13 +4166,29 @@
       <c r="D59" t="s">
         <v>193</v>
       </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
+        <v>472</v>
+      </c>
+      <c r="G59" t="s">
+        <v>473</v>
+      </c>
       <c r="H59">
         <v>2</v>
       </c>
+      <c r="I59">
+        <v>0.04</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B60" t="s">
         <v>149</v>
@@ -4175,7 +4221,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B61">
         <v>10</v>
@@ -4186,13 +4232,29 @@
       <c r="D61" t="s">
         <v>193</v>
       </c>
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" t="s">
+        <v>474</v>
+      </c>
+      <c r="G61" t="s">
+        <v>475</v>
+      </c>
       <c r="H61">
         <v>4</v>
       </c>
+      <c r="I61">
+        <v>0.06</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B62" t="s">
         <v>153</v>
@@ -4203,13 +4265,29 @@
       <c r="D62" t="s">
         <v>193</v>
       </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
+        <v>476</v>
+      </c>
+      <c r="G62" t="s">
+        <v>477</v>
+      </c>
       <c r="H62">
         <v>4</v>
       </c>
+      <c r="I62">
+        <v>0.05</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B63" t="s">
         <v>161</v>
@@ -4220,12 +4298,24 @@
       <c r="D63" t="s">
         <v>193</v>
       </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>478</v>
+      </c>
+      <c r="G63" t="s">
+        <v>479</v>
+      </c>
       <c r="H63">
         <v>2</v>
       </c>
+      <c r="I63">
+        <v>0.05</v>
+      </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -4263,7 +4353,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B65">
         <v>100</v>
@@ -4278,10 +4368,10 @@
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G65" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H65">
         <v>5</v>
@@ -4410,10 +4500,10 @@
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G69" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H69">
         <v>24</v>
@@ -4428,7 +4518,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B70">
         <v>100</v>
@@ -4791,7 +4881,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B81" t="s">
         <v>14</v>
@@ -4983,25 +5073,25 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B87" t="s">
+        <v>393</v>
+      </c>
+      <c r="C87" t="s">
+        <v>393</v>
+      </c>
+      <c r="D87" t="s">
+        <v>394</v>
+      </c>
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
         <v>396</v>
       </c>
-      <c r="C87" t="s">
-        <v>396</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>397</v>
-      </c>
-      <c r="E87" t="s">
-        <v>19</v>
-      </c>
-      <c r="F87" t="s">
-        <v>399</v>
-      </c>
-      <c r="G87" t="s">
-        <v>400</v>
       </c>
       <c r="H87">
         <v>2</v>
@@ -5016,7 +5106,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B88" t="s">
         <v>224</v>
@@ -5049,7 +5139,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B89" t="s">
         <v>228</v>
@@ -5094,13 +5184,13 @@
         <v>256</v>
       </c>
       <c r="E90" t="s">
+        <v>401</v>
+      </c>
+      <c r="F90" t="s">
         <v>404</v>
       </c>
-      <c r="F90" t="s">
-        <v>407</v>
-      </c>
       <c r="G90" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -5283,22 +5373,22 @@
         <v>257</v>
       </c>
       <c r="B96" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C96" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D96" t="s">
+        <v>400</v>
+      </c>
+      <c r="E96" t="s">
+        <v>401</v>
+      </c>
+      <c r="F96" t="s">
+        <v>402</v>
+      </c>
+      <c r="G96" t="s">
         <v>403</v>
-      </c>
-      <c r="E96" t="s">
-        <v>404</v>
-      </c>
-      <c r="F96" t="s">
-        <v>405</v>
-      </c>
-      <c r="G96" t="s">
-        <v>406</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -5313,25 +5403,25 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B97" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C97" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D97" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E97" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F97" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="G97" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H97">
         <v>5</v>
@@ -5412,13 +5502,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B100" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C100" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D100" t="s">
         <v>272</v>
@@ -5427,10 +5517,10 @@
         <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G100" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -5445,25 +5535,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B101" t="s">
+        <v>349</v>
+      </c>
+      <c r="C101" t="s">
+        <v>349</v>
+      </c>
+      <c r="D101" t="s">
         <v>351</v>
       </c>
-      <c r="C101" t="s">
-        <v>351</v>
-      </c>
-      <c r="D101" t="s">
-        <v>353</v>
-      </c>
       <c r="E101" t="s">
         <v>19</v>
       </c>
       <c r="F101" t="s">
+        <v>350</v>
+      </c>
+      <c r="G101" t="s">
         <v>352</v>
-      </c>
-      <c r="G101" t="s">
-        <v>354</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -5478,25 +5568,25 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>431</v>
+      </c>
+      <c r="B102" t="s">
+        <v>433</v>
+      </c>
+      <c r="C102" t="s">
+        <v>433</v>
+      </c>
+      <c r="D102" t="s">
+        <v>432</v>
+      </c>
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
         <v>434</v>
       </c>
-      <c r="B102" t="s">
-        <v>436</v>
-      </c>
-      <c r="C102" t="s">
-        <v>436</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="G102" t="s">
         <v>435</v>
-      </c>
-      <c r="E102" t="s">
-        <v>19</v>
-      </c>
-      <c r="F102" t="s">
-        <v>437</v>
-      </c>
-      <c r="G102" t="s">
-        <v>438</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -5511,13 +5601,13 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B103" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C103" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D103" t="s">
         <v>256</v>
@@ -5526,10 +5616,10 @@
         <v>19</v>
       </c>
       <c r="F103" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G103" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H103">
         <v>1</v>
@@ -5544,25 +5634,25 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>437</v>
+      </c>
+      <c r="B104" t="s">
+        <v>438</v>
+      </c>
+      <c r="C104" t="s">
+        <v>438</v>
+      </c>
+      <c r="D104" t="s">
+        <v>439</v>
+      </c>
+      <c r="E104" t="s">
+        <v>401</v>
+      </c>
+      <c r="F104" t="s">
         <v>440</v>
       </c>
-      <c r="B104" t="s">
-        <v>441</v>
-      </c>
-      <c r="C104" t="s">
-        <v>441</v>
-      </c>
-      <c r="D104" t="s">
-        <v>442</v>
-      </c>
-      <c r="E104" t="s">
-        <v>404</v>
-      </c>
-      <c r="F104" t="s">
-        <v>443</v>
-      </c>
       <c r="G104" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H104">
         <v>1</v>
@@ -5577,7 +5667,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B105" t="s">
         <v>273</v>
@@ -5589,10 +5679,10 @@
         <v>274</v>
       </c>
       <c r="E105" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F105" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="G105" t="s">
         <v>276</v>
@@ -5643,25 +5733,25 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B107" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C107" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D107" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E107" t="s">
         <v>275</v>
       </c>
       <c r="F107" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G107" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H107">
         <v>2</v>
@@ -5682,19 +5772,19 @@
         <v>283</v>
       </c>
       <c r="C108" t="s">
+        <v>387</v>
+      </c>
+      <c r="D108" t="s">
+        <v>388</v>
+      </c>
+      <c r="E108" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" t="s">
+        <v>389</v>
+      </c>
+      <c r="G108" t="s">
         <v>390</v>
-      </c>
-      <c r="D108" t="s">
-        <v>391</v>
-      </c>
-      <c r="E108" t="s">
-        <v>19</v>
-      </c>
-      <c r="F108" t="s">
-        <v>392</v>
-      </c>
-      <c r="G108" t="s">
-        <v>393</v>
       </c>
       <c r="H108">
         <v>1</v>

</xml_diff>

<commit_message>
Reverting the addition of the NCP699 regulator.
The FTDI debugger like the XDK uses is a much better option than
an XS-1 based XTAG. It's a single QFP48 chip that costs as much as the
XS1-64QFP would have cost alone.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/BOM-byvalue.xlsx
+++ b/Documentation/BOM-byvalue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6960"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-byvalue" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="472">
   <si>
     <t>Part</t>
   </si>
@@ -1387,39 +1387,6 @@
     <t>JP20, JP21</t>
   </si>
   <si>
-    <t>NCP699</t>
-  </si>
-  <si>
-    <t>NCP699SN18T1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>NCP699SN18T1G</t>
-  </si>
-  <si>
-    <t>C91</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>445-3451-1-ND</t>
-  </si>
-  <si>
-    <t>C1608Y5V1C225Z</t>
-  </si>
-  <si>
-    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C86, C87, C88, C89, C90</t>
-  </si>
-  <si>
-    <t>R10, R20, R139, R140, R141, R142, R143</t>
-  </si>
-  <si>
-    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7</t>
-  </si>
-  <si>
-    <t>U18</t>
-  </si>
-  <si>
     <t>445-4979-1-ND</t>
   </si>
   <si>
@@ -1454,6 +1421,15 @@
   </si>
   <si>
     <t>ERJ-2GEJ472X</t>
+  </si>
+  <si>
+    <t>C3, C4, C11, C12, C13, C14, C21, C22, C23, C25, C28, C30, C33, C38, C39, C40, C41, C42, C45, C48, C49, C55, C56, C86, C87, C88, C89</t>
+  </si>
+  <si>
+    <t>R10, R139, R140, R141, R142, R143</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6</t>
   </si>
 </sst>
 </file>
@@ -2282,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2315,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2354,10 +2330,10 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="G2" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2370,8 +2346,8 @@
         <v>0.54</v>
       </c>
       <c r="K2">
-        <f>SUM(J2:J134)</f>
-        <v>207.679</v>
+        <f>SUM(J2:J132)</f>
+        <v>206.798</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2403,13 +2379,13 @@
         <v>0.54</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J77" si="0">H3*I3</f>
+        <f t="shared" ref="J3:J76" si="0">H3*I3</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2430,14 +2406,14 @@
         <v>304</v>
       </c>
       <c r="H4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.60899999999999999</v>
+        <v>0.58800000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2524,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3099,46 +3075,46 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>460</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>461</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>462</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>463</v>
+        <v>65</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="I26">
-        <v>0.24</v>
+        <v>0.315</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
         <v>66</v>
@@ -3147,61 +3123,64 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>299</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>300</v>
       </c>
       <c r="H27">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="I27">
-        <v>0.315</v>
+        <v>0.35</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>8.19</v>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>299</v>
+        <v>335</v>
       </c>
       <c r="G28" t="s">
-        <v>300</v>
+        <v>336</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>0.4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
         <v>72</v>
@@ -3213,31 +3192,28 @@
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G29" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0.4</v>
+        <v>0.68</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L29" t="s">
-        <v>341</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>72</v>
@@ -3249,190 +3225,187 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G30" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <v>0.68</v>
+        <v>0.42</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>333</v>
+        <v>284</v>
       </c>
       <c r="G31" t="s">
-        <v>334</v>
+        <v>285</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31">
-        <v>0.42</v>
+        <v>11.91</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>35.730000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>421</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>364</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>365</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>366</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>284</v>
+        <v>367</v>
       </c>
       <c r="G32" t="s">
-        <v>285</v>
+        <v>368</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>11.91</v>
+        <v>0.44</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>35.730000000000004</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>421</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="C33" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="D33" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="G33" t="s">
-        <v>368</v>
+        <v>343</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>0.44</v>
+        <v>2.15</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>343</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>343</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>343</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>342</v>
+        <v>84</v>
       </c>
       <c r="G34" t="s">
-        <v>343</v>
+        <v>83</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>2.15</v>
+        <v>0.77</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>2.15</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>338</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>275</v>
       </c>
       <c r="F35" t="s">
-        <v>84</v>
-      </c>
-      <c r="G35" t="s">
-        <v>83</v>
+        <v>340</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>0.77</v>
+        <v>0.5</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>2.31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B36" t="s">
         <v>85</v>
@@ -3447,7 +3420,10 @@
         <v>275</v>
       </c>
       <c r="F36" t="s">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="G36" t="s">
+        <v>14</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3462,541 +3438,541 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>337</v>
+        <v>455</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>86</v>
+        <v>360</v>
       </c>
       <c r="E37" t="s">
-        <v>275</v>
+        <v>19</v>
       </c>
       <c r="F37" t="s">
-        <v>339</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>0.5</v>
+        <v>0.93</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>455</v>
+        <v>414</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>360</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>297</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>298</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I38">
-        <v>0.93</v>
+        <v>1.47</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>0.93</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" t="s">
-        <v>297</v>
+        <v>94</v>
       </c>
       <c r="G39" t="s">
-        <v>298</v>
+        <v>95</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I39">
-        <v>1.47</v>
+        <v>0.42</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>4.41</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>430</v>
-      </c>
-      <c r="B40" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>422</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>423</v>
       </c>
       <c r="E40" t="s">
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" t="s">
-        <v>95</v>
+        <v>424</v>
+      </c>
+      <c r="G40">
+        <v>702461004</v>
       </c>
       <c r="H40">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>0.42</v>
+        <v>1.64</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>5.46</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>456</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>422</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>423</v>
+        <v>98</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>424</v>
-      </c>
-      <c r="G41">
-        <v>702461004</v>
+        <v>357</v>
+      </c>
+      <c r="G41" t="s">
+        <v>358</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41">
-        <v>1.64</v>
+        <v>0.13</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>1.64</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>456</v>
-      </c>
-      <c r="B42" t="s">
-        <v>14</v>
+        <v>359</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>353</v>
       </c>
       <c r="D42" t="s">
-        <v>98</v>
+        <v>354</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G42" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0.13</v>
+        <v>0.71</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C43" t="s">
-        <v>353</v>
+        <v>451</v>
       </c>
       <c r="D43" t="s">
-        <v>354</v>
+        <v>452</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>355</v>
+        <v>454</v>
       </c>
       <c r="G43" t="s">
-        <v>356</v>
+        <v>453</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>0.71</v>
+        <v>1.58</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>361</v>
+        <v>415</v>
       </c>
       <c r="C44" t="s">
-        <v>451</v>
+        <v>416</v>
       </c>
       <c r="D44" t="s">
-        <v>452</v>
+        <v>417</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>454</v>
+        <v>418</v>
       </c>
       <c r="G44" t="s">
-        <v>453</v>
+        <v>419</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <v>1.58</v>
+        <v>1.67</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>1.58</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C45" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D45" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="G45" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I45">
-        <v>1.67</v>
+        <v>0.5</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>409</v>
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>410</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
-        <v>411</v>
+        <v>102</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>412</v>
+        <v>103</v>
       </c>
       <c r="G46" t="s">
-        <v>413</v>
+        <v>104</v>
       </c>
       <c r="H46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>0.5</v>
+        <v>2.13</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="G47" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>2.13</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="G48" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D49" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G49" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>471</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D50" t="s">
-        <v>120</v>
-      </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G50" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50">
-        <v>1.85</v>
+        <v>6</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>1.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>443</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>441</v>
       </c>
       <c r="H51">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0.55000000000000004</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>442</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
         <v>128</v>
       </c>
       <c r="C52" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D52" t="s">
-        <v>126</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" t="s">
-        <v>443</v>
+        <v>130</v>
       </c>
       <c r="G52" t="s">
-        <v>441</v>
+        <v>14</v>
       </c>
       <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>0.55000000000000004</v>
+        <v>3</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>362</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D53" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>132</v>
       </c>
       <c r="G53" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0.41</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
         <v>126</v>
@@ -4005,61 +3981,61 @@
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G54" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>363</v>
+        <v>138</v>
       </c>
       <c r="B55" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>136</v>
+        <v>286</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>287</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
         <v>140</v>
@@ -4071,28 +4047,28 @@
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>286</v>
+        <v>144</v>
       </c>
       <c r="G56" t="s">
-        <v>287</v>
+        <v>145</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>142</v>
-      </c>
-      <c r="B57" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="B57">
+        <v>470</v>
       </c>
       <c r="C57" t="s">
         <v>140</v>
@@ -4104,10 +4080,10 @@
         <v>19</v>
       </c>
       <c r="F57" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4122,109 +4098,109 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>146</v>
-      </c>
-      <c r="B58">
-        <v>470</v>
+        <v>449</v>
+      </c>
+      <c r="B58" t="s">
+        <v>176</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D58" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>147</v>
+        <v>461</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
+        <v>462</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58">
         <v>0.04</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="C59" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D59" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
       </c>
       <c r="F59" t="s">
-        <v>472</v>
+        <v>150</v>
       </c>
       <c r="G59" t="s">
-        <v>473</v>
+        <v>151</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I59">
         <v>0.04</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>448</v>
-      </c>
-      <c r="B60" t="s">
-        <v>149</v>
+        <v>447</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>150</v>
+        <v>463</v>
       </c>
       <c r="G60" t="s">
-        <v>151</v>
+        <v>464</v>
       </c>
       <c r="H60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I60">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>447</v>
-      </c>
-      <c r="B61">
-        <v>10</v>
+        <v>450</v>
+      </c>
+      <c r="B61" t="s">
+        <v>153</v>
       </c>
       <c r="C61" t="s">
         <v>192</v>
@@ -4236,28 +4212,28 @@
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="G61" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="H61">
         <v>4</v>
       </c>
       <c r="I61">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C62" t="s">
         <v>192</v>
@@ -4269,127 +4245,127 @@
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="G62" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="H62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I62">
         <v>0.05</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>444</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D63" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
       </c>
       <c r="F63" t="s">
-        <v>478</v>
+        <v>154</v>
       </c>
       <c r="G63" t="s">
-        <v>479</v>
+        <v>155</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I63">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>152</v>
-      </c>
-      <c r="B64" t="s">
-        <v>153</v>
+        <v>445</v>
+      </c>
+      <c r="B64">
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>154</v>
+        <v>375</v>
       </c>
       <c r="G64" t="s">
-        <v>155</v>
+        <v>376</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I64">
         <v>0.04</v>
       </c>
       <c r="J64">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>H64*I64</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>445</v>
-      </c>
-      <c r="B65">
-        <v>100</v>
+        <v>156</v>
+      </c>
+      <c r="B65" t="s">
+        <v>157</v>
       </c>
       <c r="C65" t="s">
-        <v>192</v>
+        <v>288</v>
       </c>
       <c r="D65" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
       </c>
       <c r="F65" t="s">
-        <v>375</v>
+        <v>289</v>
       </c>
       <c r="G65" t="s">
-        <v>376</v>
+        <v>290</v>
       </c>
       <c r="H65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I65">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J65">
-        <f>H65*I65</f>
-        <v>0.2</v>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
         <v>288</v>
@@ -4401,10 +4377,10 @@
         <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="G66" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4419,109 +4395,109 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C67" t="s">
-        <v>288</v>
+        <v>140</v>
       </c>
       <c r="D67" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
       </c>
       <c r="F67" t="s">
-        <v>295</v>
+        <v>162</v>
       </c>
       <c r="G67" t="s">
-        <v>296</v>
+        <v>163</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>160</v>
-      </c>
-      <c r="B68" t="s">
-        <v>161</v>
+        <v>164</v>
+      </c>
+      <c r="B68">
+        <v>200</v>
       </c>
       <c r="C68" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>162</v>
+        <v>372</v>
       </c>
       <c r="G68" t="s">
-        <v>163</v>
+        <v>373</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I68">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>164</v>
+        <v>374</v>
       </c>
       <c r="B69">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C69" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D69" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>372</v>
+        <v>165</v>
       </c>
       <c r="G69" t="s">
-        <v>373</v>
+        <v>166</v>
       </c>
       <c r="H69">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>374</v>
-      </c>
-      <c r="B70">
-        <v>100</v>
+        <v>167</v>
+      </c>
+      <c r="B70" t="s">
+        <v>168</v>
       </c>
       <c r="C70" t="s">
         <v>140</v>
@@ -4533,28 +4509,28 @@
         <v>19</v>
       </c>
       <c r="F70" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G70" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H70">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I70">
         <v>0.04</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B71" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C71" t="s">
         <v>140</v>
@@ -4566,28 +4542,28 @@
         <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G71" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="H71">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I71">
         <v>0.04</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B72" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C72" t="s">
         <v>140</v>
@@ -4599,28 +4575,28 @@
         <v>19</v>
       </c>
       <c r="F72" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G72" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H72">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I72">
         <v>0.04</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C73" t="s">
         <v>140</v>
@@ -4632,28 +4608,28 @@
         <v>19</v>
       </c>
       <c r="F73" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G73" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I73">
         <v>0.04</v>
       </c>
       <c r="J73">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B74" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C74" t="s">
         <v>140</v>
@@ -4665,28 +4641,28 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G74" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H74">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I74">
         <v>0.04</v>
       </c>
       <c r="J74">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B75" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C75" t="s">
         <v>140</v>
@@ -4698,10 +4674,10 @@
         <v>19</v>
       </c>
       <c r="F75" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G75" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4716,76 +4692,76 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>187</v>
-      </c>
-      <c r="B76" t="s">
-        <v>188</v>
+        <v>191</v>
+      </c>
+      <c r="B76">
+        <v>0.3</v>
       </c>
       <c r="C76" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D76" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
       </c>
       <c r="F76" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G76" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
       <c r="J76">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>191</v>
-      </c>
-      <c r="B77">
-        <v>0.3</v>
+        <v>196</v>
+      </c>
+      <c r="B77" t="s">
+        <v>197</v>
       </c>
       <c r="C77" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="D77" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G77" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>0.59</v>
+        <v>0.04</v>
       </c>
       <c r="J77">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" ref="J77:J106" si="1">H77*I77</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C78" t="s">
         <v>140</v>
@@ -4797,10 +4773,10 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G78" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -4809,16 +4785,16 @@
         <v>0.04</v>
       </c>
       <c r="J78">
-        <f t="shared" ref="J78:J108" si="1">H78*I78</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B79" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C79" t="s">
         <v>140</v>
@@ -4830,10 +4806,10 @@
         <v>19</v>
       </c>
       <c r="F79" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="G79" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -4848,10 +4824,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>204</v>
+        <v>470</v>
       </c>
       <c r="B80" t="s">
-        <v>205</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
         <v>140</v>
@@ -4862,29 +4838,23 @@
       <c r="E80" t="s">
         <v>19</v>
       </c>
-      <c r="F80" t="s">
-        <v>206</v>
-      </c>
       <c r="G80" t="s">
-        <v>207</v>
+        <v>14</v>
       </c>
       <c r="H80">
-        <v>1</v>
-      </c>
-      <c r="I80">
-        <v>0.04</v>
+        <v>6</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>465</v>
+        <v>208</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="C81" t="s">
         <v>140</v>
@@ -4895,56 +4865,62 @@
       <c r="E81" t="s">
         <v>19</v>
       </c>
+      <c r="F81" t="s">
+        <v>210</v>
+      </c>
       <c r="G81" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="H81">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>0.04</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B82" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C82" t="s">
-        <v>140</v>
+        <v>288</v>
       </c>
       <c r="D82" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="G82" t="s">
-        <v>211</v>
+        <v>292</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B83" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C83" t="s">
         <v>288</v>
@@ -4956,10 +4932,10 @@
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G83" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4974,43 +4950,43 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C84" t="s">
-        <v>288</v>
+        <v>140</v>
       </c>
       <c r="D84" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
       </c>
       <c r="F84" t="s">
-        <v>293</v>
+        <v>218</v>
       </c>
       <c r="G84" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B85" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C85" t="s">
         <v>140</v>
@@ -5022,10 +4998,10 @@
         <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G85" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -5040,759 +5016,693 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>220</v>
+        <v>395</v>
       </c>
       <c r="B86" t="s">
-        <v>221</v>
+        <v>393</v>
       </c>
       <c r="C86" t="s">
-        <v>140</v>
+        <v>393</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>394</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
       </c>
       <c r="F86" t="s">
-        <v>222</v>
+        <v>396</v>
       </c>
       <c r="G86" t="s">
-        <v>223</v>
+        <v>397</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I86">
-        <v>0.04</v>
+        <v>15.1</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B87" t="s">
-        <v>393</v>
+        <v>224</v>
       </c>
       <c r="C87" t="s">
-        <v>393</v>
+        <v>224</v>
       </c>
       <c r="D87" t="s">
-        <v>394</v>
+        <v>225</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>396</v>
+        <v>226</v>
       </c>
       <c r="G87" t="s">
-        <v>397</v>
+        <v>227</v>
       </c>
       <c r="H87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I87">
-        <v>15.1</v>
+        <v>6.6</v>
       </c>
       <c r="J87">
-        <f t="shared" si="1"/>
-        <v>30.2</v>
+        <f t="shared" ref="J87:J96" si="2">H87*I87</f>
+        <v>6.6</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B88" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D88" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="G88" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>6.6</v>
+        <v>0.79</v>
       </c>
       <c r="J88">
-        <f t="shared" ref="J88:J97" si="2">H88*I88</f>
-        <v>6.6</v>
+        <f t="shared" si="2"/>
+        <v>0.79</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>399</v>
+        <v>233</v>
       </c>
       <c r="B89" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
       <c r="C89" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="D89" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="E89" t="s">
-        <v>19</v>
+        <v>401</v>
       </c>
       <c r="F89" t="s">
-        <v>231</v>
+        <v>404</v>
       </c>
       <c r="G89" t="s">
-        <v>232</v>
+        <v>405</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B90" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C90" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D90" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E90" t="s">
-        <v>401</v>
+        <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>404</v>
+        <v>260</v>
       </c>
       <c r="G90" t="s">
-        <v>405</v>
+        <v>261</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B91" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="C91" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="D91" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
       </c>
       <c r="F91" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="G91" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>0.47</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B92" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C92" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D92" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="G92" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>0.67</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B93" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C93" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="D93" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="G93" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="H93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
       <c r="J93">
         <f t="shared" si="2"/>
-        <v>6.63</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B94" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C94" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D94" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G94" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
       <c r="J94">
         <f t="shared" si="2"/>
-        <v>1.67</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B95" t="s">
-        <v>249</v>
+        <v>392</v>
       </c>
       <c r="C95" t="s">
-        <v>249</v>
+        <v>392</v>
       </c>
       <c r="D95" t="s">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="E95" t="s">
-        <v>19</v>
+        <v>401</v>
       </c>
       <c r="F95" t="s">
-        <v>251</v>
+        <v>402</v>
       </c>
       <c r="G95" t="s">
-        <v>252</v>
+        <v>403</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
       <c r="J95">
         <f t="shared" si="2"/>
-        <v>5.88</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>257</v>
+        <v>420</v>
       </c>
       <c r="B96" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C96" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D96" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="E96" t="s">
         <v>401</v>
       </c>
       <c r="F96" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="G96" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I96">
-        <v>1.23</v>
+        <v>2.76</v>
       </c>
       <c r="J96">
         <f t="shared" si="2"/>
-        <v>1.23</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>420</v>
+        <v>266</v>
       </c>
       <c r="B97" t="s">
-        <v>391</v>
+        <v>262</v>
       </c>
       <c r="C97" t="s">
-        <v>391</v>
+        <v>262</v>
       </c>
       <c r="D97" t="s">
-        <v>406</v>
+        <v>263</v>
       </c>
       <c r="E97" t="s">
-        <v>401</v>
+        <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>407</v>
+        <v>264</v>
       </c>
       <c r="G97" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
       <c r="H97">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>2.76</v>
+        <v>3.79</v>
       </c>
       <c r="J97">
-        <f t="shared" si="2"/>
-        <v>13.799999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3.79</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B98" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C98" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D98" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="G98" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
       <c r="J98">
         <f t="shared" si="1"/>
-        <v>3.79</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>271</v>
+        <v>348</v>
       </c>
       <c r="B99" t="s">
-        <v>267</v>
+        <v>369</v>
       </c>
       <c r="C99" t="s">
-        <v>267</v>
+        <v>369</v>
       </c>
       <c r="D99" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
       </c>
       <c r="F99" t="s">
-        <v>269</v>
+        <v>370</v>
       </c>
       <c r="G99" t="s">
-        <v>270</v>
+        <v>371</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99">
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
       <c r="J99">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>348</v>
+        <v>386</v>
       </c>
       <c r="B100" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="C100" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="D100" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="G100" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100">
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
       <c r="J100">
         <f t="shared" si="1"/>
-        <v>8.48</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>386</v>
+        <v>431</v>
       </c>
       <c r="B101" t="s">
-        <v>349</v>
+        <v>433</v>
       </c>
       <c r="C101" t="s">
-        <v>349</v>
+        <v>433</v>
       </c>
       <c r="D101" t="s">
-        <v>351</v>
+        <v>432</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
       </c>
       <c r="F101" t="s">
-        <v>350</v>
+        <v>434</v>
       </c>
       <c r="G101" t="s">
-        <v>352</v>
+        <v>435</v>
       </c>
       <c r="H101">
         <v>1</v>
       </c>
       <c r="I101">
-        <v>6.84</v>
+        <v>3.15</v>
       </c>
       <c r="J101">
         <f t="shared" si="1"/>
-        <v>6.84</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="B102" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="C102" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="D102" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="E102" t="s">
-        <v>19</v>
+        <v>401</v>
       </c>
       <c r="F102" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="G102" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="H102">
         <v>1</v>
       </c>
       <c r="I102">
-        <v>3.15</v>
+        <v>5.71</v>
       </c>
       <c r="J102">
         <f t="shared" si="1"/>
-        <v>3.15</v>
+        <v>5.71</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="B103" t="s">
-        <v>457</v>
+        <v>273</v>
       </c>
       <c r="C103" t="s">
-        <v>457</v>
+        <v>273</v>
       </c>
       <c r="D103" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r=